<commit_message>
Ghillie Tarnwirkung ggü. Zombies, Quest Update, Mod Liste angepasst
</commit_message>
<xml_diff>
--- a/ressources/DayZ Mods.xlsx
+++ b/ressources/DayZ Mods.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\projects\Immersive-DayZ-Experience\ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D780B5-E33E-44D0-AC39-C5B8F412BCCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB00993-D91E-473A-A17C-30768229314C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="260" activeTab="1" xr2:uid="{FAEB3C3F-74B0-4C80-8C8B-4522341FA132}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="260" xr2:uid="{FAEB3C3F-74B0-4C80-8C8B-4522341FA132}"/>
   </bookViews>
   <sheets>
     <sheet name="Mods" sheetId="1" r:id="rId1"/>
@@ -564,7 +564,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2219" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2226" uniqueCount="654">
   <si>
     <t>Community Frameworks</t>
   </si>
@@ -3470,7 +3470,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="191">
+  <cellXfs count="196">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3783,111 +3783,10 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="44" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3917,6 +3816,122 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4708,9 +4723,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BE2B301-FC9E-4F7D-A454-62A8C1115EDF}">
   <dimension ref="A1:Q87"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T66" sqref="T66"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6758,15 +6773,36 @@
       </c>
     </row>
     <row r="58" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="93"/>
-      <c r="C58" s="85"/>
-      <c r="D58" s="38"/>
-      <c r="E58" s="89"/>
-      <c r="F58" s="87"/>
-      <c r="G58" s="38"/>
-      <c r="H58" s="38"/>
-      <c r="I58" s="38"/>
-      <c r="J58" s="38"/>
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" s="93">
+        <v>3108865421</v>
+      </c>
+      <c r="C58" s="85" t="s">
+        <v>615</v>
+      </c>
+      <c r="D58" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" s="89" t="s">
+        <v>616</v>
+      </c>
+      <c r="F58" s="87" t="s">
+        <v>8</v>
+      </c>
+      <c r="G58" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="H58" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="I58" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="J58" s="38" t="s">
+        <v>8</v>
+      </c>
       <c r="K58" s="38"/>
       <c r="L58" s="38"/>
     </row>
@@ -6775,102 +6811,102 @@
         <v>58</v>
       </c>
       <c r="B59" s="93">
-        <v>3108865421</v>
+        <v>1828439124</v>
       </c>
       <c r="C59" s="85" t="s">
-        <v>615</v>
-      </c>
-      <c r="D59" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="E59" s="89" t="s">
-        <v>616</v>
-      </c>
+        <v>617</v>
+      </c>
+      <c r="D59" s="38"/>
+      <c r="E59" s="89"/>
       <c r="F59" s="87" t="s">
         <v>8</v>
       </c>
       <c r="G59" s="38" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="H59" s="38" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="I59" s="38" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="J59" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="K59" s="38"/>
-      <c r="L59" s="38"/>
+        <v>36</v>
+      </c>
+      <c r="K59" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="L59" s="38" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="60" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" s="93">
-        <v>1828439124</v>
+        <v>1991570984</v>
       </c>
       <c r="C60" s="85" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="D60" s="38"/>
       <c r="E60" s="89"/>
       <c r="F60" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="G60" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="H60" s="38" t="s">
-        <v>36</v>
-      </c>
+      <c r="G60" s="5"/>
+      <c r="H60" s="5"/>
       <c r="I60" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="J60" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="K60" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="L60" s="38" t="s">
-        <v>36</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="J60" s="5"/>
+      <c r="K60" s="5"/>
+      <c r="L60" s="5"/>
     </row>
     <row r="61" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" s="93">
-        <v>1991570984</v>
+        <v>3171576913</v>
       </c>
       <c r="C61" s="85" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D61" s="38"/>
       <c r="E61" s="89"/>
       <c r="F61" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="G61" s="5"/>
-      <c r="H61" s="5"/>
+      <c r="G61" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="H61" s="38" t="s">
+        <v>36</v>
+      </c>
       <c r="I61" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="J61" s="5"/>
-      <c r="K61" s="5"/>
-      <c r="L61" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="J61" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="K61" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="L61" s="38" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="62" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" s="93">
-        <v>3171576913</v>
+        <v>2111523728</v>
       </c>
       <c r="C62" s="85" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="D62" s="38"/>
       <c r="E62" s="89"/>
@@ -6901,10 +6937,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="93">
-        <v>2111523728</v>
+        <v>2472500243</v>
       </c>
       <c r="C63" s="85" t="s">
-        <v>620</v>
+        <v>634</v>
       </c>
       <c r="D63" s="38"/>
       <c r="E63" s="89"/>
@@ -6935,10 +6971,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="93">
-        <v>2472500243</v>
+        <v>2224593910</v>
       </c>
       <c r="C64" s="85" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="D64" s="38"/>
       <c r="E64" s="89"/>
@@ -6969,55 +7005,41 @@
         <v>64</v>
       </c>
       <c r="B65" s="93">
-        <v>2224593910</v>
+        <v>1832448183</v>
       </c>
       <c r="C65" s="85" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="D65" s="38"/>
       <c r="E65" s="89"/>
-      <c r="F65" s="87" t="s">
-        <v>8</v>
-      </c>
+      <c r="F65" s="87"/>
       <c r="G65" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="H65" s="38" t="s">
-        <v>36</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="H65" s="38"/>
       <c r="I65" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="J65" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="K65" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="L65" s="38" t="s">
-        <v>36</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="J65" s="38"/>
+      <c r="K65" s="38"/>
+      <c r="L65" s="38"/>
     </row>
     <row r="66" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66" s="93">
-        <v>1832448183</v>
+        <v>1895432270</v>
       </c>
       <c r="C66" s="85" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="D66" s="38"/>
       <c r="E66" s="89"/>
       <c r="F66" s="87"/>
-      <c r="G66" s="38" t="s">
-        <v>8</v>
-      </c>
+      <c r="G66" s="38"/>
       <c r="H66" s="38"/>
-      <c r="I66" s="38" t="s">
-        <v>8</v>
-      </c>
+      <c r="I66" s="38"/>
       <c r="J66" s="38"/>
       <c r="K66" s="38"/>
       <c r="L66" s="38"/>
@@ -7027,10 +7049,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="93">
-        <v>1895432270</v>
+        <v>2912241382</v>
       </c>
       <c r="C67" s="85" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="D67" s="38"/>
       <c r="E67" s="89"/>
@@ -7047,10 +7069,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="93">
-        <v>2912241382</v>
+        <v>2307297070</v>
       </c>
       <c r="C68" s="85" t="s">
-        <v>638</v>
+        <v>644</v>
       </c>
       <c r="D68" s="38"/>
       <c r="E68" s="89"/>
@@ -7063,11 +7085,14 @@
       <c r="L68" s="38"/>
     </row>
     <row r="69" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
       <c r="B69" s="93">
-        <v>2307297070</v>
+        <v>1710977250</v>
       </c>
       <c r="C69" s="85" t="s">
-        <v>644</v>
+        <v>639</v>
       </c>
       <c r="D69" s="38"/>
       <c r="E69" s="89"/>
@@ -7079,12 +7104,15 @@
       <c r="K69" s="38"/>
       <c r="L69" s="38"/>
     </row>
-    <row r="70" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
       <c r="B70" s="93">
-        <v>1710977250</v>
+        <v>2895049000</v>
       </c>
       <c r="C70" s="85" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="D70" s="38"/>
       <c r="E70" s="89"/>
@@ -7096,12 +7124,15 @@
       <c r="K70" s="38"/>
       <c r="L70" s="38"/>
     </row>
-    <row r="71" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
       <c r="B71" s="93">
-        <v>2895049000</v>
+        <v>2651195301</v>
       </c>
       <c r="C71" s="85" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="D71" s="38"/>
       <c r="E71" s="89"/>
@@ -7114,11 +7145,14 @@
       <c r="L71" s="38"/>
     </row>
     <row r="72" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
       <c r="B72" s="93">
-        <v>2651195301</v>
+        <v>2874589934</v>
       </c>
       <c r="C72" s="85" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="D72" s="38"/>
       <c r="E72" s="89"/>
@@ -7131,11 +7165,14 @@
       <c r="L72" s="38"/>
     </row>
     <row r="73" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
       <c r="B73" s="93">
-        <v>2874589934</v>
+        <v>3119592638</v>
       </c>
       <c r="C73" s="85" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="D73" s="38"/>
       <c r="E73" s="89"/>
@@ -7148,50 +7185,46 @@
       <c r="L73" s="38"/>
     </row>
     <row r="74" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="93">
-        <v>3119592638</v>
-      </c>
-      <c r="C74" s="85" t="s">
-        <v>643</v>
-      </c>
-      <c r="D74" s="38"/>
-      <c r="E74" s="89"/>
-      <c r="F74" s="87"/>
-      <c r="G74" s="38"/>
-      <c r="H74" s="38"/>
-      <c r="I74" s="38"/>
-      <c r="J74" s="38"/>
-      <c r="K74" s="38"/>
-      <c r="L74" s="38"/>
+      <c r="B74" s="191"/>
+      <c r="C74" s="192"/>
+      <c r="D74" s="193"/>
+      <c r="E74" s="194"/>
+      <c r="F74" s="195"/>
+      <c r="G74" s="193"/>
+      <c r="H74" s="193"/>
+      <c r="I74" s="193"/>
+      <c r="J74" s="193"/>
+      <c r="K74" s="193"/>
+      <c r="L74" s="193"/>
     </row>
     <row r="76" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="92">
+      <c r="B76" s="117">
         <v>2856976851</v>
       </c>
-      <c r="C76" s="84" t="s">
+      <c r="C76" s="113" t="s">
         <v>22</v>
       </c>
-      <c r="D76" s="38" t="s">
+      <c r="D76" s="114" t="s">
         <v>9</v>
       </c>
-      <c r="E76" s="89"/>
-      <c r="F76" s="87" t="s">
-        <v>8</v>
-      </c>
-      <c r="G76" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="H76" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="I76" s="38"/>
-      <c r="J76" s="91" t="s">
-        <v>8</v>
-      </c>
-      <c r="K76" s="91" t="s">
-        <v>8</v>
-      </c>
-      <c r="L76" s="5"/>
+      <c r="E76" s="115"/>
+      <c r="F76" s="116" t="s">
+        <v>8</v>
+      </c>
+      <c r="G76" s="114" t="s">
+        <v>8</v>
+      </c>
+      <c r="H76" s="114" t="s">
+        <v>8</v>
+      </c>
+      <c r="I76" s="114"/>
+      <c r="J76" s="118" t="s">
+        <v>8</v>
+      </c>
+      <c r="K76" s="114" t="s">
+        <v>8</v>
+      </c>
+      <c r="L76" s="119"/>
     </row>
     <row r="77" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="117">
@@ -7530,8 +7563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FF4763-6B65-4CE2-BD87-511E98A2E639}">
   <dimension ref="A1:V225"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7557,31 +7590,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="S1" s="176"/>
+      <c r="S1"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="S2" s="176"/>
+      <c r="S2"/>
     </row>
     <row r="3" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="144" t="s">
+      <c r="C3" s="156" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="144"/>
-      <c r="E3" s="144"/>
-      <c r="F3" s="144"/>
-      <c r="G3" s="144"/>
-      <c r="H3" s="144"/>
-      <c r="I3" s="144"/>
-      <c r="J3" s="144"/>
-      <c r="K3" s="144"/>
-      <c r="L3" s="144"/>
-      <c r="M3" s="144"/>
-      <c r="N3" s="144"/>
-      <c r="O3" s="144"/>
-      <c r="P3" s="144"/>
-      <c r="Q3" s="144"/>
-      <c r="R3" s="144"/>
-      <c r="S3" s="144"/>
+      <c r="D3" s="156"/>
+      <c r="E3" s="156"/>
+      <c r="F3" s="156"/>
+      <c r="G3" s="156"/>
+      <c r="H3" s="156"/>
+      <c r="I3" s="156"/>
+      <c r="J3" s="156"/>
+      <c r="K3" s="156"/>
+      <c r="L3" s="156"/>
+      <c r="M3" s="156"/>
+      <c r="N3" s="156"/>
+      <c r="O3" s="156"/>
+      <c r="P3" s="156"/>
+      <c r="Q3" s="156"/>
+      <c r="R3" s="156"/>
+      <c r="S3" s="156"/>
     </row>
     <row r="4" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
@@ -7596,19 +7629,19 @@
       <c r="F4" s="3" t="s">
         <v>653</v>
       </c>
-      <c r="G4" s="146"/>
-      <c r="H4" s="146"/>
-      <c r="I4" s="146"/>
-      <c r="J4" s="146"/>
-      <c r="K4" s="146"/>
-      <c r="L4" s="146"/>
-      <c r="M4" s="146"/>
-      <c r="N4" s="146"/>
-      <c r="O4" s="146"/>
-      <c r="P4" s="146"/>
-      <c r="Q4" s="146"/>
-      <c r="R4" s="146"/>
-      <c r="S4" s="146"/>
+      <c r="G4" s="180"/>
+      <c r="H4" s="180"/>
+      <c r="I4" s="180"/>
+      <c r="J4" s="180"/>
+      <c r="K4" s="180"/>
+      <c r="L4" s="180"/>
+      <c r="M4" s="180"/>
+      <c r="N4" s="180"/>
+      <c r="O4" s="180"/>
+      <c r="P4" s="180"/>
+      <c r="Q4" s="180"/>
+      <c r="R4" s="180"/>
+      <c r="S4" s="180"/>
     </row>
     <row r="5" spans="1:22" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="3"/>
@@ -7659,10 +7692,10 @@
       </c>
     </row>
     <row r="6" spans="1:22" s="23" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="145" t="s">
+      <c r="A6" s="179" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="147" t="s">
+      <c r="B6" s="181" t="s">
         <v>55</v>
       </c>
       <c r="C6" s="18" t="s">
@@ -7719,13 +7752,13 @@
       <c r="T6" s="19" t="s">
         <v>274</v>
       </c>
-      <c r="V6" s="171" t="s">
+      <c r="V6" s="138" t="s">
         <v>651</v>
       </c>
     </row>
     <row r="7" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="145"/>
-      <c r="B7" s="148"/>
+      <c r="A7" s="179"/>
+      <c r="B7" s="158"/>
       <c r="C7" s="60" t="s">
         <v>46</v>
       </c>
@@ -7735,7 +7768,7 @@
       <c r="E7" s="45" t="s">
         <v>458</v>
       </c>
-      <c r="F7" s="172" t="s">
+      <c r="F7" s="139" t="s">
         <v>652</v>
       </c>
       <c r="G7" s="24" t="s">
@@ -7771,13 +7804,13 @@
       <c r="S7" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="V7" s="172" t="s">
+      <c r="V7" s="139" t="s">
         <v>652</v>
       </c>
     </row>
     <row r="8" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="145"/>
-      <c r="B8" s="148"/>
+      <c r="A8" s="179"/>
+      <c r="B8" s="158"/>
       <c r="C8" s="60" t="s">
         <v>53</v>
       </c>
@@ -7787,7 +7820,7 @@
       <c r="E8" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="171" t="s">
+      <c r="F8" s="138" t="s">
         <v>651</v>
       </c>
       <c r="G8" s="24" t="s">
@@ -7821,13 +7854,13 @@
       <c r="Q8" s="41"/>
       <c r="R8" s="130"/>
       <c r="S8" s="26"/>
-      <c r="V8" s="173" t="s">
+      <c r="V8" s="140" t="s">
         <v>647</v>
       </c>
     </row>
     <row r="9" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="145"/>
-      <c r="B9" s="148"/>
+      <c r="A9" s="179"/>
+      <c r="B9" s="158"/>
       <c r="C9" s="60" t="s">
         <v>287</v>
       </c>
@@ -7837,7 +7870,7 @@
       <c r="E9" s="23" t="s">
         <v>459</v>
       </c>
-      <c r="F9" s="171" t="s">
+      <c r="F9" s="138" t="s">
         <v>651</v>
       </c>
       <c r="G9" s="24" t="s">
@@ -7873,13 +7906,13 @@
       <c r="S9" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="V9" s="175" t="s">
+      <c r="V9" s="141" t="s">
         <v>649</v>
       </c>
     </row>
     <row r="10" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="145"/>
-      <c r="B10" s="148"/>
+      <c r="A10" s="179"/>
+      <c r="B10" s="158"/>
       <c r="C10" s="60" t="s">
         <v>47</v>
       </c>
@@ -7889,7 +7922,7 @@
       <c r="E10" s="23" t="s">
         <v>460</v>
       </c>
-      <c r="F10" s="175" t="s">
+      <c r="F10" s="141" t="s">
         <v>649</v>
       </c>
       <c r="G10" s="24" t="s">
@@ -7923,13 +7956,13 @@
       <c r="Q10" s="41"/>
       <c r="R10" s="130"/>
       <c r="S10" s="26"/>
-      <c r="V10" s="174" t="s">
+      <c r="V10" s="190" t="s">
         <v>648</v>
       </c>
     </row>
     <row r="11" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="145"/>
-      <c r="B11" s="148"/>
+      <c r="A11" s="179"/>
+      <c r="B11" s="158"/>
       <c r="C11" s="60" t="s">
         <v>63</v>
       </c>
@@ -7939,7 +7972,7 @@
       <c r="E11" s="23" t="s">
         <v>461</v>
       </c>
-      <c r="F11" s="171" t="s">
+      <c r="F11" s="138" t="s">
         <v>651</v>
       </c>
       <c r="G11" s="24" t="s">
@@ -7977,8 +8010,8 @@
       </c>
     </row>
     <row r="12" spans="1:22" s="23" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="145"/>
-      <c r="B12" s="148"/>
+      <c r="A12" s="179"/>
+      <c r="B12" s="158"/>
       <c r="C12" s="60" t="s">
         <v>48</v>
       </c>
@@ -7988,7 +8021,7 @@
       <c r="E12" s="23" t="s">
         <v>462</v>
       </c>
-      <c r="F12" s="171" t="s">
+      <c r="F12" s="138" t="s">
         <v>651</v>
       </c>
       <c r="G12" s="24" t="s">
@@ -8024,8 +8057,8 @@
       <c r="S12" s="26"/>
     </row>
     <row r="13" spans="1:22" s="23" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="145"/>
-      <c r="B13" s="148"/>
+      <c r="A13" s="179"/>
+      <c r="B13" s="158"/>
       <c r="C13" s="60" t="s">
         <v>645</v>
       </c>
@@ -8035,7 +8068,7 @@
       <c r="E13" s="23" t="s">
         <v>462</v>
       </c>
-      <c r="F13" s="171" t="s">
+      <c r="F13" s="138" t="s">
         <v>651</v>
       </c>
       <c r="G13" s="24" t="s">
@@ -8059,8 +8092,8 @@
       <c r="S13" s="26"/>
     </row>
     <row r="14" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="145"/>
-      <c r="B14" s="148"/>
+      <c r="A14" s="179"/>
+      <c r="B14" s="158"/>
       <c r="C14" s="60" t="s">
         <v>49</v>
       </c>
@@ -8070,7 +8103,7 @@
       <c r="E14" s="23" t="s">
         <v>463</v>
       </c>
-      <c r="F14" s="175" t="s">
+      <c r="F14" s="141" t="s">
         <v>649</v>
       </c>
       <c r="G14" s="24" t="s">
@@ -8106,8 +8139,8 @@
       <c r="S14" s="26"/>
     </row>
     <row r="15" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="145"/>
-      <c r="B15" s="148"/>
+      <c r="A15" s="179"/>
+      <c r="B15" s="158"/>
       <c r="C15" s="60" t="s">
         <v>78</v>
       </c>
@@ -8117,7 +8150,7 @@
       <c r="E15" s="23" t="s">
         <v>464</v>
       </c>
-      <c r="F15" s="175" t="s">
+      <c r="F15" s="141" t="s">
         <v>649</v>
       </c>
       <c r="G15" s="24" t="s">
@@ -8153,8 +8186,8 @@
       <c r="S15" s="26"/>
     </row>
     <row r="16" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="145"/>
-      <c r="B16" s="148"/>
+      <c r="A16" s="179"/>
+      <c r="B16" s="158"/>
       <c r="C16" s="60" t="s">
         <v>50</v>
       </c>
@@ -8164,7 +8197,7 @@
       <c r="E16" s="23" t="s">
         <v>465</v>
       </c>
-      <c r="F16" s="174" t="s">
+      <c r="F16" s="190" t="s">
         <v>648</v>
       </c>
       <c r="G16" s="24" t="s">
@@ -8198,8 +8231,8 @@
       <c r="S16" s="26"/>
     </row>
     <row r="17" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="145"/>
-      <c r="B17" s="148"/>
+      <c r="A17" s="179"/>
+      <c r="B17" s="158"/>
       <c r="C17" s="60" t="s">
         <v>51</v>
       </c>
@@ -8209,7 +8242,7 @@
       <c r="E17" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="174" t="s">
+      <c r="F17" s="190" t="s">
         <v>648</v>
       </c>
       <c r="G17" s="24" t="s">
@@ -8243,8 +8276,8 @@
       <c r="S17" s="26"/>
     </row>
     <row r="18" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="145"/>
-      <c r="B18" s="148"/>
+      <c r="A18" s="179"/>
+      <c r="B18" s="158"/>
       <c r="C18" s="60" t="s">
         <v>52</v>
       </c>
@@ -8254,7 +8287,7 @@
       <c r="E18" s="23" t="s">
         <v>466</v>
       </c>
-      <c r="F18" s="174" t="s">
+      <c r="F18" s="190" t="s">
         <v>648</v>
       </c>
       <c r="G18" s="24" t="s">
@@ -8288,8 +8321,8 @@
       <c r="S18" s="26"/>
     </row>
     <row r="19" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="145"/>
-      <c r="B19" s="148"/>
+      <c r="A19" s="179"/>
+      <c r="B19" s="158"/>
       <c r="C19" s="60" t="s">
         <v>350</v>
       </c>
@@ -8299,7 +8332,7 @@
       <c r="E19" s="23" t="s">
         <v>467</v>
       </c>
-      <c r="F19" s="174" t="s">
+      <c r="F19" s="190" t="s">
         <v>648</v>
       </c>
       <c r="G19" s="24" t="s">
@@ -8335,8 +8368,8 @@
       <c r="S19" s="26"/>
     </row>
     <row r="20" spans="1:20" s="40" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="145"/>
-      <c r="B20" s="149"/>
+      <c r="A20" s="179"/>
+      <c r="B20" s="182"/>
       <c r="C20" s="61" t="s">
         <v>54</v>
       </c>
@@ -8346,7 +8379,7 @@
       <c r="E20" s="28" t="s">
         <v>468</v>
       </c>
-      <c r="F20" s="177" t="s">
+      <c r="F20" s="142" t="s">
         <v>649</v>
       </c>
       <c r="G20" s="29" t="s">
@@ -8378,8 +8411,8 @@
       <c r="S20" s="31"/>
     </row>
     <row r="21" spans="1:20" s="33" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="145"/>
-      <c r="B21" s="141" t="s">
+      <c r="A21" s="179"/>
+      <c r="B21" s="178" t="s">
         <v>250</v>
       </c>
       <c r="C21" s="120" t="s">
@@ -8391,7 +8424,7 @@
       <c r="E21" s="121" t="s">
         <v>283</v>
       </c>
-      <c r="F21" s="178" t="s">
+      <c r="F21" s="143" t="s">
         <v>652</v>
       </c>
       <c r="G21" s="122" t="s">
@@ -8430,8 +8463,8 @@
       </c>
     </row>
     <row r="22" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="145"/>
-      <c r="B22" s="142"/>
+      <c r="A22" s="179"/>
+      <c r="B22" s="165"/>
       <c r="C22" s="61" t="s">
         <v>237</v>
       </c>
@@ -8441,7 +8474,7 @@
       <c r="E22" s="28" t="s">
         <v>285</v>
       </c>
-      <c r="F22" s="171" t="s">
+      <c r="F22" s="138" t="s">
         <v>651</v>
       </c>
       <c r="G22" s="29" t="s">
@@ -8475,8 +8508,8 @@
       <c r="S22" s="26"/>
     </row>
     <row r="23" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="145"/>
-      <c r="B23" s="142"/>
+      <c r="A23" s="179"/>
+      <c r="B23" s="165"/>
       <c r="C23" s="60" t="s">
         <v>49</v>
       </c>
@@ -8486,7 +8519,7 @@
       <c r="E23" s="23" t="s">
         <v>278</v>
       </c>
-      <c r="F23" s="175" t="s">
+      <c r="F23" s="141" t="s">
         <v>649</v>
       </c>
       <c r="G23" s="24" t="s">
@@ -8520,8 +8553,8 @@
       <c r="S23" s="26"/>
     </row>
     <row r="24" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="145"/>
-      <c r="B24" s="142"/>
+      <c r="A24" s="179"/>
+      <c r="B24" s="165"/>
       <c r="C24" s="60" t="s">
         <v>124</v>
       </c>
@@ -8531,7 +8564,7 @@
       <c r="E24" s="23" t="s">
         <v>282</v>
       </c>
-      <c r="F24" s="171" t="s">
+      <c r="F24" s="138" t="s">
         <v>651</v>
       </c>
       <c r="G24" s="24" t="s">
@@ -8567,8 +8600,8 @@
       <c r="S24" s="26"/>
     </row>
     <row r="25" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="145"/>
-      <c r="B25" s="142"/>
+      <c r="A25" s="179"/>
+      <c r="B25" s="165"/>
       <c r="C25" s="60" t="s">
         <v>239</v>
       </c>
@@ -8578,7 +8611,7 @@
       <c r="E25" s="23" t="s">
         <v>383</v>
       </c>
-      <c r="F25" s="171" t="s">
+      <c r="F25" s="138" t="s">
         <v>651</v>
       </c>
       <c r="G25" s="24" t="s">
@@ -8616,8 +8649,8 @@
       <c r="S25" s="26"/>
     </row>
     <row r="26" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="145"/>
-      <c r="B26" s="142"/>
+      <c r="A26" s="179"/>
+      <c r="B26" s="165"/>
       <c r="C26" s="60" t="s">
         <v>354</v>
       </c>
@@ -8627,7 +8660,7 @@
       <c r="E26" s="23" t="s">
         <v>394</v>
       </c>
-      <c r="F26" s="175" t="s">
+      <c r="F26" s="141" t="s">
         <v>649</v>
       </c>
       <c r="G26" s="24" t="s">
@@ -8661,8 +8694,8 @@
       <c r="S26" s="26"/>
     </row>
     <row r="27" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="145"/>
-      <c r="B27" s="142"/>
+      <c r="A27" s="179"/>
+      <c r="B27" s="165"/>
       <c r="C27" s="60" t="s">
         <v>123</v>
       </c>
@@ -8672,7 +8705,7 @@
       <c r="E27" s="23" t="s">
         <v>275</v>
       </c>
-      <c r="F27" s="171" t="s">
+      <c r="F27" s="138" t="s">
         <v>651</v>
       </c>
       <c r="G27" s="24" t="s">
@@ -8706,8 +8739,8 @@
       <c r="S27" s="26"/>
     </row>
     <row r="28" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="145"/>
-      <c r="B28" s="142"/>
+      <c r="A28" s="179"/>
+      <c r="B28" s="165"/>
       <c r="C28" s="60" t="s">
         <v>469</v>
       </c>
@@ -8717,7 +8750,7 @@
       <c r="E28" s="23" t="s">
         <v>277</v>
       </c>
-      <c r="F28" s="171" t="s">
+      <c r="F28" s="138" t="s">
         <v>651</v>
       </c>
       <c r="G28" s="24" t="s">
@@ -8751,8 +8784,8 @@
       <c r="S28" s="26"/>
     </row>
     <row r="29" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="145"/>
-      <c r="B29" s="142"/>
+      <c r="A29" s="179"/>
+      <c r="B29" s="165"/>
       <c r="C29" s="60" t="s">
         <v>389</v>
       </c>
@@ -8762,7 +8795,7 @@
       <c r="E29" s="23" t="s">
         <v>390</v>
       </c>
-      <c r="F29" s="171" t="s">
+      <c r="F29" s="138" t="s">
         <v>651</v>
       </c>
       <c r="G29" s="24" t="s">
@@ -8798,8 +8831,8 @@
       <c r="S29" s="26"/>
     </row>
     <row r="30" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="145"/>
-      <c r="B30" s="142"/>
+      <c r="A30" s="179"/>
+      <c r="B30" s="165"/>
       <c r="C30" s="60" t="s">
         <v>242</v>
       </c>
@@ -8809,7 +8842,7 @@
       <c r="E30" s="23" t="s">
         <v>281</v>
       </c>
-      <c r="F30" s="172" t="s">
+      <c r="F30" s="139" t="s">
         <v>652</v>
       </c>
       <c r="G30" s="24" t="s">
@@ -8846,8 +8879,8 @@
       <c r="T30" s="23"/>
     </row>
     <row r="31" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="145"/>
-      <c r="B31" s="142"/>
+      <c r="A31" s="179"/>
+      <c r="B31" s="165"/>
       <c r="C31" s="60" t="s">
         <v>355</v>
       </c>
@@ -8857,7 +8890,7 @@
       <c r="E31" s="23" t="s">
         <v>470</v>
       </c>
-      <c r="F31" s="171" t="s">
+      <c r="F31" s="138" t="s">
         <v>651</v>
       </c>
       <c r="G31" s="24" t="s">
@@ -8893,8 +8926,8 @@
       <c r="S31" s="26"/>
     </row>
     <row r="32" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="145"/>
-      <c r="B32" s="142"/>
+      <c r="A32" s="179"/>
+      <c r="B32" s="165"/>
       <c r="C32" s="60" t="s">
         <v>220</v>
       </c>
@@ -8904,7 +8937,7 @@
       <c r="E32" s="23" t="s">
         <v>276</v>
       </c>
-      <c r="F32" s="171" t="s">
+      <c r="F32" s="138" t="s">
         <v>651</v>
       </c>
       <c r="G32" s="24" t="s">
@@ -8941,8 +8974,8 @@
       <c r="T32" s="23"/>
     </row>
     <row r="33" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="145"/>
-      <c r="B33" s="142"/>
+      <c r="A33" s="179"/>
+      <c r="B33" s="165"/>
       <c r="C33" s="60" t="s">
         <v>246</v>
       </c>
@@ -8952,7 +8985,7 @@
       <c r="E33" s="23" t="s">
         <v>280</v>
       </c>
-      <c r="F33" s="171" t="s">
+      <c r="F33" s="138" t="s">
         <v>651</v>
       </c>
       <c r="G33" s="24" t="s">
@@ -8988,8 +9021,8 @@
       <c r="S33" s="26"/>
     </row>
     <row r="34" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="145"/>
-      <c r="B34" s="142"/>
+      <c r="A34" s="179"/>
+      <c r="B34" s="165"/>
       <c r="C34" s="60" t="s">
         <v>379</v>
       </c>
@@ -8999,7 +9032,7 @@
       <c r="E34" s="23" t="s">
         <v>380</v>
       </c>
-      <c r="F34" s="174" t="s">
+      <c r="F34" s="190" t="s">
         <v>648</v>
       </c>
       <c r="G34" s="24" t="s">
@@ -9033,8 +9066,8 @@
       <c r="S34" s="26"/>
     </row>
     <row r="35" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="145"/>
-      <c r="B35" s="142"/>
+      <c r="A35" s="179"/>
+      <c r="B35" s="165"/>
       <c r="C35" s="60" t="s">
         <v>392</v>
       </c>
@@ -9044,7 +9077,7 @@
       <c r="E35" s="23" t="s">
         <v>393</v>
       </c>
-      <c r="F35" s="174" t="s">
+      <c r="F35" s="190" t="s">
         <v>648</v>
       </c>
       <c r="G35" s="24" t="s">
@@ -9078,8 +9111,8 @@
       <c r="S35" s="26"/>
     </row>
     <row r="36" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="145"/>
-      <c r="B36" s="143"/>
+      <c r="A36" s="179"/>
+      <c r="B36" s="170"/>
       <c r="C36" s="65" t="s">
         <v>238</v>
       </c>
@@ -9089,7 +9122,7 @@
       <c r="E36" s="23" t="s">
         <v>284</v>
       </c>
-      <c r="F36" s="172" t="s">
+      <c r="F36" s="139" t="s">
         <v>652</v>
       </c>
       <c r="G36" s="24" t="s">
@@ -9123,10 +9156,10 @@
       <c r="S36" s="26"/>
     </row>
     <row r="37" spans="1:20" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="155" t="s">
+      <c r="A37" s="186" t="s">
         <v>270</v>
       </c>
-      <c r="B37" s="150" t="s">
+      <c r="B37" s="157" t="s">
         <v>55</v>
       </c>
       <c r="C37" s="62" t="s">
@@ -9138,7 +9171,9 @@
       <c r="E37" s="33" t="s">
         <v>345</v>
       </c>
-      <c r="F37" s="33"/>
+      <c r="F37" s="143" t="s">
+        <v>652</v>
+      </c>
       <c r="G37" s="34" t="s">
         <v>8</v>
       </c>
@@ -9169,8 +9204,8 @@
       <c r="T37" s="33"/>
     </row>
     <row r="38" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="156"/>
-      <c r="B38" s="148"/>
+      <c r="A38" s="187"/>
+      <c r="B38" s="158"/>
       <c r="C38" s="60" t="s">
         <v>111</v>
       </c>
@@ -9180,7 +9215,9 @@
       <c r="E38" s="47" t="s">
         <v>343</v>
       </c>
-      <c r="F38" s="45"/>
+      <c r="F38" s="145" t="s">
+        <v>652</v>
+      </c>
       <c r="G38" s="24" t="s">
         <v>8</v>
       </c>
@@ -9210,8 +9247,8 @@
       <c r="S38" s="26"/>
     </row>
     <row r="39" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="156"/>
-      <c r="B39" s="148"/>
+      <c r="A39" s="187"/>
+      <c r="B39" s="158"/>
       <c r="C39" s="60" t="s">
         <v>112</v>
       </c>
@@ -9221,7 +9258,9 @@
       <c r="E39" s="47" t="s">
         <v>344</v>
       </c>
-      <c r="F39" s="45"/>
+      <c r="F39" s="145" t="s">
+        <v>652</v>
+      </c>
       <c r="G39" s="24" t="s">
         <v>8</v>
       </c>
@@ -9252,8 +9291,8 @@
       <c r="T39" s="23"/>
     </row>
     <row r="40" spans="1:20" s="28" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="156"/>
-      <c r="B40" s="148"/>
+      <c r="A40" s="187"/>
+      <c r="B40" s="158"/>
       <c r="C40" s="61" t="s">
         <v>113</v>
       </c>
@@ -9263,7 +9302,9 @@
       <c r="E40" s="44" t="s">
         <v>496</v>
       </c>
-      <c r="F40" s="44"/>
+      <c r="F40" s="189" t="s">
+        <v>652</v>
+      </c>
       <c r="G40" s="29" t="s">
         <v>8</v>
       </c>
@@ -9299,8 +9340,8 @@
       <c r="S40" s="31"/>
     </row>
     <row r="41" spans="1:20" s="28" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="156"/>
-      <c r="B41" s="153" t="s">
+      <c r="A41" s="187"/>
+      <c r="B41" s="164" t="s">
         <v>197</v>
       </c>
       <c r="C41" s="63" t="s">
@@ -9312,7 +9353,7 @@
       <c r="E41" s="53" t="s">
         <v>445</v>
       </c>
-      <c r="F41" s="181" t="s">
+      <c r="F41" s="146" t="s">
         <v>647</v>
       </c>
       <c r="G41" s="54" t="s">
@@ -9346,8 +9387,8 @@
       <c r="S41" s="57"/>
     </row>
     <row r="42" spans="1:20" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="156"/>
-      <c r="B42" s="142"/>
+      <c r="A42" s="187"/>
+      <c r="B42" s="165"/>
       <c r="C42" s="60" t="s">
         <v>222</v>
       </c>
@@ -9387,8 +9428,8 @@
       <c r="S42" s="26"/>
     </row>
     <row r="43" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="156"/>
-      <c r="B43" s="142"/>
+      <c r="A43" s="187"/>
+      <c r="B43" s="165"/>
       <c r="C43" s="60" t="s">
         <v>262</v>
       </c>
@@ -9428,8 +9469,8 @@
       <c r="S43" s="26"/>
     </row>
     <row r="44" spans="1:20" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="156"/>
-      <c r="B44" s="142"/>
+      <c r="A44" s="187"/>
+      <c r="B44" s="165"/>
       <c r="C44" s="60" t="s">
         <v>223</v>
       </c>
@@ -9439,7 +9480,9 @@
       <c r="E44" s="47" t="s">
         <v>346</v>
       </c>
-      <c r="F44" s="45"/>
+      <c r="F44" s="138" t="s">
+        <v>651</v>
+      </c>
       <c r="G44" s="24" t="s">
         <v>8</v>
       </c>
@@ -9469,8 +9512,8 @@
       <c r="S44" s="26"/>
     </row>
     <row r="45" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="156"/>
-      <c r="B45" s="142"/>
+      <c r="A45" s="187"/>
+      <c r="B45" s="165"/>
       <c r="C45" s="60" t="s">
         <v>494</v>
       </c>
@@ -9513,8 +9556,8 @@
       <c r="T45" s="28"/>
     </row>
     <row r="46" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="156"/>
-      <c r="B46" s="142"/>
+      <c r="A46" s="187"/>
+      <c r="B46" s="165"/>
       <c r="C46" s="60" t="s">
         <v>417</v>
       </c>
@@ -9524,7 +9567,9 @@
       <c r="E46" s="47" t="s">
         <v>416</v>
       </c>
-      <c r="F46" s="47"/>
+      <c r="F46" s="138" t="s">
+        <v>651</v>
+      </c>
       <c r="G46" s="24" t="s">
         <v>8</v>
       </c>
@@ -9554,8 +9599,8 @@
       <c r="S46" s="26"/>
     </row>
     <row r="47" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="156"/>
-      <c r="B47" s="142"/>
+      <c r="A47" s="187"/>
+      <c r="B47" s="165"/>
       <c r="C47" s="60" t="s">
         <v>414</v>
       </c>
@@ -9595,8 +9640,8 @@
       <c r="S47" s="26"/>
     </row>
     <row r="48" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="156"/>
-      <c r="B48" s="142"/>
+      <c r="A48" s="187"/>
+      <c r="B48" s="165"/>
       <c r="C48" s="60" t="s">
         <v>412</v>
       </c>
@@ -9606,7 +9651,9 @@
       <c r="E48" s="47" t="s">
         <v>413</v>
       </c>
-      <c r="F48" s="47"/>
+      <c r="F48" s="155" t="s">
+        <v>647</v>
+      </c>
       <c r="G48" s="24" t="s">
         <v>8</v>
       </c>
@@ -9640,8 +9687,8 @@
       <c r="S48" s="26"/>
     </row>
     <row r="49" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="156"/>
-      <c r="B49" s="142"/>
+      <c r="A49" s="187"/>
+      <c r="B49" s="165"/>
       <c r="C49" s="60" t="s">
         <v>261</v>
       </c>
@@ -9683,8 +9730,8 @@
       <c r="S49" s="26"/>
     </row>
     <row r="50" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="157"/>
-      <c r="B50" s="143"/>
+      <c r="A50" s="188"/>
+      <c r="B50" s="170"/>
       <c r="C50" s="65" t="s">
         <v>535</v>
       </c>
@@ -9726,10 +9773,10 @@
       <c r="S50" s="26"/>
     </row>
     <row r="51" spans="1:20" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="158" t="s">
+      <c r="A51" s="159" t="s">
         <v>93</v>
       </c>
-      <c r="B51" s="150" t="s">
+      <c r="B51" s="157" t="s">
         <v>55</v>
       </c>
       <c r="C51" s="62" t="s">
@@ -9741,7 +9788,7 @@
       <c r="E51" s="33" t="s">
         <v>330</v>
       </c>
-      <c r="F51" s="178" t="s">
+      <c r="F51" s="143" t="s">
         <v>652</v>
       </c>
       <c r="G51" s="34" t="s">
@@ -9776,8 +9823,8 @@
       <c r="T51" s="33"/>
     </row>
     <row r="52" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="159"/>
-      <c r="B52" s="148"/>
+      <c r="A52" s="160"/>
+      <c r="B52" s="158"/>
       <c r="C52" s="60" t="s">
         <v>70</v>
       </c>
@@ -9787,7 +9834,7 @@
       <c r="E52" s="23" t="s">
         <v>333</v>
       </c>
-      <c r="F52" s="175" t="s">
+      <c r="F52" s="141" t="s">
         <v>649</v>
       </c>
       <c r="G52" s="24" t="s">
@@ -9823,8 +9870,8 @@
       <c r="S52" s="26"/>
     </row>
     <row r="53" spans="1:20" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="159"/>
-      <c r="B53" s="148"/>
+      <c r="A53" s="160"/>
+      <c r="B53" s="158"/>
       <c r="C53" s="60" t="s">
         <v>71</v>
       </c>
@@ -9834,7 +9881,7 @@
       <c r="E53" s="23" t="s">
         <v>331</v>
       </c>
-      <c r="F53" s="171" t="s">
+      <c r="F53" s="138" t="s">
         <v>651</v>
       </c>
       <c r="G53" s="24" t="s">
@@ -9870,8 +9917,8 @@
       <c r="S53" s="26"/>
     </row>
     <row r="54" spans="1:20" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="159"/>
-      <c r="B54" s="148"/>
+      <c r="A54" s="160"/>
+      <c r="B54" s="158"/>
       <c r="C54" s="61" t="s">
         <v>72</v>
       </c>
@@ -9881,7 +9928,7 @@
       <c r="E54" s="28" t="s">
         <v>332</v>
       </c>
-      <c r="F54" s="171" t="s">
+      <c r="F54" s="138" t="s">
         <v>651</v>
       </c>
       <c r="G54" s="29" t="s">
@@ -9917,8 +9964,8 @@
       <c r="S54" s="26"/>
     </row>
     <row r="55" spans="1:20" s="23" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="159"/>
-      <c r="B55" s="148"/>
+      <c r="A55" s="160"/>
+      <c r="B55" s="158"/>
       <c r="C55" s="65" t="s">
         <v>612</v>
       </c>
@@ -9928,7 +9975,7 @@
       <c r="E55" s="23" t="s">
         <v>613</v>
       </c>
-      <c r="F55" s="172" t="s">
+      <c r="F55" s="139" t="s">
         <v>652</v>
       </c>
       <c r="G55" s="24" t="s">
@@ -9962,8 +10009,8 @@
       <c r="S55" s="31"/>
     </row>
     <row r="56" spans="1:20" s="23" customFormat="1" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="159"/>
-      <c r="B56" s="153" t="s">
+      <c r="A56" s="160"/>
+      <c r="B56" s="164" t="s">
         <v>197</v>
       </c>
       <c r="C56" s="63" t="s">
@@ -9975,7 +10022,7 @@
       <c r="E56" s="53" t="s">
         <v>341</v>
       </c>
-      <c r="F56" s="183" t="s">
+      <c r="F56" s="148" t="s">
         <v>649</v>
       </c>
       <c r="G56" s="54" t="s">
@@ -10009,8 +10056,8 @@
       <c r="S56" s="57"/>
     </row>
     <row r="57" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="159"/>
-      <c r="B57" s="142"/>
+      <c r="A57" s="160"/>
+      <c r="B57" s="165"/>
       <c r="C57" s="60" t="s">
         <v>213</v>
       </c>
@@ -10020,7 +10067,7 @@
       <c r="E57" s="47" t="s">
         <v>342</v>
       </c>
-      <c r="F57" s="171" t="s">
+      <c r="F57" s="138" t="s">
         <v>651</v>
       </c>
       <c r="G57" s="24" t="s">
@@ -10056,8 +10103,8 @@
       <c r="S57" s="26"/>
     </row>
     <row r="58" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="159"/>
-      <c r="B58" s="142"/>
+      <c r="A58" s="160"/>
+      <c r="B58" s="165"/>
       <c r="C58" s="60" t="s">
         <v>206</v>
       </c>
@@ -10099,8 +10146,8 @@
       <c r="S58" s="26"/>
     </row>
     <row r="59" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="159"/>
-      <c r="B59" s="142"/>
+      <c r="A59" s="160"/>
+      <c r="B59" s="165"/>
       <c r="C59" s="60" t="s">
         <v>201</v>
       </c>
@@ -10110,7 +10157,7 @@
       <c r="E59" s="23" t="s">
         <v>335</v>
       </c>
-      <c r="F59" s="171" t="s">
+      <c r="F59" s="138" t="s">
         <v>651</v>
       </c>
       <c r="G59" s="24" t="s">
@@ -10146,8 +10193,8 @@
       <c r="S59" s="26"/>
     </row>
     <row r="60" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="159"/>
-      <c r="B60" s="142"/>
+      <c r="A60" s="160"/>
+      <c r="B60" s="165"/>
       <c r="C60" s="60" t="s">
         <v>202</v>
       </c>
@@ -10157,7 +10204,7 @@
       <c r="E60" s="23" t="s">
         <v>337</v>
       </c>
-      <c r="F60" s="171" t="s">
+      <c r="F60" s="138" t="s">
         <v>651</v>
       </c>
       <c r="G60" s="24" t="s">
@@ -10193,8 +10240,8 @@
       <c r="S60" s="26"/>
     </row>
     <row r="61" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="159"/>
-      <c r="B61" s="142"/>
+      <c r="A61" s="160"/>
+      <c r="B61" s="165"/>
       <c r="C61" s="60" t="s">
         <v>95</v>
       </c>
@@ -10204,7 +10251,7 @@
       <c r="E61" s="23" t="s">
         <v>334</v>
       </c>
-      <c r="F61" s="171" t="s">
+      <c r="F61" s="138" t="s">
         <v>651</v>
       </c>
       <c r="G61" s="24" t="s">
@@ -10238,8 +10285,8 @@
       <c r="S61" s="26"/>
     </row>
     <row r="62" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="159"/>
-      <c r="B62" s="142"/>
+      <c r="A62" s="160"/>
+      <c r="B62" s="165"/>
       <c r="C62" s="60" t="s">
         <v>419</v>
       </c>
@@ -10249,7 +10296,7 @@
       <c r="E62" s="23" t="s">
         <v>420</v>
       </c>
-      <c r="F62" s="171" t="s">
+      <c r="F62" s="138" t="s">
         <v>651</v>
       </c>
       <c r="G62" s="24" t="s">
@@ -10283,8 +10330,8 @@
       <c r="S62" s="26"/>
     </row>
     <row r="63" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="159"/>
-      <c r="B63" s="142"/>
+      <c r="A63" s="160"/>
+      <c r="B63" s="165"/>
       <c r="C63" s="60" t="s">
         <v>203</v>
       </c>
@@ -10294,7 +10341,7 @@
       <c r="E63" s="23" t="s">
         <v>338</v>
       </c>
-      <c r="F63" s="171" t="s">
+      <c r="F63" s="138" t="s">
         <v>651</v>
       </c>
       <c r="G63" s="24" t="s">
@@ -10330,8 +10377,8 @@
       <c r="S63" s="26"/>
     </row>
     <row r="64" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="159"/>
-      <c r="B64" s="142"/>
+      <c r="A64" s="160"/>
+      <c r="B64" s="165"/>
       <c r="C64" s="60" t="s">
         <v>433</v>
       </c>
@@ -10341,7 +10388,7 @@
       <c r="E64" s="47" t="s">
         <v>434</v>
       </c>
-      <c r="F64" s="179" t="s">
+      <c r="F64" s="144" t="s">
         <v>652</v>
       </c>
       <c r="G64" s="24" t="s">
@@ -10377,8 +10424,8 @@
       <c r="S64" s="26"/>
     </row>
     <row r="65" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="159"/>
-      <c r="B65" s="142"/>
+      <c r="A65" s="160"/>
+      <c r="B65" s="165"/>
       <c r="C65" s="60" t="s">
         <v>381</v>
       </c>
@@ -10388,7 +10435,7 @@
       <c r="E65" s="47" t="s">
         <v>382</v>
       </c>
-      <c r="F65" s="179" t="s">
+      <c r="F65" s="144" t="s">
         <v>652</v>
       </c>
       <c r="G65" s="24" t="s">
@@ -10423,8 +10470,8 @@
       <c r="T65" s="28"/>
     </row>
     <row r="66" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="159"/>
-      <c r="B66" s="142"/>
+      <c r="A66" s="160"/>
+      <c r="B66" s="165"/>
       <c r="C66" s="60" t="s">
         <v>398</v>
       </c>
@@ -10434,7 +10481,7 @@
       <c r="E66" s="23" t="s">
         <v>399</v>
       </c>
-      <c r="F66" s="174" t="s">
+      <c r="F66" s="190" t="s">
         <v>648</v>
       </c>
       <c r="G66" s="24" t="s">
@@ -10470,8 +10517,8 @@
       <c r="S66" s="26"/>
     </row>
     <row r="67" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="159"/>
-      <c r="B67" s="142"/>
+      <c r="A67" s="160"/>
+      <c r="B67" s="165"/>
       <c r="C67" s="60" t="s">
         <v>258</v>
       </c>
@@ -10481,7 +10528,7 @@
       <c r="E67" s="23" t="s">
         <v>336</v>
       </c>
-      <c r="F67" s="172" t="s">
+      <c r="F67" s="139" t="s">
         <v>652</v>
       </c>
       <c r="G67" s="24" t="s">
@@ -10518,8 +10565,8 @@
       <c r="T67" s="23"/>
     </row>
     <row r="68" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="159"/>
-      <c r="B68" s="142"/>
+      <c r="A68" s="160"/>
+      <c r="B68" s="165"/>
       <c r="C68" s="60" t="s">
         <v>436</v>
       </c>
@@ -10529,7 +10576,7 @@
       <c r="E68" s="47" t="s">
         <v>435</v>
       </c>
-      <c r="F68" s="182" t="s">
+      <c r="F68" s="147" t="s">
         <v>647</v>
       </c>
       <c r="G68" s="24" t="s">
@@ -10563,8 +10610,8 @@
       <c r="S68" s="26"/>
     </row>
     <row r="69" spans="1:20" s="33" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="159"/>
-      <c r="B69" s="142"/>
+      <c r="A69" s="160"/>
+      <c r="B69" s="165"/>
       <c r="C69" s="61" t="s">
         <v>207</v>
       </c>
@@ -10574,7 +10621,7 @@
       <c r="E69" s="47" t="s">
         <v>339</v>
       </c>
-      <c r="F69" s="180" t="s">
+      <c r="F69" s="145" t="s">
         <v>652</v>
       </c>
       <c r="G69" s="29" t="s">
@@ -10609,10 +10656,10 @@
       <c r="T69" s="28"/>
     </row>
     <row r="70" spans="1:20" s="23" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="168" t="s">
+      <c r="A70" s="172" t="s">
         <v>101</v>
       </c>
-      <c r="B70" s="167"/>
+      <c r="B70" s="171"/>
       <c r="C70" s="62" t="s">
         <v>83</v>
       </c>
@@ -10622,7 +10669,7 @@
       <c r="E70" s="33" t="s">
         <v>623</v>
       </c>
-      <c r="F70" s="184" t="s">
+      <c r="F70" s="149" t="s">
         <v>651</v>
       </c>
       <c r="G70" s="34" t="s">
@@ -10659,8 +10706,8 @@
       <c r="T70" s="33"/>
     </row>
     <row r="71" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="169"/>
-      <c r="B71" s="148"/>
+      <c r="A71" s="173"/>
+      <c r="B71" s="158"/>
       <c r="C71" s="60" t="s">
         <v>84</v>
       </c>
@@ -10670,7 +10717,7 @@
       <c r="E71" s="23" t="s">
         <v>308</v>
       </c>
-      <c r="F71" s="171" t="s">
+      <c r="F71" s="138" t="s">
         <v>651</v>
       </c>
       <c r="G71" s="24" t="s">
@@ -10706,8 +10753,8 @@
       <c r="S71" s="26"/>
     </row>
     <row r="72" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="169"/>
-      <c r="B72" s="148"/>
+      <c r="A72" s="173"/>
+      <c r="B72" s="158"/>
       <c r="C72" s="60" t="s">
         <v>85</v>
       </c>
@@ -10717,7 +10764,7 @@
       <c r="E72" s="23" t="s">
         <v>301</v>
       </c>
-      <c r="F72" s="179" t="s">
+      <c r="F72" s="144" t="s">
         <v>652</v>
       </c>
       <c r="G72" s="24" t="s">
@@ -10755,8 +10802,8 @@
       <c r="S72" s="26"/>
     </row>
     <row r="73" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="169"/>
-      <c r="B73" s="148"/>
+      <c r="A73" s="173"/>
+      <c r="B73" s="158"/>
       <c r="C73" s="60" t="s">
         <v>86</v>
       </c>
@@ -10766,7 +10813,7 @@
       <c r="E73" s="23" t="s">
         <v>302</v>
       </c>
-      <c r="F73" s="179" t="s">
+      <c r="F73" s="144" t="s">
         <v>652</v>
       </c>
       <c r="G73" s="24" t="s">
@@ -10802,8 +10849,8 @@
       <c r="S73" s="26"/>
     </row>
     <row r="74" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="169"/>
-      <c r="B74" s="148"/>
+      <c r="A74" s="173"/>
+      <c r="B74" s="158"/>
       <c r="C74" s="60" t="s">
         <v>87</v>
       </c>
@@ -10813,7 +10860,7 @@
       <c r="E74" s="23" t="s">
         <v>303</v>
       </c>
-      <c r="F74" s="179" t="s">
+      <c r="F74" s="144" t="s">
         <v>652</v>
       </c>
       <c r="G74" s="37" t="s">
@@ -10851,8 +10898,8 @@
       <c r="S74" s="26"/>
     </row>
     <row r="75" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="169"/>
-      <c r="B75" s="148"/>
+      <c r="A75" s="173"/>
+      <c r="B75" s="158"/>
       <c r="C75" s="60" t="s">
         <v>88</v>
       </c>
@@ -10862,7 +10909,7 @@
       <c r="E75" s="23" t="s">
         <v>304</v>
       </c>
-      <c r="F75" s="179" t="s">
+      <c r="F75" s="144" t="s">
         <v>652</v>
       </c>
       <c r="G75" s="24" t="s">
@@ -10898,8 +10945,8 @@
       <c r="S75" s="26"/>
     </row>
     <row r="76" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="169"/>
-      <c r="B76" s="148"/>
+      <c r="A76" s="173"/>
+      <c r="B76" s="158"/>
       <c r="C76" s="60" t="s">
         <v>89</v>
       </c>
@@ -10909,7 +10956,7 @@
       <c r="E76" s="23" t="s">
         <v>624</v>
       </c>
-      <c r="F76" s="171" t="s">
+      <c r="F76" s="138" t="s">
         <v>651</v>
       </c>
       <c r="G76" s="24" t="s">
@@ -10943,8 +10990,8 @@
       <c r="S76" s="26"/>
     </row>
     <row r="77" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="169"/>
-      <c r="B77" s="148"/>
+      <c r="A77" s="173"/>
+      <c r="B77" s="158"/>
       <c r="C77" s="60" t="s">
         <v>90</v>
       </c>
@@ -10954,7 +11001,7 @@
       <c r="E77" s="23" t="s">
         <v>305</v>
       </c>
-      <c r="F77" s="171" t="s">
+      <c r="F77" s="138" t="s">
         <v>651</v>
       </c>
       <c r="G77" s="24" t="s">
@@ -10990,8 +11037,8 @@
       <c r="S77" s="26"/>
     </row>
     <row r="78" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="169"/>
-      <c r="B78" s="148"/>
+      <c r="A78" s="173"/>
+      <c r="B78" s="158"/>
       <c r="C78" s="60" t="s">
         <v>91</v>
       </c>
@@ -11001,7 +11048,7 @@
       <c r="E78" s="23" t="s">
         <v>306</v>
       </c>
-      <c r="F78" s="171" t="s">
+      <c r="F78" s="138" t="s">
         <v>651</v>
       </c>
       <c r="G78" s="24" t="s">
@@ -11039,8 +11086,8 @@
       <c r="S78" s="26"/>
     </row>
     <row r="79" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="169"/>
-      <c r="B79" s="148"/>
+      <c r="A79" s="173"/>
+      <c r="B79" s="158"/>
       <c r="C79" s="60" t="s">
         <v>229</v>
       </c>
@@ -11050,7 +11097,7 @@
       <c r="E79" s="23" t="s">
         <v>307</v>
       </c>
-      <c r="F79" s="179" t="s">
+      <c r="F79" s="144" t="s">
         <v>652</v>
       </c>
       <c r="G79" s="24" t="s">
@@ -11086,8 +11133,8 @@
       <c r="S79" s="26"/>
     </row>
     <row r="80" spans="1:20" s="23" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="169"/>
-      <c r="B80" s="166"/>
+      <c r="A80" s="173"/>
+      <c r="B80" s="169"/>
       <c r="C80" s="61" t="s">
         <v>94</v>
       </c>
@@ -11097,7 +11144,7 @@
       <c r="E80" s="28" t="s">
         <v>309</v>
       </c>
-      <c r="F80" s="185" t="s">
+      <c r="F80" s="150" t="s">
         <v>651</v>
       </c>
       <c r="G80" s="29" t="s">
@@ -11133,8 +11180,8 @@
       <c r="S80" s="31"/>
     </row>
     <row r="81" spans="1:19" s="23" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="169"/>
-      <c r="B81" s="142" t="s">
+      <c r="A81" s="173"/>
+      <c r="B81" s="165" t="s">
         <v>197</v>
       </c>
       <c r="C81" s="63" t="s">
@@ -11178,8 +11225,8 @@
       <c r="S81" s="57"/>
     </row>
     <row r="82" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="169"/>
-      <c r="B82" s="142"/>
+      <c r="A82" s="173"/>
+      <c r="B82" s="165"/>
       <c r="C82" s="60" t="s">
         <v>217</v>
       </c>
@@ -11222,8 +11269,8 @@
       <c r="S82" s="26"/>
     </row>
     <row r="83" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="169"/>
-      <c r="B83" s="142"/>
+      <c r="A83" s="173"/>
+      <c r="B83" s="165"/>
       <c r="C83" s="60" t="s">
         <v>431</v>
       </c>
@@ -11233,7 +11280,7 @@
       <c r="E83" s="23" t="s">
         <v>432</v>
       </c>
-      <c r="F83" s="179" t="s">
+      <c r="F83" s="144" t="s">
         <v>652</v>
       </c>
       <c r="G83" s="24" t="s">
@@ -11267,8 +11314,8 @@
       <c r="S83" s="26"/>
     </row>
     <row r="84" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="169"/>
-      <c r="B84" s="142"/>
+      <c r="A84" s="173"/>
+      <c r="B84" s="165"/>
       <c r="C84" s="60" t="s">
         <v>299</v>
       </c>
@@ -11278,7 +11325,7 @@
       <c r="E84" s="23" t="s">
         <v>310</v>
       </c>
-      <c r="F84" s="179" t="s">
+      <c r="F84" s="144" t="s">
         <v>652</v>
       </c>
       <c r="G84" s="24" t="s">
@@ -11312,8 +11359,8 @@
       <c r="S84" s="26"/>
     </row>
     <row r="85" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="169"/>
-      <c r="B85" s="142"/>
+      <c r="A85" s="173"/>
+      <c r="B85" s="165"/>
       <c r="C85" s="60" t="s">
         <v>372</v>
       </c>
@@ -11323,7 +11370,7 @@
       <c r="E85" s="23" t="s">
         <v>373</v>
       </c>
-      <c r="F85" s="186" t="s">
+      <c r="F85" s="151" t="s">
         <v>649</v>
       </c>
       <c r="G85" s="24" t="s">
@@ -11357,8 +11404,8 @@
       <c r="S85" s="26"/>
     </row>
     <row r="86" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="169"/>
-      <c r="B86" s="142"/>
+      <c r="A86" s="173"/>
+      <c r="B86" s="165"/>
       <c r="C86" s="60" t="s">
         <v>225</v>
       </c>
@@ -11368,7 +11415,7 @@
       <c r="E86" s="45" t="s">
         <v>328</v>
       </c>
-      <c r="F86" s="179" t="s">
+      <c r="F86" s="144" t="s">
         <v>652</v>
       </c>
       <c r="G86" s="24" t="s">
@@ -11402,8 +11449,8 @@
       <c r="S86" s="26"/>
     </row>
     <row r="87" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="169"/>
-      <c r="B87" s="142"/>
+      <c r="A87" s="173"/>
+      <c r="B87" s="165"/>
       <c r="C87" s="60" t="s">
         <v>326</v>
       </c>
@@ -11413,7 +11460,7 @@
       <c r="E87" s="45" t="s">
         <v>327</v>
       </c>
-      <c r="F87" s="179" t="s">
+      <c r="F87" s="144" t="s">
         <v>652</v>
       </c>
       <c r="G87" s="24" t="s">
@@ -11449,8 +11496,8 @@
       <c r="S87" s="26"/>
     </row>
     <row r="88" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="169"/>
-      <c r="B88" s="142"/>
+      <c r="A88" s="173"/>
+      <c r="B88" s="165"/>
       <c r="C88" s="61" t="s">
         <v>253</v>
       </c>
@@ -11460,7 +11507,7 @@
       <c r="E88" s="28" t="s">
         <v>503</v>
       </c>
-      <c r="F88" s="179" t="s">
+      <c r="F88" s="144" t="s">
         <v>652</v>
       </c>
       <c r="G88" s="29" t="s">
@@ -11494,8 +11541,8 @@
       <c r="S88" s="26"/>
     </row>
     <row r="89" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="169"/>
-      <c r="B89" s="142"/>
+      <c r="A89" s="173"/>
+      <c r="B89" s="165"/>
       <c r="C89" s="60" t="s">
         <v>408</v>
       </c>
@@ -11536,8 +11583,8 @@
       <c r="S89" s="26"/>
     </row>
     <row r="90" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="169"/>
-      <c r="B90" s="142"/>
+      <c r="A90" s="173"/>
+      <c r="B90" s="165"/>
       <c r="C90" s="60" t="s">
         <v>374</v>
       </c>
@@ -11579,8 +11626,8 @@
       <c r="S90" s="26"/>
     </row>
     <row r="91" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="169"/>
-      <c r="B91" s="142"/>
+      <c r="A91" s="173"/>
+      <c r="B91" s="165"/>
       <c r="C91" s="60" t="s">
         <v>361</v>
       </c>
@@ -11624,8 +11671,8 @@
       <c r="S91" s="26"/>
     </row>
     <row r="92" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="169"/>
-      <c r="B92" s="142"/>
+      <c r="A92" s="173"/>
+      <c r="B92" s="165"/>
       <c r="C92" s="60" t="s">
         <v>357</v>
       </c>
@@ -11669,8 +11716,8 @@
       <c r="S92" s="26"/>
     </row>
     <row r="93" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="169"/>
-      <c r="B93" s="142"/>
+      <c r="A93" s="173"/>
+      <c r="B93" s="165"/>
       <c r="C93" s="60" t="s">
         <v>216</v>
       </c>
@@ -11713,8 +11760,8 @@
       <c r="S93" s="26"/>
     </row>
     <row r="94" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="169"/>
-      <c r="B94" s="142"/>
+      <c r="A94" s="173"/>
+      <c r="B94" s="165"/>
       <c r="C94" s="60" t="s">
         <v>377</v>
       </c>
@@ -11724,7 +11771,7 @@
       <c r="E94" s="47" t="s">
         <v>378</v>
       </c>
-      <c r="F94" s="179" t="s">
+      <c r="F94" s="144" t="s">
         <v>652</v>
       </c>
       <c r="G94" s="24" t="s">
@@ -11758,8 +11805,8 @@
       <c r="S94" s="26"/>
     </row>
     <row r="95" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="169"/>
-      <c r="B95" s="142"/>
+      <c r="A95" s="173"/>
+      <c r="B95" s="165"/>
       <c r="C95" s="60" t="s">
         <v>226</v>
       </c>
@@ -11769,7 +11816,7 @@
       <c r="E95" s="23" t="s">
         <v>318</v>
       </c>
-      <c r="F95" s="171" t="s">
+      <c r="F95" s="138" t="s">
         <v>651</v>
       </c>
       <c r="G95" s="24" t="s">
@@ -11803,8 +11850,8 @@
       <c r="S95" s="26"/>
     </row>
     <row r="96" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="169"/>
-      <c r="B96" s="142"/>
+      <c r="A96" s="173"/>
+      <c r="B96" s="165"/>
       <c r="C96" s="60" t="s">
         <v>251</v>
       </c>
@@ -11814,7 +11861,7 @@
       <c r="E96" s="23" t="s">
         <v>317</v>
       </c>
-      <c r="F96" s="171" t="s">
+      <c r="F96" s="138" t="s">
         <v>651</v>
       </c>
       <c r="G96" s="24" t="s">
@@ -11848,8 +11895,8 @@
       <c r="S96" s="26"/>
     </row>
     <row r="97" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="169"/>
-      <c r="B97" s="142"/>
+      <c r="A97" s="173"/>
+      <c r="B97" s="165"/>
       <c r="C97" s="60" t="s">
         <v>298</v>
       </c>
@@ -11859,7 +11906,7 @@
       <c r="E97" s="23" t="s">
         <v>319</v>
       </c>
-      <c r="F97" s="171" t="s">
+      <c r="F97" s="138" t="s">
         <v>651</v>
       </c>
       <c r="G97" s="24" t="s">
@@ -11893,8 +11940,8 @@
       <c r="S97" s="26"/>
     </row>
     <row r="98" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="169"/>
-      <c r="B98" s="142"/>
+      <c r="A98" s="173"/>
+      <c r="B98" s="165"/>
       <c r="C98" s="60" t="s">
         <v>228</v>
       </c>
@@ -11904,7 +11951,7 @@
       <c r="E98" s="23" t="s">
         <v>502</v>
       </c>
-      <c r="F98" s="171" t="s">
+      <c r="F98" s="138" t="s">
         <v>651</v>
       </c>
       <c r="G98" s="24" t="s">
@@ -11938,8 +11985,8 @@
       <c r="S98" s="26"/>
     </row>
     <row r="99" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="169"/>
-      <c r="B99" s="142"/>
+      <c r="A99" s="173"/>
+      <c r="B99" s="165"/>
       <c r="C99" s="60" t="s">
         <v>236</v>
       </c>
@@ -11978,8 +12025,8 @@
       <c r="S99" s="26"/>
     </row>
     <row r="100" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="169"/>
-      <c r="B100" s="142"/>
+      <c r="A100" s="173"/>
+      <c r="B100" s="165"/>
       <c r="C100" s="60" t="s">
         <v>227</v>
       </c>
@@ -12020,8 +12067,8 @@
       <c r="S100" s="26"/>
     </row>
     <row r="101" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="169"/>
-      <c r="B101" s="142"/>
+      <c r="A101" s="173"/>
+      <c r="B101" s="165"/>
       <c r="C101" s="65" t="s">
         <v>221</v>
       </c>
@@ -12031,7 +12078,7 @@
       <c r="E101" s="23" t="s">
         <v>311</v>
       </c>
-      <c r="F101" s="171" t="s">
+      <c r="F101" s="138" t="s">
         <v>651</v>
       </c>
       <c r="G101" s="24" t="s">
@@ -12067,8 +12114,8 @@
       <c r="S101" s="26"/>
     </row>
     <row r="102" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="169"/>
-      <c r="B102" s="142"/>
+      <c r="A102" s="173"/>
+      <c r="B102" s="165"/>
       <c r="C102" s="60" t="s">
         <v>218</v>
       </c>
@@ -12078,7 +12125,7 @@
       <c r="E102" s="45" t="s">
         <v>296</v>
       </c>
-      <c r="F102" s="189"/>
+      <c r="F102" s="154"/>
       <c r="G102" s="24" t="s">
         <v>8</v>
       </c>
@@ -12110,8 +12157,8 @@
       <c r="S102" s="26"/>
     </row>
     <row r="103" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="169"/>
-      <c r="B103" s="142"/>
+      <c r="A103" s="173"/>
+      <c r="B103" s="165"/>
       <c r="C103" s="60" t="s">
         <v>219</v>
       </c>
@@ -12121,7 +12168,7 @@
       <c r="E103" s="45" t="s">
         <v>300</v>
       </c>
-      <c r="F103" s="189"/>
+      <c r="F103" s="154"/>
       <c r="G103" s="24" t="s">
         <v>8</v>
       </c>
@@ -12155,15 +12202,15 @@
       <c r="S103" s="26"/>
     </row>
     <row r="104" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="169"/>
-      <c r="B104" s="142"/>
+      <c r="A104" s="173"/>
+      <c r="B104" s="165"/>
       <c r="C104" s="60" t="s">
         <v>363</v>
       </c>
       <c r="D104" s="23" t="s">
         <v>171</v>
       </c>
-      <c r="E104" s="187" t="s">
+      <c r="E104" s="152" t="s">
         <v>364</v>
       </c>
       <c r="G104" s="24" t="s">
@@ -12197,15 +12244,15 @@
       <c r="S104" s="26"/>
     </row>
     <row r="105" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="169"/>
-      <c r="B105" s="142"/>
+      <c r="A105" s="173"/>
+      <c r="B105" s="165"/>
       <c r="C105" s="60" t="s">
         <v>235</v>
       </c>
       <c r="D105" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="E105" s="187" t="s">
+      <c r="E105" s="152" t="s">
         <v>608</v>
       </c>
       <c r="G105" s="24" t="s">
@@ -12239,8 +12286,8 @@
       <c r="S105" s="26"/>
     </row>
     <row r="106" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="169"/>
-      <c r="B106" s="142"/>
+      <c r="A106" s="173"/>
+      <c r="B106" s="165"/>
       <c r="C106" s="60" t="s">
         <v>210</v>
       </c>
@@ -12250,7 +12297,7 @@
       <c r="E106" s="45" t="s">
         <v>295</v>
       </c>
-      <c r="F106" s="189"/>
+      <c r="F106" s="154"/>
       <c r="G106" s="24" t="s">
         <v>8</v>
       </c>
@@ -12282,8 +12329,8 @@
       <c r="S106" s="26"/>
     </row>
     <row r="107" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="169"/>
-      <c r="B107" s="142"/>
+      <c r="A107" s="173"/>
+      <c r="B107" s="165"/>
       <c r="C107" s="60" t="s">
         <v>211</v>
       </c>
@@ -12293,7 +12340,7 @@
       <c r="E107" s="45" t="s">
         <v>315</v>
       </c>
-      <c r="F107" s="189"/>
+      <c r="F107" s="154"/>
       <c r="G107" s="24" t="s">
         <v>8</v>
       </c>
@@ -12325,15 +12372,15 @@
       <c r="S107" s="26"/>
     </row>
     <row r="108" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="169"/>
-      <c r="B108" s="142"/>
+      <c r="A108" s="173"/>
+      <c r="B108" s="165"/>
       <c r="C108" s="60" t="s">
         <v>506</v>
       </c>
       <c r="D108" s="23" t="s">
         <v>171</v>
       </c>
-      <c r="E108" s="187" t="s">
+      <c r="E108" s="152" t="s">
         <v>351</v>
       </c>
       <c r="G108" s="24" t="s">
@@ -12367,15 +12414,15 @@
       <c r="S108" s="26"/>
     </row>
     <row r="109" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="169"/>
-      <c r="B109" s="142"/>
+      <c r="A109" s="173"/>
+      <c r="B109" s="165"/>
       <c r="C109" s="60" t="s">
         <v>252</v>
       </c>
       <c r="D109" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="E109" s="187" t="s">
+      <c r="E109" s="152" t="s">
         <v>321</v>
       </c>
       <c r="G109" s="24" t="s">
@@ -12409,18 +12456,18 @@
       <c r="S109" s="26"/>
     </row>
     <row r="110" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="169"/>
-      <c r="B110" s="142"/>
+      <c r="A110" s="173"/>
+      <c r="B110" s="165"/>
       <c r="C110" s="60" t="s">
         <v>255</v>
       </c>
       <c r="D110" s="23" t="s">
         <v>256</v>
       </c>
-      <c r="E110" s="187" t="s">
+      <c r="E110" s="152" t="s">
         <v>320</v>
       </c>
-      <c r="F110" s="174" t="s">
+      <c r="F110" s="190" t="s">
         <v>648</v>
       </c>
       <c r="G110" s="24" t="s">
@@ -12454,8 +12501,8 @@
       <c r="S110" s="26"/>
     </row>
     <row r="111" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="169"/>
-      <c r="B111" s="142"/>
+      <c r="A111" s="173"/>
+      <c r="B111" s="165"/>
       <c r="C111" s="60" t="s">
         <v>232</v>
       </c>
@@ -12465,7 +12512,7 @@
       <c r="E111" s="45" t="s">
         <v>293</v>
       </c>
-      <c r="F111" s="190" t="s">
+      <c r="F111" s="155" t="s">
         <v>647</v>
       </c>
       <c r="G111" s="24" t="s">
@@ -12501,8 +12548,8 @@
       <c r="S111" s="26"/>
     </row>
     <row r="112" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="169"/>
-      <c r="B112" s="142"/>
+      <c r="A112" s="173"/>
+      <c r="B112" s="165"/>
       <c r="C112" s="60" t="s">
         <v>233</v>
       </c>
@@ -12512,7 +12559,7 @@
       <c r="E112" s="45" t="s">
         <v>294</v>
       </c>
-      <c r="F112" s="190" t="s">
+      <c r="F112" s="155" t="s">
         <v>647</v>
       </c>
       <c r="G112" s="24" t="s">
@@ -12548,16 +12595,16 @@
       <c r="S112" s="26"/>
     </row>
     <row r="113" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="169"/>
-      <c r="B113" s="142"/>
+      <c r="A113" s="173"/>
+      <c r="B113" s="165"/>
       <c r="C113" s="65" t="s">
         <v>606</v>
       </c>
       <c r="D113" s="23"/>
-      <c r="E113" s="188" t="s">
+      <c r="E113" s="153" t="s">
         <v>607</v>
       </c>
-      <c r="F113" s="179" t="s">
+      <c r="F113" s="144" t="s">
         <v>652</v>
       </c>
       <c r="G113" s="24"/>
@@ -12576,8 +12623,8 @@
       <c r="T113" s="23"/>
     </row>
     <row r="114" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="169"/>
-      <c r="B114" s="142"/>
+      <c r="A114" s="173"/>
+      <c r="B114" s="165"/>
       <c r="C114" s="60" t="s">
         <v>329</v>
       </c>
@@ -12587,7 +12634,7 @@
       <c r="E114" s="23" t="s">
         <v>297</v>
       </c>
-      <c r="F114" s="186" t="s">
+      <c r="F114" s="151" t="s">
         <v>649</v>
       </c>
       <c r="G114" s="24" t="s">
@@ -12622,8 +12669,8 @@
       <c r="T114" s="23"/>
     </row>
     <row r="115" spans="1:20" s="33" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="170"/>
-      <c r="B115" s="143"/>
+      <c r="A115" s="174"/>
+      <c r="B115" s="170"/>
       <c r="C115" s="61" t="s">
         <v>322</v>
       </c>
@@ -12633,7 +12680,7 @@
       <c r="E115" s="45" t="s">
         <v>324</v>
       </c>
-      <c r="F115" s="171" t="s">
+      <c r="F115" s="138" t="s">
         <v>651</v>
       </c>
       <c r="G115" s="29" t="s">
@@ -12676,10 +12723,10 @@
       <c r="T115" s="28"/>
     </row>
     <row r="116" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="163" t="s">
+      <c r="A116" s="166" t="s">
         <v>504</v>
       </c>
-      <c r="B116" s="150" t="s">
+      <c r="B116" s="157" t="s">
         <v>55</v>
       </c>
       <c r="C116" s="62" t="s">
@@ -12722,8 +12769,8 @@
       <c r="T116" s="33"/>
     </row>
     <row r="117" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="164"/>
-      <c r="B117" s="148"/>
+      <c r="A117" s="167"/>
+      <c r="B117" s="158"/>
       <c r="C117" s="60" t="s">
         <v>96</v>
       </c>
@@ -12767,8 +12814,8 @@
       <c r="S117" s="26"/>
     </row>
     <row r="118" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="164"/>
-      <c r="B118" s="148"/>
+      <c r="A118" s="167"/>
+      <c r="B118" s="158"/>
       <c r="C118" s="60" t="s">
         <v>97</v>
       </c>
@@ -12812,8 +12859,8 @@
       <c r="S118" s="26"/>
     </row>
     <row r="119" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="164"/>
-      <c r="B119" s="148"/>
+      <c r="A119" s="167"/>
+      <c r="B119" s="158"/>
       <c r="C119" s="60" t="s">
         <v>108</v>
       </c>
@@ -12853,8 +12900,8 @@
       <c r="S119" s="26"/>
     </row>
     <row r="120" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="164"/>
-      <c r="B120" s="148"/>
+      <c r="A120" s="167"/>
+      <c r="B120" s="158"/>
       <c r="C120" s="61" t="s">
         <v>98</v>
       </c>
@@ -12895,8 +12942,8 @@
       <c r="T120" s="28"/>
     </row>
     <row r="121" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="164"/>
-      <c r="B121" s="148"/>
+      <c r="A121" s="167"/>
+      <c r="B121" s="158"/>
       <c r="C121" s="60" t="s">
         <v>183</v>
       </c>
@@ -12937,8 +12984,8 @@
       <c r="T121" s="28"/>
     </row>
     <row r="122" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="164"/>
-      <c r="B122" s="148"/>
+      <c r="A122" s="167"/>
+      <c r="B122" s="158"/>
       <c r="C122" s="61" t="s">
         <v>120</v>
       </c>
@@ -12979,8 +13026,8 @@
       <c r="T122" s="28"/>
     </row>
     <row r="123" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="164"/>
-      <c r="B123" s="148"/>
+      <c r="A123" s="167"/>
+      <c r="B123" s="158"/>
       <c r="C123" s="60" t="s">
         <v>100</v>
       </c>
@@ -13022,8 +13069,8 @@
       <c r="S123" s="26"/>
     </row>
     <row r="124" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="164"/>
-      <c r="B124" s="148"/>
+      <c r="A124" s="167"/>
+      <c r="B124" s="158"/>
       <c r="C124" s="60" t="s">
         <v>505</v>
       </c>
@@ -13065,8 +13112,8 @@
       <c r="S124" s="26"/>
     </row>
     <row r="125" spans="1:20" s="23" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="164"/>
-      <c r="B125" s="166"/>
+      <c r="A125" s="167"/>
+      <c r="B125" s="169"/>
       <c r="C125" s="60" t="s">
         <v>180</v>
       </c>
@@ -13106,8 +13153,8 @@
       <c r="S125" s="26"/>
     </row>
     <row r="126" spans="1:20" s="28" customFormat="1" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="164"/>
-      <c r="B126" s="153" t="s">
+      <c r="A126" s="167"/>
+      <c r="B126" s="164" t="s">
         <v>197</v>
       </c>
       <c r="C126" s="63" t="s">
@@ -13152,8 +13199,8 @@
       <c r="T126" s="23"/>
     </row>
     <row r="127" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="164"/>
-      <c r="B127" s="142"/>
+      <c r="A127" s="167"/>
+      <c r="B127" s="165"/>
       <c r="C127" s="60" t="s">
         <v>452</v>
       </c>
@@ -13194,8 +13241,8 @@
       <c r="T127" s="23"/>
     </row>
     <row r="128" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="164"/>
-      <c r="B128" s="142"/>
+      <c r="A128" s="167"/>
+      <c r="B128" s="165"/>
       <c r="C128" s="60" t="s">
         <v>455</v>
       </c>
@@ -13236,8 +13283,8 @@
       <c r="T128" s="23"/>
     </row>
     <row r="129" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="164"/>
-      <c r="B129" s="142"/>
+      <c r="A129" s="167"/>
+      <c r="B129" s="165"/>
       <c r="C129" s="61" t="s">
         <v>429</v>
       </c>
@@ -13280,8 +13327,8 @@
       <c r="T129" s="23"/>
     </row>
     <row r="130" spans="1:20" s="33" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="164"/>
-      <c r="B130" s="142"/>
+      <c r="A130" s="167"/>
+      <c r="B130" s="165"/>
       <c r="C130" s="60" t="s">
         <v>234</v>
       </c>
@@ -13322,8 +13369,8 @@
       <c r="T130" s="23"/>
     </row>
     <row r="131" spans="1:20" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="164"/>
-      <c r="B131" s="142"/>
+      <c r="A131" s="167"/>
+      <c r="B131" s="165"/>
       <c r="C131" s="60" t="s">
         <v>212</v>
       </c>
@@ -13364,8 +13411,8 @@
       <c r="T131" s="23"/>
     </row>
     <row r="132" spans="1:20" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="165"/>
-      <c r="B132" s="142"/>
+      <c r="A132" s="168"/>
+      <c r="B132" s="165"/>
       <c r="C132" s="65" t="s">
         <v>632</v>
       </c>
@@ -13388,10 +13435,10 @@
       <c r="T132" s="23"/>
     </row>
     <row r="133" spans="1:20" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="160" t="s">
+      <c r="A133" s="161" t="s">
         <v>115</v>
       </c>
-      <c r="B133" s="150" t="s">
+      <c r="B133" s="157" t="s">
         <v>55</v>
       </c>
       <c r="C133" s="62" t="s">
@@ -13434,8 +13481,8 @@
       <c r="T133" s="33"/>
     </row>
     <row r="134" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="161"/>
-      <c r="B134" s="148"/>
+      <c r="A134" s="162"/>
+      <c r="B134" s="158"/>
       <c r="C134" s="61" t="s">
         <v>99</v>
       </c>
@@ -13475,8 +13522,8 @@
       <c r="S134" s="31"/>
     </row>
     <row r="135" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="161"/>
-      <c r="B135" s="148"/>
+      <c r="A135" s="162"/>
+      <c r="B135" s="158"/>
       <c r="C135" s="65" t="s">
         <v>610</v>
       </c>
@@ -13519,8 +13566,8 @@
       <c r="T135" s="19"/>
     </row>
     <row r="136" spans="1:20" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="161"/>
-      <c r="B136" s="148"/>
+      <c r="A136" s="162"/>
+      <c r="B136" s="158"/>
       <c r="C136" s="60" t="s">
         <v>119</v>
       </c>
@@ -13562,8 +13609,8 @@
       <c r="T136" s="19"/>
     </row>
     <row r="137" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A137" s="161"/>
-      <c r="B137" s="148"/>
+      <c r="A137" s="162"/>
+      <c r="B137" s="158"/>
       <c r="C137" s="60" t="s">
         <v>118</v>
       </c>
@@ -13605,8 +13652,8 @@
       <c r="T137" s="19"/>
     </row>
     <row r="138" spans="1:20" s="23" customFormat="1" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="161"/>
-      <c r="B138" s="153" t="s">
+      <c r="A138" s="162"/>
+      <c r="B138" s="164" t="s">
         <v>197</v>
       </c>
       <c r="C138" s="63" t="s">
@@ -13648,8 +13695,8 @@
       <c r="S138" s="57"/>
     </row>
     <row r="139" spans="1:20" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="161"/>
-      <c r="B139" s="142"/>
+      <c r="A139" s="162"/>
+      <c r="B139" s="165"/>
       <c r="C139" s="60" t="s">
         <v>403</v>
       </c>
@@ -13688,8 +13735,8 @@
       <c r="S139" s="26"/>
     </row>
     <row r="140" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="161"/>
-      <c r="B140" s="142"/>
+      <c r="A140" s="162"/>
+      <c r="B140" s="165"/>
       <c r="C140" s="60" t="s">
         <v>259</v>
       </c>
@@ -13729,8 +13776,8 @@
       <c r="S140" s="26"/>
     </row>
     <row r="141" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="161"/>
-      <c r="B141" s="142"/>
+      <c r="A141" s="162"/>
+      <c r="B141" s="165"/>
       <c r="C141" s="65" t="s">
         <v>626</v>
       </c>
@@ -13764,8 +13811,8 @@
       <c r="S141" s="26"/>
     </row>
     <row r="142" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="161"/>
-      <c r="B142" s="142"/>
+      <c r="A142" s="162"/>
+      <c r="B142" s="165"/>
       <c r="C142" s="60" t="s">
         <v>426</v>
       </c>
@@ -13805,8 +13852,8 @@
       <c r="S142" s="26"/>
     </row>
     <row r="143" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="161"/>
-      <c r="B143" s="142"/>
+      <c r="A143" s="162"/>
+      <c r="B143" s="165"/>
       <c r="C143" s="60" t="s">
         <v>384</v>
       </c>
@@ -13846,8 +13893,8 @@
       <c r="S143" s="26"/>
     </row>
     <row r="144" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="161"/>
-      <c r="B144" s="142"/>
+      <c r="A144" s="162"/>
+      <c r="B144" s="165"/>
       <c r="C144" s="60" t="s">
         <v>443</v>
       </c>
@@ -13887,8 +13934,8 @@
       <c r="S144" s="26"/>
     </row>
     <row r="145" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="161"/>
-      <c r="B145" s="142"/>
+      <c r="A145" s="162"/>
+      <c r="B145" s="165"/>
       <c r="C145" s="60" t="s">
         <v>362</v>
       </c>
@@ -13928,8 +13975,8 @@
       <c r="S145" s="26"/>
     </row>
     <row r="146" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="161"/>
-      <c r="B146" s="142"/>
+      <c r="A146" s="162"/>
+      <c r="B146" s="165"/>
       <c r="C146" s="60" t="s">
         <v>230</v>
       </c>
@@ -13969,8 +14016,8 @@
       <c r="S146" s="26"/>
     </row>
     <row r="147" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="161"/>
-      <c r="B147" s="142"/>
+      <c r="A147" s="162"/>
+      <c r="B147" s="165"/>
       <c r="C147" s="60" t="s">
         <v>425</v>
       </c>
@@ -14010,8 +14057,8 @@
       <c r="S147" s="26"/>
     </row>
     <row r="148" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="161"/>
-      <c r="B148" s="142"/>
+      <c r="A148" s="162"/>
+      <c r="B148" s="165"/>
       <c r="C148" s="60" t="s">
         <v>400</v>
       </c>
@@ -14051,8 +14098,8 @@
       <c r="S148" s="26"/>
     </row>
     <row r="149" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="161"/>
-      <c r="B149" s="142"/>
+      <c r="A149" s="162"/>
+      <c r="B149" s="165"/>
       <c r="C149" s="60" t="s">
         <v>437</v>
       </c>
@@ -14092,8 +14139,8 @@
       <c r="S149" s="26"/>
     </row>
     <row r="150" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="161"/>
-      <c r="B150" s="142"/>
+      <c r="A150" s="162"/>
+      <c r="B150" s="165"/>
       <c r="C150" s="60" t="s">
         <v>410</v>
       </c>
@@ -14133,8 +14180,8 @@
       <c r="S150" s="26"/>
     </row>
     <row r="151" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="161"/>
-      <c r="B151" s="142"/>
+      <c r="A151" s="162"/>
+      <c r="B151" s="165"/>
       <c r="C151" s="65" t="s">
         <v>525</v>
       </c>
@@ -14174,8 +14221,8 @@
       <c r="S151" s="26"/>
     </row>
     <row r="152" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="161"/>
-      <c r="B152" s="142"/>
+      <c r="A152" s="162"/>
+      <c r="B152" s="165"/>
       <c r="C152" s="65" t="s">
         <v>260</v>
       </c>
@@ -14215,8 +14262,8 @@
       <c r="S152" s="26"/>
     </row>
     <row r="153" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="161"/>
-      <c r="B153" s="142"/>
+      <c r="A153" s="162"/>
+      <c r="B153" s="165"/>
       <c r="C153" s="65" t="s">
         <v>450</v>
       </c>
@@ -14256,8 +14303,8 @@
       <c r="S153" s="26"/>
     </row>
     <row r="154" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="161"/>
-      <c r="B154" s="142"/>
+      <c r="A154" s="162"/>
+      <c r="B154" s="165"/>
       <c r="C154" s="65" t="s">
         <v>439</v>
       </c>
@@ -14297,8 +14344,8 @@
       <c r="S154" s="26"/>
     </row>
     <row r="155" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="161"/>
-      <c r="B155" s="142"/>
+      <c r="A155" s="162"/>
+      <c r="B155" s="165"/>
       <c r="C155" s="65" t="s">
         <v>323</v>
       </c>
@@ -14340,8 +14387,8 @@
       <c r="S155" s="26"/>
     </row>
     <row r="156" spans="1:19" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="161"/>
-      <c r="B156" s="142"/>
+      <c r="A156" s="162"/>
+      <c r="B156" s="165"/>
       <c r="C156" s="65" t="s">
         <v>370</v>
       </c>
@@ -14381,8 +14428,8 @@
       <c r="S156" s="26"/>
     </row>
     <row r="157" spans="1:19" s="23" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A157" s="162"/>
-      <c r="B157" s="142"/>
+      <c r="A157" s="163"/>
+      <c r="B157" s="165"/>
       <c r="C157" s="65" t="s">
         <v>215</v>
       </c>
@@ -14422,10 +14469,10 @@
       <c r="S157" s="31"/>
     </row>
     <row r="158" spans="1:19" s="33" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A158" s="151" t="s">
+      <c r="A158" s="183" t="s">
         <v>116</v>
       </c>
-      <c r="B158" s="141" t="s">
+      <c r="B158" s="178" t="s">
         <v>197</v>
       </c>
       <c r="C158" s="62" t="s">
@@ -14469,8 +14516,8 @@
       <c r="S158" s="36"/>
     </row>
     <row r="159" spans="1:19" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A159" s="151"/>
-      <c r="B159" s="142"/>
+      <c r="A159" s="183"/>
+      <c r="B159" s="165"/>
       <c r="C159" s="60" t="s">
         <v>366</v>
       </c>
@@ -14512,8 +14559,8 @@
       <c r="S159" s="26"/>
     </row>
     <row r="160" spans="1:19" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A160" s="151"/>
-      <c r="B160" s="142"/>
+      <c r="A160" s="183"/>
+      <c r="B160" s="165"/>
       <c r="C160" s="60" t="s">
         <v>385</v>
       </c>
@@ -14555,8 +14602,8 @@
       <c r="S160" s="26"/>
     </row>
     <row r="161" spans="1:19" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A161" s="151"/>
-      <c r="B161" s="142"/>
+      <c r="A161" s="183"/>
+      <c r="B161" s="165"/>
       <c r="C161" s="60" t="s">
         <v>396</v>
       </c>
@@ -14598,8 +14645,8 @@
       <c r="S161" s="26"/>
     </row>
     <row r="162" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A162" s="151"/>
-      <c r="B162" s="142"/>
+      <c r="A162" s="183"/>
+      <c r="B162" s="165"/>
       <c r="C162" s="60" t="s">
         <v>254</v>
       </c>
@@ -14639,8 +14686,8 @@
       <c r="S162" s="26"/>
     </row>
     <row r="163" spans="1:19" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A163" s="151"/>
-      <c r="B163" s="142"/>
+      <c r="A163" s="183"/>
+      <c r="B163" s="165"/>
       <c r="C163" s="61" t="s">
         <v>405</v>
       </c>
@@ -14682,8 +14729,8 @@
       <c r="S163" s="26"/>
     </row>
     <row r="164" spans="1:19" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A164" s="151"/>
-      <c r="B164" s="142"/>
+      <c r="A164" s="183"/>
+      <c r="B164" s="165"/>
       <c r="C164" s="60" t="s">
         <v>376</v>
       </c>
@@ -14723,8 +14770,8 @@
       <c r="S164" s="26"/>
     </row>
     <row r="165" spans="1:19" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A165" s="151"/>
-      <c r="B165" s="143"/>
+      <c r="A165" s="183"/>
+      <c r="B165" s="170"/>
       <c r="C165" s="60" t="s">
         <v>406</v>
       </c>
@@ -14764,7 +14811,7 @@
       <c r="S165" s="31"/>
     </row>
     <row r="166" spans="1:19" s="33" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A166" s="152" t="s">
+      <c r="A166" s="184" t="s">
         <v>539</v>
       </c>
       <c r="B166" s="72" t="s">
@@ -14807,8 +14854,8 @@
       <c r="S166" s="71"/>
     </row>
     <row r="167" spans="1:19" s="23" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A167" s="152"/>
-      <c r="B167" s="153" t="s">
+      <c r="A167" s="184"/>
+      <c r="B167" s="164" t="s">
         <v>197</v>
       </c>
       <c r="C167" s="60" t="s">
@@ -14846,8 +14893,8 @@
       <c r="S167" s="57"/>
     </row>
     <row r="168" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A168" s="152"/>
-      <c r="B168" s="142"/>
+      <c r="A168" s="184"/>
+      <c r="B168" s="165"/>
       <c r="C168" s="60" t="s">
         <v>199</v>
       </c>
@@ -14882,8 +14929,8 @@
       <c r="S168" s="26"/>
     </row>
     <row r="169" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="152"/>
-      <c r="B169" s="142"/>
+      <c r="A169" s="184"/>
+      <c r="B169" s="165"/>
       <c r="C169" s="60" t="s">
         <v>263</v>
       </c>
@@ -14921,8 +14968,8 @@
       <c r="S169" s="26"/>
     </row>
     <row r="170" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A170" s="152"/>
-      <c r="B170" s="142"/>
+      <c r="A170" s="184"/>
+      <c r="B170" s="165"/>
       <c r="C170" s="60" t="s">
         <v>421</v>
       </c>
@@ -14959,8 +15006,8 @@
       <c r="S170" s="26"/>
     </row>
     <row r="171" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A171" s="152"/>
-      <c r="B171" s="154"/>
+      <c r="A171" s="184"/>
+      <c r="B171" s="185"/>
       <c r="C171" s="60" t="s">
         <v>422</v>
       </c>
@@ -14998,10 +15045,10 @@
       <c r="S171" s="26"/>
     </row>
     <row r="172" spans="1:19" s="33" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A172" s="140" t="s">
+      <c r="A172" s="177" t="s">
         <v>117</v>
       </c>
-      <c r="B172" s="147" t="s">
+      <c r="B172" s="181" t="s">
         <v>55</v>
       </c>
       <c r="C172" s="62" t="s">
@@ -15041,8 +15088,8 @@
       <c r="S172" s="36"/>
     </row>
     <row r="173" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A173" s="140"/>
-      <c r="B173" s="148"/>
+      <c r="A173" s="177"/>
+      <c r="B173" s="158"/>
       <c r="C173" s="60" t="s">
         <v>188</v>
       </c>
@@ -15080,8 +15127,8 @@
       <c r="S173" s="26"/>
     </row>
     <row r="174" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A174" s="140"/>
-      <c r="B174" s="148"/>
+      <c r="A174" s="177"/>
+      <c r="B174" s="158"/>
       <c r="C174" s="60" t="s">
         <v>187</v>
       </c>
@@ -15119,8 +15166,8 @@
       <c r="S174" s="26"/>
     </row>
     <row r="175" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A175" s="140"/>
-      <c r="B175" s="148"/>
+      <c r="A175" s="177"/>
+      <c r="B175" s="158"/>
       <c r="C175" s="61" t="s">
         <v>189</v>
       </c>
@@ -15158,8 +15205,8 @@
       <c r="S175" s="31"/>
     </row>
     <row r="176" spans="1:19" s="23" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A176" s="140"/>
-      <c r="B176" s="138" t="s">
+      <c r="A176" s="177"/>
+      <c r="B176" s="175" t="s">
         <v>197</v>
       </c>
       <c r="C176" s="63" t="s">
@@ -15193,8 +15240,8 @@
       <c r="S176" s="57"/>
     </row>
     <row r="177" spans="1:19" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A177" s="140"/>
-      <c r="B177" s="139"/>
+      <c r="A177" s="177"/>
+      <c r="B177" s="176"/>
       <c r="C177" s="64"/>
       <c r="E177" s="49"/>
       <c r="F177" s="49"/>
@@ -15923,18 +15970,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="C3:S3"/>
-    <mergeCell ref="B51:B55"/>
-    <mergeCell ref="A51:A69"/>
-    <mergeCell ref="A133:A157"/>
-    <mergeCell ref="B138:B157"/>
-    <mergeCell ref="A116:A132"/>
-    <mergeCell ref="B116:B125"/>
-    <mergeCell ref="B81:B115"/>
-    <mergeCell ref="B56:B69"/>
-    <mergeCell ref="B70:B80"/>
-    <mergeCell ref="A70:A115"/>
-    <mergeCell ref="B133:B137"/>
     <mergeCell ref="B176:B177"/>
     <mergeCell ref="A172:A177"/>
     <mergeCell ref="B158:B165"/>
@@ -15950,6 +15985,18 @@
     <mergeCell ref="B126:B132"/>
     <mergeCell ref="A37:A50"/>
     <mergeCell ref="B41:B50"/>
+    <mergeCell ref="C3:S3"/>
+    <mergeCell ref="B51:B55"/>
+    <mergeCell ref="A51:A69"/>
+    <mergeCell ref="A133:A157"/>
+    <mergeCell ref="B138:B157"/>
+    <mergeCell ref="A116:A132"/>
+    <mergeCell ref="B116:B125"/>
+    <mergeCell ref="B81:B115"/>
+    <mergeCell ref="B56:B69"/>
+    <mergeCell ref="B70:B80"/>
+    <mergeCell ref="A70:A115"/>
+    <mergeCell ref="B133:B137"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Airdrop Waffen Übersicht zugefuegt
</commit_message>
<xml_diff>
--- a/ressources/DayZ Mods.xlsx
+++ b/ressources/DayZ Mods.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\projects\Immersive-DayZ-Experience\ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB00993-D91E-473A-A17C-30768229314C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4225BFAF-50C1-405C-BEB1-6B799BEBC9F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="260" xr2:uid="{FAEB3C3F-74B0-4C80-8C8B-4522341FA132}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="260" activeTab="1" xr2:uid="{FAEB3C3F-74B0-4C80-8C8B-4522341FA132}"/>
   </bookViews>
   <sheets>
     <sheet name="Mods" sheetId="1" r:id="rId1"/>
@@ -3470,7 +3470,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="196">
+  <cellXfs count="192">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3817,14 +3817,70 @@
     <xf numFmtId="0" fontId="2" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -3841,12 +3897,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -3857,9 +3907,6 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3873,65 +3920,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4723,7 +4711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BE2B301-FC9E-4F7D-A454-62A8C1115EDF}">
   <dimension ref="A1:Q87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="O28" sqref="O28"/>
     </sheetView>
@@ -7185,17 +7173,13 @@
       <c r="L73" s="38"/>
     </row>
     <row r="74" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="191"/>
-      <c r="C74" s="192"/>
-      <c r="D74" s="193"/>
-      <c r="E74" s="194"/>
-      <c r="F74" s="195"/>
-      <c r="G74" s="193"/>
-      <c r="H74" s="193"/>
-      <c r="I74" s="193"/>
-      <c r="J74" s="193"/>
-      <c r="K74" s="193"/>
-      <c r="L74" s="193"/>
+      <c r="B74" s="158"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2"/>
+      <c r="I74" s="2"/>
+      <c r="J74" s="2"/>
+      <c r="K74" s="2"/>
+      <c r="L74" s="2"/>
     </row>
     <row r="76" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="117">
@@ -7563,8 +7547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FF4763-6B65-4CE2-BD87-511E98A2E639}">
   <dimension ref="A1:V225"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W124" sqref="W124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7585,7 +7569,7 @@
     <col min="14" max="14" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.28515625" style="2" customWidth="1"/>
     <col min="16" max="18" width="11.140625" style="2" customWidth="1"/>
-    <col min="19" max="19" width="9.7109375" style="17" customWidth="1"/>
+    <col min="19" max="19" width="9.85546875" style="17" customWidth="1"/>
     <col min="20" max="20" width="77.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7596,25 +7580,25 @@
       <c r="S2"/>
     </row>
     <row r="3" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="156" t="s">
+      <c r="C3" s="178" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="156"/>
-      <c r="E3" s="156"/>
-      <c r="F3" s="156"/>
-      <c r="G3" s="156"/>
-      <c r="H3" s="156"/>
-      <c r="I3" s="156"/>
-      <c r="J3" s="156"/>
-      <c r="K3" s="156"/>
-      <c r="L3" s="156"/>
-      <c r="M3" s="156"/>
-      <c r="N3" s="156"/>
-      <c r="O3" s="156"/>
-      <c r="P3" s="156"/>
-      <c r="Q3" s="156"/>
-      <c r="R3" s="156"/>
-      <c r="S3" s="156"/>
+      <c r="D3" s="178"/>
+      <c r="E3" s="178"/>
+      <c r="F3" s="178"/>
+      <c r="G3" s="178"/>
+      <c r="H3" s="178"/>
+      <c r="I3" s="178"/>
+      <c r="J3" s="178"/>
+      <c r="K3" s="178"/>
+      <c r="L3" s="178"/>
+      <c r="M3" s="178"/>
+      <c r="N3" s="178"/>
+      <c r="O3" s="178"/>
+      <c r="P3" s="178"/>
+      <c r="Q3" s="178"/>
+      <c r="R3" s="178"/>
+      <c r="S3" s="178"/>
     </row>
     <row r="4" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
@@ -7629,19 +7613,19 @@
       <c r="F4" s="3" t="s">
         <v>653</v>
       </c>
-      <c r="G4" s="180"/>
-      <c r="H4" s="180"/>
-      <c r="I4" s="180"/>
-      <c r="J4" s="180"/>
-      <c r="K4" s="180"/>
-      <c r="L4" s="180"/>
-      <c r="M4" s="180"/>
-      <c r="N4" s="180"/>
-      <c r="O4" s="180"/>
-      <c r="P4" s="180"/>
-      <c r="Q4" s="180"/>
-      <c r="R4" s="180"/>
-      <c r="S4" s="180"/>
+      <c r="G4" s="166"/>
+      <c r="H4" s="166"/>
+      <c r="I4" s="166"/>
+      <c r="J4" s="166"/>
+      <c r="K4" s="166"/>
+      <c r="L4" s="166"/>
+      <c r="M4" s="166"/>
+      <c r="N4" s="166"/>
+      <c r="O4" s="166"/>
+      <c r="P4" s="166"/>
+      <c r="Q4" s="166"/>
+      <c r="R4" s="166"/>
+      <c r="S4" s="166"/>
     </row>
     <row r="5" spans="1:22" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="3"/>
@@ -7692,10 +7676,10 @@
       </c>
     </row>
     <row r="6" spans="1:22" s="23" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="179" t="s">
+      <c r="A6" s="165" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="181" t="s">
+      <c r="B6" s="167" t="s">
         <v>55</v>
       </c>
       <c r="C6" s="18" t="s">
@@ -7757,8 +7741,8 @@
       </c>
     </row>
     <row r="7" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="179"/>
-      <c r="B7" s="158"/>
+      <c r="A7" s="165"/>
+      <c r="B7" s="168"/>
       <c r="C7" s="60" t="s">
         <v>46</v>
       </c>
@@ -7809,8 +7793,8 @@
       </c>
     </row>
     <row r="8" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="179"/>
-      <c r="B8" s="158"/>
+      <c r="A8" s="165"/>
+      <c r="B8" s="168"/>
       <c r="C8" s="60" t="s">
         <v>53</v>
       </c>
@@ -7859,8 +7843,8 @@
       </c>
     </row>
     <row r="9" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="179"/>
-      <c r="B9" s="158"/>
+      <c r="A9" s="165"/>
+      <c r="B9" s="168"/>
       <c r="C9" s="60" t="s">
         <v>287</v>
       </c>
@@ -7911,8 +7895,8 @@
       </c>
     </row>
     <row r="10" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="179"/>
-      <c r="B10" s="158"/>
+      <c r="A10" s="165"/>
+      <c r="B10" s="168"/>
       <c r="C10" s="60" t="s">
         <v>47</v>
       </c>
@@ -7956,13 +7940,13 @@
       <c r="Q10" s="41"/>
       <c r="R10" s="130"/>
       <c r="S10" s="26"/>
-      <c r="V10" s="190" t="s">
+      <c r="V10" s="157" t="s">
         <v>648</v>
       </c>
     </row>
     <row r="11" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="179"/>
-      <c r="B11" s="158"/>
+      <c r="A11" s="165"/>
+      <c r="B11" s="168"/>
       <c r="C11" s="60" t="s">
         <v>63</v>
       </c>
@@ -8010,8 +7994,8 @@
       </c>
     </row>
     <row r="12" spans="1:22" s="23" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="179"/>
-      <c r="B12" s="158"/>
+      <c r="A12" s="165"/>
+      <c r="B12" s="168"/>
       <c r="C12" s="60" t="s">
         <v>48</v>
       </c>
@@ -8057,8 +8041,8 @@
       <c r="S12" s="26"/>
     </row>
     <row r="13" spans="1:22" s="23" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="179"/>
-      <c r="B13" s="158"/>
+      <c r="A13" s="165"/>
+      <c r="B13" s="168"/>
       <c r="C13" s="60" t="s">
         <v>645</v>
       </c>
@@ -8092,8 +8076,8 @@
       <c r="S13" s="26"/>
     </row>
     <row r="14" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="179"/>
-      <c r="B14" s="158"/>
+      <c r="A14" s="165"/>
+      <c r="B14" s="168"/>
       <c r="C14" s="60" t="s">
         <v>49</v>
       </c>
@@ -8139,8 +8123,8 @@
       <c r="S14" s="26"/>
     </row>
     <row r="15" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="179"/>
-      <c r="B15" s="158"/>
+      <c r="A15" s="165"/>
+      <c r="B15" s="168"/>
       <c r="C15" s="60" t="s">
         <v>78</v>
       </c>
@@ -8186,8 +8170,8 @@
       <c r="S15" s="26"/>
     </row>
     <row r="16" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="179"/>
-      <c r="B16" s="158"/>
+      <c r="A16" s="165"/>
+      <c r="B16" s="168"/>
       <c r="C16" s="60" t="s">
         <v>50</v>
       </c>
@@ -8197,7 +8181,7 @@
       <c r="E16" s="23" t="s">
         <v>465</v>
       </c>
-      <c r="F16" s="190" t="s">
+      <c r="F16" s="157" t="s">
         <v>648</v>
       </c>
       <c r="G16" s="24" t="s">
@@ -8231,8 +8215,8 @@
       <c r="S16" s="26"/>
     </row>
     <row r="17" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="179"/>
-      <c r="B17" s="158"/>
+      <c r="A17" s="165"/>
+      <c r="B17" s="168"/>
       <c r="C17" s="60" t="s">
         <v>51</v>
       </c>
@@ -8242,7 +8226,7 @@
       <c r="E17" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="190" t="s">
+      <c r="F17" s="157" t="s">
         <v>648</v>
       </c>
       <c r="G17" s="24" t="s">
@@ -8276,8 +8260,8 @@
       <c r="S17" s="26"/>
     </row>
     <row r="18" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="179"/>
-      <c r="B18" s="158"/>
+      <c r="A18" s="165"/>
+      <c r="B18" s="168"/>
       <c r="C18" s="60" t="s">
         <v>52</v>
       </c>
@@ -8287,7 +8271,7 @@
       <c r="E18" s="23" t="s">
         <v>466</v>
       </c>
-      <c r="F18" s="190" t="s">
+      <c r="F18" s="157" t="s">
         <v>648</v>
       </c>
       <c r="G18" s="24" t="s">
@@ -8321,8 +8305,8 @@
       <c r="S18" s="26"/>
     </row>
     <row r="19" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="179"/>
-      <c r="B19" s="158"/>
+      <c r="A19" s="165"/>
+      <c r="B19" s="168"/>
       <c r="C19" s="60" t="s">
         <v>350</v>
       </c>
@@ -8332,7 +8316,7 @@
       <c r="E19" s="23" t="s">
         <v>467</v>
       </c>
-      <c r="F19" s="190" t="s">
+      <c r="F19" s="157" t="s">
         <v>648</v>
       </c>
       <c r="G19" s="24" t="s">
@@ -8368,8 +8352,8 @@
       <c r="S19" s="26"/>
     </row>
     <row r="20" spans="1:20" s="40" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="179"/>
-      <c r="B20" s="182"/>
+      <c r="A20" s="165"/>
+      <c r="B20" s="169"/>
       <c r="C20" s="61" t="s">
         <v>54</v>
       </c>
@@ -8411,8 +8395,8 @@
       <c r="S20" s="31"/>
     </row>
     <row r="21" spans="1:20" s="33" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="179"/>
-      <c r="B21" s="178" t="s">
+      <c r="A21" s="165"/>
+      <c r="B21" s="162" t="s">
         <v>250</v>
       </c>
       <c r="C21" s="120" t="s">
@@ -8463,8 +8447,8 @@
       </c>
     </row>
     <row r="22" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="179"/>
-      <c r="B22" s="165"/>
+      <c r="A22" s="165"/>
+      <c r="B22" s="163"/>
       <c r="C22" s="61" t="s">
         <v>237</v>
       </c>
@@ -8508,8 +8492,8 @@
       <c r="S22" s="26"/>
     </row>
     <row r="23" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="179"/>
-      <c r="B23" s="165"/>
+      <c r="A23" s="165"/>
+      <c r="B23" s="163"/>
       <c r="C23" s="60" t="s">
         <v>49</v>
       </c>
@@ -8553,8 +8537,8 @@
       <c r="S23" s="26"/>
     </row>
     <row r="24" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="179"/>
-      <c r="B24" s="165"/>
+      <c r="A24" s="165"/>
+      <c r="B24" s="163"/>
       <c r="C24" s="60" t="s">
         <v>124</v>
       </c>
@@ -8600,8 +8584,8 @@
       <c r="S24" s="26"/>
     </row>
     <row r="25" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="179"/>
-      <c r="B25" s="165"/>
+      <c r="A25" s="165"/>
+      <c r="B25" s="163"/>
       <c r="C25" s="60" t="s">
         <v>239</v>
       </c>
@@ -8649,8 +8633,8 @@
       <c r="S25" s="26"/>
     </row>
     <row r="26" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="179"/>
-      <c r="B26" s="165"/>
+      <c r="A26" s="165"/>
+      <c r="B26" s="163"/>
       <c r="C26" s="60" t="s">
         <v>354</v>
       </c>
@@ -8694,8 +8678,8 @@
       <c r="S26" s="26"/>
     </row>
     <row r="27" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="179"/>
-      <c r="B27" s="165"/>
+      <c r="A27" s="165"/>
+      <c r="B27" s="163"/>
       <c r="C27" s="60" t="s">
         <v>123</v>
       </c>
@@ -8739,8 +8723,8 @@
       <c r="S27" s="26"/>
     </row>
     <row r="28" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="179"/>
-      <c r="B28" s="165"/>
+      <c r="A28" s="165"/>
+      <c r="B28" s="163"/>
       <c r="C28" s="60" t="s">
         <v>469</v>
       </c>
@@ -8784,8 +8768,8 @@
       <c r="S28" s="26"/>
     </row>
     <row r="29" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="179"/>
-      <c r="B29" s="165"/>
+      <c r="A29" s="165"/>
+      <c r="B29" s="163"/>
       <c r="C29" s="60" t="s">
         <v>389</v>
       </c>
@@ -8831,8 +8815,8 @@
       <c r="S29" s="26"/>
     </row>
     <row r="30" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="179"/>
-      <c r="B30" s="165"/>
+      <c r="A30" s="165"/>
+      <c r="B30" s="163"/>
       <c r="C30" s="60" t="s">
         <v>242</v>
       </c>
@@ -8879,8 +8863,8 @@
       <c r="T30" s="23"/>
     </row>
     <row r="31" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="179"/>
-      <c r="B31" s="165"/>
+      <c r="A31" s="165"/>
+      <c r="B31" s="163"/>
       <c r="C31" s="60" t="s">
         <v>355</v>
       </c>
@@ -8926,8 +8910,8 @@
       <c r="S31" s="26"/>
     </row>
     <row r="32" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="179"/>
-      <c r="B32" s="165"/>
+      <c r="A32" s="165"/>
+      <c r="B32" s="163"/>
       <c r="C32" s="60" t="s">
         <v>220</v>
       </c>
@@ -8974,8 +8958,8 @@
       <c r="T32" s="23"/>
     </row>
     <row r="33" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="179"/>
-      <c r="B33" s="165"/>
+      <c r="A33" s="165"/>
+      <c r="B33" s="163"/>
       <c r="C33" s="60" t="s">
         <v>246</v>
       </c>
@@ -9021,8 +9005,8 @@
       <c r="S33" s="26"/>
     </row>
     <row r="34" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="179"/>
-      <c r="B34" s="165"/>
+      <c r="A34" s="165"/>
+      <c r="B34" s="163"/>
       <c r="C34" s="60" t="s">
         <v>379</v>
       </c>
@@ -9032,7 +9016,7 @@
       <c r="E34" s="23" t="s">
         <v>380</v>
       </c>
-      <c r="F34" s="190" t="s">
+      <c r="F34" s="157" t="s">
         <v>648</v>
       </c>
       <c r="G34" s="24" t="s">
@@ -9066,8 +9050,8 @@
       <c r="S34" s="26"/>
     </row>
     <row r="35" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="179"/>
-      <c r="B35" s="165"/>
+      <c r="A35" s="165"/>
+      <c r="B35" s="163"/>
       <c r="C35" s="60" t="s">
         <v>392</v>
       </c>
@@ -9077,7 +9061,7 @@
       <c r="E35" s="23" t="s">
         <v>393</v>
       </c>
-      <c r="F35" s="190" t="s">
+      <c r="F35" s="157" t="s">
         <v>648</v>
       </c>
       <c r="G35" s="24" t="s">
@@ -9111,8 +9095,8 @@
       <c r="S35" s="26"/>
     </row>
     <row r="36" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="179"/>
-      <c r="B36" s="170"/>
+      <c r="A36" s="165"/>
+      <c r="B36" s="164"/>
       <c r="C36" s="65" t="s">
         <v>238</v>
       </c>
@@ -9156,10 +9140,10 @@
       <c r="S36" s="26"/>
     </row>
     <row r="37" spans="1:20" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="186" t="s">
+      <c r="A37" s="175" t="s">
         <v>270</v>
       </c>
-      <c r="B37" s="157" t="s">
+      <c r="B37" s="170" t="s">
         <v>55</v>
       </c>
       <c r="C37" s="62" t="s">
@@ -9204,8 +9188,8 @@
       <c r="T37" s="33"/>
     </row>
     <row r="38" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="187"/>
-      <c r="B38" s="158"/>
+      <c r="A38" s="176"/>
+      <c r="B38" s="168"/>
       <c r="C38" s="60" t="s">
         <v>111</v>
       </c>
@@ -9247,8 +9231,8 @@
       <c r="S38" s="26"/>
     </row>
     <row r="39" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="187"/>
-      <c r="B39" s="158"/>
+      <c r="A39" s="176"/>
+      <c r="B39" s="168"/>
       <c r="C39" s="60" t="s">
         <v>112</v>
       </c>
@@ -9291,8 +9275,8 @@
       <c r="T39" s="23"/>
     </row>
     <row r="40" spans="1:20" s="28" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="187"/>
-      <c r="B40" s="158"/>
+      <c r="A40" s="176"/>
+      <c r="B40" s="168"/>
       <c r="C40" s="61" t="s">
         <v>113</v>
       </c>
@@ -9302,7 +9286,7 @@
       <c r="E40" s="44" t="s">
         <v>496</v>
       </c>
-      <c r="F40" s="189" t="s">
+      <c r="F40" s="156" t="s">
         <v>652</v>
       </c>
       <c r="G40" s="29" t="s">
@@ -9340,8 +9324,8 @@
       <c r="S40" s="31"/>
     </row>
     <row r="41" spans="1:20" s="28" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="187"/>
-      <c r="B41" s="164" t="s">
+      <c r="A41" s="176"/>
+      <c r="B41" s="173" t="s">
         <v>197</v>
       </c>
       <c r="C41" s="63" t="s">
@@ -9387,8 +9371,8 @@
       <c r="S41" s="57"/>
     </row>
     <row r="42" spans="1:20" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="187"/>
-      <c r="B42" s="165"/>
+      <c r="A42" s="176"/>
+      <c r="B42" s="163"/>
       <c r="C42" s="60" t="s">
         <v>222</v>
       </c>
@@ -9428,8 +9412,8 @@
       <c r="S42" s="26"/>
     </row>
     <row r="43" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="187"/>
-      <c r="B43" s="165"/>
+      <c r="A43" s="176"/>
+      <c r="B43" s="163"/>
       <c r="C43" s="60" t="s">
         <v>262</v>
       </c>
@@ -9469,8 +9453,8 @@
       <c r="S43" s="26"/>
     </row>
     <row r="44" spans="1:20" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="187"/>
-      <c r="B44" s="165"/>
+      <c r="A44" s="176"/>
+      <c r="B44" s="163"/>
       <c r="C44" s="60" t="s">
         <v>223</v>
       </c>
@@ -9512,8 +9496,8 @@
       <c r="S44" s="26"/>
     </row>
     <row r="45" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="187"/>
-      <c r="B45" s="165"/>
+      <c r="A45" s="176"/>
+      <c r="B45" s="163"/>
       <c r="C45" s="60" t="s">
         <v>494</v>
       </c>
@@ -9556,8 +9540,8 @@
       <c r="T45" s="28"/>
     </row>
     <row r="46" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="187"/>
-      <c r="B46" s="165"/>
+      <c r="A46" s="176"/>
+      <c r="B46" s="163"/>
       <c r="C46" s="60" t="s">
         <v>417</v>
       </c>
@@ -9599,8 +9583,8 @@
       <c r="S46" s="26"/>
     </row>
     <row r="47" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="187"/>
-      <c r="B47" s="165"/>
+      <c r="A47" s="176"/>
+      <c r="B47" s="163"/>
       <c r="C47" s="60" t="s">
         <v>414</v>
       </c>
@@ -9640,8 +9624,8 @@
       <c r="S47" s="26"/>
     </row>
     <row r="48" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="187"/>
-      <c r="B48" s="165"/>
+      <c r="A48" s="176"/>
+      <c r="B48" s="163"/>
       <c r="C48" s="60" t="s">
         <v>412</v>
       </c>
@@ -9687,8 +9671,8 @@
       <c r="S48" s="26"/>
     </row>
     <row r="49" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="187"/>
-      <c r="B49" s="165"/>
+      <c r="A49" s="176"/>
+      <c r="B49" s="163"/>
       <c r="C49" s="60" t="s">
         <v>261</v>
       </c>
@@ -9730,8 +9714,8 @@
       <c r="S49" s="26"/>
     </row>
     <row r="50" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="188"/>
-      <c r="B50" s="170"/>
+      <c r="A50" s="177"/>
+      <c r="B50" s="164"/>
       <c r="C50" s="65" t="s">
         <v>535</v>
       </c>
@@ -9773,10 +9757,10 @@
       <c r="S50" s="26"/>
     </row>
     <row r="51" spans="1:20" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="159" t="s">
+      <c r="A51" s="179" t="s">
         <v>93</v>
       </c>
-      <c r="B51" s="157" t="s">
+      <c r="B51" s="170" t="s">
         <v>55</v>
       </c>
       <c r="C51" s="62" t="s">
@@ -9823,8 +9807,8 @@
       <c r="T51" s="33"/>
     </row>
     <row r="52" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="160"/>
-      <c r="B52" s="158"/>
+      <c r="A52" s="180"/>
+      <c r="B52" s="168"/>
       <c r="C52" s="60" t="s">
         <v>70</v>
       </c>
@@ -9870,8 +9854,8 @@
       <c r="S52" s="26"/>
     </row>
     <row r="53" spans="1:20" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="160"/>
-      <c r="B53" s="158"/>
+      <c r="A53" s="180"/>
+      <c r="B53" s="168"/>
       <c r="C53" s="60" t="s">
         <v>71</v>
       </c>
@@ -9917,8 +9901,8 @@
       <c r="S53" s="26"/>
     </row>
     <row r="54" spans="1:20" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="160"/>
-      <c r="B54" s="158"/>
+      <c r="A54" s="180"/>
+      <c r="B54" s="168"/>
       <c r="C54" s="61" t="s">
         <v>72</v>
       </c>
@@ -9964,8 +9948,8 @@
       <c r="S54" s="26"/>
     </row>
     <row r="55" spans="1:20" s="23" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="160"/>
-      <c r="B55" s="158"/>
+      <c r="A55" s="180"/>
+      <c r="B55" s="168"/>
       <c r="C55" s="65" t="s">
         <v>612</v>
       </c>
@@ -10009,8 +9993,8 @@
       <c r="S55" s="31"/>
     </row>
     <row r="56" spans="1:20" s="23" customFormat="1" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="160"/>
-      <c r="B56" s="164" t="s">
+      <c r="A56" s="180"/>
+      <c r="B56" s="173" t="s">
         <v>197</v>
       </c>
       <c r="C56" s="63" t="s">
@@ -10056,8 +10040,8 @@
       <c r="S56" s="57"/>
     </row>
     <row r="57" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="160"/>
-      <c r="B57" s="165"/>
+      <c r="A57" s="180"/>
+      <c r="B57" s="163"/>
       <c r="C57" s="60" t="s">
         <v>213</v>
       </c>
@@ -10103,8 +10087,8 @@
       <c r="S57" s="26"/>
     </row>
     <row r="58" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="160"/>
-      <c r="B58" s="165"/>
+      <c r="A58" s="180"/>
+      <c r="B58" s="163"/>
       <c r="C58" s="60" t="s">
         <v>206</v>
       </c>
@@ -10146,8 +10130,8 @@
       <c r="S58" s="26"/>
     </row>
     <row r="59" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="160"/>
-      <c r="B59" s="165"/>
+      <c r="A59" s="180"/>
+      <c r="B59" s="163"/>
       <c r="C59" s="60" t="s">
         <v>201</v>
       </c>
@@ -10193,8 +10177,8 @@
       <c r="S59" s="26"/>
     </row>
     <row r="60" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="160"/>
-      <c r="B60" s="165"/>
+      <c r="A60" s="180"/>
+      <c r="B60" s="163"/>
       <c r="C60" s="60" t="s">
         <v>202</v>
       </c>
@@ -10240,8 +10224,8 @@
       <c r="S60" s="26"/>
     </row>
     <row r="61" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="160"/>
-      <c r="B61" s="165"/>
+      <c r="A61" s="180"/>
+      <c r="B61" s="163"/>
       <c r="C61" s="60" t="s">
         <v>95</v>
       </c>
@@ -10285,8 +10269,8 @@
       <c r="S61" s="26"/>
     </row>
     <row r="62" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="160"/>
-      <c r="B62" s="165"/>
+      <c r="A62" s="180"/>
+      <c r="B62" s="163"/>
       <c r="C62" s="60" t="s">
         <v>419</v>
       </c>
@@ -10330,8 +10314,8 @@
       <c r="S62" s="26"/>
     </row>
     <row r="63" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="160"/>
-      <c r="B63" s="165"/>
+      <c r="A63" s="180"/>
+      <c r="B63" s="163"/>
       <c r="C63" s="60" t="s">
         <v>203</v>
       </c>
@@ -10377,8 +10361,8 @@
       <c r="S63" s="26"/>
     </row>
     <row r="64" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="160"/>
-      <c r="B64" s="165"/>
+      <c r="A64" s="180"/>
+      <c r="B64" s="163"/>
       <c r="C64" s="60" t="s">
         <v>433</v>
       </c>
@@ -10424,8 +10408,8 @@
       <c r="S64" s="26"/>
     </row>
     <row r="65" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="160"/>
-      <c r="B65" s="165"/>
+      <c r="A65" s="180"/>
+      <c r="B65" s="163"/>
       <c r="C65" s="60" t="s">
         <v>381</v>
       </c>
@@ -10470,8 +10454,8 @@
       <c r="T65" s="28"/>
     </row>
     <row r="66" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="160"/>
-      <c r="B66" s="165"/>
+      <c r="A66" s="180"/>
+      <c r="B66" s="163"/>
       <c r="C66" s="60" t="s">
         <v>398</v>
       </c>
@@ -10481,7 +10465,7 @@
       <c r="E66" s="23" t="s">
         <v>399</v>
       </c>
-      <c r="F66" s="190" t="s">
+      <c r="F66" s="157" t="s">
         <v>648</v>
       </c>
       <c r="G66" s="24" t="s">
@@ -10517,8 +10501,8 @@
       <c r="S66" s="26"/>
     </row>
     <row r="67" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="160"/>
-      <c r="B67" s="165"/>
+      <c r="A67" s="180"/>
+      <c r="B67" s="163"/>
       <c r="C67" s="60" t="s">
         <v>258</v>
       </c>
@@ -10565,8 +10549,8 @@
       <c r="T67" s="23"/>
     </row>
     <row r="68" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="160"/>
-      <c r="B68" s="165"/>
+      <c r="A68" s="180"/>
+      <c r="B68" s="163"/>
       <c r="C68" s="60" t="s">
         <v>436</v>
       </c>
@@ -10610,8 +10594,8 @@
       <c r="S68" s="26"/>
     </row>
     <row r="69" spans="1:20" s="33" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="160"/>
-      <c r="B69" s="165"/>
+      <c r="A69" s="180"/>
+      <c r="B69" s="163"/>
       <c r="C69" s="61" t="s">
         <v>207</v>
       </c>
@@ -10656,10 +10640,10 @@
       <c r="T69" s="28"/>
     </row>
     <row r="70" spans="1:20" s="23" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="172" t="s">
+      <c r="A70" s="189" t="s">
         <v>101</v>
       </c>
-      <c r="B70" s="171"/>
+      <c r="B70" s="188"/>
       <c r="C70" s="62" t="s">
         <v>83</v>
       </c>
@@ -10706,8 +10690,8 @@
       <c r="T70" s="33"/>
     </row>
     <row r="71" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="173"/>
-      <c r="B71" s="158"/>
+      <c r="A71" s="190"/>
+      <c r="B71" s="168"/>
       <c r="C71" s="60" t="s">
         <v>84</v>
       </c>
@@ -10753,8 +10737,8 @@
       <c r="S71" s="26"/>
     </row>
     <row r="72" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="173"/>
-      <c r="B72" s="158"/>
+      <c r="A72" s="190"/>
+      <c r="B72" s="168"/>
       <c r="C72" s="60" t="s">
         <v>85</v>
       </c>
@@ -10802,8 +10786,8 @@
       <c r="S72" s="26"/>
     </row>
     <row r="73" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="173"/>
-      <c r="B73" s="158"/>
+      <c r="A73" s="190"/>
+      <c r="B73" s="168"/>
       <c r="C73" s="60" t="s">
         <v>86</v>
       </c>
@@ -10849,8 +10833,8 @@
       <c r="S73" s="26"/>
     </row>
     <row r="74" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="173"/>
-      <c r="B74" s="158"/>
+      <c r="A74" s="190"/>
+      <c r="B74" s="168"/>
       <c r="C74" s="60" t="s">
         <v>87</v>
       </c>
@@ -10898,8 +10882,8 @@
       <c r="S74" s="26"/>
     </row>
     <row r="75" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="173"/>
-      <c r="B75" s="158"/>
+      <c r="A75" s="190"/>
+      <c r="B75" s="168"/>
       <c r="C75" s="60" t="s">
         <v>88</v>
       </c>
@@ -10945,8 +10929,8 @@
       <c r="S75" s="26"/>
     </row>
     <row r="76" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="173"/>
-      <c r="B76" s="158"/>
+      <c r="A76" s="190"/>
+      <c r="B76" s="168"/>
       <c r="C76" s="60" t="s">
         <v>89</v>
       </c>
@@ -10990,8 +10974,8 @@
       <c r="S76" s="26"/>
     </row>
     <row r="77" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="173"/>
-      <c r="B77" s="158"/>
+      <c r="A77" s="190"/>
+      <c r="B77" s="168"/>
       <c r="C77" s="60" t="s">
         <v>90</v>
       </c>
@@ -11037,8 +11021,8 @@
       <c r="S77" s="26"/>
     </row>
     <row r="78" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="173"/>
-      <c r="B78" s="158"/>
+      <c r="A78" s="190"/>
+      <c r="B78" s="168"/>
       <c r="C78" s="60" t="s">
         <v>91</v>
       </c>
@@ -11086,8 +11070,8 @@
       <c r="S78" s="26"/>
     </row>
     <row r="79" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="173"/>
-      <c r="B79" s="158"/>
+      <c r="A79" s="190"/>
+      <c r="B79" s="168"/>
       <c r="C79" s="60" t="s">
         <v>229</v>
       </c>
@@ -11133,8 +11117,8 @@
       <c r="S79" s="26"/>
     </row>
     <row r="80" spans="1:20" s="23" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="173"/>
-      <c r="B80" s="169"/>
+      <c r="A80" s="190"/>
+      <c r="B80" s="187"/>
       <c r="C80" s="61" t="s">
         <v>94</v>
       </c>
@@ -11180,8 +11164,8 @@
       <c r="S80" s="31"/>
     </row>
     <row r="81" spans="1:19" s="23" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="173"/>
-      <c r="B81" s="165" t="s">
+      <c r="A81" s="190"/>
+      <c r="B81" s="163" t="s">
         <v>197</v>
       </c>
       <c r="C81" s="63" t="s">
@@ -11225,8 +11209,8 @@
       <c r="S81" s="57"/>
     </row>
     <row r="82" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="173"/>
-      <c r="B82" s="165"/>
+      <c r="A82" s="190"/>
+      <c r="B82" s="163"/>
       <c r="C82" s="60" t="s">
         <v>217</v>
       </c>
@@ -11269,8 +11253,8 @@
       <c r="S82" s="26"/>
     </row>
     <row r="83" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="173"/>
-      <c r="B83" s="165"/>
+      <c r="A83" s="190"/>
+      <c r="B83" s="163"/>
       <c r="C83" s="60" t="s">
         <v>431</v>
       </c>
@@ -11314,8 +11298,8 @@
       <c r="S83" s="26"/>
     </row>
     <row r="84" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="173"/>
-      <c r="B84" s="165"/>
+      <c r="A84" s="190"/>
+      <c r="B84" s="163"/>
       <c r="C84" s="60" t="s">
         <v>299</v>
       </c>
@@ -11359,8 +11343,8 @@
       <c r="S84" s="26"/>
     </row>
     <row r="85" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="173"/>
-      <c r="B85" s="165"/>
+      <c r="A85" s="190"/>
+      <c r="B85" s="163"/>
       <c r="C85" s="60" t="s">
         <v>372</v>
       </c>
@@ -11404,8 +11388,8 @@
       <c r="S85" s="26"/>
     </row>
     <row r="86" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="173"/>
-      <c r="B86" s="165"/>
+      <c r="A86" s="190"/>
+      <c r="B86" s="163"/>
       <c r="C86" s="60" t="s">
         <v>225</v>
       </c>
@@ -11449,8 +11433,8 @@
       <c r="S86" s="26"/>
     </row>
     <row r="87" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="173"/>
-      <c r="B87" s="165"/>
+      <c r="A87" s="190"/>
+      <c r="B87" s="163"/>
       <c r="C87" s="60" t="s">
         <v>326</v>
       </c>
@@ -11496,8 +11480,8 @@
       <c r="S87" s="26"/>
     </row>
     <row r="88" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="173"/>
-      <c r="B88" s="165"/>
+      <c r="A88" s="190"/>
+      <c r="B88" s="163"/>
       <c r="C88" s="61" t="s">
         <v>253</v>
       </c>
@@ -11541,8 +11525,8 @@
       <c r="S88" s="26"/>
     </row>
     <row r="89" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="173"/>
-      <c r="B89" s="165"/>
+      <c r="A89" s="190"/>
+      <c r="B89" s="163"/>
       <c r="C89" s="60" t="s">
         <v>408</v>
       </c>
@@ -11583,8 +11567,8 @@
       <c r="S89" s="26"/>
     </row>
     <row r="90" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="173"/>
-      <c r="B90" s="165"/>
+      <c r="A90" s="190"/>
+      <c r="B90" s="163"/>
       <c r="C90" s="60" t="s">
         <v>374</v>
       </c>
@@ -11626,8 +11610,8 @@
       <c r="S90" s="26"/>
     </row>
     <row r="91" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="173"/>
-      <c r="B91" s="165"/>
+      <c r="A91" s="190"/>
+      <c r="B91" s="163"/>
       <c r="C91" s="60" t="s">
         <v>361</v>
       </c>
@@ -11671,8 +11655,8 @@
       <c r="S91" s="26"/>
     </row>
     <row r="92" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="173"/>
-      <c r="B92" s="165"/>
+      <c r="A92" s="190"/>
+      <c r="B92" s="163"/>
       <c r="C92" s="60" t="s">
         <v>357</v>
       </c>
@@ -11716,8 +11700,8 @@
       <c r="S92" s="26"/>
     </row>
     <row r="93" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="173"/>
-      <c r="B93" s="165"/>
+      <c r="A93" s="190"/>
+      <c r="B93" s="163"/>
       <c r="C93" s="60" t="s">
         <v>216</v>
       </c>
@@ -11760,8 +11744,8 @@
       <c r="S93" s="26"/>
     </row>
     <row r="94" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="173"/>
-      <c r="B94" s="165"/>
+      <c r="A94" s="190"/>
+      <c r="B94" s="163"/>
       <c r="C94" s="60" t="s">
         <v>377</v>
       </c>
@@ -11805,8 +11789,8 @@
       <c r="S94" s="26"/>
     </row>
     <row r="95" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="173"/>
-      <c r="B95" s="165"/>
+      <c r="A95" s="190"/>
+      <c r="B95" s="163"/>
       <c r="C95" s="60" t="s">
         <v>226</v>
       </c>
@@ -11850,8 +11834,8 @@
       <c r="S95" s="26"/>
     </row>
     <row r="96" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="173"/>
-      <c r="B96" s="165"/>
+      <c r="A96" s="190"/>
+      <c r="B96" s="163"/>
       <c r="C96" s="60" t="s">
         <v>251</v>
       </c>
@@ -11895,8 +11879,8 @@
       <c r="S96" s="26"/>
     </row>
     <row r="97" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="173"/>
-      <c r="B97" s="165"/>
+      <c r="A97" s="190"/>
+      <c r="B97" s="163"/>
       <c r="C97" s="60" t="s">
         <v>298</v>
       </c>
@@ -11940,8 +11924,8 @@
       <c r="S97" s="26"/>
     </row>
     <row r="98" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="173"/>
-      <c r="B98" s="165"/>
+      <c r="A98" s="190"/>
+      <c r="B98" s="163"/>
       <c r="C98" s="60" t="s">
         <v>228</v>
       </c>
@@ -11985,8 +11969,8 @@
       <c r="S98" s="26"/>
     </row>
     <row r="99" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="173"/>
-      <c r="B99" s="165"/>
+      <c r="A99" s="190"/>
+      <c r="B99" s="163"/>
       <c r="C99" s="60" t="s">
         <v>236</v>
       </c>
@@ -12025,8 +12009,8 @@
       <c r="S99" s="26"/>
     </row>
     <row r="100" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="173"/>
-      <c r="B100" s="165"/>
+      <c r="A100" s="190"/>
+      <c r="B100" s="163"/>
       <c r="C100" s="60" t="s">
         <v>227</v>
       </c>
@@ -12067,8 +12051,8 @@
       <c r="S100" s="26"/>
     </row>
     <row r="101" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="173"/>
-      <c r="B101" s="165"/>
+      <c r="A101" s="190"/>
+      <c r="B101" s="163"/>
       <c r="C101" s="65" t="s">
         <v>221</v>
       </c>
@@ -12114,8 +12098,8 @@
       <c r="S101" s="26"/>
     </row>
     <row r="102" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="173"/>
-      <c r="B102" s="165"/>
+      <c r="A102" s="190"/>
+      <c r="B102" s="163"/>
       <c r="C102" s="60" t="s">
         <v>218</v>
       </c>
@@ -12157,8 +12141,8 @@
       <c r="S102" s="26"/>
     </row>
     <row r="103" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="173"/>
-      <c r="B103" s="165"/>
+      <c r="A103" s="190"/>
+      <c r="B103" s="163"/>
       <c r="C103" s="60" t="s">
         <v>219</v>
       </c>
@@ -12202,8 +12186,8 @@
       <c r="S103" s="26"/>
     </row>
     <row r="104" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="173"/>
-      <c r="B104" s="165"/>
+      <c r="A104" s="190"/>
+      <c r="B104" s="163"/>
       <c r="C104" s="60" t="s">
         <v>363</v>
       </c>
@@ -12244,8 +12228,8 @@
       <c r="S104" s="26"/>
     </row>
     <row r="105" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="173"/>
-      <c r="B105" s="165"/>
+      <c r="A105" s="190"/>
+      <c r="B105" s="163"/>
       <c r="C105" s="60" t="s">
         <v>235</v>
       </c>
@@ -12286,8 +12270,8 @@
       <c r="S105" s="26"/>
     </row>
     <row r="106" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="173"/>
-      <c r="B106" s="165"/>
+      <c r="A106" s="190"/>
+      <c r="B106" s="163"/>
       <c r="C106" s="60" t="s">
         <v>210</v>
       </c>
@@ -12329,8 +12313,8 @@
       <c r="S106" s="26"/>
     </row>
     <row r="107" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="173"/>
-      <c r="B107" s="165"/>
+      <c r="A107" s="190"/>
+      <c r="B107" s="163"/>
       <c r="C107" s="60" t="s">
         <v>211</v>
       </c>
@@ -12372,8 +12356,8 @@
       <c r="S107" s="26"/>
     </row>
     <row r="108" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="173"/>
-      <c r="B108" s="165"/>
+      <c r="A108" s="190"/>
+      <c r="B108" s="163"/>
       <c r="C108" s="60" t="s">
         <v>506</v>
       </c>
@@ -12414,8 +12398,8 @@
       <c r="S108" s="26"/>
     </row>
     <row r="109" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="173"/>
-      <c r="B109" s="165"/>
+      <c r="A109" s="190"/>
+      <c r="B109" s="163"/>
       <c r="C109" s="60" t="s">
         <v>252</v>
       </c>
@@ -12456,8 +12440,8 @@
       <c r="S109" s="26"/>
     </row>
     <row r="110" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="173"/>
-      <c r="B110" s="165"/>
+      <c r="A110" s="190"/>
+      <c r="B110" s="163"/>
       <c r="C110" s="60" t="s">
         <v>255</v>
       </c>
@@ -12467,7 +12451,7 @@
       <c r="E110" s="152" t="s">
         <v>320</v>
       </c>
-      <c r="F110" s="190" t="s">
+      <c r="F110" s="157" t="s">
         <v>648</v>
       </c>
       <c r="G110" s="24" t="s">
@@ -12501,8 +12485,8 @@
       <c r="S110" s="26"/>
     </row>
     <row r="111" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="173"/>
-      <c r="B111" s="165"/>
+      <c r="A111" s="190"/>
+      <c r="B111" s="163"/>
       <c r="C111" s="60" t="s">
         <v>232</v>
       </c>
@@ -12548,8 +12532,8 @@
       <c r="S111" s="26"/>
     </row>
     <row r="112" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="173"/>
-      <c r="B112" s="165"/>
+      <c r="A112" s="190"/>
+      <c r="B112" s="163"/>
       <c r="C112" s="60" t="s">
         <v>233</v>
       </c>
@@ -12595,8 +12579,8 @@
       <c r="S112" s="26"/>
     </row>
     <row r="113" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="173"/>
-      <c r="B113" s="165"/>
+      <c r="A113" s="190"/>
+      <c r="B113" s="163"/>
       <c r="C113" s="65" t="s">
         <v>606</v>
       </c>
@@ -12623,8 +12607,8 @@
       <c r="T113" s="23"/>
     </row>
     <row r="114" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="173"/>
-      <c r="B114" s="165"/>
+      <c r="A114" s="190"/>
+      <c r="B114" s="163"/>
       <c r="C114" s="60" t="s">
         <v>329</v>
       </c>
@@ -12669,8 +12653,8 @@
       <c r="T114" s="23"/>
     </row>
     <row r="115" spans="1:20" s="33" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="174"/>
-      <c r="B115" s="170"/>
+      <c r="A115" s="191"/>
+      <c r="B115" s="164"/>
       <c r="C115" s="61" t="s">
         <v>322</v>
       </c>
@@ -12723,10 +12707,10 @@
       <c r="T115" s="28"/>
     </row>
     <row r="116" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="166" t="s">
+      <c r="A116" s="184" t="s">
         <v>504</v>
       </c>
-      <c r="B116" s="157" t="s">
+      <c r="B116" s="170" t="s">
         <v>55</v>
       </c>
       <c r="C116" s="62" t="s">
@@ -12769,8 +12753,8 @@
       <c r="T116" s="33"/>
     </row>
     <row r="117" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="167"/>
-      <c r="B117" s="158"/>
+      <c r="A117" s="185"/>
+      <c r="B117" s="168"/>
       <c r="C117" s="60" t="s">
         <v>96</v>
       </c>
@@ -12814,8 +12798,8 @@
       <c r="S117" s="26"/>
     </row>
     <row r="118" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="167"/>
-      <c r="B118" s="158"/>
+      <c r="A118" s="185"/>
+      <c r="B118" s="168"/>
       <c r="C118" s="60" t="s">
         <v>97</v>
       </c>
@@ -12859,8 +12843,8 @@
       <c r="S118" s="26"/>
     </row>
     <row r="119" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="167"/>
-      <c r="B119" s="158"/>
+      <c r="A119" s="185"/>
+      <c r="B119" s="168"/>
       <c r="C119" s="60" t="s">
         <v>108</v>
       </c>
@@ -12900,8 +12884,8 @@
       <c r="S119" s="26"/>
     </row>
     <row r="120" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="167"/>
-      <c r="B120" s="158"/>
+      <c r="A120" s="185"/>
+      <c r="B120" s="168"/>
       <c r="C120" s="61" t="s">
         <v>98</v>
       </c>
@@ -12942,8 +12926,8 @@
       <c r="T120" s="28"/>
     </row>
     <row r="121" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="167"/>
-      <c r="B121" s="158"/>
+      <c r="A121" s="185"/>
+      <c r="B121" s="168"/>
       <c r="C121" s="60" t="s">
         <v>183</v>
       </c>
@@ -12984,8 +12968,8 @@
       <c r="T121" s="28"/>
     </row>
     <row r="122" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="167"/>
-      <c r="B122" s="158"/>
+      <c r="A122" s="185"/>
+      <c r="B122" s="168"/>
       <c r="C122" s="61" t="s">
         <v>120</v>
       </c>
@@ -13026,8 +13010,8 @@
       <c r="T122" s="28"/>
     </row>
     <row r="123" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="167"/>
-      <c r="B123" s="158"/>
+      <c r="A123" s="185"/>
+      <c r="B123" s="168"/>
       <c r="C123" s="60" t="s">
         <v>100</v>
       </c>
@@ -13069,8 +13053,8 @@
       <c r="S123" s="26"/>
     </row>
     <row r="124" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="167"/>
-      <c r="B124" s="158"/>
+      <c r="A124" s="185"/>
+      <c r="B124" s="168"/>
       <c r="C124" s="60" t="s">
         <v>505</v>
       </c>
@@ -13112,8 +13096,8 @@
       <c r="S124" s="26"/>
     </row>
     <row r="125" spans="1:20" s="23" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="167"/>
-      <c r="B125" s="169"/>
+      <c r="A125" s="185"/>
+      <c r="B125" s="187"/>
       <c r="C125" s="60" t="s">
         <v>180</v>
       </c>
@@ -13153,8 +13137,8 @@
       <c r="S125" s="26"/>
     </row>
     <row r="126" spans="1:20" s="28" customFormat="1" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="167"/>
-      <c r="B126" s="164" t="s">
+      <c r="A126" s="185"/>
+      <c r="B126" s="173" t="s">
         <v>197</v>
       </c>
       <c r="C126" s="63" t="s">
@@ -13199,8 +13183,8 @@
       <c r="T126" s="23"/>
     </row>
     <row r="127" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="167"/>
-      <c r="B127" s="165"/>
+      <c r="A127" s="185"/>
+      <c r="B127" s="163"/>
       <c r="C127" s="60" t="s">
         <v>452</v>
       </c>
@@ -13241,8 +13225,8 @@
       <c r="T127" s="23"/>
     </row>
     <row r="128" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="167"/>
-      <c r="B128" s="165"/>
+      <c r="A128" s="185"/>
+      <c r="B128" s="163"/>
       <c r="C128" s="60" t="s">
         <v>455</v>
       </c>
@@ -13283,8 +13267,8 @@
       <c r="T128" s="23"/>
     </row>
     <row r="129" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="167"/>
-      <c r="B129" s="165"/>
+      <c r="A129" s="185"/>
+      <c r="B129" s="163"/>
       <c r="C129" s="61" t="s">
         <v>429</v>
       </c>
@@ -13327,8 +13311,8 @@
       <c r="T129" s="23"/>
     </row>
     <row r="130" spans="1:20" s="33" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="167"/>
-      <c r="B130" s="165"/>
+      <c r="A130" s="185"/>
+      <c r="B130" s="163"/>
       <c r="C130" s="60" t="s">
         <v>234</v>
       </c>
@@ -13369,8 +13353,8 @@
       <c r="T130" s="23"/>
     </row>
     <row r="131" spans="1:20" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="167"/>
-      <c r="B131" s="165"/>
+      <c r="A131" s="185"/>
+      <c r="B131" s="163"/>
       <c r="C131" s="60" t="s">
         <v>212</v>
       </c>
@@ -13411,8 +13395,8 @@
       <c r="T131" s="23"/>
     </row>
     <row r="132" spans="1:20" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="168"/>
-      <c r="B132" s="165"/>
+      <c r="A132" s="186"/>
+      <c r="B132" s="163"/>
       <c r="C132" s="65" t="s">
         <v>632</v>
       </c>
@@ -13435,10 +13419,10 @@
       <c r="T132" s="23"/>
     </row>
     <row r="133" spans="1:20" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="161" t="s">
+      <c r="A133" s="181" t="s">
         <v>115</v>
       </c>
-      <c r="B133" s="157" t="s">
+      <c r="B133" s="170" t="s">
         <v>55</v>
       </c>
       <c r="C133" s="62" t="s">
@@ -13481,8 +13465,8 @@
       <c r="T133" s="33"/>
     </row>
     <row r="134" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="162"/>
-      <c r="B134" s="158"/>
+      <c r="A134" s="182"/>
+      <c r="B134" s="168"/>
       <c r="C134" s="61" t="s">
         <v>99</v>
       </c>
@@ -13522,8 +13506,8 @@
       <c r="S134" s="31"/>
     </row>
     <row r="135" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="162"/>
-      <c r="B135" s="158"/>
+      <c r="A135" s="182"/>
+      <c r="B135" s="168"/>
       <c r="C135" s="65" t="s">
         <v>610</v>
       </c>
@@ -13566,8 +13550,8 @@
       <c r="T135" s="19"/>
     </row>
     <row r="136" spans="1:20" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="162"/>
-      <c r="B136" s="158"/>
+      <c r="A136" s="182"/>
+      <c r="B136" s="168"/>
       <c r="C136" s="60" t="s">
         <v>119</v>
       </c>
@@ -13609,8 +13593,8 @@
       <c r="T136" s="19"/>
     </row>
     <row r="137" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A137" s="162"/>
-      <c r="B137" s="158"/>
+      <c r="A137" s="182"/>
+      <c r="B137" s="168"/>
       <c r="C137" s="60" t="s">
         <v>118</v>
       </c>
@@ -13652,8 +13636,8 @@
       <c r="T137" s="19"/>
     </row>
     <row r="138" spans="1:20" s="23" customFormat="1" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="162"/>
-      <c r="B138" s="164" t="s">
+      <c r="A138" s="182"/>
+      <c r="B138" s="173" t="s">
         <v>197</v>
       </c>
       <c r="C138" s="63" t="s">
@@ -13695,8 +13679,8 @@
       <c r="S138" s="57"/>
     </row>
     <row r="139" spans="1:20" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="162"/>
-      <c r="B139" s="165"/>
+      <c r="A139" s="182"/>
+      <c r="B139" s="163"/>
       <c r="C139" s="60" t="s">
         <v>403</v>
       </c>
@@ -13735,8 +13719,8 @@
       <c r="S139" s="26"/>
     </row>
     <row r="140" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="162"/>
-      <c r="B140" s="165"/>
+      <c r="A140" s="182"/>
+      <c r="B140" s="163"/>
       <c r="C140" s="60" t="s">
         <v>259</v>
       </c>
@@ -13776,8 +13760,8 @@
       <c r="S140" s="26"/>
     </row>
     <row r="141" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="162"/>
-      <c r="B141" s="165"/>
+      <c r="A141" s="182"/>
+      <c r="B141" s="163"/>
       <c r="C141" s="65" t="s">
         <v>626</v>
       </c>
@@ -13811,8 +13795,8 @@
       <c r="S141" s="26"/>
     </row>
     <row r="142" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="162"/>
-      <c r="B142" s="165"/>
+      <c r="A142" s="182"/>
+      <c r="B142" s="163"/>
       <c r="C142" s="60" t="s">
         <v>426</v>
       </c>
@@ -13852,8 +13836,8 @@
       <c r="S142" s="26"/>
     </row>
     <row r="143" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="162"/>
-      <c r="B143" s="165"/>
+      <c r="A143" s="182"/>
+      <c r="B143" s="163"/>
       <c r="C143" s="60" t="s">
         <v>384</v>
       </c>
@@ -13893,8 +13877,8 @@
       <c r="S143" s="26"/>
     </row>
     <row r="144" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="162"/>
-      <c r="B144" s="165"/>
+      <c r="A144" s="182"/>
+      <c r="B144" s="163"/>
       <c r="C144" s="60" t="s">
         <v>443</v>
       </c>
@@ -13934,8 +13918,8 @@
       <c r="S144" s="26"/>
     </row>
     <row r="145" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="162"/>
-      <c r="B145" s="165"/>
+      <c r="A145" s="182"/>
+      <c r="B145" s="163"/>
       <c r="C145" s="60" t="s">
         <v>362</v>
       </c>
@@ -13975,8 +13959,8 @@
       <c r="S145" s="26"/>
     </row>
     <row r="146" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="162"/>
-      <c r="B146" s="165"/>
+      <c r="A146" s="182"/>
+      <c r="B146" s="163"/>
       <c r="C146" s="60" t="s">
         <v>230</v>
       </c>
@@ -14016,8 +14000,8 @@
       <c r="S146" s="26"/>
     </row>
     <row r="147" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="162"/>
-      <c r="B147" s="165"/>
+      <c r="A147" s="182"/>
+      <c r="B147" s="163"/>
       <c r="C147" s="60" t="s">
         <v>425</v>
       </c>
@@ -14057,8 +14041,8 @@
       <c r="S147" s="26"/>
     </row>
     <row r="148" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="162"/>
-      <c r="B148" s="165"/>
+      <c r="A148" s="182"/>
+      <c r="B148" s="163"/>
       <c r="C148" s="60" t="s">
         <v>400</v>
       </c>
@@ -14098,8 +14082,8 @@
       <c r="S148" s="26"/>
     </row>
     <row r="149" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="162"/>
-      <c r="B149" s="165"/>
+      <c r="A149" s="182"/>
+      <c r="B149" s="163"/>
       <c r="C149" s="60" t="s">
         <v>437</v>
       </c>
@@ -14139,8 +14123,8 @@
       <c r="S149" s="26"/>
     </row>
     <row r="150" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="162"/>
-      <c r="B150" s="165"/>
+      <c r="A150" s="182"/>
+      <c r="B150" s="163"/>
       <c r="C150" s="60" t="s">
         <v>410</v>
       </c>
@@ -14180,8 +14164,8 @@
       <c r="S150" s="26"/>
     </row>
     <row r="151" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="162"/>
-      <c r="B151" s="165"/>
+      <c r="A151" s="182"/>
+      <c r="B151" s="163"/>
       <c r="C151" s="65" t="s">
         <v>525</v>
       </c>
@@ -14221,8 +14205,8 @@
       <c r="S151" s="26"/>
     </row>
     <row r="152" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="162"/>
-      <c r="B152" s="165"/>
+      <c r="A152" s="182"/>
+      <c r="B152" s="163"/>
       <c r="C152" s="65" t="s">
         <v>260</v>
       </c>
@@ -14262,8 +14246,8 @@
       <c r="S152" s="26"/>
     </row>
     <row r="153" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="162"/>
-      <c r="B153" s="165"/>
+      <c r="A153" s="182"/>
+      <c r="B153" s="163"/>
       <c r="C153" s="65" t="s">
         <v>450</v>
       </c>
@@ -14303,8 +14287,8 @@
       <c r="S153" s="26"/>
     </row>
     <row r="154" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="162"/>
-      <c r="B154" s="165"/>
+      <c r="A154" s="182"/>
+      <c r="B154" s="163"/>
       <c r="C154" s="65" t="s">
         <v>439</v>
       </c>
@@ -14344,8 +14328,8 @@
       <c r="S154" s="26"/>
     </row>
     <row r="155" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="162"/>
-      <c r="B155" s="165"/>
+      <c r="A155" s="182"/>
+      <c r="B155" s="163"/>
       <c r="C155" s="65" t="s">
         <v>323</v>
       </c>
@@ -14387,8 +14371,8 @@
       <c r="S155" s="26"/>
     </row>
     <row r="156" spans="1:19" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="162"/>
-      <c r="B156" s="165"/>
+      <c r="A156" s="182"/>
+      <c r="B156" s="163"/>
       <c r="C156" s="65" t="s">
         <v>370</v>
       </c>
@@ -14428,8 +14412,8 @@
       <c r="S156" s="26"/>
     </row>
     <row r="157" spans="1:19" s="23" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A157" s="163"/>
-      <c r="B157" s="165"/>
+      <c r="A157" s="183"/>
+      <c r="B157" s="163"/>
       <c r="C157" s="65" t="s">
         <v>215</v>
       </c>
@@ -14469,10 +14453,10 @@
       <c r="S157" s="31"/>
     </row>
     <row r="158" spans="1:19" s="33" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A158" s="183" t="s">
+      <c r="A158" s="171" t="s">
         <v>116</v>
       </c>
-      <c r="B158" s="178" t="s">
+      <c r="B158" s="162" t="s">
         <v>197</v>
       </c>
       <c r="C158" s="62" t="s">
@@ -14516,8 +14500,8 @@
       <c r="S158" s="36"/>
     </row>
     <row r="159" spans="1:19" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A159" s="183"/>
-      <c r="B159" s="165"/>
+      <c r="A159" s="171"/>
+      <c r="B159" s="163"/>
       <c r="C159" s="60" t="s">
         <v>366</v>
       </c>
@@ -14559,8 +14543,8 @@
       <c r="S159" s="26"/>
     </row>
     <row r="160" spans="1:19" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A160" s="183"/>
-      <c r="B160" s="165"/>
+      <c r="A160" s="171"/>
+      <c r="B160" s="163"/>
       <c r="C160" s="60" t="s">
         <v>385</v>
       </c>
@@ -14602,8 +14586,8 @@
       <c r="S160" s="26"/>
     </row>
     <row r="161" spans="1:19" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A161" s="183"/>
-      <c r="B161" s="165"/>
+      <c r="A161" s="171"/>
+      <c r="B161" s="163"/>
       <c r="C161" s="60" t="s">
         <v>396</v>
       </c>
@@ -14645,8 +14629,8 @@
       <c r="S161" s="26"/>
     </row>
     <row r="162" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A162" s="183"/>
-      <c r="B162" s="165"/>
+      <c r="A162" s="171"/>
+      <c r="B162" s="163"/>
       <c r="C162" s="60" t="s">
         <v>254</v>
       </c>
@@ -14686,8 +14670,8 @@
       <c r="S162" s="26"/>
     </row>
     <row r="163" spans="1:19" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A163" s="183"/>
-      <c r="B163" s="165"/>
+      <c r="A163" s="171"/>
+      <c r="B163" s="163"/>
       <c r="C163" s="61" t="s">
         <v>405</v>
       </c>
@@ -14729,8 +14713,8 @@
       <c r="S163" s="26"/>
     </row>
     <row r="164" spans="1:19" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A164" s="183"/>
-      <c r="B164" s="165"/>
+      <c r="A164" s="171"/>
+      <c r="B164" s="163"/>
       <c r="C164" s="60" t="s">
         <v>376</v>
       </c>
@@ -14770,8 +14754,8 @@
       <c r="S164" s="26"/>
     </row>
     <row r="165" spans="1:19" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A165" s="183"/>
-      <c r="B165" s="170"/>
+      <c r="A165" s="171"/>
+      <c r="B165" s="164"/>
       <c r="C165" s="60" t="s">
         <v>406</v>
       </c>
@@ -14811,7 +14795,7 @@
       <c r="S165" s="31"/>
     </row>
     <row r="166" spans="1:19" s="33" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A166" s="184" t="s">
+      <c r="A166" s="172" t="s">
         <v>539</v>
       </c>
       <c r="B166" s="72" t="s">
@@ -14854,8 +14838,8 @@
       <c r="S166" s="71"/>
     </row>
     <row r="167" spans="1:19" s="23" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A167" s="184"/>
-      <c r="B167" s="164" t="s">
+      <c r="A167" s="172"/>
+      <c r="B167" s="173" t="s">
         <v>197</v>
       </c>
       <c r="C167" s="60" t="s">
@@ -14893,8 +14877,8 @@
       <c r="S167" s="57"/>
     </row>
     <row r="168" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A168" s="184"/>
-      <c r="B168" s="165"/>
+      <c r="A168" s="172"/>
+      <c r="B168" s="163"/>
       <c r="C168" s="60" t="s">
         <v>199</v>
       </c>
@@ -14929,8 +14913,8 @@
       <c r="S168" s="26"/>
     </row>
     <row r="169" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="184"/>
-      <c r="B169" s="165"/>
+      <c r="A169" s="172"/>
+      <c r="B169" s="163"/>
       <c r="C169" s="60" t="s">
         <v>263</v>
       </c>
@@ -14968,8 +14952,8 @@
       <c r="S169" s="26"/>
     </row>
     <row r="170" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A170" s="184"/>
-      <c r="B170" s="165"/>
+      <c r="A170" s="172"/>
+      <c r="B170" s="163"/>
       <c r="C170" s="60" t="s">
         <v>421</v>
       </c>
@@ -15006,8 +14990,8 @@
       <c r="S170" s="26"/>
     </row>
     <row r="171" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A171" s="184"/>
-      <c r="B171" s="185"/>
+      <c r="A171" s="172"/>
+      <c r="B171" s="174"/>
       <c r="C171" s="60" t="s">
         <v>422</v>
       </c>
@@ -15045,10 +15029,10 @@
       <c r="S171" s="26"/>
     </row>
     <row r="172" spans="1:19" s="33" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A172" s="177" t="s">
+      <c r="A172" s="161" t="s">
         <v>117</v>
       </c>
-      <c r="B172" s="181" t="s">
+      <c r="B172" s="167" t="s">
         <v>55</v>
       </c>
       <c r="C172" s="62" t="s">
@@ -15088,8 +15072,8 @@
       <c r="S172" s="36"/>
     </row>
     <row r="173" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A173" s="177"/>
-      <c r="B173" s="158"/>
+      <c r="A173" s="161"/>
+      <c r="B173" s="168"/>
       <c r="C173" s="60" t="s">
         <v>188</v>
       </c>
@@ -15127,8 +15111,8 @@
       <c r="S173" s="26"/>
     </row>
     <row r="174" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A174" s="177"/>
-      <c r="B174" s="158"/>
+      <c r="A174" s="161"/>
+      <c r="B174" s="168"/>
       <c r="C174" s="60" t="s">
         <v>187</v>
       </c>
@@ -15166,8 +15150,8 @@
       <c r="S174" s="26"/>
     </row>
     <row r="175" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A175" s="177"/>
-      <c r="B175" s="158"/>
+      <c r="A175" s="161"/>
+      <c r="B175" s="168"/>
       <c r="C175" s="61" t="s">
         <v>189</v>
       </c>
@@ -15205,8 +15189,8 @@
       <c r="S175" s="31"/>
     </row>
     <row r="176" spans="1:19" s="23" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A176" s="177"/>
-      <c r="B176" s="175" t="s">
+      <c r="A176" s="161"/>
+      <c r="B176" s="159" t="s">
         <v>197</v>
       </c>
       <c r="C176" s="63" t="s">
@@ -15240,8 +15224,8 @@
       <c r="S176" s="57"/>
     </row>
     <row r="177" spans="1:19" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A177" s="177"/>
-      <c r="B177" s="176"/>
+      <c r="A177" s="161"/>
+      <c r="B177" s="160"/>
       <c r="C177" s="64"/>
       <c r="E177" s="49"/>
       <c r="F177" s="49"/>
@@ -15970,6 +15954,18 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="C3:S3"/>
+    <mergeCell ref="B51:B55"/>
+    <mergeCell ref="A51:A69"/>
+    <mergeCell ref="A133:A157"/>
+    <mergeCell ref="B138:B157"/>
+    <mergeCell ref="A116:A132"/>
+    <mergeCell ref="B116:B125"/>
+    <mergeCell ref="B81:B115"/>
+    <mergeCell ref="B56:B69"/>
+    <mergeCell ref="B70:B80"/>
+    <mergeCell ref="A70:A115"/>
+    <mergeCell ref="B133:B137"/>
     <mergeCell ref="B176:B177"/>
     <mergeCell ref="A172:A177"/>
     <mergeCell ref="B158:B165"/>
@@ -15985,18 +15981,6 @@
     <mergeCell ref="B126:B132"/>
     <mergeCell ref="A37:A50"/>
     <mergeCell ref="B41:B50"/>
-    <mergeCell ref="C3:S3"/>
-    <mergeCell ref="B51:B55"/>
-    <mergeCell ref="A51:A69"/>
-    <mergeCell ref="A133:A157"/>
-    <mergeCell ref="B138:B157"/>
-    <mergeCell ref="A116:A132"/>
-    <mergeCell ref="B116:B125"/>
-    <mergeCell ref="B81:B115"/>
-    <mergeCell ref="B56:B69"/>
-    <mergeCell ref="B70:B80"/>
-    <mergeCell ref="A70:A115"/>
-    <mergeCell ref="B133:B137"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Mein Kommentar zur Modliste
</commit_message>
<xml_diff>
--- a/ressources/DayZ Mods.xlsx
+++ b/ressources/DayZ Mods.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\projects\Immersive-DayZ-Experience\ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBB29C1-448D-44A3-9E2F-43F4F331166C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C90447-4F4A-48A8-A10B-4C06CB926B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="260" xr2:uid="{FAEB3C3F-74B0-4C80-8C8B-4522341FA132}"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="260" xr2:uid="{FAEB3C3F-74B0-4C80-8C8B-4522341FA132}"/>
   </bookViews>
   <sheets>
     <sheet name="Mods" sheetId="1" r:id="rId1"/>
@@ -564,7 +564,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2339" uniqueCount="680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2410" uniqueCount="690">
   <si>
     <t>Community Frameworks</t>
   </si>
@@ -2707,6 +2707,36 @@
   </si>
   <si>
     <t>View Inventory Animation</t>
+  </si>
+  <si>
+    <t>Kommentar Ali</t>
+  </si>
+  <si>
+    <t>Keep</t>
+  </si>
+  <si>
+    <t>Keep (aber wurde seit 3 Jahren nicht geupdated)</t>
+  </si>
+  <si>
+    <t>Drop (sehe keinen Mehrwert)</t>
+  </si>
+  <si>
+    <t>Maybe keep</t>
+  </si>
+  <si>
+    <t>Benötigt?</t>
+  </si>
+  <si>
+    <t>Meinetwegen :D</t>
+  </si>
+  <si>
+    <t>Keep (aber dann auch einarbeiten, nicht nur beim Trader)</t>
+  </si>
+  <si>
+    <t>Notwendig?</t>
+  </si>
+  <si>
+    <t>Inaktiv?</t>
   </si>
 </sst>
 </file>
@@ -2988,7 +3018,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="46">
+  <borders count="47">
     <border>
       <left/>
       <right/>
@@ -3583,6 +3613,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -3590,7 +3629,7 @@
     <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="204">
+  <cellXfs count="207">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3958,14 +3997,83 @@
     <xf numFmtId="0" fontId="18" fillId="21" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="35" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="36" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -3982,12 +4090,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -3998,9 +4100,6 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4015,65 +4114,14 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="35" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="36" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -4569,9 +4617,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4609,7 +4657,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -4715,7 +4763,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4857,7 +4905,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4867,9 +4915,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BE2B301-FC9E-4F7D-A454-62A8C1115EDF}">
   <dimension ref="A1:S115"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B66" sqref="A66:XFD66"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4883,6 +4931,8 @@
     <col min="7" max="7" width="39.28515625" style="90" customWidth="1"/>
     <col min="8" max="8" width="12.85546875" style="88" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" customWidth="1"/>
+    <col min="10" max="14" width="11.42578125" customWidth="1"/>
+    <col min="15" max="15" width="42.42578125" style="206" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4922,9 +4972,12 @@
       <c r="N1" s="102" t="s">
         <v>56</v>
       </c>
+      <c r="O1" s="204" t="s">
+        <v>680</v>
+      </c>
     </row>
     <row r="2" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="202" t="s">
+      <c r="A2" s="170" t="s">
         <v>669</v>
       </c>
       <c r="C2" s="159">
@@ -4941,27 +4994,30 @@
       <c r="H2" s="95" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="198" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" s="198" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" s="198" t="s">
-        <v>33</v>
-      </c>
-      <c r="L2" s="199" t="s">
-        <v>33</v>
-      </c>
-      <c r="M2" s="199" t="s">
-        <v>33</v>
-      </c>
-      <c r="N2" s="198" t="s">
-        <v>33</v>
+      <c r="I2" s="165" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="165" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="165" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="166" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="166" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="165" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="205" t="s">
+        <v>681</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="202"/>
+      <c r="A3" s="170"/>
       <c r="C3" s="160">
         <v>1564026768</v>
       </c>
@@ -4976,27 +5032,30 @@
       <c r="H3" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="K3" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="L3" s="201" t="s">
-        <v>33</v>
-      </c>
-      <c r="M3" s="199" t="s">
-        <v>33</v>
-      </c>
-      <c r="N3" s="200" t="s">
-        <v>33</v>
+      <c r="I3" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="168" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" s="166" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" s="205" t="s">
+        <v>681</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="202" t="s">
+      <c r="A4" s="170" t="s">
         <v>670</v>
       </c>
       <c r="C4" s="161">
@@ -5013,27 +5072,30 @@
       <c r="H4" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="J4" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="K4" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="L4" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="M4" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="N4" s="200" t="s">
-        <v>33</v>
+      <c r="I4" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="N4" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="O4" s="205" t="s">
+        <v>681</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="202"/>
+      <c r="A5" s="170"/>
       <c r="C5" s="161">
         <v>2614334381</v>
       </c>
@@ -5048,27 +5110,30 @@
       <c r="H5" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="J5" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="K5" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="L5" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="M5" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="N5" s="200" t="s">
-        <v>33</v>
+      <c r="I5" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="M5" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="N5" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" s="205" t="s">
+        <v>681</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="202"/>
+      <c r="A6" s="170"/>
       <c r="C6" s="161">
         <v>2507204412</v>
       </c>
@@ -5083,27 +5148,30 @@
       <c r="H6" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="K6" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="L6" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="M6" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="N6" s="200" t="s">
-        <v>33</v>
+      <c r="I6" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="L6" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="M6" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="N6" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" s="205" t="s">
+        <v>681</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="202" t="s">
+      <c r="A7" s="170" t="s">
         <v>53</v>
       </c>
       <c r="C7" s="160">
@@ -5120,27 +5188,30 @@
       <c r="H7" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="J7" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="K7" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="L7" s="201" t="s">
-        <v>33</v>
-      </c>
-      <c r="M7" s="199" t="s">
-        <v>33</v>
-      </c>
-      <c r="N7" s="200" t="s">
-        <v>33</v>
+      <c r="I7" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="K7" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" s="168" t="s">
+        <v>33</v>
+      </c>
+      <c r="M7" s="166" t="s">
+        <v>33</v>
+      </c>
+      <c r="N7" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="O7" s="205" t="s">
+        <v>681</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="202"/>
+      <c r="A8" s="170"/>
       <c r="C8" s="160">
         <v>2572331007</v>
       </c>
@@ -5175,9 +5246,12 @@
       <c r="N8" s="38" t="s">
         <v>8</v>
       </c>
+      <c r="O8" s="205" t="s">
+        <v>681</v>
+      </c>
     </row>
     <row r="9" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="202"/>
+      <c r="A9" s="170"/>
       <c r="C9" s="161">
         <v>2116157322</v>
       </c>
@@ -5192,29 +5266,32 @@
       <c r="H9" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="J9" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="K9" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="L9" s="201" t="s">
-        <v>33</v>
-      </c>
-      <c r="M9" s="199" t="s">
-        <v>33</v>
-      </c>
-      <c r="N9" s="200" t="s">
-        <v>33</v>
+      <c r="I9" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="L9" s="168" t="s">
+        <v>33</v>
+      </c>
+      <c r="M9" s="166" t="s">
+        <v>33</v>
+      </c>
+      <c r="N9" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="O9" s="205" t="s">
+        <v>681</v>
       </c>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
     </row>
     <row r="10" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="202"/>
+      <c r="A10" s="170"/>
       <c r="C10" s="161">
         <v>2793893086</v>
       </c>
@@ -5229,29 +5306,32 @@
       <c r="H10" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="J10" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="K10" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="L10" s="201" t="s">
-        <v>33</v>
-      </c>
-      <c r="M10" s="199" t="s">
-        <v>33</v>
-      </c>
-      <c r="N10" s="200" t="s">
-        <v>33</v>
+      <c r="I10" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="K10" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="L10" s="168" t="s">
+        <v>33</v>
+      </c>
+      <c r="M10" s="166" t="s">
+        <v>33</v>
+      </c>
+      <c r="N10" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="O10" s="205" t="s">
+        <v>681</v>
       </c>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
     </row>
     <row r="11" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="202" t="s">
+      <c r="A11" s="170" t="s">
         <v>671</v>
       </c>
       <c r="C11" s="161">
@@ -5270,27 +5350,30 @@
       <c r="H11" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="I11" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="J11" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="K11" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="L11" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="M11" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="N11" s="200" t="s">
-        <v>33</v>
+      <c r="I11" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="J11" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="K11" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="L11" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="M11" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="N11" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="O11" s="205" t="s">
+        <v>681</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="202"/>
+      <c r="A12" s="170"/>
       <c r="C12" s="161">
         <v>3031784065</v>
       </c>
@@ -5307,27 +5390,30 @@
       <c r="H12" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="I12" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="J12" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="K12" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="L12" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="M12" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="N12" s="200" t="s">
-        <v>33</v>
+      <c r="I12" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="J12" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="K12" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="L12" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="M12" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="N12" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="O12" s="205" t="s">
+        <v>681</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="202"/>
+      <c r="A13" s="170"/>
       <c r="C13" s="161">
         <v>2977703357</v>
       </c>
@@ -5342,27 +5428,30 @@
       <c r="H13" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="I13" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="J13" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="K13" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="L13" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="M13" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="N13" s="200" t="s">
-        <v>33</v>
+      <c r="I13" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="J13" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="K13" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="L13" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="M13" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="N13" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="O13" s="205" t="s">
+        <v>682</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="202"/>
+      <c r="A14" s="170"/>
       <c r="C14" s="161">
         <v>2980235854</v>
       </c>
@@ -5377,27 +5466,30 @@
       <c r="H14" s="87" t="s">
         <v>614</v>
       </c>
-      <c r="I14" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="J14" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="K14" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="L14" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="M14" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="N14" s="200" t="s">
-        <v>33</v>
+      <c r="I14" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="J14" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="K14" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="L14" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="M14" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="N14" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="O14" s="205" t="s">
+        <v>683</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="202"/>
+      <c r="A15" s="170"/>
       <c r="C15" s="161">
         <v>2111523728</v>
       </c>
@@ -5432,9 +5524,12 @@
       <c r="N15" s="38" t="s">
         <v>33</v>
       </c>
+      <c r="O15" s="205" t="s">
+        <v>681</v>
+      </c>
     </row>
     <row r="16" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="202" t="s">
+      <c r="A16" s="170" t="s">
         <v>675</v>
       </c>
       <c r="C16" s="161">
@@ -5471,9 +5566,12 @@
       <c r="N16" s="38" t="s">
         <v>33</v>
       </c>
+      <c r="O16" s="205" t="s">
+        <v>683</v>
+      </c>
     </row>
     <row r="17" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="202"/>
+      <c r="A17" s="170"/>
       <c r="C17" s="161">
         <v>2822531337</v>
       </c>
@@ -5506,9 +5604,12 @@
       <c r="N17" s="91" t="s">
         <v>8</v>
       </c>
+      <c r="O17" s="205" t="s">
+        <v>681</v>
+      </c>
     </row>
     <row r="18" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="202" t="s">
+      <c r="A18" s="170" t="s">
         <v>672</v>
       </c>
       <c r="C18" s="160">
@@ -5527,29 +5628,32 @@
       <c r="H18" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="I18" s="200" t="s">
+      <c r="I18" s="167" t="s">
         <v>33</v>
       </c>
       <c r="J18" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="K18" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="L18" s="201" t="s">
-        <v>33</v>
-      </c>
-      <c r="M18" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="N18" s="200" t="s">
-        <v>33</v>
+      <c r="K18" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="L18" s="168" t="s">
+        <v>33</v>
+      </c>
+      <c r="M18" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="N18" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="O18" s="205" t="s">
+        <v>681</v>
       </c>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
     </row>
     <row r="19" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="202"/>
+      <c r="A19" s="170"/>
       <c r="C19" s="160">
         <v>2166325582</v>
       </c>
@@ -5564,27 +5668,30 @@
       <c r="H19" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="I19" s="200" t="s">
+      <c r="I19" s="167" t="s">
         <v>33</v>
       </c>
       <c r="J19" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="K19" s="201" t="s">
-        <v>33</v>
-      </c>
-      <c r="L19" s="201" t="s">
-        <v>33</v>
-      </c>
-      <c r="M19" s="199" t="s">
-        <v>33</v>
-      </c>
-      <c r="N19" s="200" t="s">
-        <v>33</v>
+      <c r="K19" s="168" t="s">
+        <v>33</v>
+      </c>
+      <c r="L19" s="168" t="s">
+        <v>33</v>
+      </c>
+      <c r="M19" s="166" t="s">
+        <v>33</v>
+      </c>
+      <c r="N19" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="O19" s="205" t="s">
+        <v>681</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="202"/>
+      <c r="A20" s="170"/>
       <c r="C20" s="160">
         <v>2208230845</v>
       </c>
@@ -5601,32 +5708,35 @@
       <c r="H20" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="I20" s="200" t="s">
+      <c r="I20" s="167" t="s">
         <v>33</v>
       </c>
       <c r="J20" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="K20" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="L20" s="201" t="s">
-        <v>33</v>
-      </c>
-      <c r="M20" s="199" t="s">
-        <v>33</v>
-      </c>
-      <c r="N20" s="200" t="s">
-        <v>33</v>
+      <c r="K20" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="L20" s="168" t="s">
+        <v>33</v>
+      </c>
+      <c r="M20" s="166" t="s">
+        <v>33</v>
+      </c>
+      <c r="N20" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="O20" s="205" t="s">
+        <v>684</v>
       </c>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
     </row>
     <row r="21" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="202" t="s">
+      <c r="A21" s="170" t="s">
         <v>673</v>
       </c>
-      <c r="B21" s="203"/>
+      <c r="B21" s="169"/>
       <c r="C21" s="160">
         <v>1870481515</v>
       </c>
@@ -5657,10 +5767,13 @@
         <v>8</v>
       </c>
       <c r="N21" s="5"/>
+      <c r="O21" s="205" t="s">
+        <v>681</v>
+      </c>
     </row>
     <row r="22" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="202"/>
-      <c r="B22" s="203"/>
+      <c r="A22" s="170"/>
+      <c r="B22" s="169"/>
       <c r="C22" s="160">
         <v>2789302074</v>
       </c>
@@ -5691,10 +5804,13 @@
         <v>8</v>
       </c>
       <c r="N22" s="5"/>
+      <c r="O22" s="205" t="s">
+        <v>681</v>
+      </c>
     </row>
     <row r="23" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="202"/>
-      <c r="B23" s="203"/>
+      <c r="A23" s="170"/>
+      <c r="B23" s="169"/>
       <c r="C23" s="161">
         <v>1991570984</v>
       </c>
@@ -5721,10 +5837,13 @@
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
+      <c r="O23" s="205" t="s">
+        <v>681</v>
+      </c>
     </row>
     <row r="24" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="202"/>
-      <c r="B24" s="203"/>
+      <c r="A24" s="170"/>
+      <c r="B24" s="169"/>
       <c r="C24" s="161">
         <v>3171576913</v>
       </c>
@@ -5757,10 +5876,13 @@
       <c r="N24" s="38" t="s">
         <v>33</v>
       </c>
+      <c r="O24" s="205" t="s">
+        <v>681</v>
+      </c>
     </row>
     <row r="25" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="202"/>
-      <c r="B25" s="203"/>
+      <c r="A25" s="170"/>
+      <c r="B25" s="169"/>
       <c r="C25" s="160" t="s">
         <v>597</v>
       </c>
@@ -5791,10 +5913,13 @@
         <v>8</v>
       </c>
       <c r="N25" s="5"/>
+      <c r="O25" s="205" t="s">
+        <v>681</v>
+      </c>
     </row>
     <row r="26" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="202"/>
-      <c r="B26" s="203"/>
+      <c r="A26" s="170"/>
+      <c r="B26" s="169"/>
       <c r="C26" s="160">
         <v>2931560672</v>
       </c>
@@ -5825,10 +5950,13 @@
         <v>8</v>
       </c>
       <c r="N26" s="5"/>
+      <c r="O26" s="205" t="s">
+        <v>681</v>
+      </c>
     </row>
     <row r="27" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="202"/>
-      <c r="B27" s="203"/>
+      <c r="A27" s="170"/>
+      <c r="B27" s="169"/>
       <c r="C27" s="161">
         <v>3108865421</v>
       </c>
@@ -5859,10 +5987,13 @@
       </c>
       <c r="M27" s="38"/>
       <c r="N27" s="38"/>
+      <c r="O27" s="205" t="s">
+        <v>681</v>
+      </c>
     </row>
     <row r="28" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="202"/>
-      <c r="B28" s="203"/>
+      <c r="A28" s="170"/>
+      <c r="B28" s="169"/>
       <c r="C28" s="160">
         <v>1630943713</v>
       </c>
@@ -5895,10 +6026,13 @@
         <v>8</v>
       </c>
       <c r="N28" s="5"/>
+      <c r="O28" s="205" t="s">
+        <v>681</v>
+      </c>
     </row>
     <row r="29" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="202"/>
-      <c r="B29" s="203"/>
+      <c r="A29" s="170"/>
+      <c r="B29" s="169"/>
       <c r="C29" s="161">
         <v>1797720064</v>
       </c>
@@ -5931,10 +6065,13 @@
         <v>8</v>
       </c>
       <c r="N29" s="5"/>
+      <c r="O29" s="205" t="s">
+        <v>681</v>
+      </c>
     </row>
     <row r="30" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="202"/>
-      <c r="B30" s="203"/>
+      <c r="A30" s="170"/>
+      <c r="B30" s="169"/>
       <c r="C30" s="160">
         <v>2155726353</v>
       </c>
@@ -5965,10 +6102,13 @@
         <v>8</v>
       </c>
       <c r="N30" s="5"/>
+      <c r="O30" s="205" t="s">
+        <v>681</v>
+      </c>
     </row>
     <row r="31" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="202"/>
-      <c r="B31" s="203"/>
+      <c r="A31" s="170"/>
+      <c r="B31" s="169"/>
       <c r="C31" s="161">
         <v>2723807644</v>
       </c>
@@ -5999,10 +6139,13 @@
         <v>8</v>
       </c>
       <c r="N31" s="5"/>
+      <c r="O31" s="205" t="s">
+        <v>681</v>
+      </c>
     </row>
     <row r="32" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="202"/>
-      <c r="B32" s="203"/>
+      <c r="A32" s="170"/>
+      <c r="B32" s="169"/>
       <c r="C32" s="161">
         <v>2780914191</v>
       </c>
@@ -6033,10 +6176,13 @@
         <v>8</v>
       </c>
       <c r="N32" s="5"/>
-    </row>
-    <row r="33" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="202"/>
-      <c r="B33" s="203"/>
+      <c r="O32" s="205" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="170"/>
+      <c r="B33" s="169"/>
       <c r="C33" s="161">
         <v>2741271183</v>
       </c>
@@ -6067,10 +6213,13 @@
         <v>8</v>
       </c>
       <c r="N33" s="5"/>
-    </row>
-    <row r="34" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="202"/>
-      <c r="B34" s="203"/>
+      <c r="O33" s="205" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="170"/>
+      <c r="B34" s="169"/>
       <c r="C34" s="161">
         <v>2579252958</v>
       </c>
@@ -6103,10 +6252,13 @@
       <c r="N34" s="38" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="202"/>
-      <c r="B35" s="203"/>
+      <c r="O34" s="205" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="170"/>
+      <c r="B35" s="169"/>
       <c r="C35" s="161">
         <v>3034460305</v>
       </c>
@@ -6139,10 +6291,13 @@
       <c r="N35" s="38" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="202"/>
-      <c r="B36" s="203"/>
+      <c r="O35" s="205" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="170"/>
+      <c r="B36" s="169"/>
       <c r="C36" s="161">
         <v>2851058261</v>
       </c>
@@ -6175,10 +6330,13 @@
       <c r="N36" s="38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="202"/>
-      <c r="B37" s="203"/>
+      <c r="O36" s="205" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="170"/>
+      <c r="B37" s="169"/>
       <c r="C37" s="161">
         <v>2926289548</v>
       </c>
@@ -6209,10 +6367,13 @@
         <v>33</v>
       </c>
       <c r="N37" s="38"/>
-    </row>
-    <row r="38" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="202"/>
-      <c r="B38" s="203"/>
+      <c r="O37" s="205" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="170"/>
+      <c r="B38" s="169"/>
       <c r="C38" s="161">
         <v>3170285574</v>
       </c>
@@ -6245,10 +6406,13 @@
         <v>33</v>
       </c>
       <c r="N38" s="38"/>
-    </row>
-    <row r="39" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="202"/>
-      <c r="B39" s="203"/>
+      <c r="O38" s="205" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="170"/>
+      <c r="B39" s="169"/>
       <c r="C39" s="161">
         <v>3279662973</v>
       </c>
@@ -6281,10 +6445,13 @@
         <v>8</v>
       </c>
       <c r="N39" s="38"/>
-    </row>
-    <row r="40" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="202"/>
-      <c r="B40" s="203"/>
+      <c r="O39" s="205" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="170"/>
+      <c r="B40" s="169"/>
       <c r="C40" s="160">
         <v>2937138060</v>
       </c>
@@ -6317,9 +6484,12 @@
         <v>8</v>
       </c>
       <c r="N40" s="5"/>
-    </row>
-    <row r="41" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="202" t="s">
+      <c r="O40" s="205" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="170" t="s">
         <v>676</v>
       </c>
       <c r="C41" s="161">
@@ -6356,9 +6526,12 @@
       <c r="N41" s="38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="202"/>
+      <c r="O41" s="205" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="170"/>
       <c r="C42" s="161">
         <v>3114410963</v>
       </c>
@@ -6389,9 +6562,12 @@
         <v>33</v>
       </c>
       <c r="N42" s="5"/>
-    </row>
-    <row r="43" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="202"/>
+      <c r="O42" s="205" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="170"/>
       <c r="C43" s="160">
         <v>1866298408</v>
       </c>
@@ -6406,27 +6582,30 @@
       <c r="H43" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="J43" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="K43" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="L43" s="201" t="s">
-        <v>33</v>
-      </c>
-      <c r="M43" s="199" t="s">
-        <v>33</v>
-      </c>
-      <c r="N43" s="200" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="202"/>
+      <c r="I43" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="J43" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="K43" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="L43" s="168" t="s">
+        <v>33</v>
+      </c>
+      <c r="M43" s="166" t="s">
+        <v>33</v>
+      </c>
+      <c r="N43" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="O43" s="205" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="170"/>
       <c r="C44" s="161">
         <v>2874589934</v>
       </c>
@@ -6459,9 +6638,12 @@
       <c r="N44" s="38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="202" t="s">
+      <c r="O44" s="205" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="170" t="s">
         <v>677</v>
       </c>
       <c r="C45" s="161">
@@ -6484,9 +6666,12 @@
       <c r="L45" s="38"/>
       <c r="M45" s="38"/>
       <c r="N45" s="38"/>
-    </row>
-    <row r="46" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="202"/>
+      <c r="O45" s="205" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="170"/>
       <c r="C46" s="161">
         <v>1710977250</v>
       </c>
@@ -6509,9 +6694,12 @@
       <c r="L46" s="38"/>
       <c r="M46" s="38"/>
       <c r="N46" s="38"/>
-    </row>
-    <row r="47" spans="1:14" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="202"/>
+      <c r="O46" s="205" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="170"/>
       <c r="C47" s="161">
         <v>2895049000</v>
       </c>
@@ -6534,9 +6722,12 @@
       <c r="L47" s="38"/>
       <c r="M47" s="38"/>
       <c r="N47" s="38"/>
-    </row>
-    <row r="48" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="202" t="s">
+      <c r="O47" s="205" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="170" t="s">
         <v>678</v>
       </c>
       <c r="C48" s="161">
@@ -6571,9 +6762,12 @@
       <c r="N48" s="38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="202"/>
+      <c r="O48" s="205" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="170"/>
       <c r="C49" s="161">
         <v>2472500243</v>
       </c>
@@ -6606,9 +6800,12 @@
       <c r="N49" s="38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="202"/>
+      <c r="O49" s="205" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="170"/>
       <c r="C50" s="161">
         <v>1832448183</v>
       </c>
@@ -6635,9 +6832,12 @@
       <c r="L50" s="38"/>
       <c r="M50" s="38"/>
       <c r="N50" s="38"/>
-    </row>
-    <row r="51" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="202"/>
+      <c r="O50" s="205" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="170"/>
       <c r="C51" s="161">
         <v>1895432270</v>
       </c>
@@ -6668,9 +6868,12 @@
       <c r="N51" s="38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="202"/>
+      <c r="O51" s="205" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="170"/>
       <c r="C52" s="161">
         <v>2912241382</v>
       </c>
@@ -6701,9 +6904,12 @@
       <c r="N52" s="38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="202" t="s">
+      <c r="O52" s="205" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="170" t="s">
         <v>668</v>
       </c>
       <c r="C53" s="161">
@@ -6738,9 +6944,12 @@
       <c r="N53" s="38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="54" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="202"/>
+      <c r="O53" s="205" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="170"/>
       <c r="C54" s="161">
         <v>3043440124</v>
       </c>
@@ -6773,9 +6982,12 @@
       <c r="N54" s="38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="202"/>
+      <c r="O54" s="205" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="170"/>
       <c r="C55" s="160">
         <v>2550932214</v>
       </c>
@@ -6790,27 +7002,30 @@
       <c r="H55" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="I55" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="J55" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="K55" s="201" t="s">
-        <v>33</v>
-      </c>
-      <c r="L55" s="201" t="s">
-        <v>33</v>
-      </c>
-      <c r="M55" s="199" t="s">
-        <v>33</v>
-      </c>
-      <c r="N55" s="200" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="202"/>
+      <c r="I55" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="J55" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="K55" s="168" t="s">
+        <v>33</v>
+      </c>
+      <c r="L55" s="168" t="s">
+        <v>33</v>
+      </c>
+      <c r="M55" s="166" t="s">
+        <v>33</v>
+      </c>
+      <c r="N55" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="O55" s="205" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="170"/>
       <c r="C56" s="161">
         <v>3321340470</v>
       </c>
@@ -6845,9 +7060,12 @@
       <c r="N56" s="38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="57" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="202" t="s">
+      <c r="O56" s="205" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="170" t="s">
         <v>674</v>
       </c>
       <c r="C57" s="160">
@@ -6882,9 +7100,12 @@
       <c r="N57" s="38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="202"/>
+      <c r="O57" s="205" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="170"/>
       <c r="C58" s="160">
         <v>2793619401</v>
       </c>
@@ -6919,9 +7140,12 @@
       <c r="N58" s="38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="202"/>
+      <c r="O58" s="205" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="170"/>
       <c r="C59" s="161">
         <v>2924719512</v>
       </c>
@@ -6954,9 +7178,12 @@
       <c r="N59" s="38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="202"/>
+      <c r="O59" s="205" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="170"/>
       <c r="C60" s="161">
         <v>2810260908</v>
       </c>
@@ -6989,9 +7216,12 @@
       <c r="N60" s="38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="202"/>
+      <c r="O60" s="205" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="170"/>
       <c r="C61" s="161">
         <v>2877877368</v>
       </c>
@@ -7024,9 +7254,12 @@
       <c r="N61" s="38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="62" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="202"/>
+      <c r="O61" s="205" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="170"/>
       <c r="C62" s="161">
         <v>2857994912</v>
       </c>
@@ -7059,9 +7292,12 @@
       <c r="N62" s="38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="63" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="202"/>
+      <c r="O62" s="205" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="170"/>
       <c r="C63" s="161">
         <v>2817606510</v>
       </c>
@@ -7094,9 +7330,12 @@
       <c r="N63" s="38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="64" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="202"/>
+      <c r="O63" s="205" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="170"/>
       <c r="C64" s="161">
         <v>2884638645</v>
       </c>
@@ -7125,9 +7364,12 @@
       </c>
       <c r="M64" s="91"/>
       <c r="N64" s="5"/>
+      <c r="O64" s="205" t="s">
+        <v>688</v>
+      </c>
     </row>
     <row r="65" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="202"/>
+      <c r="A65" s="170"/>
       <c r="C65" s="160">
         <v>2521460498</v>
       </c>
@@ -7142,27 +7384,30 @@
       <c r="H65" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="I65" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="J65" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="K65" s="201" t="s">
-        <v>33</v>
-      </c>
-      <c r="L65" s="201" t="s">
-        <v>33</v>
-      </c>
-      <c r="M65" s="199" t="s">
-        <v>33</v>
-      </c>
-      <c r="N65" s="200" t="s">
-        <v>33</v>
+      <c r="I65" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="J65" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="K65" s="168" t="s">
+        <v>33</v>
+      </c>
+      <c r="L65" s="168" t="s">
+        <v>33</v>
+      </c>
+      <c r="M65" s="166" t="s">
+        <v>33</v>
+      </c>
+      <c r="N65" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="O65" s="205" t="s">
+        <v>681</v>
       </c>
     </row>
     <row r="66" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="202"/>
+      <c r="A66" s="170"/>
       <c r="C66" s="160">
         <v>2903112334</v>
       </c>
@@ -7179,27 +7424,30 @@
       <c r="H66" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="I66" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="J66" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="K66" s="201" t="s">
-        <v>33</v>
-      </c>
-      <c r="L66" s="201" t="s">
-        <v>33</v>
-      </c>
-      <c r="M66" s="199" t="s">
-        <v>33</v>
-      </c>
-      <c r="N66" s="200" t="s">
-        <v>33</v>
+      <c r="I66" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="J66" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="K66" s="168" t="s">
+        <v>33</v>
+      </c>
+      <c r="L66" s="168" t="s">
+        <v>33</v>
+      </c>
+      <c r="M66" s="166" t="s">
+        <v>33</v>
+      </c>
+      <c r="N66" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="O66" s="205" t="s">
+        <v>683</v>
       </c>
     </row>
     <row r="67" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="202"/>
+      <c r="A67" s="170"/>
       <c r="C67" s="160">
         <v>2833363308</v>
       </c>
@@ -7214,27 +7462,30 @@
       <c r="H67" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="I67" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="J67" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="K67" s="201" t="s">
-        <v>33</v>
-      </c>
-      <c r="L67" s="201" t="s">
-        <v>33</v>
-      </c>
-      <c r="M67" s="199" t="s">
-        <v>33</v>
-      </c>
-      <c r="N67" s="200" t="s">
-        <v>33</v>
+      <c r="I67" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="J67" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="K67" s="168" t="s">
+        <v>33</v>
+      </c>
+      <c r="L67" s="168" t="s">
+        <v>33</v>
+      </c>
+      <c r="M67" s="166" t="s">
+        <v>33</v>
+      </c>
+      <c r="N67" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="O67" s="205" t="s">
+        <v>681</v>
       </c>
     </row>
     <row r="68" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="202"/>
+      <c r="A68" s="170"/>
       <c r="C68" s="161">
         <v>2521678241</v>
       </c>
@@ -7249,29 +7500,32 @@
       <c r="H68" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="I68" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="J68" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="K68" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="L68" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="M68" s="199" t="s">
-        <v>33</v>
-      </c>
-      <c r="N68" s="200" t="s">
-        <v>33</v>
+      <c r="I68" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="J68" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="K68" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="L68" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="M68" s="166" t="s">
+        <v>33</v>
+      </c>
+      <c r="N68" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="O68" s="205" t="s">
+        <v>681</v>
       </c>
       <c r="R68" s="1"/>
       <c r="S68" s="1"/>
     </row>
     <row r="69" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="202"/>
+      <c r="A69" s="170"/>
       <c r="C69" s="161">
         <v>2895460678</v>
       </c>
@@ -7286,27 +7540,30 @@
       <c r="H69" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="I69" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="J69" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="K69" s="201" t="s">
-        <v>33</v>
-      </c>
-      <c r="L69" s="201" t="s">
-        <v>33</v>
-      </c>
-      <c r="M69" s="199" t="s">
-        <v>33</v>
-      </c>
-      <c r="N69" s="200" t="s">
-        <v>33</v>
+      <c r="I69" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="J69" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="K69" s="168" t="s">
+        <v>33</v>
+      </c>
+      <c r="L69" s="168" t="s">
+        <v>33</v>
+      </c>
+      <c r="M69" s="166" t="s">
+        <v>33</v>
+      </c>
+      <c r="N69" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="O69" s="205" t="s">
+        <v>681</v>
       </c>
     </row>
     <row r="70" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="202"/>
+      <c r="A70" s="170"/>
       <c r="C70" s="161">
         <v>2985895498</v>
       </c>
@@ -7339,9 +7596,12 @@
       <c r="N70" s="38" t="s">
         <v>33</v>
       </c>
+      <c r="O70" s="205" t="s">
+        <v>683</v>
+      </c>
     </row>
     <row r="71" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="202"/>
+      <c r="A71" s="170"/>
       <c r="C71" s="161">
         <v>2224593910</v>
       </c>
@@ -7373,6 +7633,9 @@
       </c>
       <c r="N71" s="38" t="s">
         <v>33</v>
+      </c>
+      <c r="O71" s="205" t="s">
+        <v>681</v>
       </c>
     </row>
     <row r="72" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7894,6 +8157,11 @@
     <sortCondition ref="B2:B98"/>
   </sortState>
   <mergeCells count="12">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A41:A44"/>
     <mergeCell ref="A11:A15"/>
     <mergeCell ref="A48:A52"/>
     <mergeCell ref="A57:A71"/>
@@ -7901,11 +8169,6 @@
     <mergeCell ref="A45:A47"/>
     <mergeCell ref="A21:A40"/>
     <mergeCell ref="A53:A56"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A41:A44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7916,8 +8179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FF4763-6B65-4CE2-BD87-511E98A2E639}">
   <dimension ref="A1:V225"/>
   <sheetViews>
-    <sheetView topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V11" sqref="V11"/>
+    <sheetView topLeftCell="A87" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K97" sqref="K97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7949,25 +8212,25 @@
       <c r="S2"/>
     </row>
     <row r="3" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="165" t="s">
+      <c r="C3" s="190" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="165"/>
-      <c r="E3" s="165"/>
-      <c r="F3" s="165"/>
-      <c r="G3" s="165"/>
-      <c r="H3" s="165"/>
-      <c r="I3" s="165"/>
-      <c r="J3" s="165"/>
-      <c r="K3" s="165"/>
-      <c r="L3" s="165"/>
-      <c r="M3" s="165"/>
-      <c r="N3" s="165"/>
-      <c r="O3" s="165"/>
-      <c r="P3" s="165"/>
-      <c r="Q3" s="165"/>
-      <c r="R3" s="165"/>
-      <c r="S3" s="165"/>
+      <c r="D3" s="190"/>
+      <c r="E3" s="190"/>
+      <c r="F3" s="190"/>
+      <c r="G3" s="190"/>
+      <c r="H3" s="190"/>
+      <c r="I3" s="190"/>
+      <c r="J3" s="190"/>
+      <c r="K3" s="190"/>
+      <c r="L3" s="190"/>
+      <c r="M3" s="190"/>
+      <c r="N3" s="190"/>
+      <c r="O3" s="190"/>
+      <c r="P3" s="190"/>
+      <c r="Q3" s="190"/>
+      <c r="R3" s="190"/>
+      <c r="S3" s="190"/>
     </row>
     <row r="4" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
@@ -7982,19 +8245,19 @@
       <c r="F4" s="3" t="s">
         <v>645</v>
       </c>
-      <c r="G4" s="189"/>
-      <c r="H4" s="189"/>
-      <c r="I4" s="189"/>
-      <c r="J4" s="189"/>
-      <c r="K4" s="189"/>
-      <c r="L4" s="189"/>
-      <c r="M4" s="189"/>
-      <c r="N4" s="189"/>
-      <c r="O4" s="189"/>
-      <c r="P4" s="189"/>
-      <c r="Q4" s="189"/>
-      <c r="R4" s="189"/>
-      <c r="S4" s="189"/>
+      <c r="G4" s="178"/>
+      <c r="H4" s="178"/>
+      <c r="I4" s="178"/>
+      <c r="J4" s="178"/>
+      <c r="K4" s="178"/>
+      <c r="L4" s="178"/>
+      <c r="M4" s="178"/>
+      <c r="N4" s="178"/>
+      <c r="O4" s="178"/>
+      <c r="P4" s="178"/>
+      <c r="Q4" s="178"/>
+      <c r="R4" s="178"/>
+      <c r="S4" s="178"/>
     </row>
     <row r="5" spans="1:22" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="3"/>
@@ -8045,10 +8308,10 @@
       </c>
     </row>
     <row r="6" spans="1:22" s="23" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="188" t="s">
+      <c r="A6" s="177" t="s">
         <v>88</v>
       </c>
-      <c r="B6" s="190" t="s">
+      <c r="B6" s="179" t="s">
         <v>51</v>
       </c>
       <c r="C6" s="18" t="s">
@@ -8110,8 +8373,8 @@
       </c>
     </row>
     <row r="7" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="188"/>
-      <c r="B7" s="167"/>
+      <c r="A7" s="177"/>
+      <c r="B7" s="180"/>
       <c r="C7" s="60" t="s">
         <v>42</v>
       </c>
@@ -8162,8 +8425,8 @@
       </c>
     </row>
     <row r="8" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="188"/>
-      <c r="B8" s="167"/>
+      <c r="A8" s="177"/>
+      <c r="B8" s="180"/>
       <c r="C8" s="60" t="s">
         <v>49</v>
       </c>
@@ -8212,8 +8475,8 @@
       </c>
     </row>
     <row r="9" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="188"/>
-      <c r="B9" s="167"/>
+      <c r="A9" s="177"/>
+      <c r="B9" s="180"/>
       <c r="C9" s="60" t="s">
         <v>283</v>
       </c>
@@ -8264,8 +8527,8 @@
       </c>
     </row>
     <row r="10" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="188"/>
-      <c r="B10" s="167"/>
+      <c r="A10" s="177"/>
+      <c r="B10" s="180"/>
       <c r="C10" s="60" t="s">
         <v>43</v>
       </c>
@@ -8314,8 +8577,8 @@
       </c>
     </row>
     <row r="11" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="188"/>
-      <c r="B11" s="167"/>
+      <c r="A11" s="177"/>
+      <c r="B11" s="180"/>
       <c r="C11" s="60" t="s">
         <v>59</v>
       </c>
@@ -8366,8 +8629,8 @@
       </c>
     </row>
     <row r="12" spans="1:22" s="23" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="188"/>
-      <c r="B12" s="167"/>
+      <c r="A12" s="177"/>
+      <c r="B12" s="180"/>
       <c r="C12" s="60" t="s">
         <v>44</v>
       </c>
@@ -8413,8 +8676,8 @@
       <c r="S12" s="26"/>
     </row>
     <row r="13" spans="1:22" s="23" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="188"/>
-      <c r="B13" s="167"/>
+      <c r="A13" s="177"/>
+      <c r="B13" s="180"/>
       <c r="C13" s="60" t="s">
         <v>637</v>
       </c>
@@ -8448,8 +8711,8 @@
       <c r="S13" s="26"/>
     </row>
     <row r="14" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="188"/>
-      <c r="B14" s="167"/>
+      <c r="A14" s="177"/>
+      <c r="B14" s="180"/>
       <c r="C14" s="60" t="s">
         <v>45</v>
       </c>
@@ -8495,8 +8758,8 @@
       <c r="S14" s="26"/>
     </row>
     <row r="15" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="188"/>
-      <c r="B15" s="167"/>
+      <c r="A15" s="177"/>
+      <c r="B15" s="180"/>
       <c r="C15" s="60" t="s">
         <v>74</v>
       </c>
@@ -8542,8 +8805,8 @@
       <c r="S15" s="26"/>
     </row>
     <row r="16" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="188"/>
-      <c r="B16" s="167"/>
+      <c r="A16" s="177"/>
+      <c r="B16" s="180"/>
       <c r="C16" s="60" t="s">
         <v>46</v>
       </c>
@@ -8587,8 +8850,8 @@
       <c r="S16" s="26"/>
     </row>
     <row r="17" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="188"/>
-      <c r="B17" s="167"/>
+      <c r="A17" s="177"/>
+      <c r="B17" s="180"/>
       <c r="C17" s="60" t="s">
         <v>47</v>
       </c>
@@ -8632,8 +8895,8 @@
       <c r="S17" s="26"/>
     </row>
     <row r="18" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="188"/>
-      <c r="B18" s="167"/>
+      <c r="A18" s="177"/>
+      <c r="B18" s="180"/>
       <c r="C18" s="60" t="s">
         <v>48</v>
       </c>
@@ -8677,8 +8940,8 @@
       <c r="S18" s="26"/>
     </row>
     <row r="19" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="188"/>
-      <c r="B19" s="167"/>
+      <c r="A19" s="177"/>
+      <c r="B19" s="180"/>
       <c r="C19" s="60" t="s">
         <v>346</v>
       </c>
@@ -8724,8 +8987,8 @@
       <c r="S19" s="26"/>
     </row>
     <row r="20" spans="1:20" s="40" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="188"/>
-      <c r="B20" s="191"/>
+      <c r="A20" s="177"/>
+      <c r="B20" s="181"/>
       <c r="C20" s="61" t="s">
         <v>50</v>
       </c>
@@ -8767,8 +9030,8 @@
       <c r="S20" s="31"/>
     </row>
     <row r="21" spans="1:20" s="33" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="188"/>
-      <c r="B21" s="187" t="s">
+      <c r="A21" s="177"/>
+      <c r="B21" s="174" t="s">
         <v>246</v>
       </c>
       <c r="C21" s="117" t="s">
@@ -8819,8 +9082,8 @@
       </c>
     </row>
     <row r="22" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="188"/>
-      <c r="B22" s="174"/>
+      <c r="A22" s="177"/>
+      <c r="B22" s="175"/>
       <c r="C22" s="61" t="s">
         <v>233</v>
       </c>
@@ -8864,8 +9127,8 @@
       <c r="S22" s="26"/>
     </row>
     <row r="23" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="188"/>
-      <c r="B23" s="174"/>
+      <c r="A23" s="177"/>
+      <c r="B23" s="175"/>
       <c r="C23" s="60" t="s">
         <v>45</v>
       </c>
@@ -8909,8 +9172,8 @@
       <c r="S23" s="26"/>
     </row>
     <row r="24" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="188"/>
-      <c r="B24" s="174"/>
+      <c r="A24" s="177"/>
+      <c r="B24" s="175"/>
       <c r="C24" s="60" t="s">
         <v>120</v>
       </c>
@@ -8956,8 +9219,8 @@
       <c r="S24" s="26"/>
     </row>
     <row r="25" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="188"/>
-      <c r="B25" s="174"/>
+      <c r="A25" s="177"/>
+      <c r="B25" s="175"/>
       <c r="C25" s="60" t="s">
         <v>235</v>
       </c>
@@ -9005,8 +9268,8 @@
       <c r="S25" s="26"/>
     </row>
     <row r="26" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="188"/>
-      <c r="B26" s="174"/>
+      <c r="A26" s="177"/>
+      <c r="B26" s="175"/>
       <c r="C26" s="60" t="s">
         <v>350</v>
       </c>
@@ -9050,8 +9313,8 @@
       <c r="S26" s="26"/>
     </row>
     <row r="27" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="188"/>
-      <c r="B27" s="174"/>
+      <c r="A27" s="177"/>
+      <c r="B27" s="175"/>
       <c r="C27" s="60" t="s">
         <v>119</v>
       </c>
@@ -9095,8 +9358,8 @@
       <c r="S27" s="26"/>
     </row>
     <row r="28" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="188"/>
-      <c r="B28" s="174"/>
+      <c r="A28" s="177"/>
+      <c r="B28" s="175"/>
       <c r="C28" s="60" t="s">
         <v>465</v>
       </c>
@@ -9140,8 +9403,8 @@
       <c r="S28" s="26"/>
     </row>
     <row r="29" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="188"/>
-      <c r="B29" s="174"/>
+      <c r="A29" s="177"/>
+      <c r="B29" s="175"/>
       <c r="C29" s="60" t="s">
         <v>385</v>
       </c>
@@ -9187,8 +9450,8 @@
       <c r="S29" s="26"/>
     </row>
     <row r="30" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="188"/>
-      <c r="B30" s="174"/>
+      <c r="A30" s="177"/>
+      <c r="B30" s="175"/>
       <c r="C30" s="60" t="s">
         <v>238</v>
       </c>
@@ -9235,8 +9498,8 @@
       <c r="T30" s="23"/>
     </row>
     <row r="31" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="188"/>
-      <c r="B31" s="174"/>
+      <c r="A31" s="177"/>
+      <c r="B31" s="175"/>
       <c r="C31" s="60" t="s">
         <v>351</v>
       </c>
@@ -9282,8 +9545,8 @@
       <c r="S31" s="26"/>
     </row>
     <row r="32" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="188"/>
-      <c r="B32" s="174"/>
+      <c r="A32" s="177"/>
+      <c r="B32" s="175"/>
       <c r="C32" s="60" t="s">
         <v>216</v>
       </c>
@@ -9330,8 +9593,8 @@
       <c r="T32" s="23"/>
     </row>
     <row r="33" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="188"/>
-      <c r="B33" s="174"/>
+      <c r="A33" s="177"/>
+      <c r="B33" s="175"/>
       <c r="C33" s="60" t="s">
         <v>242</v>
       </c>
@@ -9377,8 +9640,8 @@
       <c r="S33" s="26"/>
     </row>
     <row r="34" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="188"/>
-      <c r="B34" s="174"/>
+      <c r="A34" s="177"/>
+      <c r="B34" s="175"/>
       <c r="C34" s="60" t="s">
         <v>375</v>
       </c>
@@ -9422,8 +9685,8 @@
       <c r="S34" s="26"/>
     </row>
     <row r="35" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="188"/>
-      <c r="B35" s="174"/>
+      <c r="A35" s="177"/>
+      <c r="B35" s="175"/>
       <c r="C35" s="60" t="s">
         <v>388</v>
       </c>
@@ -9467,8 +9730,8 @@
       <c r="S35" s="26"/>
     </row>
     <row r="36" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="188"/>
-      <c r="B36" s="179"/>
+      <c r="A36" s="177"/>
+      <c r="B36" s="176"/>
       <c r="C36" s="65" t="s">
         <v>234</v>
       </c>
@@ -9512,10 +9775,10 @@
       <c r="S36" s="26"/>
     </row>
     <row r="37" spans="1:20" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="195" t="s">
+      <c r="A37" s="187" t="s">
         <v>266</v>
       </c>
-      <c r="B37" s="166" t="s">
+      <c r="B37" s="182" t="s">
         <v>51</v>
       </c>
       <c r="C37" s="62" t="s">
@@ -9560,8 +9823,8 @@
       <c r="T37" s="33"/>
     </row>
     <row r="38" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="196"/>
-      <c r="B38" s="167"/>
+      <c r="A38" s="188"/>
+      <c r="B38" s="180"/>
       <c r="C38" s="60" t="s">
         <v>107</v>
       </c>
@@ -9603,8 +9866,8 @@
       <c r="S38" s="26"/>
     </row>
     <row r="39" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="196"/>
-      <c r="B39" s="167"/>
+      <c r="A39" s="188"/>
+      <c r="B39" s="180"/>
       <c r="C39" s="60" t="s">
         <v>108</v>
       </c>
@@ -9647,8 +9910,8 @@
       <c r="T39" s="23"/>
     </row>
     <row r="40" spans="1:20" s="28" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="196"/>
-      <c r="B40" s="167"/>
+      <c r="A40" s="188"/>
+      <c r="B40" s="180"/>
       <c r="C40" s="61" t="s">
         <v>109</v>
       </c>
@@ -9696,8 +9959,8 @@
       <c r="S40" s="31"/>
     </row>
     <row r="41" spans="1:20" s="28" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="196"/>
-      <c r="B41" s="173" t="s">
+      <c r="A41" s="188"/>
+      <c r="B41" s="185" t="s">
         <v>193</v>
       </c>
       <c r="C41" s="63" t="s">
@@ -9743,8 +10006,8 @@
       <c r="S41" s="57"/>
     </row>
     <row r="42" spans="1:20" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="196"/>
-      <c r="B42" s="174"/>
+      <c r="A42" s="188"/>
+      <c r="B42" s="175"/>
       <c r="C42" s="60" t="s">
         <v>218</v>
       </c>
@@ -9786,8 +10049,8 @@
       <c r="S42" s="26"/>
     </row>
     <row r="43" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="196"/>
-      <c r="B43" s="174"/>
+      <c r="A43" s="188"/>
+      <c r="B43" s="175"/>
       <c r="C43" s="60" t="s">
         <v>258</v>
       </c>
@@ -9829,8 +10092,8 @@
       <c r="S43" s="26"/>
     </row>
     <row r="44" spans="1:20" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="196"/>
-      <c r="B44" s="174"/>
+      <c r="A44" s="188"/>
+      <c r="B44" s="175"/>
       <c r="C44" s="60" t="s">
         <v>219</v>
       </c>
@@ -9872,8 +10135,8 @@
       <c r="S44" s="26"/>
     </row>
     <row r="45" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="196"/>
-      <c r="B45" s="174"/>
+      <c r="A45" s="188"/>
+      <c r="B45" s="175"/>
       <c r="C45" s="60" t="s">
         <v>490</v>
       </c>
@@ -9918,8 +10181,8 @@
       <c r="T45" s="28"/>
     </row>
     <row r="46" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="196"/>
-      <c r="B46" s="174"/>
+      <c r="A46" s="188"/>
+      <c r="B46" s="175"/>
       <c r="C46" s="60" t="s">
         <v>413</v>
       </c>
@@ -9961,8 +10224,8 @@
       <c r="S46" s="26"/>
     </row>
     <row r="47" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="196"/>
-      <c r="B47" s="174"/>
+      <c r="A47" s="188"/>
+      <c r="B47" s="175"/>
       <c r="C47" s="60" t="s">
         <v>410</v>
       </c>
@@ -10004,8 +10267,8 @@
       <c r="S47" s="26"/>
     </row>
     <row r="48" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="196"/>
-      <c r="B48" s="174"/>
+      <c r="A48" s="188"/>
+      <c r="B48" s="175"/>
       <c r="C48" s="60" t="s">
         <v>408</v>
       </c>
@@ -10051,8 +10314,8 @@
       <c r="S48" s="26"/>
     </row>
     <row r="49" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="196"/>
-      <c r="B49" s="174"/>
+      <c r="A49" s="188"/>
+      <c r="B49" s="175"/>
       <c r="C49" s="60" t="s">
         <v>257</v>
       </c>
@@ -10096,8 +10359,8 @@
       <c r="S49" s="26"/>
     </row>
     <row r="50" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="197"/>
-      <c r="B50" s="179"/>
+      <c r="A50" s="189"/>
+      <c r="B50" s="176"/>
       <c r="C50" s="65" t="s">
         <v>531</v>
       </c>
@@ -10141,10 +10404,10 @@
       <c r="S50" s="26"/>
     </row>
     <row r="51" spans="1:20" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="168" t="s">
+      <c r="A51" s="191" t="s">
         <v>89</v>
       </c>
-      <c r="B51" s="166" t="s">
+      <c r="B51" s="182" t="s">
         <v>51</v>
       </c>
       <c r="C51" s="62" t="s">
@@ -10191,8 +10454,8 @@
       <c r="T51" s="33"/>
     </row>
     <row r="52" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="169"/>
-      <c r="B52" s="167"/>
+      <c r="A52" s="192"/>
+      <c r="B52" s="180"/>
       <c r="C52" s="60" t="s">
         <v>66</v>
       </c>
@@ -10238,8 +10501,8 @@
       <c r="S52" s="26"/>
     </row>
     <row r="53" spans="1:20" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="169"/>
-      <c r="B53" s="167"/>
+      <c r="A53" s="192"/>
+      <c r="B53" s="180"/>
       <c r="C53" s="60" t="s">
         <v>67</v>
       </c>
@@ -10285,8 +10548,8 @@
       <c r="S53" s="26"/>
     </row>
     <row r="54" spans="1:20" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="169"/>
-      <c r="B54" s="167"/>
+      <c r="A54" s="192"/>
+      <c r="B54" s="180"/>
       <c r="C54" s="61" t="s">
         <v>68</v>
       </c>
@@ -10332,8 +10595,8 @@
       <c r="S54" s="26"/>
     </row>
     <row r="55" spans="1:20" s="23" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="169"/>
-      <c r="B55" s="167"/>
+      <c r="A55" s="192"/>
+      <c r="B55" s="180"/>
       <c r="C55" s="65" t="s">
         <v>604</v>
       </c>
@@ -10377,8 +10640,8 @@
       <c r="S55" s="31"/>
     </row>
     <row r="56" spans="1:20" s="23" customFormat="1" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="169"/>
-      <c r="B56" s="173" t="s">
+      <c r="A56" s="192"/>
+      <c r="B56" s="185" t="s">
         <v>193</v>
       </c>
       <c r="C56" s="63" t="s">
@@ -10424,8 +10687,8 @@
       <c r="S56" s="57"/>
     </row>
     <row r="57" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="169"/>
-      <c r="B57" s="174"/>
+      <c r="A57" s="192"/>
+      <c r="B57" s="175"/>
       <c r="C57" s="60" t="s">
         <v>209</v>
       </c>
@@ -10471,8 +10734,8 @@
       <c r="S57" s="26"/>
     </row>
     <row r="58" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="169"/>
-      <c r="B58" s="174"/>
+      <c r="A58" s="192"/>
+      <c r="B58" s="175"/>
       <c r="C58" s="60" t="s">
         <v>202</v>
       </c>
@@ -10516,8 +10779,8 @@
       <c r="S58" s="26"/>
     </row>
     <row r="59" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="169"/>
-      <c r="B59" s="174"/>
+      <c r="A59" s="192"/>
+      <c r="B59" s="175"/>
       <c r="C59" s="60" t="s">
         <v>197</v>
       </c>
@@ -10563,8 +10826,8 @@
       <c r="S59" s="26"/>
     </row>
     <row r="60" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="169"/>
-      <c r="B60" s="174"/>
+      <c r="A60" s="192"/>
+      <c r="B60" s="175"/>
       <c r="C60" s="60" t="s">
         <v>198</v>
       </c>
@@ -10610,8 +10873,8 @@
       <c r="S60" s="26"/>
     </row>
     <row r="61" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="169"/>
-      <c r="B61" s="174"/>
+      <c r="A61" s="192"/>
+      <c r="B61" s="175"/>
       <c r="C61" s="60" t="s">
         <v>91</v>
       </c>
@@ -10655,8 +10918,8 @@
       <c r="S61" s="26"/>
     </row>
     <row r="62" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="169"/>
-      <c r="B62" s="174"/>
+      <c r="A62" s="192"/>
+      <c r="B62" s="175"/>
       <c r="C62" s="60" t="s">
         <v>415</v>
       </c>
@@ -10700,8 +10963,8 @@
       <c r="S62" s="26"/>
     </row>
     <row r="63" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="169"/>
-      <c r="B63" s="174"/>
+      <c r="A63" s="192"/>
+      <c r="B63" s="175"/>
       <c r="C63" s="60" t="s">
         <v>199</v>
       </c>
@@ -10747,8 +11010,8 @@
       <c r="S63" s="26"/>
     </row>
     <row r="64" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="169"/>
-      <c r="B64" s="174"/>
+      <c r="A64" s="192"/>
+      <c r="B64" s="175"/>
       <c r="C64" s="60" t="s">
         <v>429</v>
       </c>
@@ -10794,8 +11057,8 @@
       <c r="S64" s="26"/>
     </row>
     <row r="65" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="169"/>
-      <c r="B65" s="174"/>
+      <c r="A65" s="192"/>
+      <c r="B65" s="175"/>
       <c r="C65" s="60" t="s">
         <v>377</v>
       </c>
@@ -10840,8 +11103,8 @@
       <c r="T65" s="28"/>
     </row>
     <row r="66" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="169"/>
-      <c r="B66" s="174"/>
+      <c r="A66" s="192"/>
+      <c r="B66" s="175"/>
       <c r="C66" s="60" t="s">
         <v>394</v>
       </c>
@@ -10887,8 +11150,8 @@
       <c r="S66" s="26"/>
     </row>
     <row r="67" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="169"/>
-      <c r="B67" s="174"/>
+      <c r="A67" s="192"/>
+      <c r="B67" s="175"/>
       <c r="C67" s="60" t="s">
         <v>254</v>
       </c>
@@ -10935,8 +11198,8 @@
       <c r="T67" s="23"/>
     </row>
     <row r="68" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="169"/>
-      <c r="B68" s="174"/>
+      <c r="A68" s="192"/>
+      <c r="B68" s="175"/>
       <c r="C68" s="60" t="s">
         <v>432</v>
       </c>
@@ -10980,8 +11243,8 @@
       <c r="S68" s="26"/>
     </row>
     <row r="69" spans="1:20" s="33" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="169"/>
-      <c r="B69" s="174"/>
+      <c r="A69" s="192"/>
+      <c r="B69" s="175"/>
       <c r="C69" s="61" t="s">
         <v>203</v>
       </c>
@@ -11026,10 +11289,10 @@
       <c r="T69" s="28"/>
     </row>
     <row r="70" spans="1:20" s="23" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="181" t="s">
+      <c r="A70" s="201" t="s">
         <v>97</v>
       </c>
-      <c r="B70" s="180"/>
+      <c r="B70" s="200"/>
       <c r="C70" s="62" t="s">
         <v>79</v>
       </c>
@@ -11076,8 +11339,8 @@
       <c r="T70" s="33"/>
     </row>
     <row r="71" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="182"/>
-      <c r="B71" s="167"/>
+      <c r="A71" s="202"/>
+      <c r="B71" s="180"/>
       <c r="C71" s="60" t="s">
         <v>80</v>
       </c>
@@ -11123,8 +11386,8 @@
       <c r="S71" s="26"/>
     </row>
     <row r="72" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="182"/>
-      <c r="B72" s="167"/>
+      <c r="A72" s="202"/>
+      <c r="B72" s="180"/>
       <c r="C72" s="60" t="s">
         <v>81</v>
       </c>
@@ -11172,8 +11435,8 @@
       <c r="S72" s="26"/>
     </row>
     <row r="73" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="182"/>
-      <c r="B73" s="167"/>
+      <c r="A73" s="202"/>
+      <c r="B73" s="180"/>
       <c r="C73" s="60" t="s">
         <v>82</v>
       </c>
@@ -11219,8 +11482,8 @@
       <c r="S73" s="26"/>
     </row>
     <row r="74" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="182"/>
-      <c r="B74" s="167"/>
+      <c r="A74" s="202"/>
+      <c r="B74" s="180"/>
       <c r="C74" s="60" t="s">
         <v>83</v>
       </c>
@@ -11268,8 +11531,8 @@
       <c r="S74" s="26"/>
     </row>
     <row r="75" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="182"/>
-      <c r="B75" s="167"/>
+      <c r="A75" s="202"/>
+      <c r="B75" s="180"/>
       <c r="C75" s="60" t="s">
         <v>84</v>
       </c>
@@ -11315,8 +11578,8 @@
       <c r="S75" s="26"/>
     </row>
     <row r="76" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="182"/>
-      <c r="B76" s="167"/>
+      <c r="A76" s="202"/>
+      <c r="B76" s="180"/>
       <c r="C76" s="60" t="s">
         <v>85</v>
       </c>
@@ -11360,8 +11623,8 @@
       <c r="S76" s="26"/>
     </row>
     <row r="77" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="182"/>
-      <c r="B77" s="167"/>
+      <c r="A77" s="202"/>
+      <c r="B77" s="180"/>
       <c r="C77" s="60" t="s">
         <v>86</v>
       </c>
@@ -11407,8 +11670,8 @@
       <c r="S77" s="26"/>
     </row>
     <row r="78" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="182"/>
-      <c r="B78" s="167"/>
+      <c r="A78" s="202"/>
+      <c r="B78" s="180"/>
       <c r="C78" s="60" t="s">
         <v>87</v>
       </c>
@@ -11456,8 +11719,8 @@
       <c r="S78" s="26"/>
     </row>
     <row r="79" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="182"/>
-      <c r="B79" s="167"/>
+      <c r="A79" s="202"/>
+      <c r="B79" s="180"/>
       <c r="C79" s="60" t="s">
         <v>225</v>
       </c>
@@ -11503,8 +11766,8 @@
       <c r="S79" s="26"/>
     </row>
     <row r="80" spans="1:20" s="23" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="182"/>
-      <c r="B80" s="178"/>
+      <c r="A80" s="202"/>
+      <c r="B80" s="199"/>
       <c r="C80" s="61" t="s">
         <v>90</v>
       </c>
@@ -11550,8 +11813,8 @@
       <c r="S80" s="31"/>
     </row>
     <row r="81" spans="1:19" s="23" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="182"/>
-      <c r="B81" s="174" t="s">
+      <c r="A81" s="202"/>
+      <c r="B81" s="175" t="s">
         <v>193</v>
       </c>
       <c r="C81" s="63" t="s">
@@ -11595,8 +11858,8 @@
       <c r="S81" s="57"/>
     </row>
     <row r="82" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="182"/>
-      <c r="B82" s="174"/>
+      <c r="A82" s="202"/>
+      <c r="B82" s="175"/>
       <c r="C82" s="60" t="s">
         <v>213</v>
       </c>
@@ -11642,8 +11905,8 @@
       <c r="S82" s="26"/>
     </row>
     <row r="83" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="182"/>
-      <c r="B83" s="174"/>
+      <c r="A83" s="202"/>
+      <c r="B83" s="175"/>
       <c r="C83" s="60" t="s">
         <v>427</v>
       </c>
@@ -11687,8 +11950,8 @@
       <c r="S83" s="26"/>
     </row>
     <row r="84" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="182"/>
-      <c r="B84" s="174"/>
+      <c r="A84" s="202"/>
+      <c r="B84" s="175"/>
       <c r="C84" s="60" t="s">
         <v>295</v>
       </c>
@@ -11732,8 +11995,8 @@
       <c r="S84" s="26"/>
     </row>
     <row r="85" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="182"/>
-      <c r="B85" s="174"/>
+      <c r="A85" s="202"/>
+      <c r="B85" s="175"/>
       <c r="C85" s="60" t="s">
         <v>368</v>
       </c>
@@ -11777,8 +12040,8 @@
       <c r="S85" s="26"/>
     </row>
     <row r="86" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="182"/>
-      <c r="B86" s="174"/>
+      <c r="A86" s="202"/>
+      <c r="B86" s="175"/>
       <c r="C86" s="60" t="s">
         <v>221</v>
       </c>
@@ -11822,8 +12085,8 @@
       <c r="S86" s="26"/>
     </row>
     <row r="87" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="182"/>
-      <c r="B87" s="174"/>
+      <c r="A87" s="202"/>
+      <c r="B87" s="175"/>
       <c r="C87" s="60" t="s">
         <v>322</v>
       </c>
@@ -11869,8 +12132,8 @@
       <c r="S87" s="26"/>
     </row>
     <row r="88" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="182"/>
-      <c r="B88" s="174"/>
+      <c r="A88" s="202"/>
+      <c r="B88" s="175"/>
       <c r="C88" s="61" t="s">
         <v>249</v>
       </c>
@@ -11914,8 +12177,8 @@
       <c r="S88" s="26"/>
     </row>
     <row r="89" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="182"/>
-      <c r="B89" s="174"/>
+      <c r="A89" s="202"/>
+      <c r="B89" s="175"/>
       <c r="C89" s="60" t="s">
         <v>404</v>
       </c>
@@ -11956,8 +12219,8 @@
       <c r="S89" s="26"/>
     </row>
     <row r="90" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="182"/>
-      <c r="B90" s="174"/>
+      <c r="A90" s="202"/>
+      <c r="B90" s="175"/>
       <c r="C90" s="60" t="s">
         <v>370</v>
       </c>
@@ -11999,8 +12262,8 @@
       <c r="S90" s="26"/>
     </row>
     <row r="91" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="182"/>
-      <c r="B91" s="174"/>
+      <c r="A91" s="202"/>
+      <c r="B91" s="175"/>
       <c r="C91" s="60" t="s">
         <v>357</v>
       </c>
@@ -12046,8 +12309,8 @@
       <c r="S91" s="26"/>
     </row>
     <row r="92" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="182"/>
-      <c r="B92" s="174"/>
+      <c r="A92" s="202"/>
+      <c r="B92" s="175"/>
       <c r="C92" s="60" t="s">
         <v>353</v>
       </c>
@@ -12093,8 +12356,8 @@
       <c r="S92" s="26"/>
     </row>
     <row r="93" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="182"/>
-      <c r="B93" s="174"/>
+      <c r="A93" s="202"/>
+      <c r="B93" s="175"/>
       <c r="C93" s="60" t="s">
         <v>212</v>
       </c>
@@ -12137,8 +12400,8 @@
       <c r="S93" s="26"/>
     </row>
     <row r="94" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="182"/>
-      <c r="B94" s="174"/>
+      <c r="A94" s="202"/>
+      <c r="B94" s="175"/>
       <c r="C94" s="60" t="s">
         <v>373</v>
       </c>
@@ -12182,8 +12445,8 @@
       <c r="S94" s="26"/>
     </row>
     <row r="95" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="182"/>
-      <c r="B95" s="174"/>
+      <c r="A95" s="202"/>
+      <c r="B95" s="175"/>
       <c r="C95" s="60" t="s">
         <v>222</v>
       </c>
@@ -12227,8 +12490,8 @@
       <c r="S95" s="26"/>
     </row>
     <row r="96" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="182"/>
-      <c r="B96" s="174"/>
+      <c r="A96" s="202"/>
+      <c r="B96" s="175"/>
       <c r="C96" s="60" t="s">
         <v>247</v>
       </c>
@@ -12272,8 +12535,8 @@
       <c r="S96" s="26"/>
     </row>
     <row r="97" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="182"/>
-      <c r="B97" s="174"/>
+      <c r="A97" s="202"/>
+      <c r="B97" s="175"/>
       <c r="C97" s="60" t="s">
         <v>294</v>
       </c>
@@ -12317,8 +12580,8 @@
       <c r="S97" s="26"/>
     </row>
     <row r="98" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="182"/>
-      <c r="B98" s="174"/>
+      <c r="A98" s="202"/>
+      <c r="B98" s="175"/>
       <c r="C98" s="60" t="s">
         <v>224</v>
       </c>
@@ -12362,8 +12625,8 @@
       <c r="S98" s="26"/>
     </row>
     <row r="99" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="182"/>
-      <c r="B99" s="174"/>
+      <c r="A99" s="202"/>
+      <c r="B99" s="175"/>
       <c r="C99" s="60" t="s">
         <v>232</v>
       </c>
@@ -12402,8 +12665,8 @@
       <c r="S99" s="26"/>
     </row>
     <row r="100" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="182"/>
-      <c r="B100" s="174"/>
+      <c r="A100" s="202"/>
+      <c r="B100" s="175"/>
       <c r="C100" s="60" t="s">
         <v>223</v>
       </c>
@@ -12444,8 +12707,8 @@
       <c r="S100" s="26"/>
     </row>
     <row r="101" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="182"/>
-      <c r="B101" s="174"/>
+      <c r="A101" s="202"/>
+      <c r="B101" s="175"/>
       <c r="C101" s="65" t="s">
         <v>217</v>
       </c>
@@ -12491,8 +12754,8 @@
       <c r="S101" s="26"/>
     </row>
     <row r="102" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="182"/>
-      <c r="B102" s="174"/>
+      <c r="A102" s="202"/>
+      <c r="B102" s="175"/>
       <c r="C102" s="60" t="s">
         <v>214</v>
       </c>
@@ -12534,8 +12797,8 @@
       <c r="S102" s="26"/>
     </row>
     <row r="103" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="182"/>
-      <c r="B103" s="174"/>
+      <c r="A103" s="202"/>
+      <c r="B103" s="175"/>
       <c r="C103" s="60" t="s">
         <v>215</v>
       </c>
@@ -12579,8 +12842,8 @@
       <c r="S103" s="26"/>
     </row>
     <row r="104" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="182"/>
-      <c r="B104" s="174"/>
+      <c r="A104" s="202"/>
+      <c r="B104" s="175"/>
       <c r="C104" s="60" t="s">
         <v>359</v>
       </c>
@@ -12621,8 +12884,8 @@
       <c r="S104" s="26"/>
     </row>
     <row r="105" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="182"/>
-      <c r="B105" s="174"/>
+      <c r="A105" s="202"/>
+      <c r="B105" s="175"/>
       <c r="C105" s="60" t="s">
         <v>231</v>
       </c>
@@ -12663,8 +12926,8 @@
       <c r="S105" s="26"/>
     </row>
     <row r="106" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="182"/>
-      <c r="B106" s="174"/>
+      <c r="A106" s="202"/>
+      <c r="B106" s="175"/>
       <c r="C106" s="60" t="s">
         <v>206</v>
       </c>
@@ -12706,8 +12969,8 @@
       <c r="S106" s="26"/>
     </row>
     <row r="107" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="182"/>
-      <c r="B107" s="174"/>
+      <c r="A107" s="202"/>
+      <c r="B107" s="175"/>
       <c r="C107" s="60" t="s">
         <v>207</v>
       </c>
@@ -12749,8 +13012,8 @@
       <c r="S107" s="26"/>
     </row>
     <row r="108" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="182"/>
-      <c r="B108" s="174"/>
+      <c r="A108" s="202"/>
+      <c r="B108" s="175"/>
       <c r="C108" s="60" t="s">
         <v>502</v>
       </c>
@@ -12791,8 +13054,8 @@
       <c r="S108" s="26"/>
     </row>
     <row r="109" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="182"/>
-      <c r="B109" s="174"/>
+      <c r="A109" s="202"/>
+      <c r="B109" s="175"/>
       <c r="C109" s="60" t="s">
         <v>248</v>
       </c>
@@ -12833,8 +13096,8 @@
       <c r="S109" s="26"/>
     </row>
     <row r="110" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="182"/>
-      <c r="B110" s="174"/>
+      <c r="A110" s="202"/>
+      <c r="B110" s="175"/>
       <c r="C110" s="60" t="s">
         <v>251</v>
       </c>
@@ -12878,8 +13141,8 @@
       <c r="S110" s="26"/>
     </row>
     <row r="111" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="182"/>
-      <c r="B111" s="174"/>
+      <c r="A111" s="202"/>
+      <c r="B111" s="175"/>
       <c r="C111" s="60" t="s">
         <v>228</v>
       </c>
@@ -12925,8 +13188,8 @@
       <c r="S111" s="26"/>
     </row>
     <row r="112" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="182"/>
-      <c r="B112" s="174"/>
+      <c r="A112" s="202"/>
+      <c r="B112" s="175"/>
       <c r="C112" s="60" t="s">
         <v>229</v>
       </c>
@@ -12972,8 +13235,8 @@
       <c r="S112" s="26"/>
     </row>
     <row r="113" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="182"/>
-      <c r="B113" s="174"/>
+      <c r="A113" s="202"/>
+      <c r="B113" s="175"/>
       <c r="C113" s="65" t="s">
         <v>598</v>
       </c>
@@ -13000,8 +13263,8 @@
       <c r="T113" s="23"/>
     </row>
     <row r="114" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="182"/>
-      <c r="B114" s="174"/>
+      <c r="A114" s="202"/>
+      <c r="B114" s="175"/>
       <c r="C114" s="60" t="s">
         <v>325</v>
       </c>
@@ -13046,8 +13309,8 @@
       <c r="T114" s="23"/>
     </row>
     <row r="115" spans="1:20" s="33" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="183"/>
-      <c r="B115" s="179"/>
+      <c r="A115" s="203"/>
+      <c r="B115" s="176"/>
       <c r="C115" s="61" t="s">
         <v>318</v>
       </c>
@@ -13100,10 +13363,10 @@
       <c r="T115" s="28"/>
     </row>
     <row r="116" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="175" t="s">
+      <c r="A116" s="196" t="s">
         <v>500</v>
       </c>
-      <c r="B116" s="166" t="s">
+      <c r="B116" s="182" t="s">
         <v>51</v>
       </c>
       <c r="C116" s="62" t="s">
@@ -13148,8 +13411,8 @@
       <c r="T116" s="33"/>
     </row>
     <row r="117" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="176"/>
-      <c r="B117" s="167"/>
+      <c r="A117" s="197"/>
+      <c r="B117" s="180"/>
       <c r="C117" s="60" t="s">
         <v>92</v>
       </c>
@@ -13195,8 +13458,8 @@
       <c r="S117" s="26"/>
     </row>
     <row r="118" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="176"/>
-      <c r="B118" s="167"/>
+      <c r="A118" s="197"/>
+      <c r="B118" s="180"/>
       <c r="C118" s="60" t="s">
         <v>93</v>
       </c>
@@ -13242,8 +13505,8 @@
       <c r="S118" s="26"/>
     </row>
     <row r="119" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="176"/>
-      <c r="B119" s="167"/>
+      <c r="A119" s="197"/>
+      <c r="B119" s="180"/>
       <c r="C119" s="60" t="s">
         <v>104</v>
       </c>
@@ -13285,8 +13548,8 @@
       <c r="S119" s="26"/>
     </row>
     <row r="120" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="176"/>
-      <c r="B120" s="167"/>
+      <c r="A120" s="197"/>
+      <c r="B120" s="180"/>
       <c r="C120" s="61" t="s">
         <v>94</v>
       </c>
@@ -13329,8 +13592,8 @@
       <c r="T120" s="28"/>
     </row>
     <row r="121" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="176"/>
-      <c r="B121" s="167"/>
+      <c r="A121" s="197"/>
+      <c r="B121" s="180"/>
       <c r="C121" s="60" t="s">
         <v>179</v>
       </c>
@@ -13373,8 +13636,8 @@
       <c r="T121" s="28"/>
     </row>
     <row r="122" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="176"/>
-      <c r="B122" s="167"/>
+      <c r="A122" s="197"/>
+      <c r="B122" s="180"/>
       <c r="C122" s="61" t="s">
         <v>116</v>
       </c>
@@ -13417,8 +13680,8 @@
       <c r="T122" s="28"/>
     </row>
     <row r="123" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="176"/>
-      <c r="B123" s="167"/>
+      <c r="A123" s="197"/>
+      <c r="B123" s="180"/>
       <c r="C123" s="60" t="s">
         <v>96</v>
       </c>
@@ -13462,8 +13725,8 @@
       <c r="S123" s="26"/>
     </row>
     <row r="124" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="176"/>
-      <c r="B124" s="167"/>
+      <c r="A124" s="197"/>
+      <c r="B124" s="180"/>
       <c r="C124" s="60" t="s">
         <v>501</v>
       </c>
@@ -13507,8 +13770,8 @@
       <c r="S124" s="26"/>
     </row>
     <row r="125" spans="1:20" s="23" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="176"/>
-      <c r="B125" s="178"/>
+      <c r="A125" s="197"/>
+      <c r="B125" s="199"/>
       <c r="C125" s="60" t="s">
         <v>176</v>
       </c>
@@ -13550,8 +13813,8 @@
       <c r="S125" s="26"/>
     </row>
     <row r="126" spans="1:20" s="28" customFormat="1" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="176"/>
-      <c r="B126" s="173" t="s">
+      <c r="A126" s="197"/>
+      <c r="B126" s="185" t="s">
         <v>193</v>
       </c>
       <c r="C126" s="63" t="s">
@@ -13596,8 +13859,8 @@
       <c r="T126" s="23"/>
     </row>
     <row r="127" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="176"/>
-      <c r="B127" s="174"/>
+      <c r="A127" s="197"/>
+      <c r="B127" s="175"/>
       <c r="C127" s="60" t="s">
         <v>448</v>
       </c>
@@ -13638,8 +13901,8 @@
       <c r="T127" s="23"/>
     </row>
     <row r="128" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="176"/>
-      <c r="B128" s="174"/>
+      <c r="A128" s="197"/>
+      <c r="B128" s="175"/>
       <c r="C128" s="60" t="s">
         <v>451</v>
       </c>
@@ -13680,8 +13943,8 @@
       <c r="T128" s="23"/>
     </row>
     <row r="129" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="176"/>
-      <c r="B129" s="174"/>
+      <c r="A129" s="197"/>
+      <c r="B129" s="175"/>
       <c r="C129" s="61" t="s">
         <v>425</v>
       </c>
@@ -13724,8 +13987,8 @@
       <c r="T129" s="23"/>
     </row>
     <row r="130" spans="1:20" s="33" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="176"/>
-      <c r="B130" s="174"/>
+      <c r="A130" s="197"/>
+      <c r="B130" s="175"/>
       <c r="C130" s="60" t="s">
         <v>230</v>
       </c>
@@ -13766,8 +14029,8 @@
       <c r="T130" s="23"/>
     </row>
     <row r="131" spans="1:20" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="176"/>
-      <c r="B131" s="174"/>
+      <c r="A131" s="197"/>
+      <c r="B131" s="175"/>
       <c r="C131" s="60" t="s">
         <v>208</v>
       </c>
@@ -13808,8 +14071,8 @@
       <c r="T131" s="23"/>
     </row>
     <row r="132" spans="1:20" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="177"/>
-      <c r="B132" s="174"/>
+      <c r="A132" s="198"/>
+      <c r="B132" s="175"/>
       <c r="C132" s="65" t="s">
         <v>624</v>
       </c>
@@ -13832,10 +14095,10 @@
       <c r="T132" s="23"/>
     </row>
     <row r="133" spans="1:20" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="170" t="s">
+      <c r="A133" s="193" t="s">
         <v>111</v>
       </c>
-      <c r="B133" s="166" t="s">
+      <c r="B133" s="182" t="s">
         <v>51</v>
       </c>
       <c r="C133" s="62" t="s">
@@ -13878,8 +14141,8 @@
       <c r="T133" s="33"/>
     </row>
     <row r="134" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="171"/>
-      <c r="B134" s="167"/>
+      <c r="A134" s="194"/>
+      <c r="B134" s="180"/>
       <c r="C134" s="61" t="s">
         <v>95</v>
       </c>
@@ -13919,8 +14182,8 @@
       <c r="S134" s="31"/>
     </row>
     <row r="135" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="171"/>
-      <c r="B135" s="167"/>
+      <c r="A135" s="194"/>
+      <c r="B135" s="180"/>
       <c r="C135" s="65" t="s">
         <v>602</v>
       </c>
@@ -13963,8 +14226,8 @@
       <c r="T135" s="19"/>
     </row>
     <row r="136" spans="1:20" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="171"/>
-      <c r="B136" s="167"/>
+      <c r="A136" s="194"/>
+      <c r="B136" s="180"/>
       <c r="C136" s="60" t="s">
         <v>115</v>
       </c>
@@ -14006,8 +14269,8 @@
       <c r="T136" s="19"/>
     </row>
     <row r="137" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A137" s="171"/>
-      <c r="B137" s="167"/>
+      <c r="A137" s="194"/>
+      <c r="B137" s="180"/>
       <c r="C137" s="60" t="s">
         <v>114</v>
       </c>
@@ -14049,8 +14312,8 @@
       <c r="T137" s="19"/>
     </row>
     <row r="138" spans="1:20" s="23" customFormat="1" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="171"/>
-      <c r="B138" s="173" t="s">
+      <c r="A138" s="194"/>
+      <c r="B138" s="185" t="s">
         <v>193</v>
       </c>
       <c r="C138" s="63" t="s">
@@ -14092,8 +14355,8 @@
       <c r="S138" s="57"/>
     </row>
     <row r="139" spans="1:20" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="171"/>
-      <c r="B139" s="174"/>
+      <c r="A139" s="194"/>
+      <c r="B139" s="175"/>
       <c r="C139" s="60" t="s">
         <v>399</v>
       </c>
@@ -14132,8 +14395,8 @@
       <c r="S139" s="26"/>
     </row>
     <row r="140" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="171"/>
-      <c r="B140" s="174"/>
+      <c r="A140" s="194"/>
+      <c r="B140" s="175"/>
       <c r="C140" s="60" t="s">
         <v>255</v>
       </c>
@@ -14173,8 +14436,8 @@
       <c r="S140" s="26"/>
     </row>
     <row r="141" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="171"/>
-      <c r="B141" s="174"/>
+      <c r="A141" s="194"/>
+      <c r="B141" s="175"/>
       <c r="C141" s="65" t="s">
         <v>618</v>
       </c>
@@ -14208,8 +14471,8 @@
       <c r="S141" s="26"/>
     </row>
     <row r="142" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="171"/>
-      <c r="B142" s="174"/>
+      <c r="A142" s="194"/>
+      <c r="B142" s="175"/>
       <c r="C142" s="60" t="s">
         <v>422</v>
       </c>
@@ -14249,8 +14512,8 @@
       <c r="S142" s="26"/>
     </row>
     <row r="143" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="171"/>
-      <c r="B143" s="174"/>
+      <c r="A143" s="194"/>
+      <c r="B143" s="175"/>
       <c r="C143" s="60" t="s">
         <v>380</v>
       </c>
@@ -14290,8 +14553,8 @@
       <c r="S143" s="26"/>
     </row>
     <row r="144" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="171"/>
-      <c r="B144" s="174"/>
+      <c r="A144" s="194"/>
+      <c r="B144" s="175"/>
       <c r="C144" s="60" t="s">
         <v>439</v>
       </c>
@@ -14331,8 +14594,8 @@
       <c r="S144" s="26"/>
     </row>
     <row r="145" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="171"/>
-      <c r="B145" s="174"/>
+      <c r="A145" s="194"/>
+      <c r="B145" s="175"/>
       <c r="C145" s="60" t="s">
         <v>358</v>
       </c>
@@ -14372,8 +14635,8 @@
       <c r="S145" s="26"/>
     </row>
     <row r="146" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="171"/>
-      <c r="B146" s="174"/>
+      <c r="A146" s="194"/>
+      <c r="B146" s="175"/>
       <c r="C146" s="60" t="s">
         <v>226</v>
       </c>
@@ -14413,8 +14676,8 @@
       <c r="S146" s="26"/>
     </row>
     <row r="147" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="171"/>
-      <c r="B147" s="174"/>
+      <c r="A147" s="194"/>
+      <c r="B147" s="175"/>
       <c r="C147" s="60" t="s">
         <v>421</v>
       </c>
@@ -14454,8 +14717,8 @@
       <c r="S147" s="26"/>
     </row>
     <row r="148" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="171"/>
-      <c r="B148" s="174"/>
+      <c r="A148" s="194"/>
+      <c r="B148" s="175"/>
       <c r="C148" s="60" t="s">
         <v>396</v>
       </c>
@@ -14495,8 +14758,8 @@
       <c r="S148" s="26"/>
     </row>
     <row r="149" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="171"/>
-      <c r="B149" s="174"/>
+      <c r="A149" s="194"/>
+      <c r="B149" s="175"/>
       <c r="C149" s="60" t="s">
         <v>433</v>
       </c>
@@ -14536,8 +14799,8 @@
       <c r="S149" s="26"/>
     </row>
     <row r="150" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="171"/>
-      <c r="B150" s="174"/>
+      <c r="A150" s="194"/>
+      <c r="B150" s="175"/>
       <c r="C150" s="60" t="s">
         <v>406</v>
       </c>
@@ -14577,8 +14840,8 @@
       <c r="S150" s="26"/>
     </row>
     <row r="151" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="171"/>
-      <c r="B151" s="174"/>
+      <c r="A151" s="194"/>
+      <c r="B151" s="175"/>
       <c r="C151" s="65" t="s">
         <v>521</v>
       </c>
@@ -14618,8 +14881,8 @@
       <c r="S151" s="26"/>
     </row>
     <row r="152" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="171"/>
-      <c r="B152" s="174"/>
+      <c r="A152" s="194"/>
+      <c r="B152" s="175"/>
       <c r="C152" s="65" t="s">
         <v>256</v>
       </c>
@@ -14659,8 +14922,8 @@
       <c r="S152" s="26"/>
     </row>
     <row r="153" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="171"/>
-      <c r="B153" s="174"/>
+      <c r="A153" s="194"/>
+      <c r="B153" s="175"/>
       <c r="C153" s="65" t="s">
         <v>446</v>
       </c>
@@ -14700,8 +14963,8 @@
       <c r="S153" s="26"/>
     </row>
     <row r="154" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="171"/>
-      <c r="B154" s="174"/>
+      <c r="A154" s="194"/>
+      <c r="B154" s="175"/>
       <c r="C154" s="65" t="s">
         <v>435</v>
       </c>
@@ -14741,8 +15004,8 @@
       <c r="S154" s="26"/>
     </row>
     <row r="155" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="171"/>
-      <c r="B155" s="174"/>
+      <c r="A155" s="194"/>
+      <c r="B155" s="175"/>
       <c r="C155" s="65" t="s">
         <v>319</v>
       </c>
@@ -14784,8 +15047,8 @@
       <c r="S155" s="26"/>
     </row>
     <row r="156" spans="1:19" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="171"/>
-      <c r="B156" s="174"/>
+      <c r="A156" s="194"/>
+      <c r="B156" s="175"/>
       <c r="C156" s="65" t="s">
         <v>366</v>
       </c>
@@ -14825,8 +15088,8 @@
       <c r="S156" s="26"/>
     </row>
     <row r="157" spans="1:19" s="23" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A157" s="172"/>
-      <c r="B157" s="174"/>
+      <c r="A157" s="195"/>
+      <c r="B157" s="175"/>
       <c r="C157" s="65" t="s">
         <v>211</v>
       </c>
@@ -14866,10 +15129,10 @@
       <c r="S157" s="31"/>
     </row>
     <row r="158" spans="1:19" s="33" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A158" s="192" t="s">
+      <c r="A158" s="183" t="s">
         <v>112</v>
       </c>
-      <c r="B158" s="187" t="s">
+      <c r="B158" s="174" t="s">
         <v>193</v>
       </c>
       <c r="C158" s="62" t="s">
@@ -14913,8 +15176,8 @@
       <c r="S158" s="36"/>
     </row>
     <row r="159" spans="1:19" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A159" s="192"/>
-      <c r="B159" s="174"/>
+      <c r="A159" s="183"/>
+      <c r="B159" s="175"/>
       <c r="C159" s="60" t="s">
         <v>362</v>
       </c>
@@ -14956,8 +15219,8 @@
       <c r="S159" s="26"/>
     </row>
     <row r="160" spans="1:19" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A160" s="192"/>
-      <c r="B160" s="174"/>
+      <c r="A160" s="183"/>
+      <c r="B160" s="175"/>
       <c r="C160" s="60" t="s">
         <v>381</v>
       </c>
@@ -14999,8 +15262,8 @@
       <c r="S160" s="26"/>
     </row>
     <row r="161" spans="1:19" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A161" s="192"/>
-      <c r="B161" s="174"/>
+      <c r="A161" s="183"/>
+      <c r="B161" s="175"/>
       <c r="C161" s="60" t="s">
         <v>392</v>
       </c>
@@ -15042,8 +15305,8 @@
       <c r="S161" s="26"/>
     </row>
     <row r="162" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A162" s="192"/>
-      <c r="B162" s="174"/>
+      <c r="A162" s="183"/>
+      <c r="B162" s="175"/>
       <c r="C162" s="60" t="s">
         <v>250</v>
       </c>
@@ -15083,8 +15346,8 @@
       <c r="S162" s="26"/>
     </row>
     <row r="163" spans="1:19" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A163" s="192"/>
-      <c r="B163" s="174"/>
+      <c r="A163" s="183"/>
+      <c r="B163" s="175"/>
       <c r="C163" s="61" t="s">
         <v>401</v>
       </c>
@@ -15126,8 +15389,8 @@
       <c r="S163" s="26"/>
     </row>
     <row r="164" spans="1:19" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A164" s="192"/>
-      <c r="B164" s="174"/>
+      <c r="A164" s="183"/>
+      <c r="B164" s="175"/>
       <c r="C164" s="60" t="s">
         <v>372</v>
       </c>
@@ -15167,8 +15430,8 @@
       <c r="S164" s="26"/>
     </row>
     <row r="165" spans="1:19" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A165" s="192"/>
-      <c r="B165" s="179"/>
+      <c r="A165" s="183"/>
+      <c r="B165" s="176"/>
       <c r="C165" s="60" t="s">
         <v>402</v>
       </c>
@@ -15208,7 +15471,7 @@
       <c r="S165" s="31"/>
     </row>
     <row r="166" spans="1:19" s="33" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A166" s="193" t="s">
+      <c r="A166" s="184" t="s">
         <v>535</v>
       </c>
       <c r="B166" s="72" t="s">
@@ -15251,8 +15514,8 @@
       <c r="S166" s="71"/>
     </row>
     <row r="167" spans="1:19" s="23" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A167" s="193"/>
-      <c r="B167" s="173" t="s">
+      <c r="A167" s="184"/>
+      <c r="B167" s="185" t="s">
         <v>193</v>
       </c>
       <c r="C167" s="60" t="s">
@@ -15290,8 +15553,8 @@
       <c r="S167" s="57"/>
     </row>
     <row r="168" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A168" s="193"/>
-      <c r="B168" s="174"/>
+      <c r="A168" s="184"/>
+      <c r="B168" s="175"/>
       <c r="C168" s="60" t="s">
         <v>195</v>
       </c>
@@ -15326,8 +15589,8 @@
       <c r="S168" s="26"/>
     </row>
     <row r="169" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="193"/>
-      <c r="B169" s="174"/>
+      <c r="A169" s="184"/>
+      <c r="B169" s="175"/>
       <c r="C169" s="60" t="s">
         <v>259</v>
       </c>
@@ -15365,8 +15628,8 @@
       <c r="S169" s="26"/>
     </row>
     <row r="170" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A170" s="193"/>
-      <c r="B170" s="174"/>
+      <c r="A170" s="184"/>
+      <c r="B170" s="175"/>
       <c r="C170" s="60" t="s">
         <v>417</v>
       </c>
@@ -15403,8 +15666,8 @@
       <c r="S170" s="26"/>
     </row>
     <row r="171" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A171" s="193"/>
-      <c r="B171" s="194"/>
+      <c r="A171" s="184"/>
+      <c r="B171" s="186"/>
       <c r="C171" s="60" t="s">
         <v>418</v>
       </c>
@@ -15442,10 +15705,10 @@
       <c r="S171" s="26"/>
     </row>
     <row r="172" spans="1:19" s="33" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A172" s="186" t="s">
+      <c r="A172" s="173" t="s">
         <v>113</v>
       </c>
-      <c r="B172" s="190" t="s">
+      <c r="B172" s="179" t="s">
         <v>51</v>
       </c>
       <c r="C172" s="62" t="s">
@@ -15485,8 +15748,8 @@
       <c r="S172" s="36"/>
     </row>
     <row r="173" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A173" s="186"/>
-      <c r="B173" s="167"/>
+      <c r="A173" s="173"/>
+      <c r="B173" s="180"/>
       <c r="C173" s="60" t="s">
         <v>184</v>
       </c>
@@ -15524,8 +15787,8 @@
       <c r="S173" s="26"/>
     </row>
     <row r="174" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A174" s="186"/>
-      <c r="B174" s="167"/>
+      <c r="A174" s="173"/>
+      <c r="B174" s="180"/>
       <c r="C174" s="60" t="s">
         <v>183</v>
       </c>
@@ -15563,8 +15826,8 @@
       <c r="S174" s="26"/>
     </row>
     <row r="175" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A175" s="186"/>
-      <c r="B175" s="167"/>
+      <c r="A175" s="173"/>
+      <c r="B175" s="180"/>
       <c r="C175" s="61" t="s">
         <v>185</v>
       </c>
@@ -15602,8 +15865,8 @@
       <c r="S175" s="31"/>
     </row>
     <row r="176" spans="1:19" s="23" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A176" s="186"/>
-      <c r="B176" s="184" t="s">
+      <c r="A176" s="173"/>
+      <c r="B176" s="171" t="s">
         <v>193</v>
       </c>
       <c r="C176" s="63" t="s">
@@ -15637,8 +15900,8 @@
       <c r="S176" s="57"/>
     </row>
     <row r="177" spans="1:19" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A177" s="186"/>
-      <c r="B177" s="185"/>
+      <c r="A177" s="173"/>
+      <c r="B177" s="172"/>
       <c r="C177" s="64"/>
       <c r="E177" s="49"/>
       <c r="F177" s="49"/>
@@ -16367,6 +16630,18 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="C3:S3"/>
+    <mergeCell ref="B51:B55"/>
+    <mergeCell ref="A51:A69"/>
+    <mergeCell ref="A133:A157"/>
+    <mergeCell ref="B138:B157"/>
+    <mergeCell ref="A116:A132"/>
+    <mergeCell ref="B116:B125"/>
+    <mergeCell ref="B81:B115"/>
+    <mergeCell ref="B56:B69"/>
+    <mergeCell ref="B70:B80"/>
+    <mergeCell ref="A70:A115"/>
+    <mergeCell ref="B133:B137"/>
     <mergeCell ref="B176:B177"/>
     <mergeCell ref="A172:A177"/>
     <mergeCell ref="B158:B165"/>
@@ -16382,18 +16657,6 @@
     <mergeCell ref="B126:B132"/>
     <mergeCell ref="A37:A50"/>
     <mergeCell ref="B41:B50"/>
-    <mergeCell ref="C3:S3"/>
-    <mergeCell ref="B51:B55"/>
-    <mergeCell ref="A51:A69"/>
-    <mergeCell ref="A133:A157"/>
-    <mergeCell ref="B138:B157"/>
-    <mergeCell ref="A116:A132"/>
-    <mergeCell ref="B116:B125"/>
-    <mergeCell ref="B81:B115"/>
-    <mergeCell ref="B56:B69"/>
-    <mergeCell ref="B70:B80"/>
-    <mergeCell ref="A70:A115"/>
-    <mergeCell ref="B133:B137"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -16589,8 +16852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C657BEEB-4F2E-48F9-B8CF-BB37A76584AA}">
   <dimension ref="A1:A43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:XFD33"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Dateien für FOG Mod upgedatet
</commit_message>
<xml_diff>
--- a/ressources/DayZ Mods.xlsx
+++ b/ressources/DayZ Mods.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\projects\Immersive-DayZ-Experience\ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C90447-4F4A-48A8-A10B-4C06CB926B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{692D90FF-6DD1-460E-8E75-39B5F8C26C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="260" xr2:uid="{FAEB3C3F-74B0-4C80-8C8B-4522341FA132}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="260" xr2:uid="{FAEB3C3F-74B0-4C80-8C8B-4522341FA132}"/>
   </bookViews>
   <sheets>
     <sheet name="Mods" sheetId="1" r:id="rId1"/>
@@ -4012,68 +4012,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -4090,6 +4048,12 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -4100,6 +4064,9 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4114,14 +4081,47 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -4617,9 +4617,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 – 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4657,7 +4657,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 – 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -4763,7 +4763,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 – 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4905,7 +4905,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4915,9 +4915,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BE2B301-FC9E-4F7D-A454-62A8C1115EDF}">
   <dimension ref="A1:S115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O30" sqref="O30"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4932,7 +4932,7 @@
     <col min="8" max="8" width="12.85546875" style="88" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" customWidth="1"/>
     <col min="10" max="14" width="11.42578125" customWidth="1"/>
-    <col min="15" max="15" width="42.42578125" style="206" customWidth="1"/>
+    <col min="15" max="15" width="42.42578125" style="172" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4972,12 +4972,12 @@
       <c r="N1" s="102" t="s">
         <v>56</v>
       </c>
-      <c r="O1" s="204" t="s">
+      <c r="O1" s="170" t="s">
         <v>680</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="170" t="s">
+      <c r="A2" s="173" t="s">
         <v>669</v>
       </c>
       <c r="C2" s="159">
@@ -5012,12 +5012,12 @@
       <c r="N2" s="165" t="s">
         <v>33</v>
       </c>
-      <c r="O2" s="205" t="s">
+      <c r="O2" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="170"/>
+      <c r="A3" s="173"/>
       <c r="C3" s="160">
         <v>1564026768</v>
       </c>
@@ -5050,12 +5050,12 @@
       <c r="N3" s="167" t="s">
         <v>33</v>
       </c>
-      <c r="O3" s="205" t="s">
+      <c r="O3" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="170" t="s">
+      <c r="A4" s="173" t="s">
         <v>670</v>
       </c>
       <c r="C4" s="161">
@@ -5090,12 +5090,12 @@
       <c r="N4" s="167" t="s">
         <v>33</v>
       </c>
-      <c r="O4" s="205" t="s">
+      <c r="O4" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="170"/>
+      <c r="A5" s="173"/>
       <c r="C5" s="161">
         <v>2614334381</v>
       </c>
@@ -5128,12 +5128,12 @@
       <c r="N5" s="167" t="s">
         <v>33</v>
       </c>
-      <c r="O5" s="205" t="s">
+      <c r="O5" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="170"/>
+      <c r="A6" s="173"/>
       <c r="C6" s="161">
         <v>2507204412</v>
       </c>
@@ -5166,12 +5166,12 @@
       <c r="N6" s="167" t="s">
         <v>33</v>
       </c>
-      <c r="O6" s="205" t="s">
+      <c r="O6" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="170" t="s">
+      <c r="A7" s="173" t="s">
         <v>53</v>
       </c>
       <c r="C7" s="160">
@@ -5206,12 +5206,12 @@
       <c r="N7" s="167" t="s">
         <v>33</v>
       </c>
-      <c r="O7" s="205" t="s">
+      <c r="O7" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="170"/>
+      <c r="A8" s="173"/>
       <c r="C8" s="160">
         <v>2572331007</v>
       </c>
@@ -5246,12 +5246,12 @@
       <c r="N8" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="O8" s="205" t="s">
+      <c r="O8" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="170"/>
+      <c r="A9" s="173"/>
       <c r="C9" s="161">
         <v>2116157322</v>
       </c>
@@ -5284,14 +5284,14 @@
       <c r="N9" s="167" t="s">
         <v>33</v>
       </c>
-      <c r="O9" s="205" t="s">
+      <c r="O9" s="171" t="s">
         <v>681</v>
       </c>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
     </row>
     <row r="10" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="170"/>
+      <c r="A10" s="173"/>
       <c r="C10" s="161">
         <v>2793893086</v>
       </c>
@@ -5324,14 +5324,14 @@
       <c r="N10" s="167" t="s">
         <v>33</v>
       </c>
-      <c r="O10" s="205" t="s">
+      <c r="O10" s="171" t="s">
         <v>681</v>
       </c>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
     </row>
     <row r="11" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="170" t="s">
+      <c r="A11" s="173" t="s">
         <v>671</v>
       </c>
       <c r="C11" s="161">
@@ -5368,12 +5368,12 @@
       <c r="N11" s="167" t="s">
         <v>33</v>
       </c>
-      <c r="O11" s="205" t="s">
+      <c r="O11" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="170"/>
+      <c r="A12" s="173"/>
       <c r="C12" s="161">
         <v>3031784065</v>
       </c>
@@ -5390,17 +5390,17 @@
       <c r="H12" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="I12" s="167" t="s">
-        <v>33</v>
+      <c r="I12" s="38" t="s">
+        <v>8</v>
       </c>
       <c r="J12" s="167" t="s">
         <v>33</v>
       </c>
-      <c r="K12" s="167" t="s">
-        <v>33</v>
-      </c>
-      <c r="L12" s="167" t="s">
-        <v>33</v>
+      <c r="K12" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="L12" s="38" t="s">
+        <v>8</v>
       </c>
       <c r="M12" s="167" t="s">
         <v>33</v>
@@ -5408,12 +5408,12 @@
       <c r="N12" s="167" t="s">
         <v>33</v>
       </c>
-      <c r="O12" s="205" t="s">
+      <c r="O12" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="170"/>
+      <c r="A13" s="173"/>
       <c r="C13" s="161">
         <v>2977703357</v>
       </c>
@@ -5446,12 +5446,12 @@
       <c r="N13" s="167" t="s">
         <v>33</v>
       </c>
-      <c r="O13" s="205" t="s">
+      <c r="O13" s="171" t="s">
         <v>682</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="170"/>
+      <c r="A14" s="173"/>
       <c r="C14" s="161">
         <v>2980235854</v>
       </c>
@@ -5484,12 +5484,12 @@
       <c r="N14" s="167" t="s">
         <v>33</v>
       </c>
-      <c r="O14" s="205" t="s">
+      <c r="O14" s="171" t="s">
         <v>683</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="170"/>
+      <c r="A15" s="173"/>
       <c r="C15" s="161">
         <v>2111523728</v>
       </c>
@@ -5524,12 +5524,12 @@
       <c r="N15" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="O15" s="205" t="s">
+      <c r="O15" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="170" t="s">
+      <c r="A16" s="173" t="s">
         <v>675</v>
       </c>
       <c r="C16" s="161">
@@ -5566,12 +5566,12 @@
       <c r="N16" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="O16" s="205" t="s">
+      <c r="O16" s="171" t="s">
         <v>683</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="170"/>
+      <c r="A17" s="173"/>
       <c r="C17" s="161">
         <v>2822531337</v>
       </c>
@@ -5604,12 +5604,12 @@
       <c r="N17" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="O17" s="205" t="s">
+      <c r="O17" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="170" t="s">
+      <c r="A18" s="173" t="s">
         <v>672</v>
       </c>
       <c r="C18" s="160">
@@ -5646,14 +5646,14 @@
       <c r="N18" s="167" t="s">
         <v>33</v>
       </c>
-      <c r="O18" s="205" t="s">
+      <c r="O18" s="171" t="s">
         <v>681</v>
       </c>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
     </row>
     <row r="19" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="170"/>
+      <c r="A19" s="173"/>
       <c r="C19" s="160">
         <v>2166325582</v>
       </c>
@@ -5686,12 +5686,12 @@
       <c r="N19" s="167" t="s">
         <v>33</v>
       </c>
-      <c r="O19" s="205" t="s">
+      <c r="O19" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="170"/>
+      <c r="A20" s="173"/>
       <c r="C20" s="160">
         <v>2208230845</v>
       </c>
@@ -5726,14 +5726,14 @@
       <c r="N20" s="167" t="s">
         <v>33</v>
       </c>
-      <c r="O20" s="205" t="s">
+      <c r="O20" s="171" t="s">
         <v>684</v>
       </c>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
     </row>
     <row r="21" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="170" t="s">
+      <c r="A21" s="173" t="s">
         <v>673</v>
       </c>
       <c r="B21" s="169"/>
@@ -5767,12 +5767,12 @@
         <v>8</v>
       </c>
       <c r="N21" s="5"/>
-      <c r="O21" s="205" t="s">
+      <c r="O21" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="22" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="170"/>
+      <c r="A22" s="173"/>
       <c r="B22" s="169"/>
       <c r="C22" s="160">
         <v>2789302074</v>
@@ -5804,12 +5804,12 @@
         <v>8</v>
       </c>
       <c r="N22" s="5"/>
-      <c r="O22" s="205" t="s">
+      <c r="O22" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="170"/>
+      <c r="A23" s="173"/>
       <c r="B23" s="169"/>
       <c r="C23" s="161">
         <v>1991570984</v>
@@ -5837,12 +5837,12 @@
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
-      <c r="O23" s="205" t="s">
+      <c r="O23" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="24" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="170"/>
+      <c r="A24" s="173"/>
       <c r="B24" s="169"/>
       <c r="C24" s="161">
         <v>3171576913</v>
@@ -5876,12 +5876,12 @@
       <c r="N24" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="O24" s="205" t="s">
+      <c r="O24" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="25" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="170"/>
+      <c r="A25" s="173"/>
       <c r="B25" s="169"/>
       <c r="C25" s="160" t="s">
         <v>597</v>
@@ -5913,12 +5913,12 @@
         <v>8</v>
       </c>
       <c r="N25" s="5"/>
-      <c r="O25" s="205" t="s">
+      <c r="O25" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="26" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="170"/>
+      <c r="A26" s="173"/>
       <c r="B26" s="169"/>
       <c r="C26" s="160">
         <v>2931560672</v>
@@ -5950,12 +5950,12 @@
         <v>8</v>
       </c>
       <c r="N26" s="5"/>
-      <c r="O26" s="205" t="s">
+      <c r="O26" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="27" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="170"/>
+      <c r="A27" s="173"/>
       <c r="B27" s="169"/>
       <c r="C27" s="161">
         <v>3108865421</v>
@@ -5987,12 +5987,12 @@
       </c>
       <c r="M27" s="38"/>
       <c r="N27" s="38"/>
-      <c r="O27" s="205" t="s">
+      <c r="O27" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="28" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="170"/>
+      <c r="A28" s="173"/>
       <c r="B28" s="169"/>
       <c r="C28" s="160">
         <v>1630943713</v>
@@ -6026,12 +6026,12 @@
         <v>8</v>
       </c>
       <c r="N28" s="5"/>
-      <c r="O28" s="205" t="s">
+      <c r="O28" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="29" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="170"/>
+      <c r="A29" s="173"/>
       <c r="B29" s="169"/>
       <c r="C29" s="161">
         <v>1797720064</v>
@@ -6065,12 +6065,12 @@
         <v>8</v>
       </c>
       <c r="N29" s="5"/>
-      <c r="O29" s="205" t="s">
+      <c r="O29" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="30" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="170"/>
+      <c r="A30" s="173"/>
       <c r="B30" s="169"/>
       <c r="C30" s="160">
         <v>2155726353</v>
@@ -6102,12 +6102,12 @@
         <v>8</v>
       </c>
       <c r="N30" s="5"/>
-      <c r="O30" s="205" t="s">
+      <c r="O30" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="31" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="170"/>
+      <c r="A31" s="173"/>
       <c r="B31" s="169"/>
       <c r="C31" s="161">
         <v>2723807644</v>
@@ -6139,12 +6139,12 @@
         <v>8</v>
       </c>
       <c r="N31" s="5"/>
-      <c r="O31" s="205" t="s">
+      <c r="O31" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="32" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="170"/>
+      <c r="A32" s="173"/>
       <c r="B32" s="169"/>
       <c r="C32" s="161">
         <v>2780914191</v>
@@ -6176,12 +6176,12 @@
         <v>8</v>
       </c>
       <c r="N32" s="5"/>
-      <c r="O32" s="205" t="s">
+      <c r="O32" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="170"/>
+      <c r="A33" s="173"/>
       <c r="B33" s="169"/>
       <c r="C33" s="161">
         <v>2741271183</v>
@@ -6213,12 +6213,12 @@
         <v>8</v>
       </c>
       <c r="N33" s="5"/>
-      <c r="O33" s="205" t="s">
+      <c r="O33" s="171" t="s">
         <v>685</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="170"/>
+      <c r="A34" s="173"/>
       <c r="B34" s="169"/>
       <c r="C34" s="161">
         <v>2579252958</v>
@@ -6252,12 +6252,12 @@
       <c r="N34" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="O34" s="205" t="s">
+      <c r="O34" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="170"/>
+      <c r="A35" s="173"/>
       <c r="B35" s="169"/>
       <c r="C35" s="161">
         <v>3034460305</v>
@@ -6291,12 +6291,12 @@
       <c r="N35" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="O35" s="205" t="s">
+      <c r="O35" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="170"/>
+      <c r="A36" s="173"/>
       <c r="B36" s="169"/>
       <c r="C36" s="161">
         <v>2851058261</v>
@@ -6330,12 +6330,12 @@
       <c r="N36" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="O36" s="205" t="s">
+      <c r="O36" s="171" t="s">
         <v>686</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="170"/>
+      <c r="A37" s="173"/>
       <c r="B37" s="169"/>
       <c r="C37" s="161">
         <v>2926289548</v>
@@ -6367,12 +6367,12 @@
         <v>33</v>
       </c>
       <c r="N37" s="38"/>
-      <c r="O37" s="205" t="s">
+      <c r="O37" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="170"/>
+      <c r="A38" s="173"/>
       <c r="B38" s="169"/>
       <c r="C38" s="161">
         <v>3170285574</v>
@@ -6406,12 +6406,12 @@
         <v>33</v>
       </c>
       <c r="N38" s="38"/>
-      <c r="O38" s="205" t="s">
+      <c r="O38" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="39" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="170"/>
+      <c r="A39" s="173"/>
       <c r="B39" s="169"/>
       <c r="C39" s="161">
         <v>3279662973</v>
@@ -6445,12 +6445,12 @@
         <v>8</v>
       </c>
       <c r="N39" s="38"/>
-      <c r="O39" s="205" t="s">
+      <c r="O39" s="171" t="s">
         <v>683</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="170"/>
+      <c r="A40" s="173"/>
       <c r="B40" s="169"/>
       <c r="C40" s="160">
         <v>2937138060</v>
@@ -6484,12 +6484,12 @@
         <v>8</v>
       </c>
       <c r="N40" s="5"/>
-      <c r="O40" s="205" t="s">
+      <c r="O40" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="41" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="170" t="s">
+      <c r="A41" s="173" t="s">
         <v>676</v>
       </c>
       <c r="C41" s="161">
@@ -6526,12 +6526,12 @@
       <c r="N41" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="O41" s="205" t="s">
+      <c r="O41" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="170"/>
+      <c r="A42" s="173"/>
       <c r="C42" s="161">
         <v>3114410963</v>
       </c>
@@ -6562,12 +6562,12 @@
         <v>33</v>
       </c>
       <c r="N42" s="5"/>
-      <c r="O42" s="205" t="s">
+      <c r="O42" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="43" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="170"/>
+      <c r="A43" s="173"/>
       <c r="C43" s="160">
         <v>1866298408</v>
       </c>
@@ -6600,12 +6600,12 @@
       <c r="N43" s="167" t="s">
         <v>33</v>
       </c>
-      <c r="O43" s="205" t="s">
+      <c r="O43" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="170"/>
+      <c r="A44" s="173"/>
       <c r="C44" s="161">
         <v>2874589934</v>
       </c>
@@ -6638,12 +6638,12 @@
       <c r="N44" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="O44" s="205" t="s">
+      <c r="O44" s="171" t="s">
         <v>689</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="170" t="s">
+      <c r="A45" s="173" t="s">
         <v>677</v>
       </c>
       <c r="C45" s="161">
@@ -6666,12 +6666,12 @@
       <c r="L45" s="38"/>
       <c r="M45" s="38"/>
       <c r="N45" s="38"/>
-      <c r="O45" s="205" t="s">
+      <c r="O45" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="170"/>
+      <c r="A46" s="173"/>
       <c r="C46" s="161">
         <v>1710977250</v>
       </c>
@@ -6694,12 +6694,12 @@
       <c r="L46" s="38"/>
       <c r="M46" s="38"/>
       <c r="N46" s="38"/>
-      <c r="O46" s="205" t="s">
+      <c r="O46" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="47" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="170"/>
+      <c r="A47" s="173"/>
       <c r="C47" s="161">
         <v>2895049000</v>
       </c>
@@ -6722,12 +6722,12 @@
       <c r="L47" s="38"/>
       <c r="M47" s="38"/>
       <c r="N47" s="38"/>
-      <c r="O47" s="205" t="s">
+      <c r="O47" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="48" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="170" t="s">
+      <c r="A48" s="173" t="s">
         <v>678</v>
       </c>
       <c r="C48" s="161">
@@ -6762,12 +6762,12 @@
       <c r="N48" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="O48" s="205" t="s">
+      <c r="O48" s="171" t="s">
         <v>687</v>
       </c>
     </row>
     <row r="49" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="170"/>
+      <c r="A49" s="173"/>
       <c r="C49" s="161">
         <v>2472500243</v>
       </c>
@@ -6800,12 +6800,12 @@
       <c r="N49" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="O49" s="205" t="s">
+      <c r="O49" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="50" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="170"/>
+      <c r="A50" s="173"/>
       <c r="C50" s="161">
         <v>1832448183</v>
       </c>
@@ -6832,12 +6832,12 @@
       <c r="L50" s="38"/>
       <c r="M50" s="38"/>
       <c r="N50" s="38"/>
-      <c r="O50" s="205" t="s">
+      <c r="O50" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="51" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="170"/>
+      <c r="A51" s="173"/>
       <c r="C51" s="161">
         <v>1895432270</v>
       </c>
@@ -6868,12 +6868,12 @@
       <c r="N51" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="O51" s="205" t="s">
+      <c r="O51" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="52" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="170"/>
+      <c r="A52" s="173"/>
       <c r="C52" s="161">
         <v>2912241382</v>
       </c>
@@ -6904,12 +6904,12 @@
       <c r="N52" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="O52" s="205" t="s">
+      <c r="O52" s="171" t="s">
         <v>686</v>
       </c>
     </row>
     <row r="53" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="170" t="s">
+      <c r="A53" s="173" t="s">
         <v>668</v>
       </c>
       <c r="C53" s="161">
@@ -6944,12 +6944,12 @@
       <c r="N53" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="O53" s="205" t="s">
+      <c r="O53" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="54" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="170"/>
+      <c r="A54" s="173"/>
       <c r="C54" s="161">
         <v>3043440124</v>
       </c>
@@ -6982,12 +6982,12 @@
       <c r="N54" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="O54" s="205" t="s">
+      <c r="O54" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="55" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="170"/>
+      <c r="A55" s="173"/>
       <c r="C55" s="160">
         <v>2550932214</v>
       </c>
@@ -7020,12 +7020,12 @@
       <c r="N55" s="167" t="s">
         <v>33</v>
       </c>
-      <c r="O55" s="205" t="s">
+      <c r="O55" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="56" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="170"/>
+      <c r="A56" s="173"/>
       <c r="C56" s="161">
         <v>3321340470</v>
       </c>
@@ -7060,12 +7060,12 @@
       <c r="N56" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="O56" s="205" t="s">
+      <c r="O56" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="57" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="170" t="s">
+      <c r="A57" s="173" t="s">
         <v>674</v>
       </c>
       <c r="C57" s="160">
@@ -7100,12 +7100,12 @@
       <c r="N57" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="O57" s="205" t="s">
+      <c r="O57" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="58" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="170"/>
+      <c r="A58" s="173"/>
       <c r="C58" s="160">
         <v>2793619401</v>
       </c>
@@ -7140,12 +7140,12 @@
       <c r="N58" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="O58" s="205" t="s">
+      <c r="O58" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="59" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="170"/>
+      <c r="A59" s="173"/>
       <c r="C59" s="161">
         <v>2924719512</v>
       </c>
@@ -7178,12 +7178,12 @@
       <c r="N59" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="O59" s="205" t="s">
+      <c r="O59" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="60" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="170"/>
+      <c r="A60" s="173"/>
       <c r="C60" s="161">
         <v>2810260908</v>
       </c>
@@ -7216,12 +7216,12 @@
       <c r="N60" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="O60" s="205" t="s">
+      <c r="O60" s="171" t="s">
         <v>688</v>
       </c>
     </row>
     <row r="61" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="170"/>
+      <c r="A61" s="173"/>
       <c r="C61" s="161">
         <v>2877877368</v>
       </c>
@@ -7254,12 +7254,12 @@
       <c r="N61" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="O61" s="205" t="s">
+      <c r="O61" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="62" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="170"/>
+      <c r="A62" s="173"/>
       <c r="C62" s="161">
         <v>2857994912</v>
       </c>
@@ -7292,12 +7292,12 @@
       <c r="N62" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="O62" s="205" t="s">
+      <c r="O62" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="63" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="170"/>
+      <c r="A63" s="173"/>
       <c r="C63" s="161">
         <v>2817606510</v>
       </c>
@@ -7330,12 +7330,12 @@
       <c r="N63" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="O63" s="205" t="s">
+      <c r="O63" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="64" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="170"/>
+      <c r="A64" s="173"/>
       <c r="C64" s="161">
         <v>2884638645</v>
       </c>
@@ -7364,12 +7364,12 @@
       </c>
       <c r="M64" s="91"/>
       <c r="N64" s="5"/>
-      <c r="O64" s="205" t="s">
+      <c r="O64" s="171" t="s">
         <v>688</v>
       </c>
     </row>
     <row r="65" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="170"/>
+      <c r="A65" s="173"/>
       <c r="C65" s="160">
         <v>2521460498</v>
       </c>
@@ -7402,12 +7402,12 @@
       <c r="N65" s="167" t="s">
         <v>33</v>
       </c>
-      <c r="O65" s="205" t="s">
+      <c r="O65" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="66" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="170"/>
+      <c r="A66" s="173"/>
       <c r="C66" s="160">
         <v>2903112334</v>
       </c>
@@ -7442,12 +7442,12 @@
       <c r="N66" s="167" t="s">
         <v>33</v>
       </c>
-      <c r="O66" s="205" t="s">
+      <c r="O66" s="171" t="s">
         <v>683</v>
       </c>
     </row>
     <row r="67" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="170"/>
+      <c r="A67" s="173"/>
       <c r="C67" s="160">
         <v>2833363308</v>
       </c>
@@ -7480,12 +7480,12 @@
       <c r="N67" s="167" t="s">
         <v>33</v>
       </c>
-      <c r="O67" s="205" t="s">
+      <c r="O67" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="68" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="170"/>
+      <c r="A68" s="173"/>
       <c r="C68" s="161">
         <v>2521678241</v>
       </c>
@@ -7518,14 +7518,14 @@
       <c r="N68" s="167" t="s">
         <v>33</v>
       </c>
-      <c r="O68" s="205" t="s">
+      <c r="O68" s="171" t="s">
         <v>681</v>
       </c>
       <c r="R68" s="1"/>
       <c r="S68" s="1"/>
     </row>
     <row r="69" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="170"/>
+      <c r="A69" s="173"/>
       <c r="C69" s="161">
         <v>2895460678</v>
       </c>
@@ -7558,12 +7558,12 @@
       <c r="N69" s="167" t="s">
         <v>33</v>
       </c>
-      <c r="O69" s="205" t="s">
+      <c r="O69" s="171" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="70" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="170"/>
+      <c r="A70" s="173"/>
       <c r="C70" s="161">
         <v>2985895498</v>
       </c>
@@ -7596,12 +7596,12 @@
       <c r="N70" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="O70" s="205" t="s">
+      <c r="O70" s="171" t="s">
         <v>683</v>
       </c>
     </row>
     <row r="71" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="170"/>
+      <c r="A71" s="173"/>
       <c r="C71" s="161">
         <v>2224593910</v>
       </c>
@@ -7634,7 +7634,7 @@
       <c r="N71" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="O71" s="205" t="s">
+      <c r="O71" s="171" t="s">
         <v>681</v>
       </c>
     </row>
@@ -8157,18 +8157,18 @@
     <sortCondition ref="B2:B98"/>
   </sortState>
   <mergeCells count="12">
+    <mergeCell ref="A48:A52"/>
+    <mergeCell ref="A57:A71"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="A21:A40"/>
+    <mergeCell ref="A53:A56"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A7:A10"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="A41:A44"/>
     <mergeCell ref="A11:A15"/>
-    <mergeCell ref="A48:A52"/>
-    <mergeCell ref="A57:A71"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="A21:A40"/>
-    <mergeCell ref="A53:A56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8212,25 +8212,25 @@
       <c r="S2"/>
     </row>
     <row r="3" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="190" t="s">
+      <c r="C3" s="174" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="190"/>
-      <c r="E3" s="190"/>
-      <c r="F3" s="190"/>
-      <c r="G3" s="190"/>
-      <c r="H3" s="190"/>
-      <c r="I3" s="190"/>
-      <c r="J3" s="190"/>
-      <c r="K3" s="190"/>
-      <c r="L3" s="190"/>
-      <c r="M3" s="190"/>
-      <c r="N3" s="190"/>
-      <c r="O3" s="190"/>
-      <c r="P3" s="190"/>
-      <c r="Q3" s="190"/>
-      <c r="R3" s="190"/>
-      <c r="S3" s="190"/>
+      <c r="D3" s="174"/>
+      <c r="E3" s="174"/>
+      <c r="F3" s="174"/>
+      <c r="G3" s="174"/>
+      <c r="H3" s="174"/>
+      <c r="I3" s="174"/>
+      <c r="J3" s="174"/>
+      <c r="K3" s="174"/>
+      <c r="L3" s="174"/>
+      <c r="M3" s="174"/>
+      <c r="N3" s="174"/>
+      <c r="O3" s="174"/>
+      <c r="P3" s="174"/>
+      <c r="Q3" s="174"/>
+      <c r="R3" s="174"/>
+      <c r="S3" s="174"/>
     </row>
     <row r="4" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
@@ -8245,19 +8245,19 @@
       <c r="F4" s="3" t="s">
         <v>645</v>
       </c>
-      <c r="G4" s="178"/>
-      <c r="H4" s="178"/>
-      <c r="I4" s="178"/>
-      <c r="J4" s="178"/>
-      <c r="K4" s="178"/>
-      <c r="L4" s="178"/>
-      <c r="M4" s="178"/>
-      <c r="N4" s="178"/>
-      <c r="O4" s="178"/>
-      <c r="P4" s="178"/>
-      <c r="Q4" s="178"/>
-      <c r="R4" s="178"/>
-      <c r="S4" s="178"/>
+      <c r="G4" s="198"/>
+      <c r="H4" s="198"/>
+      <c r="I4" s="198"/>
+      <c r="J4" s="198"/>
+      <c r="K4" s="198"/>
+      <c r="L4" s="198"/>
+      <c r="M4" s="198"/>
+      <c r="N4" s="198"/>
+      <c r="O4" s="198"/>
+      <c r="P4" s="198"/>
+      <c r="Q4" s="198"/>
+      <c r="R4" s="198"/>
+      <c r="S4" s="198"/>
     </row>
     <row r="5" spans="1:22" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="3"/>
@@ -8308,10 +8308,10 @@
       </c>
     </row>
     <row r="6" spans="1:22" s="23" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="177" t="s">
+      <c r="A6" s="197" t="s">
         <v>88</v>
       </c>
-      <c r="B6" s="179" t="s">
+      <c r="B6" s="199" t="s">
         <v>51</v>
       </c>
       <c r="C6" s="18" t="s">
@@ -8373,8 +8373,8 @@
       </c>
     </row>
     <row r="7" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="177"/>
-      <c r="B7" s="180"/>
+      <c r="A7" s="197"/>
+      <c r="B7" s="176"/>
       <c r="C7" s="60" t="s">
         <v>42</v>
       </c>
@@ -8425,8 +8425,8 @@
       </c>
     </row>
     <row r="8" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="177"/>
-      <c r="B8" s="180"/>
+      <c r="A8" s="197"/>
+      <c r="B8" s="176"/>
       <c r="C8" s="60" t="s">
         <v>49</v>
       </c>
@@ -8475,8 +8475,8 @@
       </c>
     </row>
     <row r="9" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="177"/>
-      <c r="B9" s="180"/>
+      <c r="A9" s="197"/>
+      <c r="B9" s="176"/>
       <c r="C9" s="60" t="s">
         <v>283</v>
       </c>
@@ -8527,8 +8527,8 @@
       </c>
     </row>
     <row r="10" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="177"/>
-      <c r="B10" s="180"/>
+      <c r="A10" s="197"/>
+      <c r="B10" s="176"/>
       <c r="C10" s="60" t="s">
         <v>43</v>
       </c>
@@ -8577,8 +8577,8 @@
       </c>
     </row>
     <row r="11" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="177"/>
-      <c r="B11" s="180"/>
+      <c r="A11" s="197"/>
+      <c r="B11" s="176"/>
       <c r="C11" s="60" t="s">
         <v>59</v>
       </c>
@@ -8629,8 +8629,8 @@
       </c>
     </row>
     <row r="12" spans="1:22" s="23" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="177"/>
-      <c r="B12" s="180"/>
+      <c r="A12" s="197"/>
+      <c r="B12" s="176"/>
       <c r="C12" s="60" t="s">
         <v>44</v>
       </c>
@@ -8676,8 +8676,8 @@
       <c r="S12" s="26"/>
     </row>
     <row r="13" spans="1:22" s="23" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="177"/>
-      <c r="B13" s="180"/>
+      <c r="A13" s="197"/>
+      <c r="B13" s="176"/>
       <c r="C13" s="60" t="s">
         <v>637</v>
       </c>
@@ -8711,8 +8711,8 @@
       <c r="S13" s="26"/>
     </row>
     <row r="14" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="177"/>
-      <c r="B14" s="180"/>
+      <c r="A14" s="197"/>
+      <c r="B14" s="176"/>
       <c r="C14" s="60" t="s">
         <v>45</v>
       </c>
@@ -8758,8 +8758,8 @@
       <c r="S14" s="26"/>
     </row>
     <row r="15" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="177"/>
-      <c r="B15" s="180"/>
+      <c r="A15" s="197"/>
+      <c r="B15" s="176"/>
       <c r="C15" s="60" t="s">
         <v>74</v>
       </c>
@@ -8805,8 +8805,8 @@
       <c r="S15" s="26"/>
     </row>
     <row r="16" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="177"/>
-      <c r="B16" s="180"/>
+      <c r="A16" s="197"/>
+      <c r="B16" s="176"/>
       <c r="C16" s="60" t="s">
         <v>46</v>
       </c>
@@ -8850,8 +8850,8 @@
       <c r="S16" s="26"/>
     </row>
     <row r="17" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="177"/>
-      <c r="B17" s="180"/>
+      <c r="A17" s="197"/>
+      <c r="B17" s="176"/>
       <c r="C17" s="60" t="s">
         <v>47</v>
       </c>
@@ -8895,8 +8895,8 @@
       <c r="S17" s="26"/>
     </row>
     <row r="18" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="177"/>
-      <c r="B18" s="180"/>
+      <c r="A18" s="197"/>
+      <c r="B18" s="176"/>
       <c r="C18" s="60" t="s">
         <v>48</v>
       </c>
@@ -8940,8 +8940,8 @@
       <c r="S18" s="26"/>
     </row>
     <row r="19" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="177"/>
-      <c r="B19" s="180"/>
+      <c r="A19" s="197"/>
+      <c r="B19" s="176"/>
       <c r="C19" s="60" t="s">
         <v>346</v>
       </c>
@@ -8987,8 +8987,8 @@
       <c r="S19" s="26"/>
     </row>
     <row r="20" spans="1:20" s="40" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="177"/>
-      <c r="B20" s="181"/>
+      <c r="A20" s="197"/>
+      <c r="B20" s="200"/>
       <c r="C20" s="61" t="s">
         <v>50</v>
       </c>
@@ -9030,8 +9030,8 @@
       <c r="S20" s="31"/>
     </row>
     <row r="21" spans="1:20" s="33" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="177"/>
-      <c r="B21" s="174" t="s">
+      <c r="A21" s="197"/>
+      <c r="B21" s="196" t="s">
         <v>246</v>
       </c>
       <c r="C21" s="117" t="s">
@@ -9082,8 +9082,8 @@
       </c>
     </row>
     <row r="22" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="177"/>
-      <c r="B22" s="175"/>
+      <c r="A22" s="197"/>
+      <c r="B22" s="183"/>
       <c r="C22" s="61" t="s">
         <v>233</v>
       </c>
@@ -9127,8 +9127,8 @@
       <c r="S22" s="26"/>
     </row>
     <row r="23" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="177"/>
-      <c r="B23" s="175"/>
+      <c r="A23" s="197"/>
+      <c r="B23" s="183"/>
       <c r="C23" s="60" t="s">
         <v>45</v>
       </c>
@@ -9172,8 +9172,8 @@
       <c r="S23" s="26"/>
     </row>
     <row r="24" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="177"/>
-      <c r="B24" s="175"/>
+      <c r="A24" s="197"/>
+      <c r="B24" s="183"/>
       <c r="C24" s="60" t="s">
         <v>120</v>
       </c>
@@ -9219,8 +9219,8 @@
       <c r="S24" s="26"/>
     </row>
     <row r="25" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="177"/>
-      <c r="B25" s="175"/>
+      <c r="A25" s="197"/>
+      <c r="B25" s="183"/>
       <c r="C25" s="60" t="s">
         <v>235</v>
       </c>
@@ -9268,8 +9268,8 @@
       <c r="S25" s="26"/>
     </row>
     <row r="26" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="177"/>
-      <c r="B26" s="175"/>
+      <c r="A26" s="197"/>
+      <c r="B26" s="183"/>
       <c r="C26" s="60" t="s">
         <v>350</v>
       </c>
@@ -9313,8 +9313,8 @@
       <c r="S26" s="26"/>
     </row>
     <row r="27" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="177"/>
-      <c r="B27" s="175"/>
+      <c r="A27" s="197"/>
+      <c r="B27" s="183"/>
       <c r="C27" s="60" t="s">
         <v>119</v>
       </c>
@@ -9358,8 +9358,8 @@
       <c r="S27" s="26"/>
     </row>
     <row r="28" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="177"/>
-      <c r="B28" s="175"/>
+      <c r="A28" s="197"/>
+      <c r="B28" s="183"/>
       <c r="C28" s="60" t="s">
         <v>465</v>
       </c>
@@ -9403,8 +9403,8 @@
       <c r="S28" s="26"/>
     </row>
     <row r="29" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="177"/>
-      <c r="B29" s="175"/>
+      <c r="A29" s="197"/>
+      <c r="B29" s="183"/>
       <c r="C29" s="60" t="s">
         <v>385</v>
       </c>
@@ -9450,8 +9450,8 @@
       <c r="S29" s="26"/>
     </row>
     <row r="30" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="177"/>
-      <c r="B30" s="175"/>
+      <c r="A30" s="197"/>
+      <c r="B30" s="183"/>
       <c r="C30" s="60" t="s">
         <v>238</v>
       </c>
@@ -9498,8 +9498,8 @@
       <c r="T30" s="23"/>
     </row>
     <row r="31" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="177"/>
-      <c r="B31" s="175"/>
+      <c r="A31" s="197"/>
+      <c r="B31" s="183"/>
       <c r="C31" s="60" t="s">
         <v>351</v>
       </c>
@@ -9545,8 +9545,8 @@
       <c r="S31" s="26"/>
     </row>
     <row r="32" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="177"/>
-      <c r="B32" s="175"/>
+      <c r="A32" s="197"/>
+      <c r="B32" s="183"/>
       <c r="C32" s="60" t="s">
         <v>216</v>
       </c>
@@ -9593,8 +9593,8 @@
       <c r="T32" s="23"/>
     </row>
     <row r="33" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="177"/>
-      <c r="B33" s="175"/>
+      <c r="A33" s="197"/>
+      <c r="B33" s="183"/>
       <c r="C33" s="60" t="s">
         <v>242</v>
       </c>
@@ -9640,8 +9640,8 @@
       <c r="S33" s="26"/>
     </row>
     <row r="34" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="177"/>
-      <c r="B34" s="175"/>
+      <c r="A34" s="197"/>
+      <c r="B34" s="183"/>
       <c r="C34" s="60" t="s">
         <v>375</v>
       </c>
@@ -9685,8 +9685,8 @@
       <c r="S34" s="26"/>
     </row>
     <row r="35" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="177"/>
-      <c r="B35" s="175"/>
+      <c r="A35" s="197"/>
+      <c r="B35" s="183"/>
       <c r="C35" s="60" t="s">
         <v>388</v>
       </c>
@@ -9730,8 +9730,8 @@
       <c r="S35" s="26"/>
     </row>
     <row r="36" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="177"/>
-      <c r="B36" s="176"/>
+      <c r="A36" s="197"/>
+      <c r="B36" s="188"/>
       <c r="C36" s="65" t="s">
         <v>234</v>
       </c>
@@ -9775,10 +9775,10 @@
       <c r="S36" s="26"/>
     </row>
     <row r="37" spans="1:20" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="187" t="s">
+      <c r="A37" s="204" t="s">
         <v>266</v>
       </c>
-      <c r="B37" s="182" t="s">
+      <c r="B37" s="175" t="s">
         <v>51</v>
       </c>
       <c r="C37" s="62" t="s">
@@ -9823,8 +9823,8 @@
       <c r="T37" s="33"/>
     </row>
     <row r="38" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="188"/>
-      <c r="B38" s="180"/>
+      <c r="A38" s="205"/>
+      <c r="B38" s="176"/>
       <c r="C38" s="60" t="s">
         <v>107</v>
       </c>
@@ -9866,8 +9866,8 @@
       <c r="S38" s="26"/>
     </row>
     <row r="39" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="188"/>
-      <c r="B39" s="180"/>
+      <c r="A39" s="205"/>
+      <c r="B39" s="176"/>
       <c r="C39" s="60" t="s">
         <v>108</v>
       </c>
@@ -9910,8 +9910,8 @@
       <c r="T39" s="23"/>
     </row>
     <row r="40" spans="1:20" s="28" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="188"/>
-      <c r="B40" s="180"/>
+      <c r="A40" s="205"/>
+      <c r="B40" s="176"/>
       <c r="C40" s="61" t="s">
         <v>109</v>
       </c>
@@ -9959,8 +9959,8 @@
       <c r="S40" s="31"/>
     </row>
     <row r="41" spans="1:20" s="28" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="188"/>
-      <c r="B41" s="185" t="s">
+      <c r="A41" s="205"/>
+      <c r="B41" s="182" t="s">
         <v>193</v>
       </c>
       <c r="C41" s="63" t="s">
@@ -10006,8 +10006,8 @@
       <c r="S41" s="57"/>
     </row>
     <row r="42" spans="1:20" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="188"/>
-      <c r="B42" s="175"/>
+      <c r="A42" s="205"/>
+      <c r="B42" s="183"/>
       <c r="C42" s="60" t="s">
         <v>218</v>
       </c>
@@ -10049,8 +10049,8 @@
       <c r="S42" s="26"/>
     </row>
     <row r="43" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="188"/>
-      <c r="B43" s="175"/>
+      <c r="A43" s="205"/>
+      <c r="B43" s="183"/>
       <c r="C43" s="60" t="s">
         <v>258</v>
       </c>
@@ -10092,8 +10092,8 @@
       <c r="S43" s="26"/>
     </row>
     <row r="44" spans="1:20" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="188"/>
-      <c r="B44" s="175"/>
+      <c r="A44" s="205"/>
+      <c r="B44" s="183"/>
       <c r="C44" s="60" t="s">
         <v>219</v>
       </c>
@@ -10135,8 +10135,8 @@
       <c r="S44" s="26"/>
     </row>
     <row r="45" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="188"/>
-      <c r="B45" s="175"/>
+      <c r="A45" s="205"/>
+      <c r="B45" s="183"/>
       <c r="C45" s="60" t="s">
         <v>490</v>
       </c>
@@ -10181,8 +10181,8 @@
       <c r="T45" s="28"/>
     </row>
     <row r="46" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="188"/>
-      <c r="B46" s="175"/>
+      <c r="A46" s="205"/>
+      <c r="B46" s="183"/>
       <c r="C46" s="60" t="s">
         <v>413</v>
       </c>
@@ -10224,8 +10224,8 @@
       <c r="S46" s="26"/>
     </row>
     <row r="47" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="188"/>
-      <c r="B47" s="175"/>
+      <c r="A47" s="205"/>
+      <c r="B47" s="183"/>
       <c r="C47" s="60" t="s">
         <v>410</v>
       </c>
@@ -10267,8 +10267,8 @@
       <c r="S47" s="26"/>
     </row>
     <row r="48" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="188"/>
-      <c r="B48" s="175"/>
+      <c r="A48" s="205"/>
+      <c r="B48" s="183"/>
       <c r="C48" s="60" t="s">
         <v>408</v>
       </c>
@@ -10314,8 +10314,8 @@
       <c r="S48" s="26"/>
     </row>
     <row r="49" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="188"/>
-      <c r="B49" s="175"/>
+      <c r="A49" s="205"/>
+      <c r="B49" s="183"/>
       <c r="C49" s="60" t="s">
         <v>257</v>
       </c>
@@ -10359,8 +10359,8 @@
       <c r="S49" s="26"/>
     </row>
     <row r="50" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="189"/>
-      <c r="B50" s="176"/>
+      <c r="A50" s="206"/>
+      <c r="B50" s="188"/>
       <c r="C50" s="65" t="s">
         <v>531</v>
       </c>
@@ -10404,10 +10404,10 @@
       <c r="S50" s="26"/>
     </row>
     <row r="51" spans="1:20" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="191" t="s">
+      <c r="A51" s="177" t="s">
         <v>89</v>
       </c>
-      <c r="B51" s="182" t="s">
+      <c r="B51" s="175" t="s">
         <v>51</v>
       </c>
       <c r="C51" s="62" t="s">
@@ -10454,8 +10454,8 @@
       <c r="T51" s="33"/>
     </row>
     <row r="52" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="192"/>
-      <c r="B52" s="180"/>
+      <c r="A52" s="178"/>
+      <c r="B52" s="176"/>
       <c r="C52" s="60" t="s">
         <v>66</v>
       </c>
@@ -10501,8 +10501,8 @@
       <c r="S52" s="26"/>
     </row>
     <row r="53" spans="1:20" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="192"/>
-      <c r="B53" s="180"/>
+      <c r="A53" s="178"/>
+      <c r="B53" s="176"/>
       <c r="C53" s="60" t="s">
         <v>67</v>
       </c>
@@ -10548,8 +10548,8 @@
       <c r="S53" s="26"/>
     </row>
     <row r="54" spans="1:20" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="192"/>
-      <c r="B54" s="180"/>
+      <c r="A54" s="178"/>
+      <c r="B54" s="176"/>
       <c r="C54" s="61" t="s">
         <v>68</v>
       </c>
@@ -10595,8 +10595,8 @@
       <c r="S54" s="26"/>
     </row>
     <row r="55" spans="1:20" s="23" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="192"/>
-      <c r="B55" s="180"/>
+      <c r="A55" s="178"/>
+      <c r="B55" s="176"/>
       <c r="C55" s="65" t="s">
         <v>604</v>
       </c>
@@ -10640,8 +10640,8 @@
       <c r="S55" s="31"/>
     </row>
     <row r="56" spans="1:20" s="23" customFormat="1" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="192"/>
-      <c r="B56" s="185" t="s">
+      <c r="A56" s="178"/>
+      <c r="B56" s="182" t="s">
         <v>193</v>
       </c>
       <c r="C56" s="63" t="s">
@@ -10687,8 +10687,8 @@
       <c r="S56" s="57"/>
     </row>
     <row r="57" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="192"/>
-      <c r="B57" s="175"/>
+      <c r="A57" s="178"/>
+      <c r="B57" s="183"/>
       <c r="C57" s="60" t="s">
         <v>209</v>
       </c>
@@ -10734,8 +10734,8 @@
       <c r="S57" s="26"/>
     </row>
     <row r="58" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="192"/>
-      <c r="B58" s="175"/>
+      <c r="A58" s="178"/>
+      <c r="B58" s="183"/>
       <c r="C58" s="60" t="s">
         <v>202</v>
       </c>
@@ -10779,8 +10779,8 @@
       <c r="S58" s="26"/>
     </row>
     <row r="59" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="192"/>
-      <c r="B59" s="175"/>
+      <c r="A59" s="178"/>
+      <c r="B59" s="183"/>
       <c r="C59" s="60" t="s">
         <v>197</v>
       </c>
@@ -10826,8 +10826,8 @@
       <c r="S59" s="26"/>
     </row>
     <row r="60" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="192"/>
-      <c r="B60" s="175"/>
+      <c r="A60" s="178"/>
+      <c r="B60" s="183"/>
       <c r="C60" s="60" t="s">
         <v>198</v>
       </c>
@@ -10873,8 +10873,8 @@
       <c r="S60" s="26"/>
     </row>
     <row r="61" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="192"/>
-      <c r="B61" s="175"/>
+      <c r="A61" s="178"/>
+      <c r="B61" s="183"/>
       <c r="C61" s="60" t="s">
         <v>91</v>
       </c>
@@ -10918,8 +10918,8 @@
       <c r="S61" s="26"/>
     </row>
     <row r="62" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="192"/>
-      <c r="B62" s="175"/>
+      <c r="A62" s="178"/>
+      <c r="B62" s="183"/>
       <c r="C62" s="60" t="s">
         <v>415</v>
       </c>
@@ -10963,8 +10963,8 @@
       <c r="S62" s="26"/>
     </row>
     <row r="63" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="192"/>
-      <c r="B63" s="175"/>
+      <c r="A63" s="178"/>
+      <c r="B63" s="183"/>
       <c r="C63" s="60" t="s">
         <v>199</v>
       </c>
@@ -11010,8 +11010,8 @@
       <c r="S63" s="26"/>
     </row>
     <row r="64" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="192"/>
-      <c r="B64" s="175"/>
+      <c r="A64" s="178"/>
+      <c r="B64" s="183"/>
       <c r="C64" s="60" t="s">
         <v>429</v>
       </c>
@@ -11057,8 +11057,8 @@
       <c r="S64" s="26"/>
     </row>
     <row r="65" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="192"/>
-      <c r="B65" s="175"/>
+      <c r="A65" s="178"/>
+      <c r="B65" s="183"/>
       <c r="C65" s="60" t="s">
         <v>377</v>
       </c>
@@ -11103,8 +11103,8 @@
       <c r="T65" s="28"/>
     </row>
     <row r="66" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="192"/>
-      <c r="B66" s="175"/>
+      <c r="A66" s="178"/>
+      <c r="B66" s="183"/>
       <c r="C66" s="60" t="s">
         <v>394</v>
       </c>
@@ -11150,8 +11150,8 @@
       <c r="S66" s="26"/>
     </row>
     <row r="67" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="192"/>
-      <c r="B67" s="175"/>
+      <c r="A67" s="178"/>
+      <c r="B67" s="183"/>
       <c r="C67" s="60" t="s">
         <v>254</v>
       </c>
@@ -11198,8 +11198,8 @@
       <c r="T67" s="23"/>
     </row>
     <row r="68" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="192"/>
-      <c r="B68" s="175"/>
+      <c r="A68" s="178"/>
+      <c r="B68" s="183"/>
       <c r="C68" s="60" t="s">
         <v>432</v>
       </c>
@@ -11243,8 +11243,8 @@
       <c r="S68" s="26"/>
     </row>
     <row r="69" spans="1:20" s="33" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="192"/>
-      <c r="B69" s="175"/>
+      <c r="A69" s="178"/>
+      <c r="B69" s="183"/>
       <c r="C69" s="61" t="s">
         <v>203</v>
       </c>
@@ -11289,10 +11289,10 @@
       <c r="T69" s="28"/>
     </row>
     <row r="70" spans="1:20" s="23" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="201" t="s">
+      <c r="A70" s="190" t="s">
         <v>97</v>
       </c>
-      <c r="B70" s="200"/>
+      <c r="B70" s="189"/>
       <c r="C70" s="62" t="s">
         <v>79</v>
       </c>
@@ -11339,8 +11339,8 @@
       <c r="T70" s="33"/>
     </row>
     <row r="71" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="202"/>
-      <c r="B71" s="180"/>
+      <c r="A71" s="191"/>
+      <c r="B71" s="176"/>
       <c r="C71" s="60" t="s">
         <v>80</v>
       </c>
@@ -11386,8 +11386,8 @@
       <c r="S71" s="26"/>
     </row>
     <row r="72" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="202"/>
-      <c r="B72" s="180"/>
+      <c r="A72" s="191"/>
+      <c r="B72" s="176"/>
       <c r="C72" s="60" t="s">
         <v>81</v>
       </c>
@@ -11435,8 +11435,8 @@
       <c r="S72" s="26"/>
     </row>
     <row r="73" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="202"/>
-      <c r="B73" s="180"/>
+      <c r="A73" s="191"/>
+      <c r="B73" s="176"/>
       <c r="C73" s="60" t="s">
         <v>82</v>
       </c>
@@ -11482,8 +11482,8 @@
       <c r="S73" s="26"/>
     </row>
     <row r="74" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="202"/>
-      <c r="B74" s="180"/>
+      <c r="A74" s="191"/>
+      <c r="B74" s="176"/>
       <c r="C74" s="60" t="s">
         <v>83</v>
       </c>
@@ -11531,8 +11531,8 @@
       <c r="S74" s="26"/>
     </row>
     <row r="75" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="202"/>
-      <c r="B75" s="180"/>
+      <c r="A75" s="191"/>
+      <c r="B75" s="176"/>
       <c r="C75" s="60" t="s">
         <v>84</v>
       </c>
@@ -11578,8 +11578,8 @@
       <c r="S75" s="26"/>
     </row>
     <row r="76" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="202"/>
-      <c r="B76" s="180"/>
+      <c r="A76" s="191"/>
+      <c r="B76" s="176"/>
       <c r="C76" s="60" t="s">
         <v>85</v>
       </c>
@@ -11623,8 +11623,8 @@
       <c r="S76" s="26"/>
     </row>
     <row r="77" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="202"/>
-      <c r="B77" s="180"/>
+      <c r="A77" s="191"/>
+      <c r="B77" s="176"/>
       <c r="C77" s="60" t="s">
         <v>86</v>
       </c>
@@ -11670,8 +11670,8 @@
       <c r="S77" s="26"/>
     </row>
     <row r="78" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="202"/>
-      <c r="B78" s="180"/>
+      <c r="A78" s="191"/>
+      <c r="B78" s="176"/>
       <c r="C78" s="60" t="s">
         <v>87</v>
       </c>
@@ -11719,8 +11719,8 @@
       <c r="S78" s="26"/>
     </row>
     <row r="79" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="202"/>
-      <c r="B79" s="180"/>
+      <c r="A79" s="191"/>
+      <c r="B79" s="176"/>
       <c r="C79" s="60" t="s">
         <v>225</v>
       </c>
@@ -11766,8 +11766,8 @@
       <c r="S79" s="26"/>
     </row>
     <row r="80" spans="1:20" s="23" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="202"/>
-      <c r="B80" s="199"/>
+      <c r="A80" s="191"/>
+      <c r="B80" s="187"/>
       <c r="C80" s="61" t="s">
         <v>90</v>
       </c>
@@ -11813,8 +11813,8 @@
       <c r="S80" s="31"/>
     </row>
     <row r="81" spans="1:19" s="23" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="202"/>
-      <c r="B81" s="175" t="s">
+      <c r="A81" s="191"/>
+      <c r="B81" s="183" t="s">
         <v>193</v>
       </c>
       <c r="C81" s="63" t="s">
@@ -11858,8 +11858,8 @@
       <c r="S81" s="57"/>
     </row>
     <row r="82" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="202"/>
-      <c r="B82" s="175"/>
+      <c r="A82" s="191"/>
+      <c r="B82" s="183"/>
       <c r="C82" s="60" t="s">
         <v>213</v>
       </c>
@@ -11905,8 +11905,8 @@
       <c r="S82" s="26"/>
     </row>
     <row r="83" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="202"/>
-      <c r="B83" s="175"/>
+      <c r="A83" s="191"/>
+      <c r="B83" s="183"/>
       <c r="C83" s="60" t="s">
         <v>427</v>
       </c>
@@ -11950,8 +11950,8 @@
       <c r="S83" s="26"/>
     </row>
     <row r="84" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="202"/>
-      <c r="B84" s="175"/>
+      <c r="A84" s="191"/>
+      <c r="B84" s="183"/>
       <c r="C84" s="60" t="s">
         <v>295</v>
       </c>
@@ -11995,8 +11995,8 @@
       <c r="S84" s="26"/>
     </row>
     <row r="85" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="202"/>
-      <c r="B85" s="175"/>
+      <c r="A85" s="191"/>
+      <c r="B85" s="183"/>
       <c r="C85" s="60" t="s">
         <v>368</v>
       </c>
@@ -12040,8 +12040,8 @@
       <c r="S85" s="26"/>
     </row>
     <row r="86" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="202"/>
-      <c r="B86" s="175"/>
+      <c r="A86" s="191"/>
+      <c r="B86" s="183"/>
       <c r="C86" s="60" t="s">
         <v>221</v>
       </c>
@@ -12085,8 +12085,8 @@
       <c r="S86" s="26"/>
     </row>
     <row r="87" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="202"/>
-      <c r="B87" s="175"/>
+      <c r="A87" s="191"/>
+      <c r="B87" s="183"/>
       <c r="C87" s="60" t="s">
         <v>322</v>
       </c>
@@ -12132,8 +12132,8 @@
       <c r="S87" s="26"/>
     </row>
     <row r="88" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="202"/>
-      <c r="B88" s="175"/>
+      <c r="A88" s="191"/>
+      <c r="B88" s="183"/>
       <c r="C88" s="61" t="s">
         <v>249</v>
       </c>
@@ -12177,8 +12177,8 @@
       <c r="S88" s="26"/>
     </row>
     <row r="89" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="202"/>
-      <c r="B89" s="175"/>
+      <c r="A89" s="191"/>
+      <c r="B89" s="183"/>
       <c r="C89" s="60" t="s">
         <v>404</v>
       </c>
@@ -12219,8 +12219,8 @@
       <c r="S89" s="26"/>
     </row>
     <row r="90" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="202"/>
-      <c r="B90" s="175"/>
+      <c r="A90" s="191"/>
+      <c r="B90" s="183"/>
       <c r="C90" s="60" t="s">
         <v>370</v>
       </c>
@@ -12262,8 +12262,8 @@
       <c r="S90" s="26"/>
     </row>
     <row r="91" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="202"/>
-      <c r="B91" s="175"/>
+      <c r="A91" s="191"/>
+      <c r="B91" s="183"/>
       <c r="C91" s="60" t="s">
         <v>357</v>
       </c>
@@ -12309,8 +12309,8 @@
       <c r="S91" s="26"/>
     </row>
     <row r="92" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="202"/>
-      <c r="B92" s="175"/>
+      <c r="A92" s="191"/>
+      <c r="B92" s="183"/>
       <c r="C92" s="60" t="s">
         <v>353</v>
       </c>
@@ -12356,8 +12356,8 @@
       <c r="S92" s="26"/>
     </row>
     <row r="93" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="202"/>
-      <c r="B93" s="175"/>
+      <c r="A93" s="191"/>
+      <c r="B93" s="183"/>
       <c r="C93" s="60" t="s">
         <v>212</v>
       </c>
@@ -12400,8 +12400,8 @@
       <c r="S93" s="26"/>
     </row>
     <row r="94" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="202"/>
-      <c r="B94" s="175"/>
+      <c r="A94" s="191"/>
+      <c r="B94" s="183"/>
       <c r="C94" s="60" t="s">
         <v>373</v>
       </c>
@@ -12445,8 +12445,8 @@
       <c r="S94" s="26"/>
     </row>
     <row r="95" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="202"/>
-      <c r="B95" s="175"/>
+      <c r="A95" s="191"/>
+      <c r="B95" s="183"/>
       <c r="C95" s="60" t="s">
         <v>222</v>
       </c>
@@ -12490,8 +12490,8 @@
       <c r="S95" s="26"/>
     </row>
     <row r="96" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="202"/>
-      <c r="B96" s="175"/>
+      <c r="A96" s="191"/>
+      <c r="B96" s="183"/>
       <c r="C96" s="60" t="s">
         <v>247</v>
       </c>
@@ -12535,8 +12535,8 @@
       <c r="S96" s="26"/>
     </row>
     <row r="97" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="202"/>
-      <c r="B97" s="175"/>
+      <c r="A97" s="191"/>
+      <c r="B97" s="183"/>
       <c r="C97" s="60" t="s">
         <v>294</v>
       </c>
@@ -12580,8 +12580,8 @@
       <c r="S97" s="26"/>
     </row>
     <row r="98" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="202"/>
-      <c r="B98" s="175"/>
+      <c r="A98" s="191"/>
+      <c r="B98" s="183"/>
       <c r="C98" s="60" t="s">
         <v>224</v>
       </c>
@@ -12625,8 +12625,8 @@
       <c r="S98" s="26"/>
     </row>
     <row r="99" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="202"/>
-      <c r="B99" s="175"/>
+      <c r="A99" s="191"/>
+      <c r="B99" s="183"/>
       <c r="C99" s="60" t="s">
         <v>232</v>
       </c>
@@ -12665,8 +12665,8 @@
       <c r="S99" s="26"/>
     </row>
     <row r="100" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="202"/>
-      <c r="B100" s="175"/>
+      <c r="A100" s="191"/>
+      <c r="B100" s="183"/>
       <c r="C100" s="60" t="s">
         <v>223</v>
       </c>
@@ -12707,8 +12707,8 @@
       <c r="S100" s="26"/>
     </row>
     <row r="101" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="202"/>
-      <c r="B101" s="175"/>
+      <c r="A101" s="191"/>
+      <c r="B101" s="183"/>
       <c r="C101" s="65" t="s">
         <v>217</v>
       </c>
@@ -12754,8 +12754,8 @@
       <c r="S101" s="26"/>
     </row>
     <row r="102" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="202"/>
-      <c r="B102" s="175"/>
+      <c r="A102" s="191"/>
+      <c r="B102" s="183"/>
       <c r="C102" s="60" t="s">
         <v>214</v>
       </c>
@@ -12797,8 +12797,8 @@
       <c r="S102" s="26"/>
     </row>
     <row r="103" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="202"/>
-      <c r="B103" s="175"/>
+      <c r="A103" s="191"/>
+      <c r="B103" s="183"/>
       <c r="C103" s="60" t="s">
         <v>215</v>
       </c>
@@ -12842,8 +12842,8 @@
       <c r="S103" s="26"/>
     </row>
     <row r="104" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="202"/>
-      <c r="B104" s="175"/>
+      <c r="A104" s="191"/>
+      <c r="B104" s="183"/>
       <c r="C104" s="60" t="s">
         <v>359</v>
       </c>
@@ -12884,8 +12884,8 @@
       <c r="S104" s="26"/>
     </row>
     <row r="105" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="202"/>
-      <c r="B105" s="175"/>
+      <c r="A105" s="191"/>
+      <c r="B105" s="183"/>
       <c r="C105" s="60" t="s">
         <v>231</v>
       </c>
@@ -12926,8 +12926,8 @@
       <c r="S105" s="26"/>
     </row>
     <row r="106" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="202"/>
-      <c r="B106" s="175"/>
+      <c r="A106" s="191"/>
+      <c r="B106" s="183"/>
       <c r="C106" s="60" t="s">
         <v>206</v>
       </c>
@@ -12969,8 +12969,8 @@
       <c r="S106" s="26"/>
     </row>
     <row r="107" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="202"/>
-      <c r="B107" s="175"/>
+      <c r="A107" s="191"/>
+      <c r="B107" s="183"/>
       <c r="C107" s="60" t="s">
         <v>207</v>
       </c>
@@ -13012,8 +13012,8 @@
       <c r="S107" s="26"/>
     </row>
     <row r="108" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="202"/>
-      <c r="B108" s="175"/>
+      <c r="A108" s="191"/>
+      <c r="B108" s="183"/>
       <c r="C108" s="60" t="s">
         <v>502</v>
       </c>
@@ -13054,8 +13054,8 @@
       <c r="S108" s="26"/>
     </row>
     <row r="109" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="202"/>
-      <c r="B109" s="175"/>
+      <c r="A109" s="191"/>
+      <c r="B109" s="183"/>
       <c r="C109" s="60" t="s">
         <v>248</v>
       </c>
@@ -13096,8 +13096,8 @@
       <c r="S109" s="26"/>
     </row>
     <row r="110" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="202"/>
-      <c r="B110" s="175"/>
+      <c r="A110" s="191"/>
+      <c r="B110" s="183"/>
       <c r="C110" s="60" t="s">
         <v>251</v>
       </c>
@@ -13141,8 +13141,8 @@
       <c r="S110" s="26"/>
     </row>
     <row r="111" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="202"/>
-      <c r="B111" s="175"/>
+      <c r="A111" s="191"/>
+      <c r="B111" s="183"/>
       <c r="C111" s="60" t="s">
         <v>228</v>
       </c>
@@ -13188,8 +13188,8 @@
       <c r="S111" s="26"/>
     </row>
     <row r="112" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="202"/>
-      <c r="B112" s="175"/>
+      <c r="A112" s="191"/>
+      <c r="B112" s="183"/>
       <c r="C112" s="60" t="s">
         <v>229</v>
       </c>
@@ -13235,8 +13235,8 @@
       <c r="S112" s="26"/>
     </row>
     <row r="113" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="202"/>
-      <c r="B113" s="175"/>
+      <c r="A113" s="191"/>
+      <c r="B113" s="183"/>
       <c r="C113" s="65" t="s">
         <v>598</v>
       </c>
@@ -13263,8 +13263,8 @@
       <c r="T113" s="23"/>
     </row>
     <row r="114" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="202"/>
-      <c r="B114" s="175"/>
+      <c r="A114" s="191"/>
+      <c r="B114" s="183"/>
       <c r="C114" s="60" t="s">
         <v>325</v>
       </c>
@@ -13309,8 +13309,8 @@
       <c r="T114" s="23"/>
     </row>
     <row r="115" spans="1:20" s="33" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="203"/>
-      <c r="B115" s="176"/>
+      <c r="A115" s="192"/>
+      <c r="B115" s="188"/>
       <c r="C115" s="61" t="s">
         <v>318</v>
       </c>
@@ -13363,10 +13363,10 @@
       <c r="T115" s="28"/>
     </row>
     <row r="116" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="196" t="s">
+      <c r="A116" s="184" t="s">
         <v>500</v>
       </c>
-      <c r="B116" s="182" t="s">
+      <c r="B116" s="175" t="s">
         <v>51</v>
       </c>
       <c r="C116" s="62" t="s">
@@ -13411,8 +13411,8 @@
       <c r="T116" s="33"/>
     </row>
     <row r="117" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="197"/>
-      <c r="B117" s="180"/>
+      <c r="A117" s="185"/>
+      <c r="B117" s="176"/>
       <c r="C117" s="60" t="s">
         <v>92</v>
       </c>
@@ -13458,8 +13458,8 @@
       <c r="S117" s="26"/>
     </row>
     <row r="118" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="197"/>
-      <c r="B118" s="180"/>
+      <c r="A118" s="185"/>
+      <c r="B118" s="176"/>
       <c r="C118" s="60" t="s">
         <v>93</v>
       </c>
@@ -13505,8 +13505,8 @@
       <c r="S118" s="26"/>
     </row>
     <row r="119" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="197"/>
-      <c r="B119" s="180"/>
+      <c r="A119" s="185"/>
+      <c r="B119" s="176"/>
       <c r="C119" s="60" t="s">
         <v>104</v>
       </c>
@@ -13548,8 +13548,8 @@
       <c r="S119" s="26"/>
     </row>
     <row r="120" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="197"/>
-      <c r="B120" s="180"/>
+      <c r="A120" s="185"/>
+      <c r="B120" s="176"/>
       <c r="C120" s="61" t="s">
         <v>94</v>
       </c>
@@ -13592,8 +13592,8 @@
       <c r="T120" s="28"/>
     </row>
     <row r="121" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="197"/>
-      <c r="B121" s="180"/>
+      <c r="A121" s="185"/>
+      <c r="B121" s="176"/>
       <c r="C121" s="60" t="s">
         <v>179</v>
       </c>
@@ -13636,8 +13636,8 @@
       <c r="T121" s="28"/>
     </row>
     <row r="122" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="197"/>
-      <c r="B122" s="180"/>
+      <c r="A122" s="185"/>
+      <c r="B122" s="176"/>
       <c r="C122" s="61" t="s">
         <v>116</v>
       </c>
@@ -13680,8 +13680,8 @@
       <c r="T122" s="28"/>
     </row>
     <row r="123" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="197"/>
-      <c r="B123" s="180"/>
+      <c r="A123" s="185"/>
+      <c r="B123" s="176"/>
       <c r="C123" s="60" t="s">
         <v>96</v>
       </c>
@@ -13725,8 +13725,8 @@
       <c r="S123" s="26"/>
     </row>
     <row r="124" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="197"/>
-      <c r="B124" s="180"/>
+      <c r="A124" s="185"/>
+      <c r="B124" s="176"/>
       <c r="C124" s="60" t="s">
         <v>501</v>
       </c>
@@ -13770,8 +13770,8 @@
       <c r="S124" s="26"/>
     </row>
     <row r="125" spans="1:20" s="23" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="197"/>
-      <c r="B125" s="199"/>
+      <c r="A125" s="185"/>
+      <c r="B125" s="187"/>
       <c r="C125" s="60" t="s">
         <v>176</v>
       </c>
@@ -13813,8 +13813,8 @@
       <c r="S125" s="26"/>
     </row>
     <row r="126" spans="1:20" s="28" customFormat="1" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="197"/>
-      <c r="B126" s="185" t="s">
+      <c r="A126" s="185"/>
+      <c r="B126" s="182" t="s">
         <v>193</v>
       </c>
       <c r="C126" s="63" t="s">
@@ -13859,8 +13859,8 @@
       <c r="T126" s="23"/>
     </row>
     <row r="127" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="197"/>
-      <c r="B127" s="175"/>
+      <c r="A127" s="185"/>
+      <c r="B127" s="183"/>
       <c r="C127" s="60" t="s">
         <v>448</v>
       </c>
@@ -13901,8 +13901,8 @@
       <c r="T127" s="23"/>
     </row>
     <row r="128" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="197"/>
-      <c r="B128" s="175"/>
+      <c r="A128" s="185"/>
+      <c r="B128" s="183"/>
       <c r="C128" s="60" t="s">
         <v>451</v>
       </c>
@@ -13943,8 +13943,8 @@
       <c r="T128" s="23"/>
     </row>
     <row r="129" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="197"/>
-      <c r="B129" s="175"/>
+      <c r="A129" s="185"/>
+      <c r="B129" s="183"/>
       <c r="C129" s="61" t="s">
         <v>425</v>
       </c>
@@ -13987,8 +13987,8 @@
       <c r="T129" s="23"/>
     </row>
     <row r="130" spans="1:20" s="33" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="197"/>
-      <c r="B130" s="175"/>
+      <c r="A130" s="185"/>
+      <c r="B130" s="183"/>
       <c r="C130" s="60" t="s">
         <v>230</v>
       </c>
@@ -14029,8 +14029,8 @@
       <c r="T130" s="23"/>
     </row>
     <row r="131" spans="1:20" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="197"/>
-      <c r="B131" s="175"/>
+      <c r="A131" s="185"/>
+      <c r="B131" s="183"/>
       <c r="C131" s="60" t="s">
         <v>208</v>
       </c>
@@ -14071,8 +14071,8 @@
       <c r="T131" s="23"/>
     </row>
     <row r="132" spans="1:20" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="198"/>
-      <c r="B132" s="175"/>
+      <c r="A132" s="186"/>
+      <c r="B132" s="183"/>
       <c r="C132" s="65" t="s">
         <v>624</v>
       </c>
@@ -14095,10 +14095,10 @@
       <c r="T132" s="23"/>
     </row>
     <row r="133" spans="1:20" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="193" t="s">
+      <c r="A133" s="179" t="s">
         <v>111</v>
       </c>
-      <c r="B133" s="182" t="s">
+      <c r="B133" s="175" t="s">
         <v>51</v>
       </c>
       <c r="C133" s="62" t="s">
@@ -14141,8 +14141,8 @@
       <c r="T133" s="33"/>
     </row>
     <row r="134" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="194"/>
-      <c r="B134" s="180"/>
+      <c r="A134" s="180"/>
+      <c r="B134" s="176"/>
       <c r="C134" s="61" t="s">
         <v>95</v>
       </c>
@@ -14182,8 +14182,8 @@
       <c r="S134" s="31"/>
     </row>
     <row r="135" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="194"/>
-      <c r="B135" s="180"/>
+      <c r="A135" s="180"/>
+      <c r="B135" s="176"/>
       <c r="C135" s="65" t="s">
         <v>602</v>
       </c>
@@ -14226,8 +14226,8 @@
       <c r="T135" s="19"/>
     </row>
     <row r="136" spans="1:20" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="194"/>
-      <c r="B136" s="180"/>
+      <c r="A136" s="180"/>
+      <c r="B136" s="176"/>
       <c r="C136" s="60" t="s">
         <v>115</v>
       </c>
@@ -14269,8 +14269,8 @@
       <c r="T136" s="19"/>
     </row>
     <row r="137" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A137" s="194"/>
-      <c r="B137" s="180"/>
+      <c r="A137" s="180"/>
+      <c r="B137" s="176"/>
       <c r="C137" s="60" t="s">
         <v>114</v>
       </c>
@@ -14312,8 +14312,8 @@
       <c r="T137" s="19"/>
     </row>
     <row r="138" spans="1:20" s="23" customFormat="1" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="194"/>
-      <c r="B138" s="185" t="s">
+      <c r="A138" s="180"/>
+      <c r="B138" s="182" t="s">
         <v>193</v>
       </c>
       <c r="C138" s="63" t="s">
@@ -14355,8 +14355,8 @@
       <c r="S138" s="57"/>
     </row>
     <row r="139" spans="1:20" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="194"/>
-      <c r="B139" s="175"/>
+      <c r="A139" s="180"/>
+      <c r="B139" s="183"/>
       <c r="C139" s="60" t="s">
         <v>399</v>
       </c>
@@ -14395,8 +14395,8 @@
       <c r="S139" s="26"/>
     </row>
     <row r="140" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="194"/>
-      <c r="B140" s="175"/>
+      <c r="A140" s="180"/>
+      <c r="B140" s="183"/>
       <c r="C140" s="60" t="s">
         <v>255</v>
       </c>
@@ -14436,8 +14436,8 @@
       <c r="S140" s="26"/>
     </row>
     <row r="141" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="194"/>
-      <c r="B141" s="175"/>
+      <c r="A141" s="180"/>
+      <c r="B141" s="183"/>
       <c r="C141" s="65" t="s">
         <v>618</v>
       </c>
@@ -14471,8 +14471,8 @@
       <c r="S141" s="26"/>
     </row>
     <row r="142" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="194"/>
-      <c r="B142" s="175"/>
+      <c r="A142" s="180"/>
+      <c r="B142" s="183"/>
       <c r="C142" s="60" t="s">
         <v>422</v>
       </c>
@@ -14512,8 +14512,8 @@
       <c r="S142" s="26"/>
     </row>
     <row r="143" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="194"/>
-      <c r="B143" s="175"/>
+      <c r="A143" s="180"/>
+      <c r="B143" s="183"/>
       <c r="C143" s="60" t="s">
         <v>380</v>
       </c>
@@ -14553,8 +14553,8 @@
       <c r="S143" s="26"/>
     </row>
     <row r="144" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="194"/>
-      <c r="B144" s="175"/>
+      <c r="A144" s="180"/>
+      <c r="B144" s="183"/>
       <c r="C144" s="60" t="s">
         <v>439</v>
       </c>
@@ -14594,8 +14594,8 @@
       <c r="S144" s="26"/>
     </row>
     <row r="145" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="194"/>
-      <c r="B145" s="175"/>
+      <c r="A145" s="180"/>
+      <c r="B145" s="183"/>
       <c r="C145" s="60" t="s">
         <v>358</v>
       </c>
@@ -14635,8 +14635,8 @@
       <c r="S145" s="26"/>
     </row>
     <row r="146" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="194"/>
-      <c r="B146" s="175"/>
+      <c r="A146" s="180"/>
+      <c r="B146" s="183"/>
       <c r="C146" s="60" t="s">
         <v>226</v>
       </c>
@@ -14676,8 +14676,8 @@
       <c r="S146" s="26"/>
     </row>
     <row r="147" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="194"/>
-      <c r="B147" s="175"/>
+      <c r="A147" s="180"/>
+      <c r="B147" s="183"/>
       <c r="C147" s="60" t="s">
         <v>421</v>
       </c>
@@ -14717,8 +14717,8 @@
       <c r="S147" s="26"/>
     </row>
     <row r="148" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="194"/>
-      <c r="B148" s="175"/>
+      <c r="A148" s="180"/>
+      <c r="B148" s="183"/>
       <c r="C148" s="60" t="s">
         <v>396</v>
       </c>
@@ -14758,8 +14758,8 @@
       <c r="S148" s="26"/>
     </row>
     <row r="149" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="194"/>
-      <c r="B149" s="175"/>
+      <c r="A149" s="180"/>
+      <c r="B149" s="183"/>
       <c r="C149" s="60" t="s">
         <v>433</v>
       </c>
@@ -14799,8 +14799,8 @@
       <c r="S149" s="26"/>
     </row>
     <row r="150" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="194"/>
-      <c r="B150" s="175"/>
+      <c r="A150" s="180"/>
+      <c r="B150" s="183"/>
       <c r="C150" s="60" t="s">
         <v>406</v>
       </c>
@@ -14840,8 +14840,8 @@
       <c r="S150" s="26"/>
     </row>
     <row r="151" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="194"/>
-      <c r="B151" s="175"/>
+      <c r="A151" s="180"/>
+      <c r="B151" s="183"/>
       <c r="C151" s="65" t="s">
         <v>521</v>
       </c>
@@ -14881,8 +14881,8 @@
       <c r="S151" s="26"/>
     </row>
     <row r="152" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="194"/>
-      <c r="B152" s="175"/>
+      <c r="A152" s="180"/>
+      <c r="B152" s="183"/>
       <c r="C152" s="65" t="s">
         <v>256</v>
       </c>
@@ -14922,8 +14922,8 @@
       <c r="S152" s="26"/>
     </row>
     <row r="153" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="194"/>
-      <c r="B153" s="175"/>
+      <c r="A153" s="180"/>
+      <c r="B153" s="183"/>
       <c r="C153" s="65" t="s">
         <v>446</v>
       </c>
@@ -14963,8 +14963,8 @@
       <c r="S153" s="26"/>
     </row>
     <row r="154" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="194"/>
-      <c r="B154" s="175"/>
+      <c r="A154" s="180"/>
+      <c r="B154" s="183"/>
       <c r="C154" s="65" t="s">
         <v>435</v>
       </c>
@@ -15004,8 +15004,8 @@
       <c r="S154" s="26"/>
     </row>
     <row r="155" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="194"/>
-      <c r="B155" s="175"/>
+      <c r="A155" s="180"/>
+      <c r="B155" s="183"/>
       <c r="C155" s="65" t="s">
         <v>319</v>
       </c>
@@ -15047,8 +15047,8 @@
       <c r="S155" s="26"/>
     </row>
     <row r="156" spans="1:19" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="194"/>
-      <c r="B156" s="175"/>
+      <c r="A156" s="180"/>
+      <c r="B156" s="183"/>
       <c r="C156" s="65" t="s">
         <v>366</v>
       </c>
@@ -15088,8 +15088,8 @@
       <c r="S156" s="26"/>
     </row>
     <row r="157" spans="1:19" s="23" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A157" s="195"/>
-      <c r="B157" s="175"/>
+      <c r="A157" s="181"/>
+      <c r="B157" s="183"/>
       <c r="C157" s="65" t="s">
         <v>211</v>
       </c>
@@ -15129,10 +15129,10 @@
       <c r="S157" s="31"/>
     </row>
     <row r="158" spans="1:19" s="33" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A158" s="183" t="s">
+      <c r="A158" s="201" t="s">
         <v>112</v>
       </c>
-      <c r="B158" s="174" t="s">
+      <c r="B158" s="196" t="s">
         <v>193</v>
       </c>
       <c r="C158" s="62" t="s">
@@ -15176,8 +15176,8 @@
       <c r="S158" s="36"/>
     </row>
     <row r="159" spans="1:19" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A159" s="183"/>
-      <c r="B159" s="175"/>
+      <c r="A159" s="201"/>
+      <c r="B159" s="183"/>
       <c r="C159" s="60" t="s">
         <v>362</v>
       </c>
@@ -15219,8 +15219,8 @@
       <c r="S159" s="26"/>
     </row>
     <row r="160" spans="1:19" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A160" s="183"/>
-      <c r="B160" s="175"/>
+      <c r="A160" s="201"/>
+      <c r="B160" s="183"/>
       <c r="C160" s="60" t="s">
         <v>381</v>
       </c>
@@ -15262,8 +15262,8 @@
       <c r="S160" s="26"/>
     </row>
     <row r="161" spans="1:19" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A161" s="183"/>
-      <c r="B161" s="175"/>
+      <c r="A161" s="201"/>
+      <c r="B161" s="183"/>
       <c r="C161" s="60" t="s">
         <v>392</v>
       </c>
@@ -15305,8 +15305,8 @@
       <c r="S161" s="26"/>
     </row>
     <row r="162" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A162" s="183"/>
-      <c r="B162" s="175"/>
+      <c r="A162" s="201"/>
+      <c r="B162" s="183"/>
       <c r="C162" s="60" t="s">
         <v>250</v>
       </c>
@@ -15346,8 +15346,8 @@
       <c r="S162" s="26"/>
     </row>
     <row r="163" spans="1:19" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A163" s="183"/>
-      <c r="B163" s="175"/>
+      <c r="A163" s="201"/>
+      <c r="B163" s="183"/>
       <c r="C163" s="61" t="s">
         <v>401</v>
       </c>
@@ -15389,8 +15389,8 @@
       <c r="S163" s="26"/>
     </row>
     <row r="164" spans="1:19" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A164" s="183"/>
-      <c r="B164" s="175"/>
+      <c r="A164" s="201"/>
+      <c r="B164" s="183"/>
       <c r="C164" s="60" t="s">
         <v>372</v>
       </c>
@@ -15430,8 +15430,8 @@
       <c r="S164" s="26"/>
     </row>
     <row r="165" spans="1:19" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A165" s="183"/>
-      <c r="B165" s="176"/>
+      <c r="A165" s="201"/>
+      <c r="B165" s="188"/>
       <c r="C165" s="60" t="s">
         <v>402</v>
       </c>
@@ -15471,7 +15471,7 @@
       <c r="S165" s="31"/>
     </row>
     <row r="166" spans="1:19" s="33" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A166" s="184" t="s">
+      <c r="A166" s="202" t="s">
         <v>535</v>
       </c>
       <c r="B166" s="72" t="s">
@@ -15514,8 +15514,8 @@
       <c r="S166" s="71"/>
     </row>
     <row r="167" spans="1:19" s="23" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A167" s="184"/>
-      <c r="B167" s="185" t="s">
+      <c r="A167" s="202"/>
+      <c r="B167" s="182" t="s">
         <v>193</v>
       </c>
       <c r="C167" s="60" t="s">
@@ -15553,8 +15553,8 @@
       <c r="S167" s="57"/>
     </row>
     <row r="168" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A168" s="184"/>
-      <c r="B168" s="175"/>
+      <c r="A168" s="202"/>
+      <c r="B168" s="183"/>
       <c r="C168" s="60" t="s">
         <v>195</v>
       </c>
@@ -15589,8 +15589,8 @@
       <c r="S168" s="26"/>
     </row>
     <row r="169" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="184"/>
-      <c r="B169" s="175"/>
+      <c r="A169" s="202"/>
+      <c r="B169" s="183"/>
       <c r="C169" s="60" t="s">
         <v>259</v>
       </c>
@@ -15628,8 +15628,8 @@
       <c r="S169" s="26"/>
     </row>
     <row r="170" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A170" s="184"/>
-      <c r="B170" s="175"/>
+      <c r="A170" s="202"/>
+      <c r="B170" s="183"/>
       <c r="C170" s="60" t="s">
         <v>417</v>
       </c>
@@ -15666,8 +15666,8 @@
       <c r="S170" s="26"/>
     </row>
     <row r="171" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A171" s="184"/>
-      <c r="B171" s="186"/>
+      <c r="A171" s="202"/>
+      <c r="B171" s="203"/>
       <c r="C171" s="60" t="s">
         <v>418</v>
       </c>
@@ -15705,10 +15705,10 @@
       <c r="S171" s="26"/>
     </row>
     <row r="172" spans="1:19" s="33" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A172" s="173" t="s">
+      <c r="A172" s="195" t="s">
         <v>113</v>
       </c>
-      <c r="B172" s="179" t="s">
+      <c r="B172" s="199" t="s">
         <v>51</v>
       </c>
       <c r="C172" s="62" t="s">
@@ -15748,8 +15748,8 @@
       <c r="S172" s="36"/>
     </row>
     <row r="173" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A173" s="173"/>
-      <c r="B173" s="180"/>
+      <c r="A173" s="195"/>
+      <c r="B173" s="176"/>
       <c r="C173" s="60" t="s">
         <v>184</v>
       </c>
@@ -15787,8 +15787,8 @@
       <c r="S173" s="26"/>
     </row>
     <row r="174" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A174" s="173"/>
-      <c r="B174" s="180"/>
+      <c r="A174" s="195"/>
+      <c r="B174" s="176"/>
       <c r="C174" s="60" t="s">
         <v>183</v>
       </c>
@@ -15826,8 +15826,8 @@
       <c r="S174" s="26"/>
     </row>
     <row r="175" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A175" s="173"/>
-      <c r="B175" s="180"/>
+      <c r="A175" s="195"/>
+      <c r="B175" s="176"/>
       <c r="C175" s="61" t="s">
         <v>185</v>
       </c>
@@ -15865,8 +15865,8 @@
       <c r="S175" s="31"/>
     </row>
     <row r="176" spans="1:19" s="23" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A176" s="173"/>
-      <c r="B176" s="171" t="s">
+      <c r="A176" s="195"/>
+      <c r="B176" s="193" t="s">
         <v>193</v>
       </c>
       <c r="C176" s="63" t="s">
@@ -15900,8 +15900,8 @@
       <c r="S176" s="57"/>
     </row>
     <row r="177" spans="1:19" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A177" s="173"/>
-      <c r="B177" s="172"/>
+      <c r="A177" s="195"/>
+      <c r="B177" s="194"/>
       <c r="C177" s="64"/>
       <c r="E177" s="49"/>
       <c r="F177" s="49"/>
@@ -16630,18 +16630,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="C3:S3"/>
-    <mergeCell ref="B51:B55"/>
-    <mergeCell ref="A51:A69"/>
-    <mergeCell ref="A133:A157"/>
-    <mergeCell ref="B138:B157"/>
-    <mergeCell ref="A116:A132"/>
-    <mergeCell ref="B116:B125"/>
-    <mergeCell ref="B81:B115"/>
-    <mergeCell ref="B56:B69"/>
-    <mergeCell ref="B70:B80"/>
-    <mergeCell ref="A70:A115"/>
-    <mergeCell ref="B133:B137"/>
     <mergeCell ref="B176:B177"/>
     <mergeCell ref="A172:A177"/>
     <mergeCell ref="B158:B165"/>
@@ -16657,6 +16645,18 @@
     <mergeCell ref="B126:B132"/>
     <mergeCell ref="A37:A50"/>
     <mergeCell ref="B41:B50"/>
+    <mergeCell ref="C3:S3"/>
+    <mergeCell ref="B51:B55"/>
+    <mergeCell ref="A51:A69"/>
+    <mergeCell ref="A133:A157"/>
+    <mergeCell ref="B138:B157"/>
+    <mergeCell ref="A116:A132"/>
+    <mergeCell ref="B116:B125"/>
+    <mergeCell ref="B81:B115"/>
+    <mergeCell ref="B56:B69"/>
+    <mergeCell ref="B70:B80"/>
+    <mergeCell ref="A70:A115"/>
+    <mergeCell ref="B133:B137"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Loadouts Ueberarbeitet und neue erstellt - Part I plus weitere kleine Fehleranpassungen in Market und types files
</commit_message>
<xml_diff>
--- a/ressources/DayZ Mods.xlsx
+++ b/ressources/DayZ Mods.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\projects\Immersive-DayZ-Experience\ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E60990-D99C-48E0-A64C-036ADD52425D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0883FA1-159E-4A59-89F0-3B7AF0A8E242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="260" activeTab="1" xr2:uid="{FAEB3C3F-74B0-4C80-8C8B-4522341FA132}"/>
+    <workbookView xWindow="-28920" yWindow="1575" windowWidth="29040" windowHeight="15720" tabRatio="260" activeTab="1" xr2:uid="{FAEB3C3F-74B0-4C80-8C8B-4522341FA132}"/>
   </bookViews>
   <sheets>
     <sheet name="Mods" sheetId="1" r:id="rId1"/>
@@ -4104,14 +4104,65 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -4128,12 +4179,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -4146,9 +4191,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -4159,48 +4201,6 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
@@ -8237,18 +8237,18 @@
     <sortCondition ref="B2:B98"/>
   </sortState>
   <mergeCells count="12">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A11:A15"/>
     <mergeCell ref="A48:A52"/>
     <mergeCell ref="A57:A71"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A45:A47"/>
     <mergeCell ref="A21:A40"/>
     <mergeCell ref="A53:A56"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A11:A15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8259,8 +8259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FF4763-6B65-4CE2-BD87-511E98A2E639}">
   <dimension ref="A1:V229"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T29" sqref="T29"/>
+    <sheetView tabSelected="1" topLeftCell="A134" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E105" sqref="E105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8292,25 +8292,25 @@
       <c r="S2"/>
     </row>
     <row r="3" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="173" t="s">
+      <c r="C3" s="192" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="173"/>
-      <c r="E3" s="173"/>
-      <c r="F3" s="173"/>
-      <c r="G3" s="173"/>
-      <c r="H3" s="173"/>
-      <c r="I3" s="173"/>
-      <c r="J3" s="173"/>
-      <c r="K3" s="173"/>
-      <c r="L3" s="173"/>
-      <c r="M3" s="173"/>
-      <c r="N3" s="173"/>
-      <c r="O3" s="173"/>
-      <c r="P3" s="173"/>
-      <c r="Q3" s="173"/>
-      <c r="R3" s="173"/>
-      <c r="S3" s="173"/>
+      <c r="D3" s="192"/>
+      <c r="E3" s="192"/>
+      <c r="F3" s="192"/>
+      <c r="G3" s="192"/>
+      <c r="H3" s="192"/>
+      <c r="I3" s="192"/>
+      <c r="J3" s="192"/>
+      <c r="K3" s="192"/>
+      <c r="L3" s="192"/>
+      <c r="M3" s="192"/>
+      <c r="N3" s="192"/>
+      <c r="O3" s="192"/>
+      <c r="P3" s="192"/>
+      <c r="Q3" s="192"/>
+      <c r="R3" s="192"/>
+      <c r="S3" s="192"/>
     </row>
     <row r="4" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
@@ -8325,19 +8325,19 @@
       <c r="F4" s="3" t="s">
         <v>642</v>
       </c>
-      <c r="G4" s="197"/>
-      <c r="H4" s="197"/>
-      <c r="I4" s="197"/>
-      <c r="J4" s="197"/>
-      <c r="K4" s="197"/>
-      <c r="L4" s="197"/>
-      <c r="M4" s="197"/>
-      <c r="N4" s="197"/>
-      <c r="O4" s="197"/>
-      <c r="P4" s="197"/>
-      <c r="Q4" s="197"/>
-      <c r="R4" s="197"/>
-      <c r="S4" s="197"/>
+      <c r="G4" s="180"/>
+      <c r="H4" s="180"/>
+      <c r="I4" s="180"/>
+      <c r="J4" s="180"/>
+      <c r="K4" s="180"/>
+      <c r="L4" s="180"/>
+      <c r="M4" s="180"/>
+      <c r="N4" s="180"/>
+      <c r="O4" s="180"/>
+      <c r="P4" s="180"/>
+      <c r="Q4" s="180"/>
+      <c r="R4" s="180"/>
+      <c r="S4" s="180"/>
     </row>
     <row r="5" spans="1:22" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="3"/>
@@ -8388,10 +8388,10 @@
       </c>
     </row>
     <row r="6" spans="1:22" s="23" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="196" t="s">
+      <c r="A6" s="179" t="s">
         <v>88</v>
       </c>
-      <c r="B6" s="198" t="s">
+      <c r="B6" s="181" t="s">
         <v>51</v>
       </c>
       <c r="C6" s="18" t="s">
@@ -8453,8 +8453,8 @@
       </c>
     </row>
     <row r="7" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="196"/>
-      <c r="B7" s="175"/>
+      <c r="A7" s="179"/>
+      <c r="B7" s="182"/>
       <c r="C7" s="60" t="s">
         <v>42</v>
       </c>
@@ -8505,8 +8505,8 @@
       </c>
     </row>
     <row r="8" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="196"/>
-      <c r="B8" s="175"/>
+      <c r="A8" s="179"/>
+      <c r="B8" s="182"/>
       <c r="C8" s="60" t="s">
         <v>49</v>
       </c>
@@ -8555,8 +8555,8 @@
       </c>
     </row>
     <row r="9" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="196"/>
-      <c r="B9" s="175"/>
+      <c r="A9" s="179"/>
+      <c r="B9" s="182"/>
       <c r="C9" s="60" t="s">
         <v>281</v>
       </c>
@@ -8607,8 +8607,8 @@
       </c>
     </row>
     <row r="10" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="196"/>
-      <c r="B10" s="175"/>
+      <c r="A10" s="179"/>
+      <c r="B10" s="182"/>
       <c r="C10" s="60" t="s">
         <v>43</v>
       </c>
@@ -8657,8 +8657,8 @@
       </c>
     </row>
     <row r="11" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="196"/>
-      <c r="B11" s="175"/>
+      <c r="A11" s="179"/>
+      <c r="B11" s="182"/>
       <c r="C11" s="60" t="s">
         <v>59</v>
       </c>
@@ -8709,8 +8709,8 @@
       </c>
     </row>
     <row r="12" spans="1:22" s="23" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="196"/>
-      <c r="B12" s="175"/>
+      <c r="A12" s="179"/>
+      <c r="B12" s="182"/>
       <c r="C12" s="60" t="s">
         <v>44</v>
       </c>
@@ -8756,8 +8756,8 @@
       <c r="S12" s="26"/>
     </row>
     <row r="13" spans="1:22" s="23" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="196"/>
-      <c r="B13" s="175"/>
+      <c r="A13" s="179"/>
+      <c r="B13" s="182"/>
       <c r="C13" s="60" t="s">
         <v>634</v>
       </c>
@@ -8791,8 +8791,8 @@
       <c r="S13" s="26"/>
     </row>
     <row r="14" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="196"/>
-      <c r="B14" s="175"/>
+      <c r="A14" s="179"/>
+      <c r="B14" s="182"/>
       <c r="C14" s="60" t="s">
         <v>45</v>
       </c>
@@ -8838,8 +8838,8 @@
       <c r="S14" s="26"/>
     </row>
     <row r="15" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="196"/>
-      <c r="B15" s="175"/>
+      <c r="A15" s="179"/>
+      <c r="B15" s="182"/>
       <c r="C15" s="60" t="s">
         <v>74</v>
       </c>
@@ -8885,8 +8885,8 @@
       <c r="S15" s="26"/>
     </row>
     <row r="16" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="196"/>
-      <c r="B16" s="175"/>
+      <c r="A16" s="179"/>
+      <c r="B16" s="182"/>
       <c r="C16" s="60" t="s">
         <v>46</v>
       </c>
@@ -8930,8 +8930,8 @@
       <c r="S16" s="26"/>
     </row>
     <row r="17" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="196"/>
-      <c r="B17" s="175"/>
+      <c r="A17" s="179"/>
+      <c r="B17" s="182"/>
       <c r="C17" s="60" t="s">
         <v>47</v>
       </c>
@@ -8975,8 +8975,8 @@
       <c r="S17" s="26"/>
     </row>
     <row r="18" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="196"/>
-      <c r="B18" s="175"/>
+      <c r="A18" s="179"/>
+      <c r="B18" s="182"/>
       <c r="C18" s="60" t="s">
         <v>48</v>
       </c>
@@ -9020,8 +9020,8 @@
       <c r="S18" s="26"/>
     </row>
     <row r="19" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="196"/>
-      <c r="B19" s="175"/>
+      <c r="A19" s="179"/>
+      <c r="B19" s="182"/>
       <c r="C19" s="60" t="s">
         <v>344</v>
       </c>
@@ -9067,8 +9067,8 @@
       <c r="S19" s="26"/>
     </row>
     <row r="20" spans="1:20" s="40" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="196"/>
-      <c r="B20" s="199"/>
+      <c r="A20" s="179"/>
+      <c r="B20" s="183"/>
       <c r="C20" s="61" t="s">
         <v>50</v>
       </c>
@@ -9110,8 +9110,8 @@
       <c r="S20" s="31"/>
     </row>
     <row r="21" spans="1:20" s="33" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="196"/>
-      <c r="B21" s="195" t="s">
+      <c r="A21" s="179"/>
+      <c r="B21" s="176" t="s">
         <v>244</v>
       </c>
       <c r="C21" s="117" t="s">
@@ -9162,8 +9162,8 @@
       </c>
     </row>
     <row r="22" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="196"/>
-      <c r="B22" s="182"/>
+      <c r="A22" s="179"/>
+      <c r="B22" s="177"/>
       <c r="C22" s="61" t="s">
         <v>231</v>
       </c>
@@ -9209,8 +9209,8 @@
       <c r="S22" s="26"/>
     </row>
     <row r="23" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="196"/>
-      <c r="B23" s="182"/>
+      <c r="A23" s="179"/>
+      <c r="B23" s="177"/>
       <c r="C23" s="60" t="s">
         <v>45</v>
       </c>
@@ -9254,8 +9254,8 @@
       <c r="S23" s="26"/>
     </row>
     <row r="24" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="196"/>
-      <c r="B24" s="182"/>
+      <c r="A24" s="179"/>
+      <c r="B24" s="177"/>
       <c r="C24" s="60" t="s">
         <v>120</v>
       </c>
@@ -9303,8 +9303,8 @@
       <c r="S24" s="26"/>
     </row>
     <row r="25" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="196"/>
-      <c r="B25" s="182"/>
+      <c r="A25" s="179"/>
+      <c r="B25" s="177"/>
       <c r="C25" s="60" t="s">
         <v>233</v>
       </c>
@@ -9354,8 +9354,8 @@
       <c r="S25" s="26"/>
     </row>
     <row r="26" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="196"/>
-      <c r="B26" s="182"/>
+      <c r="A26" s="179"/>
+      <c r="B26" s="177"/>
       <c r="C26" s="60" t="s">
         <v>348</v>
       </c>
@@ -9401,8 +9401,8 @@
       <c r="S26" s="26"/>
     </row>
     <row r="27" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="196"/>
-      <c r="B27" s="182"/>
+      <c r="A27" s="179"/>
+      <c r="B27" s="177"/>
       <c r="C27" s="60" t="s">
         <v>119</v>
       </c>
@@ -9448,8 +9448,8 @@
       <c r="S27" s="26"/>
     </row>
     <row r="28" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="196"/>
-      <c r="B28" s="182"/>
+      <c r="A28" s="179"/>
+      <c r="B28" s="177"/>
       <c r="C28" s="60" t="s">
         <v>462</v>
       </c>
@@ -9495,8 +9495,8 @@
       <c r="S28" s="26"/>
     </row>
     <row r="29" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="196"/>
-      <c r="B29" s="182"/>
+      <c r="A29" s="179"/>
+      <c r="B29" s="177"/>
       <c r="C29" s="60" t="s">
         <v>383</v>
       </c>
@@ -9542,8 +9542,8 @@
       <c r="S29" s="26"/>
     </row>
     <row r="30" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="196"/>
-      <c r="B30" s="182"/>
+      <c r="A30" s="179"/>
+      <c r="B30" s="177"/>
       <c r="C30" s="60" t="s">
         <v>236</v>
       </c>
@@ -9590,8 +9590,8 @@
       <c r="T30" s="23"/>
     </row>
     <row r="31" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="196"/>
-      <c r="B31" s="182"/>
+      <c r="A31" s="179"/>
+      <c r="B31" s="177"/>
       <c r="C31" s="60" t="s">
         <v>349</v>
       </c>
@@ -9637,8 +9637,8 @@
       <c r="S31" s="26"/>
     </row>
     <row r="32" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="196"/>
-      <c r="B32" s="182"/>
+      <c r="A32" s="179"/>
+      <c r="B32" s="177"/>
       <c r="C32" s="60" t="s">
         <v>349</v>
       </c>
@@ -9684,8 +9684,8 @@
       <c r="S32" s="26"/>
     </row>
     <row r="33" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="196"/>
-      <c r="B33" s="182"/>
+      <c r="A33" s="179"/>
+      <c r="B33" s="177"/>
       <c r="C33" s="60" t="s">
         <v>215</v>
       </c>
@@ -9732,8 +9732,8 @@
       <c r="T33" s="23"/>
     </row>
     <row r="34" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="196"/>
-      <c r="B34" s="182"/>
+      <c r="A34" s="179"/>
+      <c r="B34" s="177"/>
       <c r="C34" s="60" t="s">
         <v>240</v>
       </c>
@@ -9779,8 +9779,8 @@
       <c r="S34" s="26"/>
     </row>
     <row r="35" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="196"/>
-      <c r="B35" s="182"/>
+      <c r="A35" s="179"/>
+      <c r="B35" s="177"/>
       <c r="C35" s="60" t="s">
         <v>373</v>
       </c>
@@ -9824,8 +9824,8 @@
       <c r="S35" s="26"/>
     </row>
     <row r="36" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="196"/>
-      <c r="B36" s="182"/>
+      <c r="A36" s="179"/>
+      <c r="B36" s="177"/>
       <c r="C36" s="60" t="s">
         <v>688</v>
       </c>
@@ -9857,8 +9857,8 @@
       <c r="S36" s="26"/>
     </row>
     <row r="37" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="196"/>
-      <c r="B37" s="182"/>
+      <c r="A37" s="179"/>
+      <c r="B37" s="177"/>
       <c r="C37" s="60" t="s">
         <v>385</v>
       </c>
@@ -9904,8 +9904,8 @@
       <c r="S37" s="26"/>
     </row>
     <row r="38" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="196"/>
-      <c r="B38" s="187"/>
+      <c r="A38" s="179"/>
+      <c r="B38" s="178"/>
       <c r="C38" s="65" t="s">
         <v>232</v>
       </c>
@@ -9951,10 +9951,10 @@
       <c r="S38" s="26"/>
     </row>
     <row r="39" spans="1:20" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="203" t="s">
+      <c r="A39" s="189" t="s">
         <v>264</v>
       </c>
-      <c r="B39" s="174" t="s">
+      <c r="B39" s="184" t="s">
         <v>51</v>
       </c>
       <c r="C39" s="62" t="s">
@@ -9999,8 +9999,8 @@
       <c r="T39" s="33"/>
     </row>
     <row r="40" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="204"/>
-      <c r="B40" s="175"/>
+      <c r="A40" s="190"/>
+      <c r="B40" s="182"/>
       <c r="C40" s="60" t="s">
         <v>107</v>
       </c>
@@ -10042,8 +10042,8 @@
       <c r="S40" s="26"/>
     </row>
     <row r="41" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="204"/>
-      <c r="B41" s="175"/>
+      <c r="A41" s="190"/>
+      <c r="B41" s="182"/>
       <c r="C41" s="60" t="s">
         <v>108</v>
       </c>
@@ -10086,8 +10086,8 @@
       <c r="T41" s="23"/>
     </row>
     <row r="42" spans="1:20" s="28" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="204"/>
-      <c r="B42" s="175"/>
+      <c r="A42" s="190"/>
+      <c r="B42" s="182"/>
       <c r="C42" s="61" t="s">
         <v>109</v>
       </c>
@@ -10135,8 +10135,8 @@
       <c r="S42" s="31"/>
     </row>
     <row r="43" spans="1:20" s="28" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="204"/>
-      <c r="B43" s="181" t="s">
+      <c r="A43" s="190"/>
+      <c r="B43" s="187" t="s">
         <v>193</v>
       </c>
       <c r="C43" s="63" t="s">
@@ -10184,8 +10184,8 @@
       <c r="S43" s="57"/>
     </row>
     <row r="44" spans="1:20" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="204"/>
-      <c r="B44" s="182"/>
+      <c r="A44" s="190"/>
+      <c r="B44" s="177"/>
       <c r="C44" s="60" t="s">
         <v>217</v>
       </c>
@@ -10227,8 +10227,8 @@
       <c r="S44" s="26"/>
     </row>
     <row r="45" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="204"/>
-      <c r="B45" s="182"/>
+      <c r="A45" s="190"/>
+      <c r="B45" s="177"/>
       <c r="C45" s="60" t="s">
         <v>256</v>
       </c>
@@ -10270,8 +10270,8 @@
       <c r="S45" s="26"/>
     </row>
     <row r="46" spans="1:20" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="204"/>
-      <c r="B46" s="182"/>
+      <c r="A46" s="190"/>
+      <c r="B46" s="177"/>
       <c r="C46" s="60" t="s">
         <v>218</v>
       </c>
@@ -10313,8 +10313,8 @@
       <c r="S46" s="26"/>
     </row>
     <row r="47" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="204"/>
-      <c r="B47" s="182"/>
+      <c r="A47" s="190"/>
+      <c r="B47" s="177"/>
       <c r="C47" s="60" t="s">
         <v>487</v>
       </c>
@@ -10361,8 +10361,8 @@
       <c r="T47" s="28"/>
     </row>
     <row r="48" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="204"/>
-      <c r="B48" s="182"/>
+      <c r="A48" s="190"/>
+      <c r="B48" s="177"/>
       <c r="C48" s="60" t="s">
         <v>410</v>
       </c>
@@ -10406,8 +10406,8 @@
       <c r="S48" s="26"/>
     </row>
     <row r="49" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="204"/>
-      <c r="B49" s="182"/>
+      <c r="A49" s="190"/>
+      <c r="B49" s="177"/>
       <c r="C49" s="60" t="s">
         <v>407</v>
       </c>
@@ -10451,8 +10451,8 @@
       <c r="S49" s="26"/>
     </row>
     <row r="50" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="204"/>
-      <c r="B50" s="182"/>
+      <c r="A50" s="190"/>
+      <c r="B50" s="177"/>
       <c r="C50" s="60" t="s">
         <v>405</v>
       </c>
@@ -10500,8 +10500,8 @@
       <c r="S50" s="26"/>
     </row>
     <row r="51" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="204"/>
-      <c r="B51" s="182"/>
+      <c r="A51" s="190"/>
+      <c r="B51" s="177"/>
       <c r="C51" s="60" t="s">
         <v>255</v>
       </c>
@@ -10547,8 +10547,8 @@
       <c r="S51" s="26"/>
     </row>
     <row r="52" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="205"/>
-      <c r="B52" s="187"/>
+      <c r="A52" s="191"/>
+      <c r="B52" s="178"/>
       <c r="C52" s="65" t="s">
         <v>528</v>
       </c>
@@ -10592,10 +10592,10 @@
       <c r="S52" s="26"/>
     </row>
     <row r="53" spans="1:20" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="176" t="s">
+      <c r="A53" s="193" t="s">
         <v>89</v>
       </c>
-      <c r="B53" s="174" t="s">
+      <c r="B53" s="184" t="s">
         <v>51</v>
       </c>
       <c r="C53" s="62" t="s">
@@ -10642,8 +10642,8 @@
       <c r="T53" s="33"/>
     </row>
     <row r="54" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="177"/>
-      <c r="B54" s="175"/>
+      <c r="A54" s="194"/>
+      <c r="B54" s="182"/>
       <c r="C54" s="60" t="s">
         <v>66</v>
       </c>
@@ -10689,8 +10689,8 @@
       <c r="S54" s="26"/>
     </row>
     <row r="55" spans="1:20" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="177"/>
-      <c r="B55" s="175"/>
+      <c r="A55" s="194"/>
+      <c r="B55" s="182"/>
       <c r="C55" s="60" t="s">
         <v>67</v>
       </c>
@@ -10736,8 +10736,8 @@
       <c r="S55" s="26"/>
     </row>
     <row r="56" spans="1:20" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="177"/>
-      <c r="B56" s="175"/>
+      <c r="A56" s="194"/>
+      <c r="B56" s="182"/>
       <c r="C56" s="61" t="s">
         <v>68</v>
       </c>
@@ -10783,8 +10783,8 @@
       <c r="S56" s="26"/>
     </row>
     <row r="57" spans="1:20" s="23" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="177"/>
-      <c r="B57" s="175"/>
+      <c r="A57" s="194"/>
+      <c r="B57" s="182"/>
       <c r="C57" s="65" t="s">
         <v>601</v>
       </c>
@@ -10828,8 +10828,8 @@
       <c r="S57" s="31"/>
     </row>
     <row r="58" spans="1:20" s="23" customFormat="1" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="177"/>
-      <c r="B58" s="181" t="s">
+      <c r="A58" s="194"/>
+      <c r="B58" s="187" t="s">
         <v>193</v>
       </c>
       <c r="C58" s="63" t="s">
@@ -10877,8 +10877,8 @@
       <c r="S58" s="57"/>
     </row>
     <row r="59" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="177"/>
-      <c r="B59" s="182"/>
+      <c r="A59" s="194"/>
+      <c r="B59" s="177"/>
       <c r="C59" s="60" t="s">
         <v>208</v>
       </c>
@@ -10926,8 +10926,8 @@
       <c r="S59" s="26"/>
     </row>
     <row r="60" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="177"/>
-      <c r="B60" s="182"/>
+      <c r="A60" s="194"/>
+      <c r="B60" s="177"/>
       <c r="C60" s="60" t="s">
         <v>202</v>
       </c>
@@ -10971,8 +10971,8 @@
       <c r="S60" s="26"/>
     </row>
     <row r="61" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="177"/>
-      <c r="B61" s="182"/>
+      <c r="A61" s="194"/>
+      <c r="B61" s="177"/>
       <c r="C61" s="60" t="s">
         <v>197</v>
       </c>
@@ -11018,8 +11018,8 @@
       <c r="S61" s="26"/>
     </row>
     <row r="62" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="177"/>
-      <c r="B62" s="182"/>
+      <c r="A62" s="194"/>
+      <c r="B62" s="177"/>
       <c r="C62" s="60" t="s">
         <v>198</v>
       </c>
@@ -11065,8 +11065,8 @@
       <c r="S62" s="26"/>
     </row>
     <row r="63" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="177"/>
-      <c r="B63" s="182"/>
+      <c r="A63" s="194"/>
+      <c r="B63" s="177"/>
       <c r="C63" s="60" t="s">
         <v>91</v>
       </c>
@@ -11112,8 +11112,8 @@
       <c r="S63" s="26"/>
     </row>
     <row r="64" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="177"/>
-      <c r="B64" s="182"/>
+      <c r="A64" s="194"/>
+      <c r="B64" s="177"/>
       <c r="C64" s="60" t="s">
         <v>412</v>
       </c>
@@ -11159,8 +11159,8 @@
       <c r="S64" s="26"/>
     </row>
     <row r="65" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="177"/>
-      <c r="B65" s="182"/>
+      <c r="A65" s="194"/>
+      <c r="B65" s="177"/>
       <c r="C65" s="60" t="s">
         <v>199</v>
       </c>
@@ -11208,8 +11208,8 @@
       <c r="S65" s="26"/>
     </row>
     <row r="66" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="177"/>
-      <c r="B66" s="182"/>
+      <c r="A66" s="194"/>
+      <c r="B66" s="177"/>
       <c r="C66" s="60" t="s">
         <v>426</v>
       </c>
@@ -11255,8 +11255,8 @@
       <c r="S66" s="26"/>
     </row>
     <row r="67" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="177"/>
-      <c r="B67" s="182"/>
+      <c r="A67" s="194"/>
+      <c r="B67" s="177"/>
       <c r="C67" s="60" t="s">
         <v>375</v>
       </c>
@@ -11303,8 +11303,8 @@
       <c r="T67" s="28"/>
     </row>
     <row r="68" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="177"/>
-      <c r="B68" s="182"/>
+      <c r="A68" s="194"/>
+      <c r="B68" s="177"/>
       <c r="C68" s="60" t="s">
         <v>391</v>
       </c>
@@ -11352,8 +11352,8 @@
       <c r="S68" s="26"/>
     </row>
     <row r="69" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="177"/>
-      <c r="B69" s="182"/>
+      <c r="A69" s="194"/>
+      <c r="B69" s="177"/>
       <c r="C69" s="60" t="s">
         <v>252</v>
       </c>
@@ -11402,8 +11402,8 @@
       <c r="T69" s="23"/>
     </row>
     <row r="70" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="177"/>
-      <c r="B70" s="182"/>
+      <c r="A70" s="194"/>
+      <c r="B70" s="177"/>
       <c r="C70" s="60" t="s">
         <v>429</v>
       </c>
@@ -11449,8 +11449,8 @@
       <c r="S70" s="26"/>
     </row>
     <row r="71" spans="1:20" s="33" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="177"/>
-      <c r="B71" s="182"/>
+      <c r="A71" s="194"/>
+      <c r="B71" s="177"/>
       <c r="C71" s="61" t="s">
         <v>203</v>
       </c>
@@ -11495,10 +11495,10 @@
       <c r="T71" s="28"/>
     </row>
     <row r="72" spans="1:20" s="23" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="189" t="s">
+      <c r="A72" s="203" t="s">
         <v>97</v>
       </c>
-      <c r="B72" s="188"/>
+      <c r="B72" s="202"/>
       <c r="C72" s="62" t="s">
         <v>79</v>
       </c>
@@ -11545,8 +11545,8 @@
       <c r="T72" s="33"/>
     </row>
     <row r="73" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="190"/>
-      <c r="B73" s="175"/>
+      <c r="A73" s="204"/>
+      <c r="B73" s="182"/>
       <c r="C73" s="60" t="s">
         <v>80</v>
       </c>
@@ -11592,8 +11592,8 @@
       <c r="S73" s="26"/>
     </row>
     <row r="74" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="190"/>
-      <c r="B74" s="175"/>
+      <c r="A74" s="204"/>
+      <c r="B74" s="182"/>
       <c r="C74" s="60" t="s">
         <v>81</v>
       </c>
@@ -11641,8 +11641,8 @@
       <c r="S74" s="26"/>
     </row>
     <row r="75" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="190"/>
-      <c r="B75" s="175"/>
+      <c r="A75" s="204"/>
+      <c r="B75" s="182"/>
       <c r="C75" s="60" t="s">
         <v>82</v>
       </c>
@@ -11688,8 +11688,8 @@
       <c r="S75" s="26"/>
     </row>
     <row r="76" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="190"/>
-      <c r="B76" s="175"/>
+      <c r="A76" s="204"/>
+      <c r="B76" s="182"/>
       <c r="C76" s="60" t="s">
         <v>83</v>
       </c>
@@ -11737,8 +11737,8 @@
       <c r="S76" s="26"/>
     </row>
     <row r="77" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="190"/>
-      <c r="B77" s="175"/>
+      <c r="A77" s="204"/>
+      <c r="B77" s="182"/>
       <c r="C77" s="60" t="s">
         <v>84</v>
       </c>
@@ -11784,8 +11784,8 @@
       <c r="S77" s="26"/>
     </row>
     <row r="78" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="190"/>
-      <c r="B78" s="175"/>
+      <c r="A78" s="204"/>
+      <c r="B78" s="182"/>
       <c r="C78" s="60" t="s">
         <v>85</v>
       </c>
@@ -11829,8 +11829,8 @@
       <c r="S78" s="26"/>
     </row>
     <row r="79" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="190"/>
-      <c r="B79" s="175"/>
+      <c r="A79" s="204"/>
+      <c r="B79" s="182"/>
       <c r="C79" s="60" t="s">
         <v>86</v>
       </c>
@@ -11876,8 +11876,8 @@
       <c r="S79" s="26"/>
     </row>
     <row r="80" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="190"/>
-      <c r="B80" s="175"/>
+      <c r="A80" s="204"/>
+      <c r="B80" s="182"/>
       <c r="C80" s="60" t="s">
         <v>87</v>
       </c>
@@ -11925,8 +11925,8 @@
       <c r="S80" s="26"/>
     </row>
     <row r="81" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="190"/>
-      <c r="B81" s="175"/>
+      <c r="A81" s="204"/>
+      <c r="B81" s="182"/>
       <c r="C81" s="60" t="s">
         <v>223</v>
       </c>
@@ -11972,8 +11972,8 @@
       <c r="S81" s="26"/>
     </row>
     <row r="82" spans="1:19" s="23" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="190"/>
-      <c r="B82" s="186"/>
+      <c r="A82" s="204"/>
+      <c r="B82" s="201"/>
       <c r="C82" s="61" t="s">
         <v>90</v>
       </c>
@@ -12019,8 +12019,8 @@
       <c r="S82" s="31"/>
     </row>
     <row r="83" spans="1:19" s="23" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="190"/>
-      <c r="B83" s="182" t="s">
+      <c r="A83" s="204"/>
+      <c r="B83" s="177" t="s">
         <v>193</v>
       </c>
       <c r="C83" s="63" t="s">
@@ -12068,8 +12068,8 @@
       <c r="S83" s="57"/>
     </row>
     <row r="84" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="190"/>
-      <c r="B84" s="182"/>
+      <c r="A84" s="204"/>
+      <c r="B84" s="177"/>
       <c r="C84" s="60" t="s">
         <v>212</v>
       </c>
@@ -12115,8 +12115,8 @@
       <c r="S84" s="26"/>
     </row>
     <row r="85" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="190"/>
-      <c r="B85" s="182"/>
+      <c r="A85" s="204"/>
+      <c r="B85" s="177"/>
       <c r="C85" s="60" t="s">
         <v>424</v>
       </c>
@@ -12160,8 +12160,8 @@
       <c r="S85" s="26"/>
     </row>
     <row r="86" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="190"/>
-      <c r="B86" s="182"/>
+      <c r="A86" s="204"/>
+      <c r="B86" s="177"/>
       <c r="C86" s="60" t="s">
         <v>293</v>
       </c>
@@ -12207,8 +12207,8 @@
       <c r="S86" s="26"/>
     </row>
     <row r="87" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="190"/>
-      <c r="B87" s="182"/>
+      <c r="A87" s="204"/>
+      <c r="B87" s="177"/>
       <c r="C87" s="60" t="s">
         <v>366</v>
       </c>
@@ -12254,8 +12254,8 @@
       <c r="S87" s="26"/>
     </row>
     <row r="88" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="190"/>
-      <c r="B88" s="182"/>
+      <c r="A88" s="204"/>
+      <c r="B88" s="177"/>
       <c r="C88" s="60" t="s">
         <v>219</v>
       </c>
@@ -12299,8 +12299,8 @@
       <c r="S88" s="26"/>
     </row>
     <row r="89" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="190"/>
-      <c r="B89" s="182"/>
+      <c r="A89" s="204"/>
+      <c r="B89" s="177"/>
       <c r="C89" s="60" t="s">
         <v>320</v>
       </c>
@@ -12346,8 +12346,8 @@
       <c r="S89" s="26"/>
     </row>
     <row r="90" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="190"/>
-      <c r="B90" s="182"/>
+      <c r="A90" s="204"/>
+      <c r="B90" s="177"/>
       <c r="C90" s="61" t="s">
         <v>247</v>
       </c>
@@ -12393,8 +12393,8 @@
       <c r="S90" s="26"/>
     </row>
     <row r="91" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="190"/>
-      <c r="B91" s="182"/>
+      <c r="A91" s="204"/>
+      <c r="B91" s="177"/>
       <c r="C91" s="60" t="s">
         <v>401</v>
       </c>
@@ -12440,8 +12440,8 @@
       <c r="S91" s="26"/>
     </row>
     <row r="92" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="190"/>
-      <c r="B92" s="182"/>
+      <c r="A92" s="204"/>
+      <c r="B92" s="177"/>
       <c r="C92" s="65" t="s">
         <v>692</v>
       </c>
@@ -12473,8 +12473,8 @@
       <c r="S92" s="26"/>
     </row>
     <row r="93" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="190"/>
-      <c r="B93" s="182"/>
+      <c r="A93" s="204"/>
+      <c r="B93" s="177"/>
       <c r="C93" s="60" t="s">
         <v>368</v>
       </c>
@@ -12518,8 +12518,8 @@
       <c r="S93" s="26"/>
     </row>
     <row r="94" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="190"/>
-      <c r="B94" s="182"/>
+      <c r="A94" s="204"/>
+      <c r="B94" s="177"/>
       <c r="C94" s="60" t="s">
         <v>355</v>
       </c>
@@ -12565,8 +12565,8 @@
       <c r="S94" s="26"/>
     </row>
     <row r="95" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="190"/>
-      <c r="B95" s="182"/>
+      <c r="A95" s="204"/>
+      <c r="B95" s="177"/>
       <c r="C95" s="60" t="s">
         <v>351</v>
       </c>
@@ -12612,8 +12612,8 @@
       <c r="S95" s="26"/>
     </row>
     <row r="96" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="190"/>
-      <c r="B96" s="182"/>
+      <c r="A96" s="204"/>
+      <c r="B96" s="177"/>
       <c r="C96" s="60" t="s">
         <v>211</v>
       </c>
@@ -12661,8 +12661,8 @@
       <c r="S96" s="26"/>
     </row>
     <row r="97" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="190"/>
-      <c r="B97" s="182"/>
+      <c r="A97" s="204"/>
+      <c r="B97" s="177"/>
       <c r="C97" s="60" t="s">
         <v>371</v>
       </c>
@@ -12708,8 +12708,8 @@
       <c r="S97" s="26"/>
     </row>
     <row r="98" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="190"/>
-      <c r="B98" s="182"/>
+      <c r="A98" s="204"/>
+      <c r="B98" s="177"/>
       <c r="C98" s="60" t="s">
         <v>220</v>
       </c>
@@ -12755,8 +12755,8 @@
       <c r="S98" s="26"/>
     </row>
     <row r="99" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="190"/>
-      <c r="B99" s="182"/>
+      <c r="A99" s="204"/>
+      <c r="B99" s="177"/>
       <c r="C99" s="60" t="s">
         <v>245</v>
       </c>
@@ -12800,8 +12800,8 @@
       <c r="S99" s="26"/>
     </row>
     <row r="100" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="190"/>
-      <c r="B100" s="182"/>
+      <c r="A100" s="204"/>
+      <c r="B100" s="177"/>
       <c r="C100" s="60" t="s">
         <v>292</v>
       </c>
@@ -12845,8 +12845,8 @@
       <c r="S100" s="26"/>
     </row>
     <row r="101" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="190"/>
-      <c r="B101" s="182"/>
+      <c r="A101" s="204"/>
+      <c r="B101" s="177"/>
       <c r="C101" s="60" t="s">
         <v>222</v>
       </c>
@@ -12892,8 +12892,8 @@
       <c r="S101" s="26"/>
     </row>
     <row r="102" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="190"/>
-      <c r="B102" s="182"/>
+      <c r="A102" s="204"/>
+      <c r="B102" s="177"/>
       <c r="C102" s="60" t="s">
         <v>697</v>
       </c>
@@ -12937,8 +12937,8 @@
       <c r="S102" s="26"/>
     </row>
     <row r="103" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="190"/>
-      <c r="B103" s="182"/>
+      <c r="A103" s="204"/>
+      <c r="B103" s="177"/>
       <c r="C103" s="60" t="s">
         <v>230</v>
       </c>
@@ -12980,8 +12980,8 @@
       <c r="S103" s="26"/>
     </row>
     <row r="104" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="190"/>
-      <c r="B104" s="182"/>
+      <c r="A104" s="204"/>
+      <c r="B104" s="177"/>
       <c r="C104" s="60" t="s">
         <v>221</v>
       </c>
@@ -13027,8 +13027,8 @@
       <c r="S104" s="26"/>
     </row>
     <row r="105" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="190"/>
-      <c r="B105" s="182"/>
+      <c r="A105" s="204"/>
+      <c r="B105" s="177"/>
       <c r="C105" s="65" t="s">
         <v>216</v>
       </c>
@@ -13074,8 +13074,8 @@
       <c r="S105" s="26"/>
     </row>
     <row r="106" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="190"/>
-      <c r="B106" s="182"/>
+      <c r="A106" s="204"/>
+      <c r="B106" s="177"/>
       <c r="C106" s="60" t="s">
         <v>213</v>
       </c>
@@ -13121,8 +13121,8 @@
       <c r="S106" s="26"/>
     </row>
     <row r="107" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="190"/>
-      <c r="B107" s="182"/>
+      <c r="A107" s="204"/>
+      <c r="B107" s="177"/>
       <c r="C107" s="60" t="s">
         <v>214</v>
       </c>
@@ -13168,8 +13168,8 @@
       <c r="S107" s="26"/>
     </row>
     <row r="108" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="190"/>
-      <c r="B108" s="182"/>
+      <c r="A108" s="204"/>
+      <c r="B108" s="177"/>
       <c r="C108" s="60" t="s">
         <v>357</v>
       </c>
@@ -13215,8 +13215,8 @@
       <c r="S108" s="26"/>
     </row>
     <row r="109" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="190"/>
-      <c r="B109" s="182"/>
+      <c r="A109" s="204"/>
+      <c r="B109" s="177"/>
       <c r="C109" s="60" t="s">
         <v>229</v>
       </c>
@@ -13262,8 +13262,8 @@
       <c r="S109" s="26"/>
     </row>
     <row r="110" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="190"/>
-      <c r="B110" s="182"/>
+      <c r="A110" s="204"/>
+      <c r="B110" s="177"/>
       <c r="C110" s="60" t="s">
         <v>205</v>
       </c>
@@ -13309,8 +13309,8 @@
       <c r="S110" s="26"/>
     </row>
     <row r="111" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="190"/>
-      <c r="B111" s="182"/>
+      <c r="A111" s="204"/>
+      <c r="B111" s="177"/>
       <c r="C111" s="60" t="s">
         <v>206</v>
       </c>
@@ -13356,8 +13356,8 @@
       <c r="S111" s="26"/>
     </row>
     <row r="112" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="190"/>
-      <c r="B112" s="182"/>
+      <c r="A112" s="204"/>
+      <c r="B112" s="177"/>
       <c r="C112" s="60" t="s">
         <v>499</v>
       </c>
@@ -13403,8 +13403,8 @@
       <c r="S112" s="26"/>
     </row>
     <row r="113" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="190"/>
-      <c r="B113" s="182"/>
+      <c r="A113" s="204"/>
+      <c r="B113" s="177"/>
       <c r="C113" s="60" t="s">
         <v>246</v>
       </c>
@@ -13450,8 +13450,8 @@
       <c r="S113" s="26"/>
     </row>
     <row r="114" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="190"/>
-      <c r="B114" s="182"/>
+      <c r="A114" s="204"/>
+      <c r="B114" s="177"/>
       <c r="C114" s="60" t="s">
         <v>249</v>
       </c>
@@ -13495,8 +13495,8 @@
       <c r="S114" s="26"/>
     </row>
     <row r="115" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="190"/>
-      <c r="B115" s="182"/>
+      <c r="A115" s="204"/>
+      <c r="B115" s="177"/>
       <c r="C115" s="60" t="s">
         <v>226</v>
       </c>
@@ -13544,8 +13544,8 @@
       <c r="S115" s="26"/>
     </row>
     <row r="116" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="190"/>
-      <c r="B116" s="182"/>
+      <c r="A116" s="204"/>
+      <c r="B116" s="177"/>
       <c r="C116" s="60" t="s">
         <v>227</v>
       </c>
@@ -13593,8 +13593,8 @@
       <c r="S116" s="26"/>
     </row>
     <row r="117" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="190"/>
-      <c r="B117" s="182"/>
+      <c r="A117" s="204"/>
+      <c r="B117" s="177"/>
       <c r="C117" s="65" t="s">
         <v>595</v>
       </c>
@@ -13621,8 +13621,8 @@
       <c r="T117" s="23"/>
     </row>
     <row r="118" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="190"/>
-      <c r="B118" s="182"/>
+      <c r="A118" s="204"/>
+      <c r="B118" s="177"/>
       <c r="C118" s="60" t="s">
         <v>323</v>
       </c>
@@ -13669,8 +13669,8 @@
       <c r="T118" s="23"/>
     </row>
     <row r="119" spans="1:20" s="33" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="191"/>
-      <c r="B119" s="187"/>
+      <c r="A119" s="205"/>
+      <c r="B119" s="178"/>
       <c r="C119" s="61" t="s">
         <v>316</v>
       </c>
@@ -13723,10 +13723,10 @@
       <c r="T119" s="28"/>
     </row>
     <row r="120" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="183" t="s">
+      <c r="A120" s="198" t="s">
         <v>497</v>
       </c>
-      <c r="B120" s="174" t="s">
+      <c r="B120" s="184" t="s">
         <v>51</v>
       </c>
       <c r="C120" s="62" t="s">
@@ -13771,8 +13771,8 @@
       <c r="T120" s="33"/>
     </row>
     <row r="121" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="184"/>
-      <c r="B121" s="175"/>
+      <c r="A121" s="199"/>
+      <c r="B121" s="182"/>
       <c r="C121" s="60" t="s">
         <v>92</v>
       </c>
@@ -13818,8 +13818,8 @@
       <c r="S121" s="26"/>
     </row>
     <row r="122" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="184"/>
-      <c r="B122" s="175"/>
+      <c r="A122" s="199"/>
+      <c r="B122" s="182"/>
       <c r="C122" s="60" t="s">
         <v>93</v>
       </c>
@@ -13865,8 +13865,8 @@
       <c r="S122" s="26"/>
     </row>
     <row r="123" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="184"/>
-      <c r="B123" s="175"/>
+      <c r="A123" s="199"/>
+      <c r="B123" s="182"/>
       <c r="C123" s="60" t="s">
         <v>104</v>
       </c>
@@ -13908,8 +13908,8 @@
       <c r="S123" s="26"/>
     </row>
     <row r="124" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="184"/>
-      <c r="B124" s="175"/>
+      <c r="A124" s="199"/>
+      <c r="B124" s="182"/>
       <c r="C124" s="61" t="s">
         <v>94</v>
       </c>
@@ -13952,8 +13952,8 @@
       <c r="T124" s="28"/>
     </row>
     <row r="125" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="184"/>
-      <c r="B125" s="175"/>
+      <c r="A125" s="199"/>
+      <c r="B125" s="182"/>
       <c r="C125" s="60" t="s">
         <v>179</v>
       </c>
@@ -13996,8 +13996,8 @@
       <c r="T125" s="28"/>
     </row>
     <row r="126" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="184"/>
-      <c r="B126" s="175"/>
+      <c r="A126" s="199"/>
+      <c r="B126" s="182"/>
       <c r="C126" s="61" t="s">
         <v>116</v>
       </c>
@@ -14040,8 +14040,8 @@
       <c r="T126" s="28"/>
     </row>
     <row r="127" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="184"/>
-      <c r="B127" s="175"/>
+      <c r="A127" s="199"/>
+      <c r="B127" s="182"/>
       <c r="C127" s="60" t="s">
         <v>96</v>
       </c>
@@ -14085,8 +14085,8 @@
       <c r="S127" s="26"/>
     </row>
     <row r="128" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="184"/>
-      <c r="B128" s="175"/>
+      <c r="A128" s="199"/>
+      <c r="B128" s="182"/>
       <c r="C128" s="60" t="s">
         <v>498</v>
       </c>
@@ -14130,8 +14130,8 @@
       <c r="S128" s="26"/>
     </row>
     <row r="129" spans="1:20" s="23" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="184"/>
-      <c r="B129" s="186"/>
+      <c r="A129" s="199"/>
+      <c r="B129" s="201"/>
       <c r="C129" s="60" t="s">
         <v>176</v>
       </c>
@@ -14173,8 +14173,8 @@
       <c r="S129" s="26"/>
     </row>
     <row r="130" spans="1:20" s="28" customFormat="1" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="184"/>
-      <c r="B130" s="181" t="s">
+      <c r="A130" s="199"/>
+      <c r="B130" s="187" t="s">
         <v>193</v>
       </c>
       <c r="C130" s="63" t="s">
@@ -14221,8 +14221,8 @@
       <c r="T130" s="23"/>
     </row>
     <row r="131" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="184"/>
-      <c r="B131" s="182"/>
+      <c r="A131" s="199"/>
+      <c r="B131" s="177"/>
       <c r="C131" s="60" t="s">
         <v>445</v>
       </c>
@@ -14265,8 +14265,8 @@
       <c r="T131" s="23"/>
     </row>
     <row r="132" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="184"/>
-      <c r="B132" s="182"/>
+      <c r="A132" s="199"/>
+      <c r="B132" s="177"/>
       <c r="C132" s="60" t="s">
         <v>448</v>
       </c>
@@ -14309,8 +14309,8 @@
       <c r="T132" s="23"/>
     </row>
     <row r="133" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="184"/>
-      <c r="B133" s="182"/>
+      <c r="A133" s="199"/>
+      <c r="B133" s="177"/>
       <c r="C133" s="61" t="s">
         <v>422</v>
       </c>
@@ -14355,8 +14355,8 @@
       <c r="T133" s="23"/>
     </row>
     <row r="134" spans="1:20" s="33" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="184"/>
-      <c r="B134" s="182"/>
+      <c r="A134" s="199"/>
+      <c r="B134" s="177"/>
       <c r="C134" s="60" t="s">
         <v>228</v>
       </c>
@@ -14399,8 +14399,8 @@
       <c r="T134" s="23"/>
     </row>
     <row r="135" spans="1:20" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="184"/>
-      <c r="B135" s="182"/>
+      <c r="A135" s="199"/>
+      <c r="B135" s="177"/>
       <c r="C135" s="60" t="s">
         <v>207</v>
       </c>
@@ -14443,8 +14443,8 @@
       <c r="T135" s="23"/>
     </row>
     <row r="136" spans="1:20" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="185"/>
-      <c r="B136" s="182"/>
+      <c r="A136" s="200"/>
+      <c r="B136" s="177"/>
       <c r="C136" s="65" t="s">
         <v>621</v>
       </c>
@@ -14467,10 +14467,10 @@
       <c r="T136" s="23"/>
     </row>
     <row r="137" spans="1:20" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="178" t="s">
+      <c r="A137" s="195" t="s">
         <v>111</v>
       </c>
-      <c r="B137" s="174" t="s">
+      <c r="B137" s="184" t="s">
         <v>51</v>
       </c>
       <c r="C137" s="62" t="s">
@@ -14513,8 +14513,8 @@
       <c r="T137" s="33"/>
     </row>
     <row r="138" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="179"/>
-      <c r="B138" s="175"/>
+      <c r="A138" s="196"/>
+      <c r="B138" s="182"/>
       <c r="C138" s="61" t="s">
         <v>95</v>
       </c>
@@ -14554,8 +14554,8 @@
       <c r="S138" s="31"/>
     </row>
     <row r="139" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="179"/>
-      <c r="B139" s="175"/>
+      <c r="A139" s="196"/>
+      <c r="B139" s="182"/>
       <c r="C139" s="65" t="s">
         <v>599</v>
       </c>
@@ -14598,8 +14598,8 @@
       <c r="T139" s="19"/>
     </row>
     <row r="140" spans="1:20" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="179"/>
-      <c r="B140" s="175"/>
+      <c r="A140" s="196"/>
+      <c r="B140" s="182"/>
       <c r="C140" s="60" t="s">
         <v>115</v>
       </c>
@@ -14641,8 +14641,8 @@
       <c r="T140" s="19"/>
     </row>
     <row r="141" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="179"/>
-      <c r="B141" s="175"/>
+      <c r="A141" s="196"/>
+      <c r="B141" s="182"/>
       <c r="C141" s="60" t="s">
         <v>114</v>
       </c>
@@ -14684,8 +14684,8 @@
       <c r="T141" s="19"/>
     </row>
     <row r="142" spans="1:20" s="23" customFormat="1" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="179"/>
-      <c r="B142" s="181" t="s">
+      <c r="A142" s="196"/>
+      <c r="B142" s="187" t="s">
         <v>193</v>
       </c>
       <c r="C142" s="63" t="s">
@@ -14727,8 +14727,8 @@
       <c r="S142" s="57"/>
     </row>
     <row r="143" spans="1:20" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="179"/>
-      <c r="B143" s="182"/>
+      <c r="A143" s="196"/>
+      <c r="B143" s="177"/>
       <c r="C143" s="60" t="s">
         <v>396</v>
       </c>
@@ -14767,8 +14767,8 @@
       <c r="S143" s="26"/>
     </row>
     <row r="144" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="179"/>
-      <c r="B144" s="182"/>
+      <c r="A144" s="196"/>
+      <c r="B144" s="177"/>
       <c r="C144" s="60" t="s">
         <v>253</v>
       </c>
@@ -14808,8 +14808,8 @@
       <c r="S144" s="26"/>
     </row>
     <row r="145" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="179"/>
-      <c r="B145" s="182"/>
+      <c r="A145" s="196"/>
+      <c r="B145" s="177"/>
       <c r="C145" s="65" t="s">
         <v>615</v>
       </c>
@@ -14843,8 +14843,8 @@
       <c r="S145" s="26"/>
     </row>
     <row r="146" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="179"/>
-      <c r="B146" s="182"/>
+      <c r="A146" s="196"/>
+      <c r="B146" s="177"/>
       <c r="C146" s="60" t="s">
         <v>419</v>
       </c>
@@ -14884,8 +14884,8 @@
       <c r="S146" s="26"/>
     </row>
     <row r="147" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="179"/>
-      <c r="B147" s="182"/>
+      <c r="A147" s="196"/>
+      <c r="B147" s="177"/>
       <c r="C147" s="60" t="s">
         <v>378</v>
       </c>
@@ -14923,8 +14923,8 @@
       <c r="S147" s="26"/>
     </row>
     <row r="148" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="179"/>
-      <c r="B148" s="182"/>
+      <c r="A148" s="196"/>
+      <c r="B148" s="177"/>
       <c r="C148" s="60" t="s">
         <v>436</v>
       </c>
@@ -14964,8 +14964,8 @@
       <c r="S148" s="26"/>
     </row>
     <row r="149" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="179"/>
-      <c r="B149" s="182"/>
+      <c r="A149" s="196"/>
+      <c r="B149" s="177"/>
       <c r="C149" s="60" t="s">
         <v>356</v>
       </c>
@@ -15005,8 +15005,8 @@
       <c r="S149" s="26"/>
     </row>
     <row r="150" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="179"/>
-      <c r="B150" s="182"/>
+      <c r="A150" s="196"/>
+      <c r="B150" s="177"/>
       <c r="C150" s="60" t="s">
         <v>224</v>
       </c>
@@ -15048,8 +15048,8 @@
       <c r="S150" s="26"/>
     </row>
     <row r="151" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="179"/>
-      <c r="B151" s="182"/>
+      <c r="A151" s="196"/>
+      <c r="B151" s="177"/>
       <c r="C151" s="60" t="s">
         <v>418</v>
       </c>
@@ -15089,8 +15089,8 @@
       <c r="S151" s="26"/>
     </row>
     <row r="152" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="179"/>
-      <c r="B152" s="182"/>
+      <c r="A152" s="196"/>
+      <c r="B152" s="177"/>
       <c r="C152" s="60" t="s">
         <v>393</v>
       </c>
@@ -15130,8 +15130,8 @@
       <c r="S152" s="26"/>
     </row>
     <row r="153" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="179"/>
-      <c r="B153" s="182"/>
+      <c r="A153" s="196"/>
+      <c r="B153" s="177"/>
       <c r="C153" s="60" t="s">
         <v>430</v>
       </c>
@@ -15171,8 +15171,8 @@
       <c r="S153" s="26"/>
     </row>
     <row r="154" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="179"/>
-      <c r="B154" s="182"/>
+      <c r="A154" s="196"/>
+      <c r="B154" s="177"/>
       <c r="C154" s="60" t="s">
         <v>403</v>
       </c>
@@ -15212,8 +15212,8 @@
       <c r="S154" s="26"/>
     </row>
     <row r="155" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="179"/>
-      <c r="B155" s="182"/>
+      <c r="A155" s="196"/>
+      <c r="B155" s="177"/>
       <c r="C155" s="65" t="s">
         <v>518</v>
       </c>
@@ -15255,8 +15255,8 @@
       <c r="S155" s="26"/>
     </row>
     <row r="156" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="179"/>
-      <c r="B156" s="182"/>
+      <c r="A156" s="196"/>
+      <c r="B156" s="177"/>
       <c r="C156" s="65" t="s">
         <v>254</v>
       </c>
@@ -15296,8 +15296,8 @@
       <c r="S156" s="26"/>
     </row>
     <row r="157" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="179"/>
-      <c r="B157" s="182"/>
+      <c r="A157" s="196"/>
+      <c r="B157" s="177"/>
       <c r="C157" s="65" t="s">
         <v>443</v>
       </c>
@@ -15337,8 +15337,8 @@
       <c r="S157" s="26"/>
     </row>
     <row r="158" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="179"/>
-      <c r="B158" s="182"/>
+      <c r="A158" s="196"/>
+      <c r="B158" s="177"/>
       <c r="C158" s="65" t="s">
         <v>432</v>
       </c>
@@ -15378,8 +15378,8 @@
       <c r="S158" s="26"/>
     </row>
     <row r="159" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="179"/>
-      <c r="B159" s="182"/>
+      <c r="A159" s="196"/>
+      <c r="B159" s="177"/>
       <c r="C159" s="65" t="s">
         <v>317</v>
       </c>
@@ -15421,8 +15421,8 @@
       <c r="S159" s="26"/>
     </row>
     <row r="160" spans="1:19" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="179"/>
-      <c r="B160" s="182"/>
+      <c r="A160" s="196"/>
+      <c r="B160" s="177"/>
       <c r="C160" s="65" t="s">
         <v>364</v>
       </c>
@@ -15464,8 +15464,8 @@
       <c r="S160" s="26"/>
     </row>
     <row r="161" spans="1:19" s="23" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A161" s="180"/>
-      <c r="B161" s="182"/>
+      <c r="A161" s="197"/>
+      <c r="B161" s="177"/>
       <c r="C161" s="65" t="s">
         <v>210</v>
       </c>
@@ -15505,10 +15505,10 @@
       <c r="S161" s="31"/>
     </row>
     <row r="162" spans="1:19" s="33" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A162" s="200" t="s">
+      <c r="A162" s="185" t="s">
         <v>112</v>
       </c>
-      <c r="B162" s="195" t="s">
+      <c r="B162" s="176" t="s">
         <v>193</v>
       </c>
       <c r="C162" s="62" t="s">
@@ -15554,8 +15554,8 @@
       <c r="S162" s="36"/>
     </row>
     <row r="163" spans="1:19" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A163" s="200"/>
-      <c r="B163" s="182"/>
+      <c r="A163" s="185"/>
+      <c r="B163" s="177"/>
       <c r="C163" s="60" t="s">
         <v>360</v>
       </c>
@@ -15597,8 +15597,8 @@
       <c r="S163" s="26"/>
     </row>
     <row r="164" spans="1:19" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A164" s="200"/>
-      <c r="B164" s="182"/>
+      <c r="A164" s="185"/>
+      <c r="B164" s="177"/>
       <c r="C164" s="60" t="s">
         <v>379</v>
       </c>
@@ -15642,8 +15642,8 @@
       <c r="S164" s="26"/>
     </row>
     <row r="165" spans="1:19" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A165" s="200"/>
-      <c r="B165" s="182"/>
+      <c r="A165" s="185"/>
+      <c r="B165" s="177"/>
       <c r="C165" s="60" t="s">
         <v>389</v>
       </c>
@@ -15687,8 +15687,8 @@
       <c r="S165" s="26"/>
     </row>
     <row r="166" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A166" s="200"/>
-      <c r="B166" s="182"/>
+      <c r="A166" s="185"/>
+      <c r="B166" s="177"/>
       <c r="C166" s="60" t="s">
         <v>248</v>
       </c>
@@ -15730,8 +15730,8 @@
       <c r="S166" s="26"/>
     </row>
     <row r="167" spans="1:19" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A167" s="200"/>
-      <c r="B167" s="182"/>
+      <c r="A167" s="185"/>
+      <c r="B167" s="177"/>
       <c r="C167" s="61" t="s">
         <v>398</v>
       </c>
@@ -15775,8 +15775,8 @@
       <c r="S167" s="26"/>
     </row>
     <row r="168" spans="1:19" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A168" s="200"/>
-      <c r="B168" s="182"/>
+      <c r="A168" s="185"/>
+      <c r="B168" s="177"/>
       <c r="C168" s="60" t="s">
         <v>370</v>
       </c>
@@ -15818,8 +15818,8 @@
       <c r="S168" s="26"/>
     </row>
     <row r="169" spans="1:19" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="200"/>
-      <c r="B169" s="187"/>
+      <c r="A169" s="185"/>
+      <c r="B169" s="178"/>
       <c r="C169" s="60" t="s">
         <v>399</v>
       </c>
@@ -15861,7 +15861,7 @@
       <c r="S169" s="31"/>
     </row>
     <row r="170" spans="1:19" s="33" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A170" s="201" t="s">
+      <c r="A170" s="186" t="s">
         <v>532</v>
       </c>
       <c r="B170" s="72" t="s">
@@ -15904,8 +15904,8 @@
       <c r="S170" s="71"/>
     </row>
     <row r="171" spans="1:19" s="23" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A171" s="201"/>
-      <c r="B171" s="181" t="s">
+      <c r="A171" s="186"/>
+      <c r="B171" s="187" t="s">
         <v>193</v>
       </c>
       <c r="C171" s="60" t="s">
@@ -15943,8 +15943,8 @@
       <c r="S171" s="57"/>
     </row>
     <row r="172" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A172" s="201"/>
-      <c r="B172" s="182"/>
+      <c r="A172" s="186"/>
+      <c r="B172" s="177"/>
       <c r="C172" s="60" t="s">
         <v>195</v>
       </c>
@@ -15979,8 +15979,8 @@
       <c r="S172" s="26"/>
     </row>
     <row r="173" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A173" s="201"/>
-      <c r="B173" s="182"/>
+      <c r="A173" s="186"/>
+      <c r="B173" s="177"/>
       <c r="C173" s="60" t="s">
         <v>257</v>
       </c>
@@ -16020,8 +16020,8 @@
       <c r="S173" s="26"/>
     </row>
     <row r="174" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A174" s="201"/>
-      <c r="B174" s="182"/>
+      <c r="A174" s="186"/>
+      <c r="B174" s="177"/>
       <c r="C174" s="60" t="s">
         <v>414</v>
       </c>
@@ -16058,8 +16058,8 @@
       <c r="S174" s="26"/>
     </row>
     <row r="175" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A175" s="201"/>
-      <c r="B175" s="202"/>
+      <c r="A175" s="186"/>
+      <c r="B175" s="188"/>
       <c r="C175" s="60" t="s">
         <v>415</v>
       </c>
@@ -16097,10 +16097,10 @@
       <c r="S175" s="26"/>
     </row>
     <row r="176" spans="1:19" s="33" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A176" s="194" t="s">
+      <c r="A176" s="175" t="s">
         <v>113</v>
       </c>
-      <c r="B176" s="198" t="s">
+      <c r="B176" s="181" t="s">
         <v>51</v>
       </c>
       <c r="C176" s="62" t="s">
@@ -16140,8 +16140,8 @@
       <c r="S176" s="36"/>
     </row>
     <row r="177" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A177" s="194"/>
-      <c r="B177" s="175"/>
+      <c r="A177" s="175"/>
+      <c r="B177" s="182"/>
       <c r="C177" s="60" t="s">
         <v>184</v>
       </c>
@@ -16179,8 +16179,8 @@
       <c r="S177" s="26"/>
     </row>
     <row r="178" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A178" s="194"/>
-      <c r="B178" s="175"/>
+      <c r="A178" s="175"/>
+      <c r="B178" s="182"/>
       <c r="C178" s="60" t="s">
         <v>183</v>
       </c>
@@ -16218,8 +16218,8 @@
       <c r="S178" s="26"/>
     </row>
     <row r="179" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A179" s="194"/>
-      <c r="B179" s="175"/>
+      <c r="A179" s="175"/>
+      <c r="B179" s="182"/>
       <c r="C179" s="61" t="s">
         <v>185</v>
       </c>
@@ -16257,8 +16257,8 @@
       <c r="S179" s="31"/>
     </row>
     <row r="180" spans="1:19" s="23" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A180" s="194"/>
-      <c r="B180" s="192" t="s">
+      <c r="A180" s="175"/>
+      <c r="B180" s="173" t="s">
         <v>193</v>
       </c>
       <c r="C180" s="63" t="s">
@@ -16292,8 +16292,8 @@
       <c r="S180" s="57"/>
     </row>
     <row r="181" spans="1:19" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A181" s="194"/>
-      <c r="B181" s="193"/>
+      <c r="A181" s="175"/>
+      <c r="B181" s="174"/>
       <c r="C181" s="64"/>
       <c r="E181" s="49"/>
       <c r="F181" s="49"/>
@@ -17022,6 +17022,18 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="C3:S3"/>
+    <mergeCell ref="B53:B57"/>
+    <mergeCell ref="A53:A71"/>
+    <mergeCell ref="A137:A161"/>
+    <mergeCell ref="B142:B161"/>
+    <mergeCell ref="A120:A136"/>
+    <mergeCell ref="B120:B129"/>
+    <mergeCell ref="B83:B119"/>
+    <mergeCell ref="B58:B71"/>
+    <mergeCell ref="B72:B82"/>
+    <mergeCell ref="A72:A119"/>
+    <mergeCell ref="B137:B141"/>
     <mergeCell ref="B180:B181"/>
     <mergeCell ref="A176:A181"/>
     <mergeCell ref="B162:B169"/>
@@ -17037,18 +17049,6 @@
     <mergeCell ref="B130:B136"/>
     <mergeCell ref="A39:A52"/>
     <mergeCell ref="B43:B52"/>
-    <mergeCell ref="C3:S3"/>
-    <mergeCell ref="B53:B57"/>
-    <mergeCell ref="A53:A71"/>
-    <mergeCell ref="A137:A161"/>
-    <mergeCell ref="B142:B161"/>
-    <mergeCell ref="A120:A136"/>
-    <mergeCell ref="B120:B129"/>
-    <mergeCell ref="B83:B119"/>
-    <mergeCell ref="B58:B71"/>
-    <mergeCell ref="B72:B82"/>
-    <mergeCell ref="A72:A119"/>
-    <mergeCell ref="B137:B141"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
kleinere CE Anpassungen und Infected AI Balancing. AI Patrolsettings angepasst. Einige Dateien entfernt.
</commit_message>
<xml_diff>
--- a/ressources/DayZ Mods.xlsx
+++ b/ressources/DayZ Mods.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\projects\Immersive-DayZ-Experience\ressources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Documents\DayZ_Server\Immersive-DayZ-Experience\ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0883FA1-159E-4A59-89F0-3B7AF0A8E242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F61D11D-8D2D-4539-A441-2418C5CD1DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1575" windowWidth="29040" windowHeight="15720" tabRatio="260" activeTab="1" xr2:uid="{FAEB3C3F-74B0-4C80-8C8B-4522341FA132}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="15345" tabRatio="260" activeTab="1" xr2:uid="{FAEB3C3F-74B0-4C80-8C8B-4522341FA132}"/>
   </bookViews>
   <sheets>
     <sheet name="Mods" sheetId="1" r:id="rId1"/>
@@ -4104,65 +4104,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -4179,6 +4128,12 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -4191,6 +4146,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -4201,6 +4159,48 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
@@ -8237,18 +8237,18 @@
     <sortCondition ref="B2:B98"/>
   </sortState>
   <mergeCells count="12">
+    <mergeCell ref="A48:A52"/>
+    <mergeCell ref="A57:A71"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="A21:A40"/>
+    <mergeCell ref="A53:A56"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A7:A10"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="A41:A44"/>
     <mergeCell ref="A11:A15"/>
-    <mergeCell ref="A48:A52"/>
-    <mergeCell ref="A57:A71"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="A21:A40"/>
-    <mergeCell ref="A53:A56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8259,8 +8259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FF4763-6B65-4CE2-BD87-511E98A2E639}">
   <dimension ref="A1:V229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E105" sqref="E105"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M80" activeCellId="1" sqref="I83 M80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8292,25 +8292,25 @@
       <c r="S2"/>
     </row>
     <row r="3" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="192" t="s">
+      <c r="C3" s="173" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="192"/>
-      <c r="E3" s="192"/>
-      <c r="F3" s="192"/>
-      <c r="G3" s="192"/>
-      <c r="H3" s="192"/>
-      <c r="I3" s="192"/>
-      <c r="J3" s="192"/>
-      <c r="K3" s="192"/>
-      <c r="L3" s="192"/>
-      <c r="M3" s="192"/>
-      <c r="N3" s="192"/>
-      <c r="O3" s="192"/>
-      <c r="P3" s="192"/>
-      <c r="Q3" s="192"/>
-      <c r="R3" s="192"/>
-      <c r="S3" s="192"/>
+      <c r="D3" s="173"/>
+      <c r="E3" s="173"/>
+      <c r="F3" s="173"/>
+      <c r="G3" s="173"/>
+      <c r="H3" s="173"/>
+      <c r="I3" s="173"/>
+      <c r="J3" s="173"/>
+      <c r="K3" s="173"/>
+      <c r="L3" s="173"/>
+      <c r="M3" s="173"/>
+      <c r="N3" s="173"/>
+      <c r="O3" s="173"/>
+      <c r="P3" s="173"/>
+      <c r="Q3" s="173"/>
+      <c r="R3" s="173"/>
+      <c r="S3" s="173"/>
     </row>
     <row r="4" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
@@ -8325,19 +8325,19 @@
       <c r="F4" s="3" t="s">
         <v>642</v>
       </c>
-      <c r="G4" s="180"/>
-      <c r="H4" s="180"/>
-      <c r="I4" s="180"/>
-      <c r="J4" s="180"/>
-      <c r="K4" s="180"/>
-      <c r="L4" s="180"/>
-      <c r="M4" s="180"/>
-      <c r="N4" s="180"/>
-      <c r="O4" s="180"/>
-      <c r="P4" s="180"/>
-      <c r="Q4" s="180"/>
-      <c r="R4" s="180"/>
-      <c r="S4" s="180"/>
+      <c r="G4" s="197"/>
+      <c r="H4" s="197"/>
+      <c r="I4" s="197"/>
+      <c r="J4" s="197"/>
+      <c r="K4" s="197"/>
+      <c r="L4" s="197"/>
+      <c r="M4" s="197"/>
+      <c r="N4" s="197"/>
+      <c r="O4" s="197"/>
+      <c r="P4" s="197"/>
+      <c r="Q4" s="197"/>
+      <c r="R4" s="197"/>
+      <c r="S4" s="197"/>
     </row>
     <row r="5" spans="1:22" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="3"/>
@@ -8388,10 +8388,10 @@
       </c>
     </row>
     <row r="6" spans="1:22" s="23" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="179" t="s">
+      <c r="A6" s="196" t="s">
         <v>88</v>
       </c>
-      <c r="B6" s="181" t="s">
+      <c r="B6" s="198" t="s">
         <v>51</v>
       </c>
       <c r="C6" s="18" t="s">
@@ -8453,8 +8453,8 @@
       </c>
     </row>
     <row r="7" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="179"/>
-      <c r="B7" s="182"/>
+      <c r="A7" s="196"/>
+      <c r="B7" s="175"/>
       <c r="C7" s="60" t="s">
         <v>42</v>
       </c>
@@ -8505,8 +8505,8 @@
       </c>
     </row>
     <row r="8" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="179"/>
-      <c r="B8" s="182"/>
+      <c r="A8" s="196"/>
+      <c r="B8" s="175"/>
       <c r="C8" s="60" t="s">
         <v>49</v>
       </c>
@@ -8555,8 +8555,8 @@
       </c>
     </row>
     <row r="9" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="179"/>
-      <c r="B9" s="182"/>
+      <c r="A9" s="196"/>
+      <c r="B9" s="175"/>
       <c r="C9" s="60" t="s">
         <v>281</v>
       </c>
@@ -8607,8 +8607,8 @@
       </c>
     </row>
     <row r="10" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="179"/>
-      <c r="B10" s="182"/>
+      <c r="A10" s="196"/>
+      <c r="B10" s="175"/>
       <c r="C10" s="60" t="s">
         <v>43</v>
       </c>
@@ -8657,8 +8657,8 @@
       </c>
     </row>
     <row r="11" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="179"/>
-      <c r="B11" s="182"/>
+      <c r="A11" s="196"/>
+      <c r="B11" s="175"/>
       <c r="C11" s="60" t="s">
         <v>59</v>
       </c>
@@ -8709,8 +8709,8 @@
       </c>
     </row>
     <row r="12" spans="1:22" s="23" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="179"/>
-      <c r="B12" s="182"/>
+      <c r="A12" s="196"/>
+      <c r="B12" s="175"/>
       <c r="C12" s="60" t="s">
         <v>44</v>
       </c>
@@ -8756,8 +8756,8 @@
       <c r="S12" s="26"/>
     </row>
     <row r="13" spans="1:22" s="23" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="179"/>
-      <c r="B13" s="182"/>
+      <c r="A13" s="196"/>
+      <c r="B13" s="175"/>
       <c r="C13" s="60" t="s">
         <v>634</v>
       </c>
@@ -8791,8 +8791,8 @@
       <c r="S13" s="26"/>
     </row>
     <row r="14" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="179"/>
-      <c r="B14" s="182"/>
+      <c r="A14" s="196"/>
+      <c r="B14" s="175"/>
       <c r="C14" s="60" t="s">
         <v>45</v>
       </c>
@@ -8838,8 +8838,8 @@
       <c r="S14" s="26"/>
     </row>
     <row r="15" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="179"/>
-      <c r="B15" s="182"/>
+      <c r="A15" s="196"/>
+      <c r="B15" s="175"/>
       <c r="C15" s="60" t="s">
         <v>74</v>
       </c>
@@ -8885,8 +8885,8 @@
       <c r="S15" s="26"/>
     </row>
     <row r="16" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="179"/>
-      <c r="B16" s="182"/>
+      <c r="A16" s="196"/>
+      <c r="B16" s="175"/>
       <c r="C16" s="60" t="s">
         <v>46</v>
       </c>
@@ -8930,8 +8930,8 @@
       <c r="S16" s="26"/>
     </row>
     <row r="17" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="179"/>
-      <c r="B17" s="182"/>
+      <c r="A17" s="196"/>
+      <c r="B17" s="175"/>
       <c r="C17" s="60" t="s">
         <v>47</v>
       </c>
@@ -8975,8 +8975,8 @@
       <c r="S17" s="26"/>
     </row>
     <row r="18" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="179"/>
-      <c r="B18" s="182"/>
+      <c r="A18" s="196"/>
+      <c r="B18" s="175"/>
       <c r="C18" s="60" t="s">
         <v>48</v>
       </c>
@@ -9020,8 +9020,8 @@
       <c r="S18" s="26"/>
     </row>
     <row r="19" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="179"/>
-      <c r="B19" s="182"/>
+      <c r="A19" s="196"/>
+      <c r="B19" s="175"/>
       <c r="C19" s="60" t="s">
         <v>344</v>
       </c>
@@ -9067,8 +9067,8 @@
       <c r="S19" s="26"/>
     </row>
     <row r="20" spans="1:20" s="40" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="179"/>
-      <c r="B20" s="183"/>
+      <c r="A20" s="196"/>
+      <c r="B20" s="199"/>
       <c r="C20" s="61" t="s">
         <v>50</v>
       </c>
@@ -9110,8 +9110,8 @@
       <c r="S20" s="31"/>
     </row>
     <row r="21" spans="1:20" s="33" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="179"/>
-      <c r="B21" s="176" t="s">
+      <c r="A21" s="196"/>
+      <c r="B21" s="195" t="s">
         <v>244</v>
       </c>
       <c r="C21" s="117" t="s">
@@ -9162,8 +9162,8 @@
       </c>
     </row>
     <row r="22" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="179"/>
-      <c r="B22" s="177"/>
+      <c r="A22" s="196"/>
+      <c r="B22" s="182"/>
       <c r="C22" s="61" t="s">
         <v>231</v>
       </c>
@@ -9209,8 +9209,8 @@
       <c r="S22" s="26"/>
     </row>
     <row r="23" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="179"/>
-      <c r="B23" s="177"/>
+      <c r="A23" s="196"/>
+      <c r="B23" s="182"/>
       <c r="C23" s="60" t="s">
         <v>45</v>
       </c>
@@ -9254,8 +9254,8 @@
       <c r="S23" s="26"/>
     </row>
     <row r="24" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="179"/>
-      <c r="B24" s="177"/>
+      <c r="A24" s="196"/>
+      <c r="B24" s="182"/>
       <c r="C24" s="60" t="s">
         <v>120</v>
       </c>
@@ -9303,8 +9303,8 @@
       <c r="S24" s="26"/>
     </row>
     <row r="25" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="179"/>
-      <c r="B25" s="177"/>
+      <c r="A25" s="196"/>
+      <c r="B25" s="182"/>
       <c r="C25" s="60" t="s">
         <v>233</v>
       </c>
@@ -9354,8 +9354,8 @@
       <c r="S25" s="26"/>
     </row>
     <row r="26" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="179"/>
-      <c r="B26" s="177"/>
+      <c r="A26" s="196"/>
+      <c r="B26" s="182"/>
       <c r="C26" s="60" t="s">
         <v>348</v>
       </c>
@@ -9401,8 +9401,8 @@
       <c r="S26" s="26"/>
     </row>
     <row r="27" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="179"/>
-      <c r="B27" s="177"/>
+      <c r="A27" s="196"/>
+      <c r="B27" s="182"/>
       <c r="C27" s="60" t="s">
         <v>119</v>
       </c>
@@ -9448,8 +9448,8 @@
       <c r="S27" s="26"/>
     </row>
     <row r="28" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="179"/>
-      <c r="B28" s="177"/>
+      <c r="A28" s="196"/>
+      <c r="B28" s="182"/>
       <c r="C28" s="60" t="s">
         <v>462</v>
       </c>
@@ -9495,8 +9495,8 @@
       <c r="S28" s="26"/>
     </row>
     <row r="29" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="179"/>
-      <c r="B29" s="177"/>
+      <c r="A29" s="196"/>
+      <c r="B29" s="182"/>
       <c r="C29" s="60" t="s">
         <v>383</v>
       </c>
@@ -9542,8 +9542,8 @@
       <c r="S29" s="26"/>
     </row>
     <row r="30" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="179"/>
-      <c r="B30" s="177"/>
+      <c r="A30" s="196"/>
+      <c r="B30" s="182"/>
       <c r="C30" s="60" t="s">
         <v>236</v>
       </c>
@@ -9590,8 +9590,8 @@
       <c r="T30" s="23"/>
     </row>
     <row r="31" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="179"/>
-      <c r="B31" s="177"/>
+      <c r="A31" s="196"/>
+      <c r="B31" s="182"/>
       <c r="C31" s="60" t="s">
         <v>349</v>
       </c>
@@ -9637,8 +9637,8 @@
       <c r="S31" s="26"/>
     </row>
     <row r="32" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="179"/>
-      <c r="B32" s="177"/>
+      <c r="A32" s="196"/>
+      <c r="B32" s="182"/>
       <c r="C32" s="60" t="s">
         <v>349</v>
       </c>
@@ -9684,8 +9684,8 @@
       <c r="S32" s="26"/>
     </row>
     <row r="33" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="179"/>
-      <c r="B33" s="177"/>
+      <c r="A33" s="196"/>
+      <c r="B33" s="182"/>
       <c r="C33" s="60" t="s">
         <v>215</v>
       </c>
@@ -9732,8 +9732,8 @@
       <c r="T33" s="23"/>
     </row>
     <row r="34" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="179"/>
-      <c r="B34" s="177"/>
+      <c r="A34" s="196"/>
+      <c r="B34" s="182"/>
       <c r="C34" s="60" t="s">
         <v>240</v>
       </c>
@@ -9779,8 +9779,8 @@
       <c r="S34" s="26"/>
     </row>
     <row r="35" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="179"/>
-      <c r="B35" s="177"/>
+      <c r="A35" s="196"/>
+      <c r="B35" s="182"/>
       <c r="C35" s="60" t="s">
         <v>373</v>
       </c>
@@ -9824,8 +9824,8 @@
       <c r="S35" s="26"/>
     </row>
     <row r="36" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="179"/>
-      <c r="B36" s="177"/>
+      <c r="A36" s="196"/>
+      <c r="B36" s="182"/>
       <c r="C36" s="60" t="s">
         <v>688</v>
       </c>
@@ -9857,8 +9857,8 @@
       <c r="S36" s="26"/>
     </row>
     <row r="37" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="179"/>
-      <c r="B37" s="177"/>
+      <c r="A37" s="196"/>
+      <c r="B37" s="182"/>
       <c r="C37" s="60" t="s">
         <v>385</v>
       </c>
@@ -9904,8 +9904,8 @@
       <c r="S37" s="26"/>
     </row>
     <row r="38" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="179"/>
-      <c r="B38" s="178"/>
+      <c r="A38" s="196"/>
+      <c r="B38" s="187"/>
       <c r="C38" s="65" t="s">
         <v>232</v>
       </c>
@@ -9951,10 +9951,10 @@
       <c r="S38" s="26"/>
     </row>
     <row r="39" spans="1:20" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="189" t="s">
+      <c r="A39" s="203" t="s">
         <v>264</v>
       </c>
-      <c r="B39" s="184" t="s">
+      <c r="B39" s="174" t="s">
         <v>51</v>
       </c>
       <c r="C39" s="62" t="s">
@@ -9999,8 +9999,8 @@
       <c r="T39" s="33"/>
     </row>
     <row r="40" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="190"/>
-      <c r="B40" s="182"/>
+      <c r="A40" s="204"/>
+      <c r="B40" s="175"/>
       <c r="C40" s="60" t="s">
         <v>107</v>
       </c>
@@ -10042,8 +10042,8 @@
       <c r="S40" s="26"/>
     </row>
     <row r="41" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="190"/>
-      <c r="B41" s="182"/>
+      <c r="A41" s="204"/>
+      <c r="B41" s="175"/>
       <c r="C41" s="60" t="s">
         <v>108</v>
       </c>
@@ -10086,8 +10086,8 @@
       <c r="T41" s="23"/>
     </row>
     <row r="42" spans="1:20" s="28" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="190"/>
-      <c r="B42" s="182"/>
+      <c r="A42" s="204"/>
+      <c r="B42" s="175"/>
       <c r="C42" s="61" t="s">
         <v>109</v>
       </c>
@@ -10135,8 +10135,8 @@
       <c r="S42" s="31"/>
     </row>
     <row r="43" spans="1:20" s="28" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="190"/>
-      <c r="B43" s="187" t="s">
+      <c r="A43" s="204"/>
+      <c r="B43" s="181" t="s">
         <v>193</v>
       </c>
       <c r="C43" s="63" t="s">
@@ -10184,8 +10184,8 @@
       <c r="S43" s="57"/>
     </row>
     <row r="44" spans="1:20" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="190"/>
-      <c r="B44" s="177"/>
+      <c r="A44" s="204"/>
+      <c r="B44" s="182"/>
       <c r="C44" s="60" t="s">
         <v>217</v>
       </c>
@@ -10227,8 +10227,8 @@
       <c r="S44" s="26"/>
     </row>
     <row r="45" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="190"/>
-      <c r="B45" s="177"/>
+      <c r="A45" s="204"/>
+      <c r="B45" s="182"/>
       <c r="C45" s="60" t="s">
         <v>256</v>
       </c>
@@ -10270,8 +10270,8 @@
       <c r="S45" s="26"/>
     </row>
     <row r="46" spans="1:20" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="190"/>
-      <c r="B46" s="177"/>
+      <c r="A46" s="204"/>
+      <c r="B46" s="182"/>
       <c r="C46" s="60" t="s">
         <v>218</v>
       </c>
@@ -10313,8 +10313,8 @@
       <c r="S46" s="26"/>
     </row>
     <row r="47" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="190"/>
-      <c r="B47" s="177"/>
+      <c r="A47" s="204"/>
+      <c r="B47" s="182"/>
       <c r="C47" s="60" t="s">
         <v>487</v>
       </c>
@@ -10361,8 +10361,8 @@
       <c r="T47" s="28"/>
     </row>
     <row r="48" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="190"/>
-      <c r="B48" s="177"/>
+      <c r="A48" s="204"/>
+      <c r="B48" s="182"/>
       <c r="C48" s="60" t="s">
         <v>410</v>
       </c>
@@ -10406,8 +10406,8 @@
       <c r="S48" s="26"/>
     </row>
     <row r="49" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="190"/>
-      <c r="B49" s="177"/>
+      <c r="A49" s="204"/>
+      <c r="B49" s="182"/>
       <c r="C49" s="60" t="s">
         <v>407</v>
       </c>
@@ -10451,8 +10451,8 @@
       <c r="S49" s="26"/>
     </row>
     <row r="50" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="190"/>
-      <c r="B50" s="177"/>
+      <c r="A50" s="204"/>
+      <c r="B50" s="182"/>
       <c r="C50" s="60" t="s">
         <v>405</v>
       </c>
@@ -10500,8 +10500,8 @@
       <c r="S50" s="26"/>
     </row>
     <row r="51" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="190"/>
-      <c r="B51" s="177"/>
+      <c r="A51" s="204"/>
+      <c r="B51" s="182"/>
       <c r="C51" s="60" t="s">
         <v>255</v>
       </c>
@@ -10547,8 +10547,8 @@
       <c r="S51" s="26"/>
     </row>
     <row r="52" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="191"/>
-      <c r="B52" s="178"/>
+      <c r="A52" s="205"/>
+      <c r="B52" s="187"/>
       <c r="C52" s="65" t="s">
         <v>528</v>
       </c>
@@ -10592,10 +10592,10 @@
       <c r="S52" s="26"/>
     </row>
     <row r="53" spans="1:20" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="193" t="s">
+      <c r="A53" s="176" t="s">
         <v>89</v>
       </c>
-      <c r="B53" s="184" t="s">
+      <c r="B53" s="174" t="s">
         <v>51</v>
       </c>
       <c r="C53" s="62" t="s">
@@ -10642,8 +10642,8 @@
       <c r="T53" s="33"/>
     </row>
     <row r="54" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="194"/>
-      <c r="B54" s="182"/>
+      <c r="A54" s="177"/>
+      <c r="B54" s="175"/>
       <c r="C54" s="60" t="s">
         <v>66</v>
       </c>
@@ -10689,8 +10689,8 @@
       <c r="S54" s="26"/>
     </row>
     <row r="55" spans="1:20" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="194"/>
-      <c r="B55" s="182"/>
+      <c r="A55" s="177"/>
+      <c r="B55" s="175"/>
       <c r="C55" s="60" t="s">
         <v>67</v>
       </c>
@@ -10736,8 +10736,8 @@
       <c r="S55" s="26"/>
     </row>
     <row r="56" spans="1:20" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="194"/>
-      <c r="B56" s="182"/>
+      <c r="A56" s="177"/>
+      <c r="B56" s="175"/>
       <c r="C56" s="61" t="s">
         <v>68</v>
       </c>
@@ -10783,8 +10783,8 @@
       <c r="S56" s="26"/>
     </row>
     <row r="57" spans="1:20" s="23" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="194"/>
-      <c r="B57" s="182"/>
+      <c r="A57" s="177"/>
+      <c r="B57" s="175"/>
       <c r="C57" s="65" t="s">
         <v>601</v>
       </c>
@@ -10828,8 +10828,8 @@
       <c r="S57" s="31"/>
     </row>
     <row r="58" spans="1:20" s="23" customFormat="1" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="194"/>
-      <c r="B58" s="187" t="s">
+      <c r="A58" s="177"/>
+      <c r="B58" s="181" t="s">
         <v>193</v>
       </c>
       <c r="C58" s="63" t="s">
@@ -10877,8 +10877,8 @@
       <c r="S58" s="57"/>
     </row>
     <row r="59" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="194"/>
-      <c r="B59" s="177"/>
+      <c r="A59" s="177"/>
+      <c r="B59" s="182"/>
       <c r="C59" s="60" t="s">
         <v>208</v>
       </c>
@@ -10926,8 +10926,8 @@
       <c r="S59" s="26"/>
     </row>
     <row r="60" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="194"/>
-      <c r="B60" s="177"/>
+      <c r="A60" s="177"/>
+      <c r="B60" s="182"/>
       <c r="C60" s="60" t="s">
         <v>202</v>
       </c>
@@ -10971,8 +10971,8 @@
       <c r="S60" s="26"/>
     </row>
     <row r="61" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="194"/>
-      <c r="B61" s="177"/>
+      <c r="A61" s="177"/>
+      <c r="B61" s="182"/>
       <c r="C61" s="60" t="s">
         <v>197</v>
       </c>
@@ -11018,8 +11018,8 @@
       <c r="S61" s="26"/>
     </row>
     <row r="62" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="194"/>
-      <c r="B62" s="177"/>
+      <c r="A62" s="177"/>
+      <c r="B62" s="182"/>
       <c r="C62" s="60" t="s">
         <v>198</v>
       </c>
@@ -11065,8 +11065,8 @@
       <c r="S62" s="26"/>
     </row>
     <row r="63" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="194"/>
-      <c r="B63" s="177"/>
+      <c r="A63" s="177"/>
+      <c r="B63" s="182"/>
       <c r="C63" s="60" t="s">
         <v>91</v>
       </c>
@@ -11112,8 +11112,8 @@
       <c r="S63" s="26"/>
     </row>
     <row r="64" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="194"/>
-      <c r="B64" s="177"/>
+      <c r="A64" s="177"/>
+      <c r="B64" s="182"/>
       <c r="C64" s="60" t="s">
         <v>412</v>
       </c>
@@ -11159,8 +11159,8 @@
       <c r="S64" s="26"/>
     </row>
     <row r="65" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="194"/>
-      <c r="B65" s="177"/>
+      <c r="A65" s="177"/>
+      <c r="B65" s="182"/>
       <c r="C65" s="60" t="s">
         <v>199</v>
       </c>
@@ -11208,8 +11208,8 @@
       <c r="S65" s="26"/>
     </row>
     <row r="66" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="194"/>
-      <c r="B66" s="177"/>
+      <c r="A66" s="177"/>
+      <c r="B66" s="182"/>
       <c r="C66" s="60" t="s">
         <v>426</v>
       </c>
@@ -11255,8 +11255,8 @@
       <c r="S66" s="26"/>
     </row>
     <row r="67" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="194"/>
-      <c r="B67" s="177"/>
+      <c r="A67" s="177"/>
+      <c r="B67" s="182"/>
       <c r="C67" s="60" t="s">
         <v>375</v>
       </c>
@@ -11303,8 +11303,8 @@
       <c r="T67" s="28"/>
     </row>
     <row r="68" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="194"/>
-      <c r="B68" s="177"/>
+      <c r="A68" s="177"/>
+      <c r="B68" s="182"/>
       <c r="C68" s="60" t="s">
         <v>391</v>
       </c>
@@ -11352,8 +11352,8 @@
       <c r="S68" s="26"/>
     </row>
     <row r="69" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="194"/>
-      <c r="B69" s="177"/>
+      <c r="A69" s="177"/>
+      <c r="B69" s="182"/>
       <c r="C69" s="60" t="s">
         <v>252</v>
       </c>
@@ -11402,8 +11402,8 @@
       <c r="T69" s="23"/>
     </row>
     <row r="70" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="194"/>
-      <c r="B70" s="177"/>
+      <c r="A70" s="177"/>
+      <c r="B70" s="182"/>
       <c r="C70" s="60" t="s">
         <v>429</v>
       </c>
@@ -11449,8 +11449,8 @@
       <c r="S70" s="26"/>
     </row>
     <row r="71" spans="1:20" s="33" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="194"/>
-      <c r="B71" s="177"/>
+      <c r="A71" s="177"/>
+      <c r="B71" s="182"/>
       <c r="C71" s="61" t="s">
         <v>203</v>
       </c>
@@ -11495,10 +11495,10 @@
       <c r="T71" s="28"/>
     </row>
     <row r="72" spans="1:20" s="23" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="203" t="s">
+      <c r="A72" s="189" t="s">
         <v>97</v>
       </c>
-      <c r="B72" s="202"/>
+      <c r="B72" s="188"/>
       <c r="C72" s="62" t="s">
         <v>79</v>
       </c>
@@ -11545,8 +11545,8 @@
       <c r="T72" s="33"/>
     </row>
     <row r="73" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="204"/>
-      <c r="B73" s="182"/>
+      <c r="A73" s="190"/>
+      <c r="B73" s="175"/>
       <c r="C73" s="60" t="s">
         <v>80</v>
       </c>
@@ -11592,8 +11592,8 @@
       <c r="S73" s="26"/>
     </row>
     <row r="74" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="204"/>
-      <c r="B74" s="182"/>
+      <c r="A74" s="190"/>
+      <c r="B74" s="175"/>
       <c r="C74" s="60" t="s">
         <v>81</v>
       </c>
@@ -11641,8 +11641,8 @@
       <c r="S74" s="26"/>
     </row>
     <row r="75" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="204"/>
-      <c r="B75" s="182"/>
+      <c r="A75" s="190"/>
+      <c r="B75" s="175"/>
       <c r="C75" s="60" t="s">
         <v>82</v>
       </c>
@@ -11688,8 +11688,8 @@
       <c r="S75" s="26"/>
     </row>
     <row r="76" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="204"/>
-      <c r="B76" s="182"/>
+      <c r="A76" s="190"/>
+      <c r="B76" s="175"/>
       <c r="C76" s="60" t="s">
         <v>83</v>
       </c>
@@ -11737,8 +11737,8 @@
       <c r="S76" s="26"/>
     </row>
     <row r="77" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="204"/>
-      <c r="B77" s="182"/>
+      <c r="A77" s="190"/>
+      <c r="B77" s="175"/>
       <c r="C77" s="60" t="s">
         <v>84</v>
       </c>
@@ -11784,8 +11784,8 @@
       <c r="S77" s="26"/>
     </row>
     <row r="78" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="204"/>
-      <c r="B78" s="182"/>
+      <c r="A78" s="190"/>
+      <c r="B78" s="175"/>
       <c r="C78" s="60" t="s">
         <v>85</v>
       </c>
@@ -11829,8 +11829,8 @@
       <c r="S78" s="26"/>
     </row>
     <row r="79" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="204"/>
-      <c r="B79" s="182"/>
+      <c r="A79" s="190"/>
+      <c r="B79" s="175"/>
       <c r="C79" s="60" t="s">
         <v>86</v>
       </c>
@@ -11876,8 +11876,8 @@
       <c r="S79" s="26"/>
     </row>
     <row r="80" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="204"/>
-      <c r="B80" s="182"/>
+      <c r="A80" s="190"/>
+      <c r="B80" s="175"/>
       <c r="C80" s="60" t="s">
         <v>87</v>
       </c>
@@ -11925,8 +11925,8 @@
       <c r="S80" s="26"/>
     </row>
     <row r="81" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="204"/>
-      <c r="B81" s="182"/>
+      <c r="A81" s="190"/>
+      <c r="B81" s="175"/>
       <c r="C81" s="60" t="s">
         <v>223</v>
       </c>
@@ -11972,8 +11972,8 @@
       <c r="S81" s="26"/>
     </row>
     <row r="82" spans="1:19" s="23" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="204"/>
-      <c r="B82" s="201"/>
+      <c r="A82" s="190"/>
+      <c r="B82" s="186"/>
       <c r="C82" s="61" t="s">
         <v>90</v>
       </c>
@@ -12019,8 +12019,8 @@
       <c r="S82" s="31"/>
     </row>
     <row r="83" spans="1:19" s="23" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="204"/>
-      <c r="B83" s="177" t="s">
+      <c r="A83" s="190"/>
+      <c r="B83" s="182" t="s">
         <v>193</v>
       </c>
       <c r="C83" s="63" t="s">
@@ -12042,7 +12042,7 @@
         <v>99</v>
       </c>
       <c r="I83" s="55" t="s">
-        <v>694</v>
+        <v>98</v>
       </c>
       <c r="J83" s="77">
         <v>5</v>
@@ -12068,8 +12068,8 @@
       <c r="S83" s="57"/>
     </row>
     <row r="84" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="204"/>
-      <c r="B84" s="177"/>
+      <c r="A84" s="190"/>
+      <c r="B84" s="182"/>
       <c r="C84" s="60" t="s">
         <v>212</v>
       </c>
@@ -12115,8 +12115,8 @@
       <c r="S84" s="26"/>
     </row>
     <row r="85" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="204"/>
-      <c r="B85" s="177"/>
+      <c r="A85" s="190"/>
+      <c r="B85" s="182"/>
       <c r="C85" s="60" t="s">
         <v>424</v>
       </c>
@@ -12160,8 +12160,8 @@
       <c r="S85" s="26"/>
     </row>
     <row r="86" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="204"/>
-      <c r="B86" s="177"/>
+      <c r="A86" s="190"/>
+      <c r="B86" s="182"/>
       <c r="C86" s="60" t="s">
         <v>293</v>
       </c>
@@ -12207,8 +12207,8 @@
       <c r="S86" s="26"/>
     </row>
     <row r="87" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="204"/>
-      <c r="B87" s="177"/>
+      <c r="A87" s="190"/>
+      <c r="B87" s="182"/>
       <c r="C87" s="60" t="s">
         <v>366</v>
       </c>
@@ -12254,8 +12254,8 @@
       <c r="S87" s="26"/>
     </row>
     <row r="88" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="204"/>
-      <c r="B88" s="177"/>
+      <c r="A88" s="190"/>
+      <c r="B88" s="182"/>
       <c r="C88" s="60" t="s">
         <v>219</v>
       </c>
@@ -12299,8 +12299,8 @@
       <c r="S88" s="26"/>
     </row>
     <row r="89" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="204"/>
-      <c r="B89" s="177"/>
+      <c r="A89" s="190"/>
+      <c r="B89" s="182"/>
       <c r="C89" s="60" t="s">
         <v>320</v>
       </c>
@@ -12346,8 +12346,8 @@
       <c r="S89" s="26"/>
     </row>
     <row r="90" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="204"/>
-      <c r="B90" s="177"/>
+      <c r="A90" s="190"/>
+      <c r="B90" s="182"/>
       <c r="C90" s="61" t="s">
         <v>247</v>
       </c>
@@ -12393,8 +12393,8 @@
       <c r="S90" s="26"/>
     </row>
     <row r="91" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="204"/>
-      <c r="B91" s="177"/>
+      <c r="A91" s="190"/>
+      <c r="B91" s="182"/>
       <c r="C91" s="60" t="s">
         <v>401</v>
       </c>
@@ -12440,8 +12440,8 @@
       <c r="S91" s="26"/>
     </row>
     <row r="92" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="204"/>
-      <c r="B92" s="177"/>
+      <c r="A92" s="190"/>
+      <c r="B92" s="182"/>
       <c r="C92" s="65" t="s">
         <v>692</v>
       </c>
@@ -12473,8 +12473,8 @@
       <c r="S92" s="26"/>
     </row>
     <row r="93" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="204"/>
-      <c r="B93" s="177"/>
+      <c r="A93" s="190"/>
+      <c r="B93" s="182"/>
       <c r="C93" s="60" t="s">
         <v>368</v>
       </c>
@@ -12518,8 +12518,8 @@
       <c r="S93" s="26"/>
     </row>
     <row r="94" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="204"/>
-      <c r="B94" s="177"/>
+      <c r="A94" s="190"/>
+      <c r="B94" s="182"/>
       <c r="C94" s="60" t="s">
         <v>355</v>
       </c>
@@ -12565,8 +12565,8 @@
       <c r="S94" s="26"/>
     </row>
     <row r="95" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="204"/>
-      <c r="B95" s="177"/>
+      <c r="A95" s="190"/>
+      <c r="B95" s="182"/>
       <c r="C95" s="60" t="s">
         <v>351</v>
       </c>
@@ -12612,8 +12612,8 @@
       <c r="S95" s="26"/>
     </row>
     <row r="96" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="204"/>
-      <c r="B96" s="177"/>
+      <c r="A96" s="190"/>
+      <c r="B96" s="182"/>
       <c r="C96" s="60" t="s">
         <v>211</v>
       </c>
@@ -12661,8 +12661,8 @@
       <c r="S96" s="26"/>
     </row>
     <row r="97" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="204"/>
-      <c r="B97" s="177"/>
+      <c r="A97" s="190"/>
+      <c r="B97" s="182"/>
       <c r="C97" s="60" t="s">
         <v>371</v>
       </c>
@@ -12708,8 +12708,8 @@
       <c r="S97" s="26"/>
     </row>
     <row r="98" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="204"/>
-      <c r="B98" s="177"/>
+      <c r="A98" s="190"/>
+      <c r="B98" s="182"/>
       <c r="C98" s="60" t="s">
         <v>220</v>
       </c>
@@ -12755,8 +12755,8 @@
       <c r="S98" s="26"/>
     </row>
     <row r="99" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="204"/>
-      <c r="B99" s="177"/>
+      <c r="A99" s="190"/>
+      <c r="B99" s="182"/>
       <c r="C99" s="60" t="s">
         <v>245</v>
       </c>
@@ -12800,8 +12800,8 @@
       <c r="S99" s="26"/>
     </row>
     <row r="100" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="204"/>
-      <c r="B100" s="177"/>
+      <c r="A100" s="190"/>
+      <c r="B100" s="182"/>
       <c r="C100" s="60" t="s">
         <v>292</v>
       </c>
@@ -12845,8 +12845,8 @@
       <c r="S100" s="26"/>
     </row>
     <row r="101" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="204"/>
-      <c r="B101" s="177"/>
+      <c r="A101" s="190"/>
+      <c r="B101" s="182"/>
       <c r="C101" s="60" t="s">
         <v>222</v>
       </c>
@@ -12892,8 +12892,8 @@
       <c r="S101" s="26"/>
     </row>
     <row r="102" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="204"/>
-      <c r="B102" s="177"/>
+      <c r="A102" s="190"/>
+      <c r="B102" s="182"/>
       <c r="C102" s="60" t="s">
         <v>697</v>
       </c>
@@ -12937,8 +12937,8 @@
       <c r="S102" s="26"/>
     </row>
     <row r="103" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="204"/>
-      <c r="B103" s="177"/>
+      <c r="A103" s="190"/>
+      <c r="B103" s="182"/>
       <c r="C103" s="60" t="s">
         <v>230</v>
       </c>
@@ -12980,8 +12980,8 @@
       <c r="S103" s="26"/>
     </row>
     <row r="104" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="204"/>
-      <c r="B104" s="177"/>
+      <c r="A104" s="190"/>
+      <c r="B104" s="182"/>
       <c r="C104" s="60" t="s">
         <v>221</v>
       </c>
@@ -13027,8 +13027,8 @@
       <c r="S104" s="26"/>
     </row>
     <row r="105" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="204"/>
-      <c r="B105" s="177"/>
+      <c r="A105" s="190"/>
+      <c r="B105" s="182"/>
       <c r="C105" s="65" t="s">
         <v>216</v>
       </c>
@@ -13074,8 +13074,8 @@
       <c r="S105" s="26"/>
     </row>
     <row r="106" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="204"/>
-      <c r="B106" s="177"/>
+      <c r="A106" s="190"/>
+      <c r="B106" s="182"/>
       <c r="C106" s="60" t="s">
         <v>213</v>
       </c>
@@ -13121,8 +13121,8 @@
       <c r="S106" s="26"/>
     </row>
     <row r="107" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="204"/>
-      <c r="B107" s="177"/>
+      <c r="A107" s="190"/>
+      <c r="B107" s="182"/>
       <c r="C107" s="60" t="s">
         <v>214</v>
       </c>
@@ -13168,8 +13168,8 @@
       <c r="S107" s="26"/>
     </row>
     <row r="108" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="204"/>
-      <c r="B108" s="177"/>
+      <c r="A108" s="190"/>
+      <c r="B108" s="182"/>
       <c r="C108" s="60" t="s">
         <v>357</v>
       </c>
@@ -13215,8 +13215,8 @@
       <c r="S108" s="26"/>
     </row>
     <row r="109" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="204"/>
-      <c r="B109" s="177"/>
+      <c r="A109" s="190"/>
+      <c r="B109" s="182"/>
       <c r="C109" s="60" t="s">
         <v>229</v>
       </c>
@@ -13262,8 +13262,8 @@
       <c r="S109" s="26"/>
     </row>
     <row r="110" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="204"/>
-      <c r="B110" s="177"/>
+      <c r="A110" s="190"/>
+      <c r="B110" s="182"/>
       <c r="C110" s="60" t="s">
         <v>205</v>
       </c>
@@ -13309,8 +13309,8 @@
       <c r="S110" s="26"/>
     </row>
     <row r="111" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="204"/>
-      <c r="B111" s="177"/>
+      <c r="A111" s="190"/>
+      <c r="B111" s="182"/>
       <c r="C111" s="60" t="s">
         <v>206</v>
       </c>
@@ -13356,8 +13356,8 @@
       <c r="S111" s="26"/>
     </row>
     <row r="112" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="204"/>
-      <c r="B112" s="177"/>
+      <c r="A112" s="190"/>
+      <c r="B112" s="182"/>
       <c r="C112" s="60" t="s">
         <v>499</v>
       </c>
@@ -13403,8 +13403,8 @@
       <c r="S112" s="26"/>
     </row>
     <row r="113" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="204"/>
-      <c r="B113" s="177"/>
+      <c r="A113" s="190"/>
+      <c r="B113" s="182"/>
       <c r="C113" s="60" t="s">
         <v>246</v>
       </c>
@@ -13450,8 +13450,8 @@
       <c r="S113" s="26"/>
     </row>
     <row r="114" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="204"/>
-      <c r="B114" s="177"/>
+      <c r="A114" s="190"/>
+      <c r="B114" s="182"/>
       <c r="C114" s="60" t="s">
         <v>249</v>
       </c>
@@ -13495,8 +13495,8 @@
       <c r="S114" s="26"/>
     </row>
     <row r="115" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="204"/>
-      <c r="B115" s="177"/>
+      <c r="A115" s="190"/>
+      <c r="B115" s="182"/>
       <c r="C115" s="60" t="s">
         <v>226</v>
       </c>
@@ -13544,8 +13544,8 @@
       <c r="S115" s="26"/>
     </row>
     <row r="116" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="204"/>
-      <c r="B116" s="177"/>
+      <c r="A116" s="190"/>
+      <c r="B116" s="182"/>
       <c r="C116" s="60" t="s">
         <v>227</v>
       </c>
@@ -13593,8 +13593,8 @@
       <c r="S116" s="26"/>
     </row>
     <row r="117" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="204"/>
-      <c r="B117" s="177"/>
+      <c r="A117" s="190"/>
+      <c r="B117" s="182"/>
       <c r="C117" s="65" t="s">
         <v>595</v>
       </c>
@@ -13621,8 +13621,8 @@
       <c r="T117" s="23"/>
     </row>
     <row r="118" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="204"/>
-      <c r="B118" s="177"/>
+      <c r="A118" s="190"/>
+      <c r="B118" s="182"/>
       <c r="C118" s="60" t="s">
         <v>323</v>
       </c>
@@ -13669,8 +13669,8 @@
       <c r="T118" s="23"/>
     </row>
     <row r="119" spans="1:20" s="33" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="205"/>
-      <c r="B119" s="178"/>
+      <c r="A119" s="191"/>
+      <c r="B119" s="187"/>
       <c r="C119" s="61" t="s">
         <v>316</v>
       </c>
@@ -13723,10 +13723,10 @@
       <c r="T119" s="28"/>
     </row>
     <row r="120" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="198" t="s">
+      <c r="A120" s="183" t="s">
         <v>497</v>
       </c>
-      <c r="B120" s="184" t="s">
+      <c r="B120" s="174" t="s">
         <v>51</v>
       </c>
       <c r="C120" s="62" t="s">
@@ -13771,8 +13771,8 @@
       <c r="T120" s="33"/>
     </row>
     <row r="121" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="199"/>
-      <c r="B121" s="182"/>
+      <c r="A121" s="184"/>
+      <c r="B121" s="175"/>
       <c r="C121" s="60" t="s">
         <v>92</v>
       </c>
@@ -13818,8 +13818,8 @@
       <c r="S121" s="26"/>
     </row>
     <row r="122" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="199"/>
-      <c r="B122" s="182"/>
+      <c r="A122" s="184"/>
+      <c r="B122" s="175"/>
       <c r="C122" s="60" t="s">
         <v>93</v>
       </c>
@@ -13865,8 +13865,8 @@
       <c r="S122" s="26"/>
     </row>
     <row r="123" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="199"/>
-      <c r="B123" s="182"/>
+      <c r="A123" s="184"/>
+      <c r="B123" s="175"/>
       <c r="C123" s="60" t="s">
         <v>104</v>
       </c>
@@ -13908,8 +13908,8 @@
       <c r="S123" s="26"/>
     </row>
     <row r="124" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="199"/>
-      <c r="B124" s="182"/>
+      <c r="A124" s="184"/>
+      <c r="B124" s="175"/>
       <c r="C124" s="61" t="s">
         <v>94</v>
       </c>
@@ -13952,8 +13952,8 @@
       <c r="T124" s="28"/>
     </row>
     <row r="125" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="199"/>
-      <c r="B125" s="182"/>
+      <c r="A125" s="184"/>
+      <c r="B125" s="175"/>
       <c r="C125" s="60" t="s">
         <v>179</v>
       </c>
@@ -13996,8 +13996,8 @@
       <c r="T125" s="28"/>
     </row>
     <row r="126" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="199"/>
-      <c r="B126" s="182"/>
+      <c r="A126" s="184"/>
+      <c r="B126" s="175"/>
       <c r="C126" s="61" t="s">
         <v>116</v>
       </c>
@@ -14040,8 +14040,8 @@
       <c r="T126" s="28"/>
     </row>
     <row r="127" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="199"/>
-      <c r="B127" s="182"/>
+      <c r="A127" s="184"/>
+      <c r="B127" s="175"/>
       <c r="C127" s="60" t="s">
         <v>96</v>
       </c>
@@ -14085,8 +14085,8 @@
       <c r="S127" s="26"/>
     </row>
     <row r="128" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="199"/>
-      <c r="B128" s="182"/>
+      <c r="A128" s="184"/>
+      <c r="B128" s="175"/>
       <c r="C128" s="60" t="s">
         <v>498</v>
       </c>
@@ -14130,8 +14130,8 @@
       <c r="S128" s="26"/>
     </row>
     <row r="129" spans="1:20" s="23" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="199"/>
-      <c r="B129" s="201"/>
+      <c r="A129" s="184"/>
+      <c r="B129" s="186"/>
       <c r="C129" s="60" t="s">
         <v>176</v>
       </c>
@@ -14173,8 +14173,8 @@
       <c r="S129" s="26"/>
     </row>
     <row r="130" spans="1:20" s="28" customFormat="1" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="199"/>
-      <c r="B130" s="187" t="s">
+      <c r="A130" s="184"/>
+      <c r="B130" s="181" t="s">
         <v>193</v>
       </c>
       <c r="C130" s="63" t="s">
@@ -14221,8 +14221,8 @@
       <c r="T130" s="23"/>
     </row>
     <row r="131" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="199"/>
-      <c r="B131" s="177"/>
+      <c r="A131" s="184"/>
+      <c r="B131" s="182"/>
       <c r="C131" s="60" t="s">
         <v>445</v>
       </c>
@@ -14265,8 +14265,8 @@
       <c r="T131" s="23"/>
     </row>
     <row r="132" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="199"/>
-      <c r="B132" s="177"/>
+      <c r="A132" s="184"/>
+      <c r="B132" s="182"/>
       <c r="C132" s="60" t="s">
         <v>448</v>
       </c>
@@ -14309,8 +14309,8 @@
       <c r="T132" s="23"/>
     </row>
     <row r="133" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="199"/>
-      <c r="B133" s="177"/>
+      <c r="A133" s="184"/>
+      <c r="B133" s="182"/>
       <c r="C133" s="61" t="s">
         <v>422</v>
       </c>
@@ -14355,8 +14355,8 @@
       <c r="T133" s="23"/>
     </row>
     <row r="134" spans="1:20" s="33" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="199"/>
-      <c r="B134" s="177"/>
+      <c r="A134" s="184"/>
+      <c r="B134" s="182"/>
       <c r="C134" s="60" t="s">
         <v>228</v>
       </c>
@@ -14399,8 +14399,8 @@
       <c r="T134" s="23"/>
     </row>
     <row r="135" spans="1:20" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="199"/>
-      <c r="B135" s="177"/>
+      <c r="A135" s="184"/>
+      <c r="B135" s="182"/>
       <c r="C135" s="60" t="s">
         <v>207</v>
       </c>
@@ -14443,8 +14443,8 @@
       <c r="T135" s="23"/>
     </row>
     <row r="136" spans="1:20" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="200"/>
-      <c r="B136" s="177"/>
+      <c r="A136" s="185"/>
+      <c r="B136" s="182"/>
       <c r="C136" s="65" t="s">
         <v>621</v>
       </c>
@@ -14467,10 +14467,10 @@
       <c r="T136" s="23"/>
     </row>
     <row r="137" spans="1:20" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="195" t="s">
+      <c r="A137" s="178" t="s">
         <v>111</v>
       </c>
-      <c r="B137" s="184" t="s">
+      <c r="B137" s="174" t="s">
         <v>51</v>
       </c>
       <c r="C137" s="62" t="s">
@@ -14513,8 +14513,8 @@
       <c r="T137" s="33"/>
     </row>
     <row r="138" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="196"/>
-      <c r="B138" s="182"/>
+      <c r="A138" s="179"/>
+      <c r="B138" s="175"/>
       <c r="C138" s="61" t="s">
         <v>95</v>
       </c>
@@ -14554,8 +14554,8 @@
       <c r="S138" s="31"/>
     </row>
     <row r="139" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="196"/>
-      <c r="B139" s="182"/>
+      <c r="A139" s="179"/>
+      <c r="B139" s="175"/>
       <c r="C139" s="65" t="s">
         <v>599</v>
       </c>
@@ -14598,8 +14598,8 @@
       <c r="T139" s="19"/>
     </row>
     <row r="140" spans="1:20" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="196"/>
-      <c r="B140" s="182"/>
+      <c r="A140" s="179"/>
+      <c r="B140" s="175"/>
       <c r="C140" s="60" t="s">
         <v>115</v>
       </c>
@@ -14641,8 +14641,8 @@
       <c r="T140" s="19"/>
     </row>
     <row r="141" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="196"/>
-      <c r="B141" s="182"/>
+      <c r="A141" s="179"/>
+      <c r="B141" s="175"/>
       <c r="C141" s="60" t="s">
         <v>114</v>
       </c>
@@ -14684,8 +14684,8 @@
       <c r="T141" s="19"/>
     </row>
     <row r="142" spans="1:20" s="23" customFormat="1" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="196"/>
-      <c r="B142" s="187" t="s">
+      <c r="A142" s="179"/>
+      <c r="B142" s="181" t="s">
         <v>193</v>
       </c>
       <c r="C142" s="63" t="s">
@@ -14727,8 +14727,8 @@
       <c r="S142" s="57"/>
     </row>
     <row r="143" spans="1:20" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="196"/>
-      <c r="B143" s="177"/>
+      <c r="A143" s="179"/>
+      <c r="B143" s="182"/>
       <c r="C143" s="60" t="s">
         <v>396</v>
       </c>
@@ -14767,8 +14767,8 @@
       <c r="S143" s="26"/>
     </row>
     <row r="144" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="196"/>
-      <c r="B144" s="177"/>
+      <c r="A144" s="179"/>
+      <c r="B144" s="182"/>
       <c r="C144" s="60" t="s">
         <v>253</v>
       </c>
@@ -14808,8 +14808,8 @@
       <c r="S144" s="26"/>
     </row>
     <row r="145" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="196"/>
-      <c r="B145" s="177"/>
+      <c r="A145" s="179"/>
+      <c r="B145" s="182"/>
       <c r="C145" s="65" t="s">
         <v>615</v>
       </c>
@@ -14843,8 +14843,8 @@
       <c r="S145" s="26"/>
     </row>
     <row r="146" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="196"/>
-      <c r="B146" s="177"/>
+      <c r="A146" s="179"/>
+      <c r="B146" s="182"/>
       <c r="C146" s="60" t="s">
         <v>419</v>
       </c>
@@ -14884,8 +14884,8 @@
       <c r="S146" s="26"/>
     </row>
     <row r="147" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="196"/>
-      <c r="B147" s="177"/>
+      <c r="A147" s="179"/>
+      <c r="B147" s="182"/>
       <c r="C147" s="60" t="s">
         <v>378</v>
       </c>
@@ -14923,8 +14923,8 @@
       <c r="S147" s="26"/>
     </row>
     <row r="148" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="196"/>
-      <c r="B148" s="177"/>
+      <c r="A148" s="179"/>
+      <c r="B148" s="182"/>
       <c r="C148" s="60" t="s">
         <v>436</v>
       </c>
@@ -14964,8 +14964,8 @@
       <c r="S148" s="26"/>
     </row>
     <row r="149" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="196"/>
-      <c r="B149" s="177"/>
+      <c r="A149" s="179"/>
+      <c r="B149" s="182"/>
       <c r="C149" s="60" t="s">
         <v>356</v>
       </c>
@@ -15005,8 +15005,8 @@
       <c r="S149" s="26"/>
     </row>
     <row r="150" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="196"/>
-      <c r="B150" s="177"/>
+      <c r="A150" s="179"/>
+      <c r="B150" s="182"/>
       <c r="C150" s="60" t="s">
         <v>224</v>
       </c>
@@ -15048,8 +15048,8 @@
       <c r="S150" s="26"/>
     </row>
     <row r="151" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="196"/>
-      <c r="B151" s="177"/>
+      <c r="A151" s="179"/>
+      <c r="B151" s="182"/>
       <c r="C151" s="60" t="s">
         <v>418</v>
       </c>
@@ -15089,8 +15089,8 @@
       <c r="S151" s="26"/>
     </row>
     <row r="152" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="196"/>
-      <c r="B152" s="177"/>
+      <c r="A152" s="179"/>
+      <c r="B152" s="182"/>
       <c r="C152" s="60" t="s">
         <v>393</v>
       </c>
@@ -15130,8 +15130,8 @@
       <c r="S152" s="26"/>
     </row>
     <row r="153" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="196"/>
-      <c r="B153" s="177"/>
+      <c r="A153" s="179"/>
+      <c r="B153" s="182"/>
       <c r="C153" s="60" t="s">
         <v>430</v>
       </c>
@@ -15171,8 +15171,8 @@
       <c r="S153" s="26"/>
     </row>
     <row r="154" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="196"/>
-      <c r="B154" s="177"/>
+      <c r="A154" s="179"/>
+      <c r="B154" s="182"/>
       <c r="C154" s="60" t="s">
         <v>403</v>
       </c>
@@ -15212,8 +15212,8 @@
       <c r="S154" s="26"/>
     </row>
     <row r="155" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="196"/>
-      <c r="B155" s="177"/>
+      <c r="A155" s="179"/>
+      <c r="B155" s="182"/>
       <c r="C155" s="65" t="s">
         <v>518</v>
       </c>
@@ -15255,8 +15255,8 @@
       <c r="S155" s="26"/>
     </row>
     <row r="156" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="196"/>
-      <c r="B156" s="177"/>
+      <c r="A156" s="179"/>
+      <c r="B156" s="182"/>
       <c r="C156" s="65" t="s">
         <v>254</v>
       </c>
@@ -15296,8 +15296,8 @@
       <c r="S156" s="26"/>
     </row>
     <row r="157" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="196"/>
-      <c r="B157" s="177"/>
+      <c r="A157" s="179"/>
+      <c r="B157" s="182"/>
       <c r="C157" s="65" t="s">
         <v>443</v>
       </c>
@@ -15337,8 +15337,8 @@
       <c r="S157" s="26"/>
     </row>
     <row r="158" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="196"/>
-      <c r="B158" s="177"/>
+      <c r="A158" s="179"/>
+      <c r="B158" s="182"/>
       <c r="C158" s="65" t="s">
         <v>432</v>
       </c>
@@ -15378,8 +15378,8 @@
       <c r="S158" s="26"/>
     </row>
     <row r="159" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="196"/>
-      <c r="B159" s="177"/>
+      <c r="A159" s="179"/>
+      <c r="B159" s="182"/>
       <c r="C159" s="65" t="s">
         <v>317</v>
       </c>
@@ -15421,8 +15421,8 @@
       <c r="S159" s="26"/>
     </row>
     <row r="160" spans="1:19" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="196"/>
-      <c r="B160" s="177"/>
+      <c r="A160" s="179"/>
+      <c r="B160" s="182"/>
       <c r="C160" s="65" t="s">
         <v>364</v>
       </c>
@@ -15464,8 +15464,8 @@
       <c r="S160" s="26"/>
     </row>
     <row r="161" spans="1:19" s="23" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A161" s="197"/>
-      <c r="B161" s="177"/>
+      <c r="A161" s="180"/>
+      <c r="B161" s="182"/>
       <c r="C161" s="65" t="s">
         <v>210</v>
       </c>
@@ -15505,10 +15505,10 @@
       <c r="S161" s="31"/>
     </row>
     <row r="162" spans="1:19" s="33" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A162" s="185" t="s">
+      <c r="A162" s="200" t="s">
         <v>112</v>
       </c>
-      <c r="B162" s="176" t="s">
+      <c r="B162" s="195" t="s">
         <v>193</v>
       </c>
       <c r="C162" s="62" t="s">
@@ -15554,8 +15554,8 @@
       <c r="S162" s="36"/>
     </row>
     <row r="163" spans="1:19" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A163" s="185"/>
-      <c r="B163" s="177"/>
+      <c r="A163" s="200"/>
+      <c r="B163" s="182"/>
       <c r="C163" s="60" t="s">
         <v>360</v>
       </c>
@@ -15597,8 +15597,8 @@
       <c r="S163" s="26"/>
     </row>
     <row r="164" spans="1:19" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A164" s="185"/>
-      <c r="B164" s="177"/>
+      <c r="A164" s="200"/>
+      <c r="B164" s="182"/>
       <c r="C164" s="60" t="s">
         <v>379</v>
       </c>
@@ -15642,8 +15642,8 @@
       <c r="S164" s="26"/>
     </row>
     <row r="165" spans="1:19" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A165" s="185"/>
-      <c r="B165" s="177"/>
+      <c r="A165" s="200"/>
+      <c r="B165" s="182"/>
       <c r="C165" s="60" t="s">
         <v>389</v>
       </c>
@@ -15687,8 +15687,8 @@
       <c r="S165" s="26"/>
     </row>
     <row r="166" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A166" s="185"/>
-      <c r="B166" s="177"/>
+      <c r="A166" s="200"/>
+      <c r="B166" s="182"/>
       <c r="C166" s="60" t="s">
         <v>248</v>
       </c>
@@ -15730,8 +15730,8 @@
       <c r="S166" s="26"/>
     </row>
     <row r="167" spans="1:19" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A167" s="185"/>
-      <c r="B167" s="177"/>
+      <c r="A167" s="200"/>
+      <c r="B167" s="182"/>
       <c r="C167" s="61" t="s">
         <v>398</v>
       </c>
@@ -15775,8 +15775,8 @@
       <c r="S167" s="26"/>
     </row>
     <row r="168" spans="1:19" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A168" s="185"/>
-      <c r="B168" s="177"/>
+      <c r="A168" s="200"/>
+      <c r="B168" s="182"/>
       <c r="C168" s="60" t="s">
         <v>370</v>
       </c>
@@ -15818,8 +15818,8 @@
       <c r="S168" s="26"/>
     </row>
     <row r="169" spans="1:19" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="185"/>
-      <c r="B169" s="178"/>
+      <c r="A169" s="200"/>
+      <c r="B169" s="187"/>
       <c r="C169" s="60" t="s">
         <v>399</v>
       </c>
@@ -15861,7 +15861,7 @@
       <c r="S169" s="31"/>
     </row>
     <row r="170" spans="1:19" s="33" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A170" s="186" t="s">
+      <c r="A170" s="201" t="s">
         <v>532</v>
       </c>
       <c r="B170" s="72" t="s">
@@ -15904,8 +15904,8 @@
       <c r="S170" s="71"/>
     </row>
     <row r="171" spans="1:19" s="23" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A171" s="186"/>
-      <c r="B171" s="187" t="s">
+      <c r="A171" s="201"/>
+      <c r="B171" s="181" t="s">
         <v>193</v>
       </c>
       <c r="C171" s="60" t="s">
@@ -15943,8 +15943,8 @@
       <c r="S171" s="57"/>
     </row>
     <row r="172" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A172" s="186"/>
-      <c r="B172" s="177"/>
+      <c r="A172" s="201"/>
+      <c r="B172" s="182"/>
       <c r="C172" s="60" t="s">
         <v>195</v>
       </c>
@@ -15979,8 +15979,8 @@
       <c r="S172" s="26"/>
     </row>
     <row r="173" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A173" s="186"/>
-      <c r="B173" s="177"/>
+      <c r="A173" s="201"/>
+      <c r="B173" s="182"/>
       <c r="C173" s="60" t="s">
         <v>257</v>
       </c>
@@ -16020,8 +16020,8 @@
       <c r="S173" s="26"/>
     </row>
     <row r="174" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A174" s="186"/>
-      <c r="B174" s="177"/>
+      <c r="A174" s="201"/>
+      <c r="B174" s="182"/>
       <c r="C174" s="60" t="s">
         <v>414</v>
       </c>
@@ -16058,8 +16058,8 @@
       <c r="S174" s="26"/>
     </row>
     <row r="175" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A175" s="186"/>
-      <c r="B175" s="188"/>
+      <c r="A175" s="201"/>
+      <c r="B175" s="202"/>
       <c r="C175" s="60" t="s">
         <v>415</v>
       </c>
@@ -16097,10 +16097,10 @@
       <c r="S175" s="26"/>
     </row>
     <row r="176" spans="1:19" s="33" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A176" s="175" t="s">
+      <c r="A176" s="194" t="s">
         <v>113</v>
       </c>
-      <c r="B176" s="181" t="s">
+      <c r="B176" s="198" t="s">
         <v>51</v>
       </c>
       <c r="C176" s="62" t="s">
@@ -16140,8 +16140,8 @@
       <c r="S176" s="36"/>
     </row>
     <row r="177" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A177" s="175"/>
-      <c r="B177" s="182"/>
+      <c r="A177" s="194"/>
+      <c r="B177" s="175"/>
       <c r="C177" s="60" t="s">
         <v>184</v>
       </c>
@@ -16179,8 +16179,8 @@
       <c r="S177" s="26"/>
     </row>
     <row r="178" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A178" s="175"/>
-      <c r="B178" s="182"/>
+      <c r="A178" s="194"/>
+      <c r="B178" s="175"/>
       <c r="C178" s="60" t="s">
         <v>183</v>
       </c>
@@ -16218,8 +16218,8 @@
       <c r="S178" s="26"/>
     </row>
     <row r="179" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A179" s="175"/>
-      <c r="B179" s="182"/>
+      <c r="A179" s="194"/>
+      <c r="B179" s="175"/>
       <c r="C179" s="61" t="s">
         <v>185</v>
       </c>
@@ -16257,8 +16257,8 @@
       <c r="S179" s="31"/>
     </row>
     <row r="180" spans="1:19" s="23" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A180" s="175"/>
-      <c r="B180" s="173" t="s">
+      <c r="A180" s="194"/>
+      <c r="B180" s="192" t="s">
         <v>193</v>
       </c>
       <c r="C180" s="63" t="s">
@@ -16292,8 +16292,8 @@
       <c r="S180" s="57"/>
     </row>
     <row r="181" spans="1:19" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A181" s="175"/>
-      <c r="B181" s="174"/>
+      <c r="A181" s="194"/>
+      <c r="B181" s="193"/>
       <c r="C181" s="64"/>
       <c r="E181" s="49"/>
       <c r="F181" s="49"/>
@@ -17022,18 +17022,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="C3:S3"/>
-    <mergeCell ref="B53:B57"/>
-    <mergeCell ref="A53:A71"/>
-    <mergeCell ref="A137:A161"/>
-    <mergeCell ref="B142:B161"/>
-    <mergeCell ref="A120:A136"/>
-    <mergeCell ref="B120:B129"/>
-    <mergeCell ref="B83:B119"/>
-    <mergeCell ref="B58:B71"/>
-    <mergeCell ref="B72:B82"/>
-    <mergeCell ref="A72:A119"/>
-    <mergeCell ref="B137:B141"/>
     <mergeCell ref="B180:B181"/>
     <mergeCell ref="A176:A181"/>
     <mergeCell ref="B162:B169"/>
@@ -17049,6 +17037,18 @@
     <mergeCell ref="B130:B136"/>
     <mergeCell ref="A39:A52"/>
     <mergeCell ref="B43:B52"/>
+    <mergeCell ref="C3:S3"/>
+    <mergeCell ref="B53:B57"/>
+    <mergeCell ref="A53:A71"/>
+    <mergeCell ref="A137:A161"/>
+    <mergeCell ref="B142:B161"/>
+    <mergeCell ref="A120:A136"/>
+    <mergeCell ref="B120:B129"/>
+    <mergeCell ref="B83:B119"/>
+    <mergeCell ref="B58:B71"/>
+    <mergeCell ref="B72:B82"/>
+    <mergeCell ref="A72:A119"/>
+    <mergeCell ref="B137:B141"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Zu viel um hier reinzuschreiben. liest eh keiner
</commit_message>
<xml_diff>
--- a/ressources/DayZ Mods.xlsx
+++ b/ressources/DayZ Mods.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Documents\DayZ_Server\Immersive-DayZ-Experience\ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F61D11D-8D2D-4539-A441-2418C5CD1DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E93DED9-4A20-42A3-AE0E-1F7A1229CEE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="15345" tabRatio="260" activeTab="1" xr2:uid="{FAEB3C3F-74B0-4C80-8C8B-4522341FA132}"/>
+    <workbookView xWindow="4680" yWindow="4680" windowWidth="28800" windowHeight="15345" tabRatio="260" activeTab="1" xr2:uid="{FAEB3C3F-74B0-4C80-8C8B-4522341FA132}"/>
   </bookViews>
   <sheets>
     <sheet name="Mods" sheetId="1" r:id="rId1"/>
@@ -4104,14 +4104,65 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -4128,12 +4179,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -4146,9 +4191,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -4159,48 +4201,6 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
@@ -8237,18 +8237,18 @@
     <sortCondition ref="B2:B98"/>
   </sortState>
   <mergeCells count="12">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A11:A15"/>
     <mergeCell ref="A48:A52"/>
     <mergeCell ref="A57:A71"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A45:A47"/>
     <mergeCell ref="A21:A40"/>
     <mergeCell ref="A53:A56"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A11:A15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8259,8 +8259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FF4763-6B65-4CE2-BD87-511E98A2E639}">
   <dimension ref="A1:V229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M80" activeCellId="1" sqref="I83 M80"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8292,25 +8292,25 @@
       <c r="S2"/>
     </row>
     <row r="3" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="173" t="s">
+      <c r="C3" s="192" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="173"/>
-      <c r="E3" s="173"/>
-      <c r="F3" s="173"/>
-      <c r="G3" s="173"/>
-      <c r="H3" s="173"/>
-      <c r="I3" s="173"/>
-      <c r="J3" s="173"/>
-      <c r="K3" s="173"/>
-      <c r="L3" s="173"/>
-      <c r="M3" s="173"/>
-      <c r="N3" s="173"/>
-      <c r="O3" s="173"/>
-      <c r="P3" s="173"/>
-      <c r="Q3" s="173"/>
-      <c r="R3" s="173"/>
-      <c r="S3" s="173"/>
+      <c r="D3" s="192"/>
+      <c r="E3" s="192"/>
+      <c r="F3" s="192"/>
+      <c r="G3" s="192"/>
+      <c r="H3" s="192"/>
+      <c r="I3" s="192"/>
+      <c r="J3" s="192"/>
+      <c r="K3" s="192"/>
+      <c r="L3" s="192"/>
+      <c r="M3" s="192"/>
+      <c r="N3" s="192"/>
+      <c r="O3" s="192"/>
+      <c r="P3" s="192"/>
+      <c r="Q3" s="192"/>
+      <c r="R3" s="192"/>
+      <c r="S3" s="192"/>
     </row>
     <row r="4" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
@@ -8325,19 +8325,19 @@
       <c r="F4" s="3" t="s">
         <v>642</v>
       </c>
-      <c r="G4" s="197"/>
-      <c r="H4" s="197"/>
-      <c r="I4" s="197"/>
-      <c r="J4" s="197"/>
-      <c r="K4" s="197"/>
-      <c r="L4" s="197"/>
-      <c r="M4" s="197"/>
-      <c r="N4" s="197"/>
-      <c r="O4" s="197"/>
-      <c r="P4" s="197"/>
-      <c r="Q4" s="197"/>
-      <c r="R4" s="197"/>
-      <c r="S4" s="197"/>
+      <c r="G4" s="180"/>
+      <c r="H4" s="180"/>
+      <c r="I4" s="180"/>
+      <c r="J4" s="180"/>
+      <c r="K4" s="180"/>
+      <c r="L4" s="180"/>
+      <c r="M4" s="180"/>
+      <c r="N4" s="180"/>
+      <c r="O4" s="180"/>
+      <c r="P4" s="180"/>
+      <c r="Q4" s="180"/>
+      <c r="R4" s="180"/>
+      <c r="S4" s="180"/>
     </row>
     <row r="5" spans="1:22" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="3"/>
@@ -8388,10 +8388,10 @@
       </c>
     </row>
     <row r="6" spans="1:22" s="23" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="196" t="s">
+      <c r="A6" s="179" t="s">
         <v>88</v>
       </c>
-      <c r="B6" s="198" t="s">
+      <c r="B6" s="181" t="s">
         <v>51</v>
       </c>
       <c r="C6" s="18" t="s">
@@ -8453,8 +8453,8 @@
       </c>
     </row>
     <row r="7" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="196"/>
-      <c r="B7" s="175"/>
+      <c r="A7" s="179"/>
+      <c r="B7" s="182"/>
       <c r="C7" s="60" t="s">
         <v>42</v>
       </c>
@@ -8505,8 +8505,8 @@
       </c>
     </row>
     <row r="8" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="196"/>
-      <c r="B8" s="175"/>
+      <c r="A8" s="179"/>
+      <c r="B8" s="182"/>
       <c r="C8" s="60" t="s">
         <v>49</v>
       </c>
@@ -8555,8 +8555,8 @@
       </c>
     </row>
     <row r="9" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="196"/>
-      <c r="B9" s="175"/>
+      <c r="A9" s="179"/>
+      <c r="B9" s="182"/>
       <c r="C9" s="60" t="s">
         <v>281</v>
       </c>
@@ -8607,8 +8607,8 @@
       </c>
     </row>
     <row r="10" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="196"/>
-      <c r="B10" s="175"/>
+      <c r="A10" s="179"/>
+      <c r="B10" s="182"/>
       <c r="C10" s="60" t="s">
         <v>43</v>
       </c>
@@ -8657,8 +8657,8 @@
       </c>
     </row>
     <row r="11" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="196"/>
-      <c r="B11" s="175"/>
+      <c r="A11" s="179"/>
+      <c r="B11" s="182"/>
       <c r="C11" s="60" t="s">
         <v>59</v>
       </c>
@@ -8709,8 +8709,8 @@
       </c>
     </row>
     <row r="12" spans="1:22" s="23" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="196"/>
-      <c r="B12" s="175"/>
+      <c r="A12" s="179"/>
+      <c r="B12" s="182"/>
       <c r="C12" s="60" t="s">
         <v>44</v>
       </c>
@@ -8756,8 +8756,8 @@
       <c r="S12" s="26"/>
     </row>
     <row r="13" spans="1:22" s="23" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="196"/>
-      <c r="B13" s="175"/>
+      <c r="A13" s="179"/>
+      <c r="B13" s="182"/>
       <c r="C13" s="60" t="s">
         <v>634</v>
       </c>
@@ -8791,8 +8791,8 @@
       <c r="S13" s="26"/>
     </row>
     <row r="14" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="196"/>
-      <c r="B14" s="175"/>
+      <c r="A14" s="179"/>
+      <c r="B14" s="182"/>
       <c r="C14" s="60" t="s">
         <v>45</v>
       </c>
@@ -8838,8 +8838,8 @@
       <c r="S14" s="26"/>
     </row>
     <row r="15" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="196"/>
-      <c r="B15" s="175"/>
+      <c r="A15" s="179"/>
+      <c r="B15" s="182"/>
       <c r="C15" s="60" t="s">
         <v>74</v>
       </c>
@@ -8885,8 +8885,8 @@
       <c r="S15" s="26"/>
     </row>
     <row r="16" spans="1:22" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="196"/>
-      <c r="B16" s="175"/>
+      <c r="A16" s="179"/>
+      <c r="B16" s="182"/>
       <c r="C16" s="60" t="s">
         <v>46</v>
       </c>
@@ -8930,8 +8930,8 @@
       <c r="S16" s="26"/>
     </row>
     <row r="17" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="196"/>
-      <c r="B17" s="175"/>
+      <c r="A17" s="179"/>
+      <c r="B17" s="182"/>
       <c r="C17" s="60" t="s">
         <v>47</v>
       </c>
@@ -8975,8 +8975,8 @@
       <c r="S17" s="26"/>
     </row>
     <row r="18" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="196"/>
-      <c r="B18" s="175"/>
+      <c r="A18" s="179"/>
+      <c r="B18" s="182"/>
       <c r="C18" s="60" t="s">
         <v>48</v>
       </c>
@@ -9020,8 +9020,8 @@
       <c r="S18" s="26"/>
     </row>
     <row r="19" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="196"/>
-      <c r="B19" s="175"/>
+      <c r="A19" s="179"/>
+      <c r="B19" s="182"/>
       <c r="C19" s="60" t="s">
         <v>344</v>
       </c>
@@ -9067,8 +9067,8 @@
       <c r="S19" s="26"/>
     </row>
     <row r="20" spans="1:20" s="40" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="196"/>
-      <c r="B20" s="199"/>
+      <c r="A20" s="179"/>
+      <c r="B20" s="183"/>
       <c r="C20" s="61" t="s">
         <v>50</v>
       </c>
@@ -9110,8 +9110,8 @@
       <c r="S20" s="31"/>
     </row>
     <row r="21" spans="1:20" s="33" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="196"/>
-      <c r="B21" s="195" t="s">
+      <c r="A21" s="179"/>
+      <c r="B21" s="176" t="s">
         <v>244</v>
       </c>
       <c r="C21" s="117" t="s">
@@ -9162,8 +9162,8 @@
       </c>
     </row>
     <row r="22" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="196"/>
-      <c r="B22" s="182"/>
+      <c r="A22" s="179"/>
+      <c r="B22" s="177"/>
       <c r="C22" s="61" t="s">
         <v>231</v>
       </c>
@@ -9209,8 +9209,8 @@
       <c r="S22" s="26"/>
     </row>
     <row r="23" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="196"/>
-      <c r="B23" s="182"/>
+      <c r="A23" s="179"/>
+      <c r="B23" s="177"/>
       <c r="C23" s="60" t="s">
         <v>45</v>
       </c>
@@ -9254,8 +9254,8 @@
       <c r="S23" s="26"/>
     </row>
     <row r="24" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="196"/>
-      <c r="B24" s="182"/>
+      <c r="A24" s="179"/>
+      <c r="B24" s="177"/>
       <c r="C24" s="60" t="s">
         <v>120</v>
       </c>
@@ -9303,8 +9303,8 @@
       <c r="S24" s="26"/>
     </row>
     <row r="25" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="196"/>
-      <c r="B25" s="182"/>
+      <c r="A25" s="179"/>
+      <c r="B25" s="177"/>
       <c r="C25" s="60" t="s">
         <v>233</v>
       </c>
@@ -9354,8 +9354,8 @@
       <c r="S25" s="26"/>
     </row>
     <row r="26" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="196"/>
-      <c r="B26" s="182"/>
+      <c r="A26" s="179"/>
+      <c r="B26" s="177"/>
       <c r="C26" s="60" t="s">
         <v>348</v>
       </c>
@@ -9401,8 +9401,8 @@
       <c r="S26" s="26"/>
     </row>
     <row r="27" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="196"/>
-      <c r="B27" s="182"/>
+      <c r="A27" s="179"/>
+      <c r="B27" s="177"/>
       <c r="C27" s="60" t="s">
         <v>119</v>
       </c>
@@ -9448,8 +9448,8 @@
       <c r="S27" s="26"/>
     </row>
     <row r="28" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="196"/>
-      <c r="B28" s="182"/>
+      <c r="A28" s="179"/>
+      <c r="B28" s="177"/>
       <c r="C28" s="60" t="s">
         <v>462</v>
       </c>
@@ -9495,8 +9495,8 @@
       <c r="S28" s="26"/>
     </row>
     <row r="29" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="196"/>
-      <c r="B29" s="182"/>
+      <c r="A29" s="179"/>
+      <c r="B29" s="177"/>
       <c r="C29" s="60" t="s">
         <v>383</v>
       </c>
@@ -9542,8 +9542,8 @@
       <c r="S29" s="26"/>
     </row>
     <row r="30" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="196"/>
-      <c r="B30" s="182"/>
+      <c r="A30" s="179"/>
+      <c r="B30" s="177"/>
       <c r="C30" s="60" t="s">
         <v>236</v>
       </c>
@@ -9590,8 +9590,8 @@
       <c r="T30" s="23"/>
     </row>
     <row r="31" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="196"/>
-      <c r="B31" s="182"/>
+      <c r="A31" s="179"/>
+      <c r="B31" s="177"/>
       <c r="C31" s="60" t="s">
         <v>349</v>
       </c>
@@ -9637,8 +9637,8 @@
       <c r="S31" s="26"/>
     </row>
     <row r="32" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="196"/>
-      <c r="B32" s="182"/>
+      <c r="A32" s="179"/>
+      <c r="B32" s="177"/>
       <c r="C32" s="60" t="s">
         <v>349</v>
       </c>
@@ -9684,8 +9684,8 @@
       <c r="S32" s="26"/>
     </row>
     <row r="33" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="196"/>
-      <c r="B33" s="182"/>
+      <c r="A33" s="179"/>
+      <c r="B33" s="177"/>
       <c r="C33" s="60" t="s">
         <v>215</v>
       </c>
@@ -9732,8 +9732,8 @@
       <c r="T33" s="23"/>
     </row>
     <row r="34" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="196"/>
-      <c r="B34" s="182"/>
+      <c r="A34" s="179"/>
+      <c r="B34" s="177"/>
       <c r="C34" s="60" t="s">
         <v>240</v>
       </c>
@@ -9779,8 +9779,8 @@
       <c r="S34" s="26"/>
     </row>
     <row r="35" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="196"/>
-      <c r="B35" s="182"/>
+      <c r="A35" s="179"/>
+      <c r="B35" s="177"/>
       <c r="C35" s="60" t="s">
         <v>373</v>
       </c>
@@ -9824,8 +9824,8 @@
       <c r="S35" s="26"/>
     </row>
     <row r="36" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="196"/>
-      <c r="B36" s="182"/>
+      <c r="A36" s="179"/>
+      <c r="B36" s="177"/>
       <c r="C36" s="60" t="s">
         <v>688</v>
       </c>
@@ -9857,8 +9857,8 @@
       <c r="S36" s="26"/>
     </row>
     <row r="37" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="196"/>
-      <c r="B37" s="182"/>
+      <c r="A37" s="179"/>
+      <c r="B37" s="177"/>
       <c r="C37" s="60" t="s">
         <v>385</v>
       </c>
@@ -9904,8 +9904,8 @@
       <c r="S37" s="26"/>
     </row>
     <row r="38" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="196"/>
-      <c r="B38" s="187"/>
+      <c r="A38" s="179"/>
+      <c r="B38" s="178"/>
       <c r="C38" s="65" t="s">
         <v>232</v>
       </c>
@@ -9951,10 +9951,10 @@
       <c r="S38" s="26"/>
     </row>
     <row r="39" spans="1:20" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="203" t="s">
+      <c r="A39" s="189" t="s">
         <v>264</v>
       </c>
-      <c r="B39" s="174" t="s">
+      <c r="B39" s="184" t="s">
         <v>51</v>
       </c>
       <c r="C39" s="62" t="s">
@@ -9999,8 +9999,8 @@
       <c r="T39" s="33"/>
     </row>
     <row r="40" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="204"/>
-      <c r="B40" s="175"/>
+      <c r="A40" s="190"/>
+      <c r="B40" s="182"/>
       <c r="C40" s="60" t="s">
         <v>107</v>
       </c>
@@ -10042,8 +10042,8 @@
       <c r="S40" s="26"/>
     </row>
     <row r="41" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="204"/>
-      <c r="B41" s="175"/>
+      <c r="A41" s="190"/>
+      <c r="B41" s="182"/>
       <c r="C41" s="60" t="s">
         <v>108</v>
       </c>
@@ -10086,8 +10086,8 @@
       <c r="T41" s="23"/>
     </row>
     <row r="42" spans="1:20" s="28" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="204"/>
-      <c r="B42" s="175"/>
+      <c r="A42" s="190"/>
+      <c r="B42" s="182"/>
       <c r="C42" s="61" t="s">
         <v>109</v>
       </c>
@@ -10135,8 +10135,8 @@
       <c r="S42" s="31"/>
     </row>
     <row r="43" spans="1:20" s="28" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="204"/>
-      <c r="B43" s="181" t="s">
+      <c r="A43" s="190"/>
+      <c r="B43" s="187" t="s">
         <v>193</v>
       </c>
       <c r="C43" s="63" t="s">
@@ -10184,8 +10184,8 @@
       <c r="S43" s="57"/>
     </row>
     <row r="44" spans="1:20" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="204"/>
-      <c r="B44" s="182"/>
+      <c r="A44" s="190"/>
+      <c r="B44" s="177"/>
       <c r="C44" s="60" t="s">
         <v>217</v>
       </c>
@@ -10227,8 +10227,8 @@
       <c r="S44" s="26"/>
     </row>
     <row r="45" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="204"/>
-      <c r="B45" s="182"/>
+      <c r="A45" s="190"/>
+      <c r="B45" s="177"/>
       <c r="C45" s="60" t="s">
         <v>256</v>
       </c>
@@ -10270,8 +10270,8 @@
       <c r="S45" s="26"/>
     </row>
     <row r="46" spans="1:20" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="204"/>
-      <c r="B46" s="182"/>
+      <c r="A46" s="190"/>
+      <c r="B46" s="177"/>
       <c r="C46" s="60" t="s">
         <v>218</v>
       </c>
@@ -10313,8 +10313,8 @@
       <c r="S46" s="26"/>
     </row>
     <row r="47" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="204"/>
-      <c r="B47" s="182"/>
+      <c r="A47" s="190"/>
+      <c r="B47" s="177"/>
       <c r="C47" s="60" t="s">
         <v>487</v>
       </c>
@@ -10361,8 +10361,8 @@
       <c r="T47" s="28"/>
     </row>
     <row r="48" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="204"/>
-      <c r="B48" s="182"/>
+      <c r="A48" s="190"/>
+      <c r="B48" s="177"/>
       <c r="C48" s="60" t="s">
         <v>410</v>
       </c>
@@ -10406,8 +10406,8 @@
       <c r="S48" s="26"/>
     </row>
     <row r="49" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="204"/>
-      <c r="B49" s="182"/>
+      <c r="A49" s="190"/>
+      <c r="B49" s="177"/>
       <c r="C49" s="60" t="s">
         <v>407</v>
       </c>
@@ -10451,8 +10451,8 @@
       <c r="S49" s="26"/>
     </row>
     <row r="50" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="204"/>
-      <c r="B50" s="182"/>
+      <c r="A50" s="190"/>
+      <c r="B50" s="177"/>
       <c r="C50" s="60" t="s">
         <v>405</v>
       </c>
@@ -10500,8 +10500,8 @@
       <c r="S50" s="26"/>
     </row>
     <row r="51" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="204"/>
-      <c r="B51" s="182"/>
+      <c r="A51" s="190"/>
+      <c r="B51" s="177"/>
       <c r="C51" s="60" t="s">
         <v>255</v>
       </c>
@@ -10547,8 +10547,8 @@
       <c r="S51" s="26"/>
     </row>
     <row r="52" spans="1:20" s="50" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="205"/>
-      <c r="B52" s="187"/>
+      <c r="A52" s="191"/>
+      <c r="B52" s="178"/>
       <c r="C52" s="65" t="s">
         <v>528</v>
       </c>
@@ -10592,10 +10592,10 @@
       <c r="S52" s="26"/>
     </row>
     <row r="53" spans="1:20" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="176" t="s">
+      <c r="A53" s="193" t="s">
         <v>89</v>
       </c>
-      <c r="B53" s="174" t="s">
+      <c r="B53" s="184" t="s">
         <v>51</v>
       </c>
       <c r="C53" s="62" t="s">
@@ -10642,8 +10642,8 @@
       <c r="T53" s="33"/>
     </row>
     <row r="54" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="177"/>
-      <c r="B54" s="175"/>
+      <c r="A54" s="194"/>
+      <c r="B54" s="182"/>
       <c r="C54" s="60" t="s">
         <v>66</v>
       </c>
@@ -10689,8 +10689,8 @@
       <c r="S54" s="26"/>
     </row>
     <row r="55" spans="1:20" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="177"/>
-      <c r="B55" s="175"/>
+      <c r="A55" s="194"/>
+      <c r="B55" s="182"/>
       <c r="C55" s="60" t="s">
         <v>67</v>
       </c>
@@ -10736,8 +10736,8 @@
       <c r="S55" s="26"/>
     </row>
     <row r="56" spans="1:20" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="177"/>
-      <c r="B56" s="175"/>
+      <c r="A56" s="194"/>
+      <c r="B56" s="182"/>
       <c r="C56" s="61" t="s">
         <v>68</v>
       </c>
@@ -10783,8 +10783,8 @@
       <c r="S56" s="26"/>
     </row>
     <row r="57" spans="1:20" s="23" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="177"/>
-      <c r="B57" s="175"/>
+      <c r="A57" s="194"/>
+      <c r="B57" s="182"/>
       <c r="C57" s="65" t="s">
         <v>601</v>
       </c>
@@ -10828,8 +10828,8 @@
       <c r="S57" s="31"/>
     </row>
     <row r="58" spans="1:20" s="23" customFormat="1" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="177"/>
-      <c r="B58" s="181" t="s">
+      <c r="A58" s="194"/>
+      <c r="B58" s="187" t="s">
         <v>193</v>
       </c>
       <c r="C58" s="63" t="s">
@@ -10877,8 +10877,8 @@
       <c r="S58" s="57"/>
     </row>
     <row r="59" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="177"/>
-      <c r="B59" s="182"/>
+      <c r="A59" s="194"/>
+      <c r="B59" s="177"/>
       <c r="C59" s="60" t="s">
         <v>208</v>
       </c>
@@ -10926,8 +10926,8 @@
       <c r="S59" s="26"/>
     </row>
     <row r="60" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="177"/>
-      <c r="B60" s="182"/>
+      <c r="A60" s="194"/>
+      <c r="B60" s="177"/>
       <c r="C60" s="60" t="s">
         <v>202</v>
       </c>
@@ -10971,8 +10971,8 @@
       <c r="S60" s="26"/>
     </row>
     <row r="61" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="177"/>
-      <c r="B61" s="182"/>
+      <c r="A61" s="194"/>
+      <c r="B61" s="177"/>
       <c r="C61" s="60" t="s">
         <v>197</v>
       </c>
@@ -11018,8 +11018,8 @@
       <c r="S61" s="26"/>
     </row>
     <row r="62" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="177"/>
-      <c r="B62" s="182"/>
+      <c r="A62" s="194"/>
+      <c r="B62" s="177"/>
       <c r="C62" s="60" t="s">
         <v>198</v>
       </c>
@@ -11065,8 +11065,8 @@
       <c r="S62" s="26"/>
     </row>
     <row r="63" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="177"/>
-      <c r="B63" s="182"/>
+      <c r="A63" s="194"/>
+      <c r="B63" s="177"/>
       <c r="C63" s="60" t="s">
         <v>91</v>
       </c>
@@ -11112,8 +11112,8 @@
       <c r="S63" s="26"/>
     </row>
     <row r="64" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="177"/>
-      <c r="B64" s="182"/>
+      <c r="A64" s="194"/>
+      <c r="B64" s="177"/>
       <c r="C64" s="60" t="s">
         <v>412</v>
       </c>
@@ -11159,8 +11159,8 @@
       <c r="S64" s="26"/>
     </row>
     <row r="65" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="177"/>
-      <c r="B65" s="182"/>
+      <c r="A65" s="194"/>
+      <c r="B65" s="177"/>
       <c r="C65" s="60" t="s">
         <v>199</v>
       </c>
@@ -11208,8 +11208,8 @@
       <c r="S65" s="26"/>
     </row>
     <row r="66" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="177"/>
-      <c r="B66" s="182"/>
+      <c r="A66" s="194"/>
+      <c r="B66" s="177"/>
       <c r="C66" s="60" t="s">
         <v>426</v>
       </c>
@@ -11255,8 +11255,8 @@
       <c r="S66" s="26"/>
     </row>
     <row r="67" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="177"/>
-      <c r="B67" s="182"/>
+      <c r="A67" s="194"/>
+      <c r="B67" s="177"/>
       <c r="C67" s="60" t="s">
         <v>375</v>
       </c>
@@ -11303,8 +11303,8 @@
       <c r="T67" s="28"/>
     </row>
     <row r="68" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="177"/>
-      <c r="B68" s="182"/>
+      <c r="A68" s="194"/>
+      <c r="B68" s="177"/>
       <c r="C68" s="60" t="s">
         <v>391</v>
       </c>
@@ -11352,8 +11352,8 @@
       <c r="S68" s="26"/>
     </row>
     <row r="69" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="177"/>
-      <c r="B69" s="182"/>
+      <c r="A69" s="194"/>
+      <c r="B69" s="177"/>
       <c r="C69" s="60" t="s">
         <v>252</v>
       </c>
@@ -11402,8 +11402,8 @@
       <c r="T69" s="23"/>
     </row>
     <row r="70" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="177"/>
-      <c r="B70" s="182"/>
+      <c r="A70" s="194"/>
+      <c r="B70" s="177"/>
       <c r="C70" s="60" t="s">
         <v>429</v>
       </c>
@@ -11449,8 +11449,8 @@
       <c r="S70" s="26"/>
     </row>
     <row r="71" spans="1:20" s="33" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="177"/>
-      <c r="B71" s="182"/>
+      <c r="A71" s="194"/>
+      <c r="B71" s="177"/>
       <c r="C71" s="61" t="s">
         <v>203</v>
       </c>
@@ -11495,10 +11495,10 @@
       <c r="T71" s="28"/>
     </row>
     <row r="72" spans="1:20" s="23" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="189" t="s">
+      <c r="A72" s="203" t="s">
         <v>97</v>
       </c>
-      <c r="B72" s="188"/>
+      <c r="B72" s="202"/>
       <c r="C72" s="62" t="s">
         <v>79</v>
       </c>
@@ -11545,8 +11545,8 @@
       <c r="T72" s="33"/>
     </row>
     <row r="73" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="190"/>
-      <c r="B73" s="175"/>
+      <c r="A73" s="204"/>
+      <c r="B73" s="182"/>
       <c r="C73" s="60" t="s">
         <v>80</v>
       </c>
@@ -11592,8 +11592,8 @@
       <c r="S73" s="26"/>
     </row>
     <row r="74" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="190"/>
-      <c r="B74" s="175"/>
+      <c r="A74" s="204"/>
+      <c r="B74" s="182"/>
       <c r="C74" s="60" t="s">
         <v>81</v>
       </c>
@@ -11641,8 +11641,8 @@
       <c r="S74" s="26"/>
     </row>
     <row r="75" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="190"/>
-      <c r="B75" s="175"/>
+      <c r="A75" s="204"/>
+      <c r="B75" s="182"/>
       <c r="C75" s="60" t="s">
         <v>82</v>
       </c>
@@ -11688,8 +11688,8 @@
       <c r="S75" s="26"/>
     </row>
     <row r="76" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="190"/>
-      <c r="B76" s="175"/>
+      <c r="A76" s="204"/>
+      <c r="B76" s="182"/>
       <c r="C76" s="60" t="s">
         <v>83</v>
       </c>
@@ -11737,8 +11737,8 @@
       <c r="S76" s="26"/>
     </row>
     <row r="77" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="190"/>
-      <c r="B77" s="175"/>
+      <c r="A77" s="204"/>
+      <c r="B77" s="182"/>
       <c r="C77" s="60" t="s">
         <v>84</v>
       </c>
@@ -11784,8 +11784,8 @@
       <c r="S77" s="26"/>
     </row>
     <row r="78" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="190"/>
-      <c r="B78" s="175"/>
+      <c r="A78" s="204"/>
+      <c r="B78" s="182"/>
       <c r="C78" s="60" t="s">
         <v>85</v>
       </c>
@@ -11829,8 +11829,8 @@
       <c r="S78" s="26"/>
     </row>
     <row r="79" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="190"/>
-      <c r="B79" s="175"/>
+      <c r="A79" s="204"/>
+      <c r="B79" s="182"/>
       <c r="C79" s="60" t="s">
         <v>86</v>
       </c>
@@ -11876,8 +11876,8 @@
       <c r="S79" s="26"/>
     </row>
     <row r="80" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="190"/>
-      <c r="B80" s="175"/>
+      <c r="A80" s="204"/>
+      <c r="B80" s="182"/>
       <c r="C80" s="60" t="s">
         <v>87</v>
       </c>
@@ -11925,8 +11925,8 @@
       <c r="S80" s="26"/>
     </row>
     <row r="81" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="190"/>
-      <c r="B81" s="175"/>
+      <c r="A81" s="204"/>
+      <c r="B81" s="182"/>
       <c r="C81" s="60" t="s">
         <v>223</v>
       </c>
@@ -11972,8 +11972,8 @@
       <c r="S81" s="26"/>
     </row>
     <row r="82" spans="1:19" s="23" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="190"/>
-      <c r="B82" s="186"/>
+      <c r="A82" s="204"/>
+      <c r="B82" s="201"/>
       <c r="C82" s="61" t="s">
         <v>90</v>
       </c>
@@ -12019,8 +12019,8 @@
       <c r="S82" s="31"/>
     </row>
     <row r="83" spans="1:19" s="23" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="190"/>
-      <c r="B83" s="182" t="s">
+      <c r="A83" s="204"/>
+      <c r="B83" s="177" t="s">
         <v>193</v>
       </c>
       <c r="C83" s="63" t="s">
@@ -12068,8 +12068,8 @@
       <c r="S83" s="57"/>
     </row>
     <row r="84" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="190"/>
-      <c r="B84" s="182"/>
+      <c r="A84" s="204"/>
+      <c r="B84" s="177"/>
       <c r="C84" s="60" t="s">
         <v>212</v>
       </c>
@@ -12115,8 +12115,8 @@
       <c r="S84" s="26"/>
     </row>
     <row r="85" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="190"/>
-      <c r="B85" s="182"/>
+      <c r="A85" s="204"/>
+      <c r="B85" s="177"/>
       <c r="C85" s="60" t="s">
         <v>424</v>
       </c>
@@ -12160,8 +12160,8 @@
       <c r="S85" s="26"/>
     </row>
     <row r="86" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="190"/>
-      <c r="B86" s="182"/>
+      <c r="A86" s="204"/>
+      <c r="B86" s="177"/>
       <c r="C86" s="60" t="s">
         <v>293</v>
       </c>
@@ -12207,8 +12207,8 @@
       <c r="S86" s="26"/>
     </row>
     <row r="87" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="190"/>
-      <c r="B87" s="182"/>
+      <c r="A87" s="204"/>
+      <c r="B87" s="177"/>
       <c r="C87" s="60" t="s">
         <v>366</v>
       </c>
@@ -12254,8 +12254,8 @@
       <c r="S87" s="26"/>
     </row>
     <row r="88" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="190"/>
-      <c r="B88" s="182"/>
+      <c r="A88" s="204"/>
+      <c r="B88" s="177"/>
       <c r="C88" s="60" t="s">
         <v>219</v>
       </c>
@@ -12299,8 +12299,8 @@
       <c r="S88" s="26"/>
     </row>
     <row r="89" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="190"/>
-      <c r="B89" s="182"/>
+      <c r="A89" s="204"/>
+      <c r="B89" s="177"/>
       <c r="C89" s="60" t="s">
         <v>320</v>
       </c>
@@ -12346,8 +12346,8 @@
       <c r="S89" s="26"/>
     </row>
     <row r="90" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="190"/>
-      <c r="B90" s="182"/>
+      <c r="A90" s="204"/>
+      <c r="B90" s="177"/>
       <c r="C90" s="61" t="s">
         <v>247</v>
       </c>
@@ -12393,8 +12393,8 @@
       <c r="S90" s="26"/>
     </row>
     <row r="91" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="190"/>
-      <c r="B91" s="182"/>
+      <c r="A91" s="204"/>
+      <c r="B91" s="177"/>
       <c r="C91" s="60" t="s">
         <v>401</v>
       </c>
@@ -12440,8 +12440,8 @@
       <c r="S91" s="26"/>
     </row>
     <row r="92" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="190"/>
-      <c r="B92" s="182"/>
+      <c r="A92" s="204"/>
+      <c r="B92" s="177"/>
       <c r="C92" s="65" t="s">
         <v>692</v>
       </c>
@@ -12473,8 +12473,8 @@
       <c r="S92" s="26"/>
     </row>
     <row r="93" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="190"/>
-      <c r="B93" s="182"/>
+      <c r="A93" s="204"/>
+      <c r="B93" s="177"/>
       <c r="C93" s="60" t="s">
         <v>368</v>
       </c>
@@ -12518,8 +12518,8 @@
       <c r="S93" s="26"/>
     </row>
     <row r="94" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="190"/>
-      <c r="B94" s="182"/>
+      <c r="A94" s="204"/>
+      <c r="B94" s="177"/>
       <c r="C94" s="60" t="s">
         <v>355</v>
       </c>
@@ -12565,8 +12565,8 @@
       <c r="S94" s="26"/>
     </row>
     <row r="95" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="190"/>
-      <c r="B95" s="182"/>
+      <c r="A95" s="204"/>
+      <c r="B95" s="177"/>
       <c r="C95" s="60" t="s">
         <v>351</v>
       </c>
@@ -12612,8 +12612,8 @@
       <c r="S95" s="26"/>
     </row>
     <row r="96" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="190"/>
-      <c r="B96" s="182"/>
+      <c r="A96" s="204"/>
+      <c r="B96" s="177"/>
       <c r="C96" s="60" t="s">
         <v>211</v>
       </c>
@@ -12661,8 +12661,8 @@
       <c r="S96" s="26"/>
     </row>
     <row r="97" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="190"/>
-      <c r="B97" s="182"/>
+      <c r="A97" s="204"/>
+      <c r="B97" s="177"/>
       <c r="C97" s="60" t="s">
         <v>371</v>
       </c>
@@ -12708,8 +12708,8 @@
       <c r="S97" s="26"/>
     </row>
     <row r="98" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="190"/>
-      <c r="B98" s="182"/>
+      <c r="A98" s="204"/>
+      <c r="B98" s="177"/>
       <c r="C98" s="60" t="s">
         <v>220</v>
       </c>
@@ -12755,8 +12755,8 @@
       <c r="S98" s="26"/>
     </row>
     <row r="99" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="190"/>
-      <c r="B99" s="182"/>
+      <c r="A99" s="204"/>
+      <c r="B99" s="177"/>
       <c r="C99" s="60" t="s">
         <v>245</v>
       </c>
@@ -12800,8 +12800,8 @@
       <c r="S99" s="26"/>
     </row>
     <row r="100" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="190"/>
-      <c r="B100" s="182"/>
+      <c r="A100" s="204"/>
+      <c r="B100" s="177"/>
       <c r="C100" s="60" t="s">
         <v>292</v>
       </c>
@@ -12845,8 +12845,8 @@
       <c r="S100" s="26"/>
     </row>
     <row r="101" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="190"/>
-      <c r="B101" s="182"/>
+      <c r="A101" s="204"/>
+      <c r="B101" s="177"/>
       <c r="C101" s="60" t="s">
         <v>222</v>
       </c>
@@ -12892,8 +12892,8 @@
       <c r="S101" s="26"/>
     </row>
     <row r="102" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="190"/>
-      <c r="B102" s="182"/>
+      <c r="A102" s="204"/>
+      <c r="B102" s="177"/>
       <c r="C102" s="60" t="s">
         <v>697</v>
       </c>
@@ -12937,8 +12937,8 @@
       <c r="S102" s="26"/>
     </row>
     <row r="103" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="190"/>
-      <c r="B103" s="182"/>
+      <c r="A103" s="204"/>
+      <c r="B103" s="177"/>
       <c r="C103" s="60" t="s">
         <v>230</v>
       </c>
@@ -12980,8 +12980,8 @@
       <c r="S103" s="26"/>
     </row>
     <row r="104" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="190"/>
-      <c r="B104" s="182"/>
+      <c r="A104" s="204"/>
+      <c r="B104" s="177"/>
       <c r="C104" s="60" t="s">
         <v>221</v>
       </c>
@@ -13027,8 +13027,8 @@
       <c r="S104" s="26"/>
     </row>
     <row r="105" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="190"/>
-      <c r="B105" s="182"/>
+      <c r="A105" s="204"/>
+      <c r="B105" s="177"/>
       <c r="C105" s="65" t="s">
         <v>216</v>
       </c>
@@ -13074,8 +13074,8 @@
       <c r="S105" s="26"/>
     </row>
     <row r="106" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="190"/>
-      <c r="B106" s="182"/>
+      <c r="A106" s="204"/>
+      <c r="B106" s="177"/>
       <c r="C106" s="60" t="s">
         <v>213</v>
       </c>
@@ -13121,8 +13121,8 @@
       <c r="S106" s="26"/>
     </row>
     <row r="107" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="190"/>
-      <c r="B107" s="182"/>
+      <c r="A107" s="204"/>
+      <c r="B107" s="177"/>
       <c r="C107" s="60" t="s">
         <v>214</v>
       </c>
@@ -13168,8 +13168,8 @@
       <c r="S107" s="26"/>
     </row>
     <row r="108" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="190"/>
-      <c r="B108" s="182"/>
+      <c r="A108" s="204"/>
+      <c r="B108" s="177"/>
       <c r="C108" s="60" t="s">
         <v>357</v>
       </c>
@@ -13215,8 +13215,8 @@
       <c r="S108" s="26"/>
     </row>
     <row r="109" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="190"/>
-      <c r="B109" s="182"/>
+      <c r="A109" s="204"/>
+      <c r="B109" s="177"/>
       <c r="C109" s="60" t="s">
         <v>229</v>
       </c>
@@ -13262,8 +13262,8 @@
       <c r="S109" s="26"/>
     </row>
     <row r="110" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="190"/>
-      <c r="B110" s="182"/>
+      <c r="A110" s="204"/>
+      <c r="B110" s="177"/>
       <c r="C110" s="60" t="s">
         <v>205</v>
       </c>
@@ -13309,8 +13309,8 @@
       <c r="S110" s="26"/>
     </row>
     <row r="111" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="190"/>
-      <c r="B111" s="182"/>
+      <c r="A111" s="204"/>
+      <c r="B111" s="177"/>
       <c r="C111" s="60" t="s">
         <v>206</v>
       </c>
@@ -13356,8 +13356,8 @@
       <c r="S111" s="26"/>
     </row>
     <row r="112" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="190"/>
-      <c r="B112" s="182"/>
+      <c r="A112" s="204"/>
+      <c r="B112" s="177"/>
       <c r="C112" s="60" t="s">
         <v>499</v>
       </c>
@@ -13403,8 +13403,8 @@
       <c r="S112" s="26"/>
     </row>
     <row r="113" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="190"/>
-      <c r="B113" s="182"/>
+      <c r="A113" s="204"/>
+      <c r="B113" s="177"/>
       <c r="C113" s="60" t="s">
         <v>246</v>
       </c>
@@ -13450,8 +13450,8 @@
       <c r="S113" s="26"/>
     </row>
     <row r="114" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="190"/>
-      <c r="B114" s="182"/>
+      <c r="A114" s="204"/>
+      <c r="B114" s="177"/>
       <c r="C114" s="60" t="s">
         <v>249</v>
       </c>
@@ -13495,8 +13495,8 @@
       <c r="S114" s="26"/>
     </row>
     <row r="115" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="190"/>
-      <c r="B115" s="182"/>
+      <c r="A115" s="204"/>
+      <c r="B115" s="177"/>
       <c r="C115" s="60" t="s">
         <v>226</v>
       </c>
@@ -13544,8 +13544,8 @@
       <c r="S115" s="26"/>
     </row>
     <row r="116" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="190"/>
-      <c r="B116" s="182"/>
+      <c r="A116" s="204"/>
+      <c r="B116" s="177"/>
       <c r="C116" s="60" t="s">
         <v>227</v>
       </c>
@@ -13593,8 +13593,8 @@
       <c r="S116" s="26"/>
     </row>
     <row r="117" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="190"/>
-      <c r="B117" s="182"/>
+      <c r="A117" s="204"/>
+      <c r="B117" s="177"/>
       <c r="C117" s="65" t="s">
         <v>595</v>
       </c>
@@ -13621,8 +13621,8 @@
       <c r="T117" s="23"/>
     </row>
     <row r="118" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="190"/>
-      <c r="B118" s="182"/>
+      <c r="A118" s="204"/>
+      <c r="B118" s="177"/>
       <c r="C118" s="60" t="s">
         <v>323</v>
       </c>
@@ -13669,8 +13669,8 @@
       <c r="T118" s="23"/>
     </row>
     <row r="119" spans="1:20" s="33" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="191"/>
-      <c r="B119" s="187"/>
+      <c r="A119" s="205"/>
+      <c r="B119" s="178"/>
       <c r="C119" s="61" t="s">
         <v>316</v>
       </c>
@@ -13723,10 +13723,10 @@
       <c r="T119" s="28"/>
     </row>
     <row r="120" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="183" t="s">
+      <c r="A120" s="198" t="s">
         <v>497</v>
       </c>
-      <c r="B120" s="174" t="s">
+      <c r="B120" s="184" t="s">
         <v>51</v>
       </c>
       <c r="C120" s="62" t="s">
@@ -13771,8 +13771,8 @@
       <c r="T120" s="33"/>
     </row>
     <row r="121" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="184"/>
-      <c r="B121" s="175"/>
+      <c r="A121" s="199"/>
+      <c r="B121" s="182"/>
       <c r="C121" s="60" t="s">
         <v>92</v>
       </c>
@@ -13818,8 +13818,8 @@
       <c r="S121" s="26"/>
     </row>
     <row r="122" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="184"/>
-      <c r="B122" s="175"/>
+      <c r="A122" s="199"/>
+      <c r="B122" s="182"/>
       <c r="C122" s="60" t="s">
         <v>93</v>
       </c>
@@ -13865,8 +13865,8 @@
       <c r="S122" s="26"/>
     </row>
     <row r="123" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="184"/>
-      <c r="B123" s="175"/>
+      <c r="A123" s="199"/>
+      <c r="B123" s="182"/>
       <c r="C123" s="60" t="s">
         <v>104</v>
       </c>
@@ -13908,8 +13908,8 @@
       <c r="S123" s="26"/>
     </row>
     <row r="124" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="184"/>
-      <c r="B124" s="175"/>
+      <c r="A124" s="199"/>
+      <c r="B124" s="182"/>
       <c r="C124" s="61" t="s">
         <v>94</v>
       </c>
@@ -13952,8 +13952,8 @@
       <c r="T124" s="28"/>
     </row>
     <row r="125" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="184"/>
-      <c r="B125" s="175"/>
+      <c r="A125" s="199"/>
+      <c r="B125" s="182"/>
       <c r="C125" s="60" t="s">
         <v>179</v>
       </c>
@@ -13996,8 +13996,8 @@
       <c r="T125" s="28"/>
     </row>
     <row r="126" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="184"/>
-      <c r="B126" s="175"/>
+      <c r="A126" s="199"/>
+      <c r="B126" s="182"/>
       <c r="C126" s="61" t="s">
         <v>116</v>
       </c>
@@ -14040,8 +14040,8 @@
       <c r="T126" s="28"/>
     </row>
     <row r="127" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="184"/>
-      <c r="B127" s="175"/>
+      <c r="A127" s="199"/>
+      <c r="B127" s="182"/>
       <c r="C127" s="60" t="s">
         <v>96</v>
       </c>
@@ -14085,8 +14085,8 @@
       <c r="S127" s="26"/>
     </row>
     <row r="128" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="184"/>
-      <c r="B128" s="175"/>
+      <c r="A128" s="199"/>
+      <c r="B128" s="182"/>
       <c r="C128" s="60" t="s">
         <v>498</v>
       </c>
@@ -14130,8 +14130,8 @@
       <c r="S128" s="26"/>
     </row>
     <row r="129" spans="1:20" s="23" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="184"/>
-      <c r="B129" s="186"/>
+      <c r="A129" s="199"/>
+      <c r="B129" s="201"/>
       <c r="C129" s="60" t="s">
         <v>176</v>
       </c>
@@ -14173,8 +14173,8 @@
       <c r="S129" s="26"/>
     </row>
     <row r="130" spans="1:20" s="28" customFormat="1" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="184"/>
-      <c r="B130" s="181" t="s">
+      <c r="A130" s="199"/>
+      <c r="B130" s="187" t="s">
         <v>193</v>
       </c>
       <c r="C130" s="63" t="s">
@@ -14221,8 +14221,8 @@
       <c r="T130" s="23"/>
     </row>
     <row r="131" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="184"/>
-      <c r="B131" s="182"/>
+      <c r="A131" s="199"/>
+      <c r="B131" s="177"/>
       <c r="C131" s="60" t="s">
         <v>445</v>
       </c>
@@ -14265,8 +14265,8 @@
       <c r="T131" s="23"/>
     </row>
     <row r="132" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="184"/>
-      <c r="B132" s="182"/>
+      <c r="A132" s="199"/>
+      <c r="B132" s="177"/>
       <c r="C132" s="60" t="s">
         <v>448</v>
       </c>
@@ -14309,8 +14309,8 @@
       <c r="T132" s="23"/>
     </row>
     <row r="133" spans="1:20" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="184"/>
-      <c r="B133" s="182"/>
+      <c r="A133" s="199"/>
+      <c r="B133" s="177"/>
       <c r="C133" s="61" t="s">
         <v>422</v>
       </c>
@@ -14355,8 +14355,8 @@
       <c r="T133" s="23"/>
     </row>
     <row r="134" spans="1:20" s="33" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="184"/>
-      <c r="B134" s="182"/>
+      <c r="A134" s="199"/>
+      <c r="B134" s="177"/>
       <c r="C134" s="60" t="s">
         <v>228</v>
       </c>
@@ -14399,8 +14399,8 @@
       <c r="T134" s="23"/>
     </row>
     <row r="135" spans="1:20" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="184"/>
-      <c r="B135" s="182"/>
+      <c r="A135" s="199"/>
+      <c r="B135" s="177"/>
       <c r="C135" s="60" t="s">
         <v>207</v>
       </c>
@@ -14443,8 +14443,8 @@
       <c r="T135" s="23"/>
     </row>
     <row r="136" spans="1:20" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="185"/>
-      <c r="B136" s="182"/>
+      <c r="A136" s="200"/>
+      <c r="B136" s="177"/>
       <c r="C136" s="65" t="s">
         <v>621</v>
       </c>
@@ -14467,10 +14467,10 @@
       <c r="T136" s="23"/>
     </row>
     <row r="137" spans="1:20" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="178" t="s">
+      <c r="A137" s="195" t="s">
         <v>111</v>
       </c>
-      <c r="B137" s="174" t="s">
+      <c r="B137" s="184" t="s">
         <v>51</v>
       </c>
       <c r="C137" s="62" t="s">
@@ -14513,8 +14513,8 @@
       <c r="T137" s="33"/>
     </row>
     <row r="138" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="179"/>
-      <c r="B138" s="175"/>
+      <c r="A138" s="196"/>
+      <c r="B138" s="182"/>
       <c r="C138" s="61" t="s">
         <v>95</v>
       </c>
@@ -14554,8 +14554,8 @@
       <c r="S138" s="31"/>
     </row>
     <row r="139" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="179"/>
-      <c r="B139" s="175"/>
+      <c r="A139" s="196"/>
+      <c r="B139" s="182"/>
       <c r="C139" s="65" t="s">
         <v>599</v>
       </c>
@@ -14598,8 +14598,8 @@
       <c r="T139" s="19"/>
     </row>
     <row r="140" spans="1:20" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="179"/>
-      <c r="B140" s="175"/>
+      <c r="A140" s="196"/>
+      <c r="B140" s="182"/>
       <c r="C140" s="60" t="s">
         <v>115</v>
       </c>
@@ -14641,8 +14641,8 @@
       <c r="T140" s="19"/>
     </row>
     <row r="141" spans="1:20" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="179"/>
-      <c r="B141" s="175"/>
+      <c r="A141" s="196"/>
+      <c r="B141" s="182"/>
       <c r="C141" s="60" t="s">
         <v>114</v>
       </c>
@@ -14684,8 +14684,8 @@
       <c r="T141" s="19"/>
     </row>
     <row r="142" spans="1:20" s="23" customFormat="1" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="179"/>
-      <c r="B142" s="181" t="s">
+      <c r="A142" s="196"/>
+      <c r="B142" s="187" t="s">
         <v>193</v>
       </c>
       <c r="C142" s="63" t="s">
@@ -14727,8 +14727,8 @@
       <c r="S142" s="57"/>
     </row>
     <row r="143" spans="1:20" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="179"/>
-      <c r="B143" s="182"/>
+      <c r="A143" s="196"/>
+      <c r="B143" s="177"/>
       <c r="C143" s="60" t="s">
         <v>396</v>
       </c>
@@ -14767,8 +14767,8 @@
       <c r="S143" s="26"/>
     </row>
     <row r="144" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="179"/>
-      <c r="B144" s="182"/>
+      <c r="A144" s="196"/>
+      <c r="B144" s="177"/>
       <c r="C144" s="60" t="s">
         <v>253</v>
       </c>
@@ -14808,8 +14808,8 @@
       <c r="S144" s="26"/>
     </row>
     <row r="145" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="179"/>
-      <c r="B145" s="182"/>
+      <c r="A145" s="196"/>
+      <c r="B145" s="177"/>
       <c r="C145" s="65" t="s">
         <v>615</v>
       </c>
@@ -14843,8 +14843,8 @@
       <c r="S145" s="26"/>
     </row>
     <row r="146" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="179"/>
-      <c r="B146" s="182"/>
+      <c r="A146" s="196"/>
+      <c r="B146" s="177"/>
       <c r="C146" s="60" t="s">
         <v>419</v>
       </c>
@@ -14884,8 +14884,8 @@
       <c r="S146" s="26"/>
     </row>
     <row r="147" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="179"/>
-      <c r="B147" s="182"/>
+      <c r="A147" s="196"/>
+      <c r="B147" s="177"/>
       <c r="C147" s="60" t="s">
         <v>378</v>
       </c>
@@ -14923,8 +14923,8 @@
       <c r="S147" s="26"/>
     </row>
     <row r="148" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="179"/>
-      <c r="B148" s="182"/>
+      <c r="A148" s="196"/>
+      <c r="B148" s="177"/>
       <c r="C148" s="60" t="s">
         <v>436</v>
       </c>
@@ -14964,8 +14964,8 @@
       <c r="S148" s="26"/>
     </row>
     <row r="149" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="179"/>
-      <c r="B149" s="182"/>
+      <c r="A149" s="196"/>
+      <c r="B149" s="177"/>
       <c r="C149" s="60" t="s">
         <v>356</v>
       </c>
@@ -15005,8 +15005,8 @@
       <c r="S149" s="26"/>
     </row>
     <row r="150" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="179"/>
-      <c r="B150" s="182"/>
+      <c r="A150" s="196"/>
+      <c r="B150" s="177"/>
       <c r="C150" s="60" t="s">
         <v>224</v>
       </c>
@@ -15048,8 +15048,8 @@
       <c r="S150" s="26"/>
     </row>
     <row r="151" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="179"/>
-      <c r="B151" s="182"/>
+      <c r="A151" s="196"/>
+      <c r="B151" s="177"/>
       <c r="C151" s="60" t="s">
         <v>418</v>
       </c>
@@ -15089,8 +15089,8 @@
       <c r="S151" s="26"/>
     </row>
     <row r="152" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="179"/>
-      <c r="B152" s="182"/>
+      <c r="A152" s="196"/>
+      <c r="B152" s="177"/>
       <c r="C152" s="60" t="s">
         <v>393</v>
       </c>
@@ -15130,8 +15130,8 @@
       <c r="S152" s="26"/>
     </row>
     <row r="153" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="179"/>
-      <c r="B153" s="182"/>
+      <c r="A153" s="196"/>
+      <c r="B153" s="177"/>
       <c r="C153" s="60" t="s">
         <v>430</v>
       </c>
@@ -15171,8 +15171,8 @@
       <c r="S153" s="26"/>
     </row>
     <row r="154" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="179"/>
-      <c r="B154" s="182"/>
+      <c r="A154" s="196"/>
+      <c r="B154" s="177"/>
       <c r="C154" s="60" t="s">
         <v>403</v>
       </c>
@@ -15212,8 +15212,8 @@
       <c r="S154" s="26"/>
     </row>
     <row r="155" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="179"/>
-      <c r="B155" s="182"/>
+      <c r="A155" s="196"/>
+      <c r="B155" s="177"/>
       <c r="C155" s="65" t="s">
         <v>518</v>
       </c>
@@ -15255,8 +15255,8 @@
       <c r="S155" s="26"/>
     </row>
     <row r="156" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="179"/>
-      <c r="B156" s="182"/>
+      <c r="A156" s="196"/>
+      <c r="B156" s="177"/>
       <c r="C156" s="65" t="s">
         <v>254</v>
       </c>
@@ -15296,8 +15296,8 @@
       <c r="S156" s="26"/>
     </row>
     <row r="157" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="179"/>
-      <c r="B157" s="182"/>
+      <c r="A157" s="196"/>
+      <c r="B157" s="177"/>
       <c r="C157" s="65" t="s">
         <v>443</v>
       </c>
@@ -15337,8 +15337,8 @@
       <c r="S157" s="26"/>
     </row>
     <row r="158" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="179"/>
-      <c r="B158" s="182"/>
+      <c r="A158" s="196"/>
+      <c r="B158" s="177"/>
       <c r="C158" s="65" t="s">
         <v>432</v>
       </c>
@@ -15378,8 +15378,8 @@
       <c r="S158" s="26"/>
     </row>
     <row r="159" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="179"/>
-      <c r="B159" s="182"/>
+      <c r="A159" s="196"/>
+      <c r="B159" s="177"/>
       <c r="C159" s="65" t="s">
         <v>317</v>
       </c>
@@ -15421,8 +15421,8 @@
       <c r="S159" s="26"/>
     </row>
     <row r="160" spans="1:19" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="179"/>
-      <c r="B160" s="182"/>
+      <c r="A160" s="196"/>
+      <c r="B160" s="177"/>
       <c r="C160" s="65" t="s">
         <v>364</v>
       </c>
@@ -15464,8 +15464,8 @@
       <c r="S160" s="26"/>
     </row>
     <row r="161" spans="1:19" s="23" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A161" s="180"/>
-      <c r="B161" s="182"/>
+      <c r="A161" s="197"/>
+      <c r="B161" s="177"/>
       <c r="C161" s="65" t="s">
         <v>210</v>
       </c>
@@ -15505,10 +15505,10 @@
       <c r="S161" s="31"/>
     </row>
     <row r="162" spans="1:19" s="33" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A162" s="200" t="s">
+      <c r="A162" s="185" t="s">
         <v>112</v>
       </c>
-      <c r="B162" s="195" t="s">
+      <c r="B162" s="176" t="s">
         <v>193</v>
       </c>
       <c r="C162" s="62" t="s">
@@ -15554,8 +15554,8 @@
       <c r="S162" s="36"/>
     </row>
     <row r="163" spans="1:19" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A163" s="200"/>
-      <c r="B163" s="182"/>
+      <c r="A163" s="185"/>
+      <c r="B163" s="177"/>
       <c r="C163" s="60" t="s">
         <v>360</v>
       </c>
@@ -15597,8 +15597,8 @@
       <c r="S163" s="26"/>
     </row>
     <row r="164" spans="1:19" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A164" s="200"/>
-      <c r="B164" s="182"/>
+      <c r="A164" s="185"/>
+      <c r="B164" s="177"/>
       <c r="C164" s="60" t="s">
         <v>379</v>
       </c>
@@ -15642,8 +15642,8 @@
       <c r="S164" s="26"/>
     </row>
     <row r="165" spans="1:19" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A165" s="200"/>
-      <c r="B165" s="182"/>
+      <c r="A165" s="185"/>
+      <c r="B165" s="177"/>
       <c r="C165" s="60" t="s">
         <v>389</v>
       </c>
@@ -15687,8 +15687,8 @@
       <c r="S165" s="26"/>
     </row>
     <row r="166" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A166" s="200"/>
-      <c r="B166" s="182"/>
+      <c r="A166" s="185"/>
+      <c r="B166" s="177"/>
       <c r="C166" s="60" t="s">
         <v>248</v>
       </c>
@@ -15730,8 +15730,8 @@
       <c r="S166" s="26"/>
     </row>
     <row r="167" spans="1:19" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A167" s="200"/>
-      <c r="B167" s="182"/>
+      <c r="A167" s="185"/>
+      <c r="B167" s="177"/>
       <c r="C167" s="61" t="s">
         <v>398</v>
       </c>
@@ -15775,8 +15775,8 @@
       <c r="S167" s="26"/>
     </row>
     <row r="168" spans="1:19" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A168" s="200"/>
-      <c r="B168" s="182"/>
+      <c r="A168" s="185"/>
+      <c r="B168" s="177"/>
       <c r="C168" s="60" t="s">
         <v>370</v>
       </c>
@@ -15818,8 +15818,8 @@
       <c r="S168" s="26"/>
     </row>
     <row r="169" spans="1:19" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="200"/>
-      <c r="B169" s="187"/>
+      <c r="A169" s="185"/>
+      <c r="B169" s="178"/>
       <c r="C169" s="60" t="s">
         <v>399</v>
       </c>
@@ -15861,7 +15861,7 @@
       <c r="S169" s="31"/>
     </row>
     <row r="170" spans="1:19" s="33" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A170" s="201" t="s">
+      <c r="A170" s="186" t="s">
         <v>532</v>
       </c>
       <c r="B170" s="72" t="s">
@@ -15904,8 +15904,8 @@
       <c r="S170" s="71"/>
     </row>
     <row r="171" spans="1:19" s="23" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A171" s="201"/>
-      <c r="B171" s="181" t="s">
+      <c r="A171" s="186"/>
+      <c r="B171" s="187" t="s">
         <v>193</v>
       </c>
       <c r="C171" s="60" t="s">
@@ -15943,8 +15943,8 @@
       <c r="S171" s="57"/>
     </row>
     <row r="172" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A172" s="201"/>
-      <c r="B172" s="182"/>
+      <c r="A172" s="186"/>
+      <c r="B172" s="177"/>
       <c r="C172" s="60" t="s">
         <v>195</v>
       </c>
@@ -15979,8 +15979,8 @@
       <c r="S172" s="26"/>
     </row>
     <row r="173" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A173" s="201"/>
-      <c r="B173" s="182"/>
+      <c r="A173" s="186"/>
+      <c r="B173" s="177"/>
       <c r="C173" s="60" t="s">
         <v>257</v>
       </c>
@@ -16020,8 +16020,8 @@
       <c r="S173" s="26"/>
     </row>
     <row r="174" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A174" s="201"/>
-      <c r="B174" s="182"/>
+      <c r="A174" s="186"/>
+      <c r="B174" s="177"/>
       <c r="C174" s="60" t="s">
         <v>414</v>
       </c>
@@ -16058,8 +16058,8 @@
       <c r="S174" s="26"/>
     </row>
     <row r="175" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A175" s="201"/>
-      <c r="B175" s="202"/>
+      <c r="A175" s="186"/>
+      <c r="B175" s="188"/>
       <c r="C175" s="60" t="s">
         <v>415</v>
       </c>
@@ -16097,10 +16097,10 @@
       <c r="S175" s="26"/>
     </row>
     <row r="176" spans="1:19" s="33" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A176" s="194" t="s">
+      <c r="A176" s="175" t="s">
         <v>113</v>
       </c>
-      <c r="B176" s="198" t="s">
+      <c r="B176" s="181" t="s">
         <v>51</v>
       </c>
       <c r="C176" s="62" t="s">
@@ -16140,8 +16140,8 @@
       <c r="S176" s="36"/>
     </row>
     <row r="177" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A177" s="194"/>
-      <c r="B177" s="175"/>
+      <c r="A177" s="175"/>
+      <c r="B177" s="182"/>
       <c r="C177" s="60" t="s">
         <v>184</v>
       </c>
@@ -16179,8 +16179,8 @@
       <c r="S177" s="26"/>
     </row>
     <row r="178" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A178" s="194"/>
-      <c r="B178" s="175"/>
+      <c r="A178" s="175"/>
+      <c r="B178" s="182"/>
       <c r="C178" s="60" t="s">
         <v>183</v>
       </c>
@@ -16218,8 +16218,8 @@
       <c r="S178" s="26"/>
     </row>
     <row r="179" spans="1:19" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A179" s="194"/>
-      <c r="B179" s="175"/>
+      <c r="A179" s="175"/>
+      <c r="B179" s="182"/>
       <c r="C179" s="61" t="s">
         <v>185</v>
       </c>
@@ -16257,8 +16257,8 @@
       <c r="S179" s="31"/>
     </row>
     <row r="180" spans="1:19" s="23" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A180" s="194"/>
-      <c r="B180" s="192" t="s">
+      <c r="A180" s="175"/>
+      <c r="B180" s="173" t="s">
         <v>193</v>
       </c>
       <c r="C180" s="63" t="s">
@@ -16292,8 +16292,8 @@
       <c r="S180" s="57"/>
     </row>
     <row r="181" spans="1:19" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A181" s="194"/>
-      <c r="B181" s="193"/>
+      <c r="A181" s="175"/>
+      <c r="B181" s="174"/>
       <c r="C181" s="64"/>
       <c r="E181" s="49"/>
       <c r="F181" s="49"/>
@@ -17022,6 +17022,18 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="C3:S3"/>
+    <mergeCell ref="B53:B57"/>
+    <mergeCell ref="A53:A71"/>
+    <mergeCell ref="A137:A161"/>
+    <mergeCell ref="B142:B161"/>
+    <mergeCell ref="A120:A136"/>
+    <mergeCell ref="B120:B129"/>
+    <mergeCell ref="B83:B119"/>
+    <mergeCell ref="B58:B71"/>
+    <mergeCell ref="B72:B82"/>
+    <mergeCell ref="A72:A119"/>
+    <mergeCell ref="B137:B141"/>
     <mergeCell ref="B180:B181"/>
     <mergeCell ref="A176:A181"/>
     <mergeCell ref="B162:B169"/>
@@ -17037,18 +17049,6 @@
     <mergeCell ref="B130:B136"/>
     <mergeCell ref="A39:A52"/>
     <mergeCell ref="B43:B52"/>
-    <mergeCell ref="C3:S3"/>
-    <mergeCell ref="B53:B57"/>
-    <mergeCell ref="A53:A71"/>
-    <mergeCell ref="A137:A161"/>
-    <mergeCell ref="B142:B161"/>
-    <mergeCell ref="A120:A136"/>
-    <mergeCell ref="B120:B129"/>
-    <mergeCell ref="B83:B119"/>
-    <mergeCell ref="B58:B71"/>
-    <mergeCell ref="B72:B82"/>
-    <mergeCell ref="A72:A119"/>
-    <mergeCell ref="B137:B141"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>